<commit_message>
updated to the new unity System
- fixed some bugs in unity
</commit_message>
<xml_diff>
--- a/Zeitaufzeichnung_Ishjarta.xlsx
+++ b/Zeitaufzeichnung_Ishjarta.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danijel\Desktop\ishjarta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF57E6C9-3755-447E-A44E-6584FB2753ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73533DB8-503D-4ECF-B60D-15C371455013}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15180" yWindow="940" windowWidth="23220" windowHeight="20060" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vorlage" sheetId="8" r:id="rId1"/>
@@ -336,7 +336,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>Minimap</t>
+      <t>Minimap, auf das neue Unity Input System wechseln.</t>
     </r>
   </si>
 </sst>
@@ -1308,11 +1308,29 @@
     <xf numFmtId="165" fontId="1" fillId="32" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="10" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="10" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="2" borderId="20" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="10" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1326,6 +1344,27 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="10" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1338,36 +1377,6 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="6" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="2" borderId="20" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="10" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1380,20 +1389,11 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="10" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="10" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="1" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
@@ -1422,6 +1422,45 @@
     <xf numFmtId="165" fontId="1" fillId="6" borderId="7" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="6" borderId="8" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="6" borderId="1" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="5" borderId="13" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="5" borderId="3" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="5" borderId="14" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="6" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="6" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="12" xfId="6" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="6" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="165" fontId="1" fillId="3" borderId="13" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1443,98 +1482,68 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="13" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="3" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="14" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="20" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="6" borderId="13" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="6" borderId="3" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="6" borderId="14" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="6" borderId="0" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="6" borderId="20" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="165" fontId="1" fillId="6" borderId="27" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="6" borderId="9" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="6" borderId="11" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="13" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="3" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="14" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="20" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="6" borderId="27" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="6" borderId="9" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="6" borderId="11" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="5" borderId="13" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="5" borderId="3" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="5" borderId="14" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="6" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="6" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="12" xfId="6" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="6" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="6" borderId="13" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="6" borderId="3" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="6" borderId="14" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="6" borderId="0" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="6" borderId="20" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="6" borderId="8" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="6" borderId="1" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1553,15 +1562,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -1974,7 +1974,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="154" t="s">
+      <c r="A1" s="153" t="s">
         <v>14</v>
       </c>
       <c r="B1" s="116" t="s">
@@ -2016,7 +2016,7 @@
       <c r="N1" s="42"/>
     </row>
     <row r="2" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="155"/>
+      <c r="A2" s="154"/>
       <c r="B2" s="124" t="s">
         <v>0</v>
       </c>
@@ -2064,63 +2064,63 @@
       <c r="N2" s="31"/>
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="146">
+      <c r="A3" s="141">
         <v>44571</v>
       </c>
       <c r="B3" s="10">
         <v>0.33333333333333331</v>
       </c>
-      <c r="C3" s="142" t="s">
+      <c r="C3" s="155" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="143"/>
+      <c r="D3" s="156"/>
       <c r="E3" s="11">
         <v>0.33333333333333331</v>
       </c>
-      <c r="F3" s="149" t="s">
+      <c r="F3" s="152" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="150"/>
+      <c r="G3" s="149"/>
       <c r="H3" s="12">
         <v>0.33333333333333331</v>
       </c>
-      <c r="I3" s="138" t="s">
+      <c r="I3" s="144" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="139"/>
+      <c r="J3" s="145"/>
       <c r="K3" s="33">
         <v>0.33333333333333331</v>
       </c>
-      <c r="L3" s="160" t="s">
+      <c r="L3" s="136" t="s">
         <v>26</v>
       </c>
-      <c r="M3" s="161"/>
+      <c r="M3" s="137"/>
     </row>
     <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="147"/>
+      <c r="A4" s="142"/>
       <c r="B4" s="14">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C4" s="144"/>
-      <c r="D4" s="145"/>
+      <c r="C4" s="157"/>
+      <c r="D4" s="158"/>
       <c r="E4" s="15">
         <v>0.41666666666666669</v>
       </c>
-      <c r="F4" s="151"/>
-      <c r="G4" s="152"/>
+      <c r="F4" s="150"/>
+      <c r="G4" s="151"/>
       <c r="H4" s="16">
         <v>0.41666666666666669</v>
       </c>
-      <c r="I4" s="140"/>
-      <c r="J4" s="141"/>
+      <c r="I4" s="146"/>
+      <c r="J4" s="147"/>
       <c r="K4" s="39">
         <v>0.41666666666666669</v>
       </c>
-      <c r="L4" s="162"/>
-      <c r="M4" s="163"/>
+      <c r="L4" s="138"/>
+      <c r="M4" s="139"/>
     </row>
     <row r="5" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="148"/>
+      <c r="A5" s="143"/>
       <c r="B5" s="97">
         <f>B4-B3</f>
         <v>8.333333333333337E-2</v>
@@ -2147,45 +2147,45 @@
       <c r="M5" s="105"/>
     </row>
     <row r="6" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="146"/>
+      <c r="A6" s="141"/>
       <c r="B6" s="10"/>
-      <c r="C6" s="142" t="s">
+      <c r="C6" s="155" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="157"/>
+      <c r="D6" s="160"/>
       <c r="E6" s="11"/>
-      <c r="F6" s="153" t="s">
+      <c r="F6" s="148" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="150"/>
+      <c r="G6" s="149"/>
       <c r="H6" s="12"/>
-      <c r="I6" s="138" t="s">
+      <c r="I6" s="144" t="s">
         <v>24</v>
       </c>
-      <c r="J6" s="139"/>
+      <c r="J6" s="145"/>
       <c r="K6" s="13"/>
-      <c r="L6" s="164" t="s">
+      <c r="L6" s="140" t="s">
         <v>11</v>
       </c>
-      <c r="M6" s="161"/>
+      <c r="M6" s="137"/>
     </row>
     <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="147"/>
+      <c r="A7" s="142"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="158"/>
-      <c r="D7" s="159"/>
+      <c r="C7" s="161"/>
+      <c r="D7" s="162"/>
       <c r="E7" s="15"/>
-      <c r="F7" s="151"/>
-      <c r="G7" s="152"/>
+      <c r="F7" s="150"/>
+      <c r="G7" s="151"/>
       <c r="H7" s="16"/>
-      <c r="I7" s="140"/>
-      <c r="J7" s="141"/>
+      <c r="I7" s="146"/>
+      <c r="J7" s="147"/>
       <c r="K7" s="39"/>
-      <c r="L7" s="162"/>
-      <c r="M7" s="163"/>
+      <c r="L7" s="138"/>
+      <c r="M7" s="139"/>
     </row>
     <row r="8" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="148"/>
+      <c r="A8" s="143"/>
       <c r="B8" s="97">
         <f>B7-B6</f>
         <v>0</v>
@@ -2212,45 +2212,45 @@
       <c r="M8" s="111"/>
     </row>
     <row r="9" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="146"/>
+      <c r="A9" s="141"/>
       <c r="B9" s="10"/>
-      <c r="C9" s="156" t="s">
+      <c r="C9" s="159" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="143"/>
+      <c r="D9" s="156"/>
       <c r="E9" s="11"/>
-      <c r="F9" s="153" t="s">
+      <c r="F9" s="148" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="150"/>
+      <c r="G9" s="149"/>
       <c r="H9" s="12"/>
-      <c r="I9" s="138" t="s">
+      <c r="I9" s="144" t="s">
         <v>24</v>
       </c>
-      <c r="J9" s="139"/>
+      <c r="J9" s="145"/>
       <c r="K9" s="40"/>
-      <c r="L9" s="160" t="s">
+      <c r="L9" s="136" t="s">
         <v>24</v>
       </c>
-      <c r="M9" s="161"/>
+      <c r="M9" s="137"/>
     </row>
     <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="147"/>
+      <c r="A10" s="142"/>
       <c r="B10" s="14"/>
-      <c r="C10" s="144"/>
-      <c r="D10" s="145"/>
+      <c r="C10" s="157"/>
+      <c r="D10" s="158"/>
       <c r="E10" s="15"/>
-      <c r="F10" s="151"/>
-      <c r="G10" s="152"/>
+      <c r="F10" s="150"/>
+      <c r="G10" s="151"/>
       <c r="H10" s="16"/>
-      <c r="I10" s="140"/>
-      <c r="J10" s="141"/>
+      <c r="I10" s="146"/>
+      <c r="J10" s="147"/>
       <c r="K10" s="39"/>
-      <c r="L10" s="162"/>
-      <c r="M10" s="163"/>
+      <c r="L10" s="138"/>
+      <c r="M10" s="139"/>
     </row>
     <row r="11" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="148"/>
+      <c r="A11" s="143"/>
       <c r="B11" s="97">
         <f>(B10-B9)</f>
         <v>0</v>
@@ -2277,45 +2277,45 @@
       <c r="M11" s="111"/>
     </row>
     <row r="12" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="146"/>
+      <c r="A12" s="141"/>
       <c r="B12" s="10"/>
-      <c r="C12" s="142" t="s">
+      <c r="C12" s="155" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="143"/>
+      <c r="D12" s="156"/>
       <c r="E12" s="11"/>
-      <c r="F12" s="149" t="s">
+      <c r="F12" s="152" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="150"/>
+      <c r="G12" s="149"/>
       <c r="H12" s="12"/>
-      <c r="I12" s="138" t="s">
+      <c r="I12" s="144" t="s">
         <v>24</v>
       </c>
-      <c r="J12" s="139"/>
+      <c r="J12" s="145"/>
       <c r="K12" s="40"/>
-      <c r="L12" s="160" t="s">
+      <c r="L12" s="136" t="s">
         <v>24</v>
       </c>
-      <c r="M12" s="161"/>
+      <c r="M12" s="137"/>
     </row>
     <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="147"/>
+      <c r="A13" s="142"/>
       <c r="B13" s="14"/>
-      <c r="C13" s="144"/>
-      <c r="D13" s="145"/>
+      <c r="C13" s="157"/>
+      <c r="D13" s="158"/>
       <c r="E13" s="15"/>
-      <c r="F13" s="151"/>
-      <c r="G13" s="152"/>
+      <c r="F13" s="150"/>
+      <c r="G13" s="151"/>
       <c r="H13" s="16"/>
-      <c r="I13" s="140"/>
-      <c r="J13" s="141"/>
+      <c r="I13" s="146"/>
+      <c r="J13" s="147"/>
       <c r="K13" s="34"/>
-      <c r="L13" s="162"/>
-      <c r="M13" s="163"/>
+      <c r="L13" s="138"/>
+      <c r="M13" s="139"/>
     </row>
     <row r="14" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="148"/>
+      <c r="A14" s="143"/>
       <c r="B14" s="97">
         <f>(B13-B12)</f>
         <v>0</v>
@@ -2342,45 +2342,45 @@
       <c r="M14" s="113"/>
     </row>
     <row r="15" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="146"/>
+      <c r="A15" s="141"/>
       <c r="B15" s="10"/>
-      <c r="C15" s="142" t="s">
+      <c r="C15" s="155" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="143"/>
+      <c r="D15" s="156"/>
       <c r="E15" s="11"/>
-      <c r="F15" s="149" t="s">
+      <c r="F15" s="152" t="s">
         <v>24</v>
       </c>
-      <c r="G15" s="150"/>
+      <c r="G15" s="149"/>
       <c r="H15" s="12"/>
-      <c r="I15" s="138" t="s">
+      <c r="I15" s="144" t="s">
         <v>24</v>
       </c>
-      <c r="J15" s="139"/>
+      <c r="J15" s="145"/>
       <c r="K15" s="33"/>
-      <c r="L15" s="160" t="s">
+      <c r="L15" s="136" t="s">
         <v>24</v>
       </c>
-      <c r="M15" s="161"/>
+      <c r="M15" s="137"/>
     </row>
     <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="147"/>
+      <c r="A16" s="142"/>
       <c r="B16" s="14"/>
-      <c r="C16" s="144"/>
-      <c r="D16" s="145"/>
+      <c r="C16" s="157"/>
+      <c r="D16" s="158"/>
       <c r="E16" s="15"/>
-      <c r="F16" s="151"/>
-      <c r="G16" s="152"/>
+      <c r="F16" s="150"/>
+      <c r="G16" s="151"/>
       <c r="H16" s="16"/>
-      <c r="I16" s="140"/>
-      <c r="J16" s="141"/>
+      <c r="I16" s="146"/>
+      <c r="J16" s="147"/>
       <c r="K16" s="39"/>
-      <c r="L16" s="162"/>
-      <c r="M16" s="163"/>
+      <c r="L16" s="138"/>
+      <c r="M16" s="139"/>
     </row>
     <row r="17" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="148"/>
+      <c r="A17" s="143"/>
       <c r="B17" s="97">
         <f>(B16-B15)</f>
         <v>0</v>
@@ -2407,45 +2407,45 @@
       <c r="M17" s="111"/>
     </row>
     <row r="18" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="146"/>
+      <c r="A18" s="141"/>
       <c r="B18" s="10"/>
-      <c r="C18" s="142" t="s">
+      <c r="C18" s="155" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="143"/>
+      <c r="D18" s="156"/>
       <c r="E18" s="11"/>
-      <c r="F18" s="149" t="s">
+      <c r="F18" s="152" t="s">
         <v>24</v>
       </c>
-      <c r="G18" s="150"/>
+      <c r="G18" s="149"/>
       <c r="H18" s="12"/>
-      <c r="I18" s="138" t="s">
+      <c r="I18" s="144" t="s">
         <v>24</v>
       </c>
-      <c r="J18" s="139"/>
+      <c r="J18" s="145"/>
       <c r="K18" s="40"/>
-      <c r="L18" s="160" t="s">
+      <c r="L18" s="136" t="s">
         <v>24</v>
       </c>
-      <c r="M18" s="161"/>
+      <c r="M18" s="137"/>
     </row>
     <row r="19" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="147"/>
+      <c r="A19" s="142"/>
       <c r="B19" s="14"/>
-      <c r="C19" s="144"/>
-      <c r="D19" s="145"/>
+      <c r="C19" s="157"/>
+      <c r="D19" s="158"/>
       <c r="E19" s="15"/>
-      <c r="F19" s="151"/>
-      <c r="G19" s="152"/>
+      <c r="F19" s="150"/>
+      <c r="G19" s="151"/>
       <c r="H19" s="16"/>
-      <c r="I19" s="140"/>
-      <c r="J19" s="141"/>
+      <c r="I19" s="146"/>
+      <c r="J19" s="147"/>
       <c r="K19" s="39"/>
-      <c r="L19" s="162"/>
-      <c r="M19" s="163"/>
+      <c r="L19" s="138"/>
+      <c r="M19" s="139"/>
     </row>
     <row r="20" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="148"/>
+      <c r="A20" s="143"/>
       <c r="B20" s="97">
         <f>(B19-B18)</f>
         <v>0</v>
@@ -2472,45 +2472,45 @@
       <c r="M20" s="111"/>
     </row>
     <row r="21" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="146"/>
+      <c r="A21" s="141"/>
       <c r="B21" s="10"/>
-      <c r="C21" s="142" t="s">
+      <c r="C21" s="155" t="s">
         <v>23</v>
       </c>
-      <c r="D21" s="143"/>
+      <c r="D21" s="156"/>
       <c r="E21" s="11"/>
-      <c r="F21" s="149" t="s">
+      <c r="F21" s="152" t="s">
         <v>24</v>
       </c>
-      <c r="G21" s="150"/>
+      <c r="G21" s="149"/>
       <c r="H21" s="12"/>
-      <c r="I21" s="138" t="s">
+      <c r="I21" s="144" t="s">
         <v>24</v>
       </c>
-      <c r="J21" s="139"/>
+      <c r="J21" s="145"/>
       <c r="K21" s="33"/>
-      <c r="L21" s="160" t="s">
+      <c r="L21" s="136" t="s">
         <v>24</v>
       </c>
-      <c r="M21" s="161"/>
+      <c r="M21" s="137"/>
     </row>
     <row r="22" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="147"/>
+      <c r="A22" s="142"/>
       <c r="B22" s="14"/>
-      <c r="C22" s="144"/>
-      <c r="D22" s="145"/>
+      <c r="C22" s="157"/>
+      <c r="D22" s="158"/>
       <c r="E22" s="15"/>
-      <c r="F22" s="151"/>
-      <c r="G22" s="152"/>
+      <c r="F22" s="150"/>
+      <c r="G22" s="151"/>
       <c r="H22" s="16"/>
-      <c r="I22" s="140"/>
-      <c r="J22" s="141"/>
+      <c r="I22" s="146"/>
+      <c r="J22" s="147"/>
       <c r="K22" s="34"/>
-      <c r="L22" s="162"/>
-      <c r="M22" s="163"/>
+      <c r="L22" s="138"/>
+      <c r="M22" s="139"/>
     </row>
     <row r="23" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="148"/>
+      <c r="A23" s="143"/>
       <c r="B23" s="97">
         <f>(B22-B21)</f>
         <v>0</v>
@@ -2538,10 +2538,10 @@
     </row>
     <row r="24" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
     <row r="29" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A29" s="136" t="s">
+      <c r="A29" s="163" t="s">
         <v>21</v>
       </c>
-      <c r="B29" s="137"/>
+      <c r="B29" s="164"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="96" t="s">
@@ -2563,31 +2563,6 @@
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="L3:M4"/>
-    <mergeCell ref="L6:M7"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="I3:J4"/>
-    <mergeCell ref="F6:G7"/>
-    <mergeCell ref="F3:G4"/>
-    <mergeCell ref="I6:J7"/>
-    <mergeCell ref="I9:J10"/>
-    <mergeCell ref="L21:M22"/>
-    <mergeCell ref="L18:M19"/>
-    <mergeCell ref="L15:M16"/>
-    <mergeCell ref="L12:M13"/>
-    <mergeCell ref="L9:M10"/>
-    <mergeCell ref="F9:G10"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="C3:D4"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="C18:D19"/>
-    <mergeCell ref="C15:D16"/>
-    <mergeCell ref="C12:D13"/>
-    <mergeCell ref="C9:D10"/>
-    <mergeCell ref="C6:D7"/>
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="I21:J22"/>
     <mergeCell ref="I18:J19"/>
@@ -2600,6 +2575,31 @@
     <mergeCell ref="F18:G19"/>
     <mergeCell ref="F15:G16"/>
     <mergeCell ref="F12:G13"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="C3:D4"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="C18:D19"/>
+    <mergeCell ref="C15:D16"/>
+    <mergeCell ref="C12:D13"/>
+    <mergeCell ref="C9:D10"/>
+    <mergeCell ref="C6:D7"/>
+    <mergeCell ref="L21:M22"/>
+    <mergeCell ref="L18:M19"/>
+    <mergeCell ref="L15:M16"/>
+    <mergeCell ref="L12:M13"/>
+    <mergeCell ref="L9:M10"/>
+    <mergeCell ref="L3:M4"/>
+    <mergeCell ref="L6:M7"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="I3:J4"/>
+    <mergeCell ref="F6:G7"/>
+    <mergeCell ref="F3:G4"/>
+    <mergeCell ref="I6:J7"/>
+    <mergeCell ref="I9:J10"/>
+    <mergeCell ref="F9:G10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -3056,6 +3056,60 @@
     </row>
   </sheetData>
   <mergeCells count="63">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H19:I19"/>
     <mergeCell ref="A20:A22"/>
     <mergeCell ref="C20:C21"/>
     <mergeCell ref="E20:E21"/>
@@ -3065,60 +3119,6 @@
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="F22:G22"/>
     <mergeCell ref="H22:I22"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -3201,31 +3201,31 @@
       <c r="B2" s="10">
         <v>0.33333333333333298</v>
       </c>
-      <c r="C2" s="198" t="s">
+      <c r="C2" s="183" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="199"/>
+      <c r="D2" s="184"/>
       <c r="E2" s="11">
         <v>0.33333333333333298</v>
       </c>
-      <c r="F2" s="177" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="178"/>
+      <c r="F2" s="190" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="191"/>
       <c r="H2" s="12">
         <v>0.33333333333333298</v>
       </c>
-      <c r="I2" s="184" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2" s="185"/>
+      <c r="I2" s="194" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="205"/>
       <c r="K2" s="33">
         <v>0.33333333333333298</v>
       </c>
-      <c r="L2" s="188" t="s">
-        <v>4</v>
-      </c>
-      <c r="M2" s="189"/>
+      <c r="L2" s="174" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" s="175"/>
       <c r="N2" s="31"/>
     </row>
     <row r="3" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -3233,125 +3233,125 @@
       <c r="B3" s="14">
         <v>0.49166666666666697</v>
       </c>
-      <c r="C3" s="200"/>
-      <c r="D3" s="201"/>
+      <c r="C3" s="185"/>
+      <c r="D3" s="186"/>
       <c r="E3" s="15">
         <v>0.41666666666666702</v>
       </c>
-      <c r="F3" s="179"/>
-      <c r="G3" s="180"/>
+      <c r="F3" s="192"/>
+      <c r="G3" s="193"/>
       <c r="H3" s="16">
         <v>0.41666666666666702</v>
       </c>
-      <c r="I3" s="186"/>
-      <c r="J3" s="187"/>
+      <c r="I3" s="196"/>
+      <c r="J3" s="197"/>
       <c r="K3" s="39">
         <v>0.41666666666666702</v>
       </c>
-      <c r="L3" s="190"/>
-      <c r="M3" s="191"/>
+      <c r="L3" s="198"/>
+      <c r="M3" s="199"/>
     </row>
     <row r="4" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="165"/>
-      <c r="B4" s="174">
+      <c r="B4" s="187">
         <f>B3-B2</f>
         <v>0.15833333333333399</v>
       </c>
-      <c r="C4" s="175"/>
-      <c r="D4" s="176"/>
-      <c r="E4" s="181">
+      <c r="C4" s="188"/>
+      <c r="D4" s="189"/>
+      <c r="E4" s="209">
         <f>E3-E2</f>
         <v>8.3333333333334036E-2</v>
       </c>
-      <c r="F4" s="182"/>
-      <c r="G4" s="183"/>
-      <c r="H4" s="195">
+      <c r="F4" s="210"/>
+      <c r="G4" s="211"/>
+      <c r="H4" s="180">
         <f>H3-H2</f>
         <v>8.3333333333334036E-2</v>
       </c>
-      <c r="I4" s="196"/>
-      <c r="J4" s="197"/>
-      <c r="K4" s="192">
+      <c r="I4" s="181"/>
+      <c r="J4" s="182"/>
+      <c r="K4" s="206">
         <f>K3-K2</f>
         <v>8.3333333333334036E-2</v>
       </c>
-      <c r="L4" s="193"/>
-      <c r="M4" s="194"/>
+      <c r="L4" s="207"/>
+      <c r="M4" s="208"/>
     </row>
     <row r="5" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="165">
         <v>44568</v>
       </c>
       <c r="B5" s="10"/>
-      <c r="C5" s="198" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="199"/>
+      <c r="C5" s="183" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="184"/>
       <c r="E5" s="11">
         <v>0.89583333333333304</v>
       </c>
-      <c r="F5" s="177" t="s">
+      <c r="F5" s="190" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="178"/>
+      <c r="G5" s="191"/>
       <c r="H5" s="12"/>
-      <c r="I5" s="184" t="s">
-        <v>4</v>
-      </c>
-      <c r="J5" s="202"/>
+      <c r="I5" s="194" t="s">
+        <v>4</v>
+      </c>
+      <c r="J5" s="195"/>
       <c r="K5" s="13">
         <v>0.33333333333333298</v>
       </c>
-      <c r="L5" s="188" t="s">
+      <c r="L5" s="174" t="s">
         <v>7</v>
       </c>
-      <c r="M5" s="189"/>
+      <c r="M5" s="175"/>
     </row>
     <row r="6" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="165"/>
       <c r="B6" s="14"/>
-      <c r="C6" s="200"/>
-      <c r="D6" s="201"/>
+      <c r="C6" s="185"/>
+      <c r="D6" s="186"/>
       <c r="E6" s="15">
         <v>0.97916666666666696</v>
       </c>
-      <c r="F6" s="179"/>
-      <c r="G6" s="180"/>
+      <c r="F6" s="192"/>
+      <c r="G6" s="193"/>
       <c r="H6" s="16"/>
-      <c r="I6" s="186"/>
-      <c r="J6" s="187"/>
+      <c r="I6" s="196"/>
+      <c r="J6" s="197"/>
       <c r="K6" s="39">
         <v>0.625</v>
       </c>
-      <c r="L6" s="203"/>
-      <c r="M6" s="204"/>
+      <c r="L6" s="176"/>
+      <c r="M6" s="177"/>
     </row>
     <row r="7" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="165"/>
-      <c r="B7" s="174">
+      <c r="B7" s="187">
         <f>B6-B5</f>
         <v>0</v>
       </c>
-      <c r="C7" s="175"/>
-      <c r="D7" s="176"/>
-      <c r="E7" s="181">
+      <c r="C7" s="188"/>
+      <c r="D7" s="189"/>
+      <c r="E7" s="209">
         <f>E6-E5</f>
         <v>8.3333333333333925E-2</v>
       </c>
-      <c r="F7" s="182"/>
-      <c r="G7" s="183"/>
-      <c r="H7" s="195">
+      <c r="F7" s="210"/>
+      <c r="G7" s="211"/>
+      <c r="H7" s="180">
         <f>H6-H5</f>
         <v>0</v>
       </c>
-      <c r="I7" s="196"/>
-      <c r="J7" s="197"/>
-      <c r="K7" s="205">
+      <c r="I7" s="181"/>
+      <c r="J7" s="182"/>
+      <c r="K7" s="200">
         <f>K6-K5</f>
         <v>0.29166666666666702</v>
       </c>
-      <c r="L7" s="206"/>
-      <c r="M7" s="207"/>
+      <c r="L7" s="201"/>
+      <c r="M7" s="202"/>
     </row>
     <row r="8" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="165">
@@ -3360,81 +3360,81 @@
       <c r="B8" s="10">
         <v>0.72916666666666696</v>
       </c>
-      <c r="C8" s="198" t="s">
+      <c r="C8" s="183" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="199"/>
+      <c r="D8" s="184"/>
       <c r="E8" s="11">
         <v>0.77083333333333304</v>
       </c>
-      <c r="F8" s="177" t="s">
+      <c r="F8" s="190" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="178"/>
+      <c r="G8" s="191"/>
       <c r="H8" s="12">
         <v>0.77083333333333304</v>
       </c>
-      <c r="I8" s="184" t="s">
-        <v>4</v>
-      </c>
-      <c r="J8" s="202"/>
+      <c r="I8" s="194" t="s">
+        <v>4</v>
+      </c>
+      <c r="J8" s="195"/>
       <c r="K8" s="40">
         <v>0.77083333333333304</v>
       </c>
-      <c r="L8" s="190" t="s">
-        <v>4</v>
-      </c>
-      <c r="M8" s="191"/>
+      <c r="L8" s="198" t="s">
+        <v>4</v>
+      </c>
+      <c r="M8" s="199"/>
     </row>
     <row r="9" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="165"/>
       <c r="B9" s="14">
         <v>1</v>
       </c>
-      <c r="C9" s="200"/>
-      <c r="D9" s="201"/>
+      <c r="C9" s="185"/>
+      <c r="D9" s="186"/>
       <c r="E9" s="15">
         <v>0.91666666666666696</v>
       </c>
-      <c r="F9" s="179"/>
-      <c r="G9" s="180"/>
+      <c r="F9" s="192"/>
+      <c r="G9" s="193"/>
       <c r="H9" s="16">
         <v>0.9375</v>
       </c>
-      <c r="I9" s="186"/>
-      <c r="J9" s="187"/>
+      <c r="I9" s="196"/>
+      <c r="J9" s="197"/>
       <c r="K9" s="39">
         <v>0.91666666666666696</v>
       </c>
-      <c r="L9" s="190"/>
-      <c r="M9" s="191"/>
+      <c r="L9" s="198"/>
+      <c r="M9" s="199"/>
     </row>
     <row r="10" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="165"/>
-      <c r="B10" s="174">
+      <c r="B10" s="187">
         <f>(B9-B8)</f>
         <v>0.27083333333333304</v>
       </c>
-      <c r="C10" s="175"/>
-      <c r="D10" s="176"/>
-      <c r="E10" s="181">
+      <c r="C10" s="188"/>
+      <c r="D10" s="189"/>
+      <c r="E10" s="209">
         <f>E9-E8</f>
         <v>0.14583333333333393</v>
       </c>
-      <c r="F10" s="182"/>
-      <c r="G10" s="183"/>
-      <c r="H10" s="195">
+      <c r="F10" s="210"/>
+      <c r="G10" s="211"/>
+      <c r="H10" s="180">
         <f>H9-H8</f>
         <v>0.16666666666666696</v>
       </c>
-      <c r="I10" s="196"/>
-      <c r="J10" s="197"/>
-      <c r="K10" s="205">
+      <c r="I10" s="181"/>
+      <c r="J10" s="182"/>
+      <c r="K10" s="200">
         <f>K9-K8</f>
         <v>0.14583333333333393</v>
       </c>
-      <c r="L10" s="206"/>
-      <c r="M10" s="207"/>
+      <c r="L10" s="201"/>
+      <c r="M10" s="202"/>
     </row>
     <row r="11" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="165">
@@ -3443,288 +3443,319 @@
       <c r="B11" s="10">
         <v>0.66666666666666696</v>
       </c>
-      <c r="C11" s="198" t="s">
+      <c r="C11" s="183" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="199"/>
+      <c r="D11" s="184"/>
       <c r="E11" s="11">
         <v>0.66666666666666696</v>
       </c>
-      <c r="F11" s="177" t="s">
+      <c r="F11" s="190" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="178"/>
+      <c r="G11" s="191"/>
       <c r="H11" s="12">
         <v>0.75</v>
       </c>
-      <c r="I11" s="184" t="s">
-        <v>4</v>
-      </c>
-      <c r="J11" s="202"/>
+      <c r="I11" s="194" t="s">
+        <v>4</v>
+      </c>
+      <c r="J11" s="195"/>
       <c r="K11" s="40">
         <v>0.75</v>
       </c>
-      <c r="L11" s="190" t="s">
-        <v>4</v>
-      </c>
-      <c r="M11" s="191"/>
+      <c r="L11" s="198" t="s">
+        <v>4</v>
+      </c>
+      <c r="M11" s="199"/>
     </row>
     <row r="12" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="165"/>
       <c r="B12" s="14">
         <v>1</v>
       </c>
-      <c r="C12" s="200"/>
-      <c r="D12" s="201"/>
+      <c r="C12" s="185"/>
+      <c r="D12" s="186"/>
       <c r="E12" s="15">
         <v>0.95833333333333304</v>
       </c>
-      <c r="F12" s="179"/>
-      <c r="G12" s="180"/>
+      <c r="F12" s="192"/>
+      <c r="G12" s="193"/>
       <c r="H12" s="16">
         <v>1</v>
       </c>
-      <c r="I12" s="186"/>
-      <c r="J12" s="187"/>
+      <c r="I12" s="196"/>
+      <c r="J12" s="197"/>
       <c r="K12" s="34">
         <v>0.95833333333333304</v>
       </c>
-      <c r="L12" s="203"/>
-      <c r="M12" s="204"/>
+      <c r="L12" s="176"/>
+      <c r="M12" s="177"/>
     </row>
     <row r="13" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="165"/>
-      <c r="B13" s="174">
+      <c r="B13" s="187">
         <f>(B12-B11)</f>
         <v>0.33333333333333304</v>
       </c>
-      <c r="C13" s="175"/>
-      <c r="D13" s="176"/>
-      <c r="E13" s="181">
+      <c r="C13" s="188"/>
+      <c r="D13" s="189"/>
+      <c r="E13" s="209">
         <f>E12-E11</f>
         <v>0.29166666666666607</v>
       </c>
-      <c r="F13" s="182"/>
-      <c r="G13" s="183"/>
-      <c r="H13" s="195">
+      <c r="F13" s="210"/>
+      <c r="G13" s="211"/>
+      <c r="H13" s="180">
         <f>H12-H11</f>
         <v>0.25</v>
       </c>
-      <c r="I13" s="196"/>
-      <c r="J13" s="197"/>
-      <c r="K13" s="208">
+      <c r="I13" s="181"/>
+      <c r="J13" s="182"/>
+      <c r="K13" s="203">
         <f>K12-K11</f>
         <v>0.20833333333333304</v>
       </c>
-      <c r="L13" s="208"/>
-      <c r="M13" s="209"/>
+      <c r="L13" s="203"/>
+      <c r="M13" s="204"/>
     </row>
     <row r="14" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="165"/>
       <c r="B14" s="10"/>
-      <c r="C14" s="198" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="199"/>
+      <c r="C14" s="183" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="184"/>
       <c r="E14" s="11"/>
-      <c r="F14" s="177" t="s">
-        <v>4</v>
-      </c>
-      <c r="G14" s="178"/>
+      <c r="F14" s="190" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14" s="191"/>
       <c r="H14" s="12"/>
-      <c r="I14" s="184" t="s">
-        <v>4</v>
-      </c>
-      <c r="J14" s="202"/>
+      <c r="I14" s="194" t="s">
+        <v>4</v>
+      </c>
+      <c r="J14" s="195"/>
       <c r="K14" s="33"/>
-      <c r="L14" s="188" t="s">
-        <v>4</v>
-      </c>
-      <c r="M14" s="189"/>
+      <c r="L14" s="174" t="s">
+        <v>4</v>
+      </c>
+      <c r="M14" s="175"/>
     </row>
     <row r="15" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="165"/>
       <c r="B15" s="14"/>
-      <c r="C15" s="200"/>
-      <c r="D15" s="201"/>
+      <c r="C15" s="185"/>
+      <c r="D15" s="186"/>
       <c r="E15" s="15"/>
-      <c r="F15" s="179"/>
-      <c r="G15" s="180"/>
+      <c r="F15" s="192"/>
+      <c r="G15" s="193"/>
       <c r="H15" s="16"/>
-      <c r="I15" s="186"/>
-      <c r="J15" s="187"/>
+      <c r="I15" s="196"/>
+      <c r="J15" s="197"/>
       <c r="K15" s="39"/>
-      <c r="L15" s="190"/>
-      <c r="M15" s="191"/>
+      <c r="L15" s="198"/>
+      <c r="M15" s="199"/>
     </row>
     <row r="16" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="165"/>
-      <c r="B16" s="174">
+      <c r="B16" s="187">
         <f>(B15-B14)</f>
         <v>0</v>
       </c>
-      <c r="C16" s="175"/>
-      <c r="D16" s="176"/>
-      <c r="E16" s="181">
+      <c r="C16" s="188"/>
+      <c r="D16" s="189"/>
+      <c r="E16" s="209">
         <f>E15-E14</f>
         <v>0</v>
       </c>
-      <c r="F16" s="182"/>
-      <c r="G16" s="183"/>
-      <c r="H16" s="195">
+      <c r="F16" s="210"/>
+      <c r="G16" s="211"/>
+      <c r="H16" s="180">
         <f>H15-H14</f>
         <v>0</v>
       </c>
-      <c r="I16" s="196"/>
-      <c r="J16" s="197"/>
-      <c r="K16" s="205">
+      <c r="I16" s="181"/>
+      <c r="J16" s="182"/>
+      <c r="K16" s="200">
         <f>K15-K14</f>
         <v>0</v>
       </c>
-      <c r="L16" s="206"/>
-      <c r="M16" s="207"/>
+      <c r="L16" s="201"/>
+      <c r="M16" s="202"/>
     </row>
     <row r="17" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="165"/>
       <c r="B17" s="10"/>
-      <c r="C17" s="198" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" s="199"/>
+      <c r="C17" s="183" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="184"/>
       <c r="E17" s="11"/>
-      <c r="F17" s="177" t="s">
-        <v>4</v>
-      </c>
-      <c r="G17" s="178"/>
+      <c r="F17" s="190" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" s="191"/>
       <c r="H17" s="12"/>
-      <c r="I17" s="184" t="s">
-        <v>4</v>
-      </c>
-      <c r="J17" s="202"/>
+      <c r="I17" s="194" t="s">
+        <v>4</v>
+      </c>
+      <c r="J17" s="195"/>
       <c r="K17" s="40"/>
-      <c r="L17" s="190" t="s">
-        <v>4</v>
-      </c>
-      <c r="M17" s="191"/>
+      <c r="L17" s="198" t="s">
+        <v>4</v>
+      </c>
+      <c r="M17" s="199"/>
     </row>
     <row r="18" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="165"/>
       <c r="B18" s="14"/>
-      <c r="C18" s="200"/>
-      <c r="D18" s="201"/>
+      <c r="C18" s="185"/>
+      <c r="D18" s="186"/>
       <c r="E18" s="15"/>
-      <c r="F18" s="179"/>
-      <c r="G18" s="180"/>
+      <c r="F18" s="192"/>
+      <c r="G18" s="193"/>
       <c r="H18" s="16"/>
-      <c r="I18" s="186"/>
-      <c r="J18" s="187"/>
+      <c r="I18" s="196"/>
+      <c r="J18" s="197"/>
       <c r="K18" s="39"/>
-      <c r="L18" s="190"/>
-      <c r="M18" s="191"/>
+      <c r="L18" s="198"/>
+      <c r="M18" s="199"/>
     </row>
     <row r="19" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="165"/>
-      <c r="B19" s="174">
+      <c r="B19" s="187">
         <f>(B18-B17)</f>
         <v>0</v>
       </c>
-      <c r="C19" s="175"/>
-      <c r="D19" s="176"/>
-      <c r="E19" s="181">
+      <c r="C19" s="188"/>
+      <c r="D19" s="189"/>
+      <c r="E19" s="209">
         <f>E18-E17</f>
         <v>0</v>
       </c>
-      <c r="F19" s="182"/>
-      <c r="G19" s="183"/>
-      <c r="H19" s="195">
+      <c r="F19" s="210"/>
+      <c r="G19" s="211"/>
+      <c r="H19" s="180">
         <f>H18-H17</f>
         <v>0</v>
       </c>
-      <c r="I19" s="196"/>
-      <c r="J19" s="197"/>
-      <c r="K19" s="205">
+      <c r="I19" s="181"/>
+      <c r="J19" s="182"/>
+      <c r="K19" s="200">
         <f>K18-K17</f>
         <v>0</v>
       </c>
-      <c r="L19" s="206"/>
-      <c r="M19" s="207"/>
+      <c r="L19" s="201"/>
+      <c r="M19" s="202"/>
     </row>
     <row r="20" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="165"/>
       <c r="B20" s="10"/>
-      <c r="C20" s="198" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" s="199"/>
+      <c r="C20" s="183" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="184"/>
       <c r="E20" s="11"/>
-      <c r="F20" s="177" t="s">
-        <v>4</v>
-      </c>
-      <c r="G20" s="178"/>
+      <c r="F20" s="190" t="s">
+        <v>4</v>
+      </c>
+      <c r="G20" s="191"/>
       <c r="H20" s="12"/>
-      <c r="I20" s="184" t="s">
-        <v>4</v>
-      </c>
-      <c r="J20" s="202"/>
+      <c r="I20" s="194" t="s">
+        <v>4</v>
+      </c>
+      <c r="J20" s="195"/>
       <c r="K20" s="33"/>
-      <c r="L20" s="188" t="s">
-        <v>4</v>
-      </c>
-      <c r="M20" s="189"/>
+      <c r="L20" s="174" t="s">
+        <v>4</v>
+      </c>
+      <c r="M20" s="175"/>
     </row>
     <row r="21" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="165"/>
       <c r="B21" s="14"/>
-      <c r="C21" s="200"/>
-      <c r="D21" s="201"/>
+      <c r="C21" s="185"/>
+      <c r="D21" s="186"/>
       <c r="E21" s="15"/>
-      <c r="F21" s="179"/>
-      <c r="G21" s="180"/>
+      <c r="F21" s="192"/>
+      <c r="G21" s="193"/>
       <c r="H21" s="16"/>
-      <c r="I21" s="186"/>
-      <c r="J21" s="187"/>
+      <c r="I21" s="196"/>
+      <c r="J21" s="197"/>
       <c r="K21" s="34"/>
-      <c r="L21" s="203"/>
-      <c r="M21" s="204"/>
+      <c r="L21" s="176"/>
+      <c r="M21" s="177"/>
     </row>
     <row r="22" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="165"/>
-      <c r="B22" s="174">
+      <c r="B22" s="187">
         <f>(B21-B20)</f>
         <v>0</v>
       </c>
-      <c r="C22" s="175"/>
-      <c r="D22" s="176"/>
-      <c r="E22" s="181">
+      <c r="C22" s="188"/>
+      <c r="D22" s="189"/>
+      <c r="E22" s="209">
         <f>E21-E20</f>
         <v>0</v>
       </c>
-      <c r="F22" s="182"/>
-      <c r="G22" s="183"/>
-      <c r="H22" s="195">
+      <c r="F22" s="210"/>
+      <c r="G22" s="211"/>
+      <c r="H22" s="180">
         <f>H21-H20</f>
         <v>0</v>
       </c>
-      <c r="I22" s="196"/>
-      <c r="J22" s="197"/>
-      <c r="K22" s="210">
+      <c r="I22" s="181"/>
+      <c r="J22" s="182"/>
+      <c r="K22" s="178">
         <f>K21-K20</f>
         <v>0</v>
       </c>
-      <c r="L22" s="210"/>
-      <c r="M22" s="211"/>
+      <c r="L22" s="178"/>
+      <c r="M22" s="179"/>
     </row>
     <row r="23" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="63">
-    <mergeCell ref="L20:M21"/>
-    <mergeCell ref="K22:M22"/>
-    <mergeCell ref="H22:J22"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="C20:D21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="F20:G21"/>
-    <mergeCell ref="I20:J21"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="F2:G3"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="I2:J3"/>
+    <mergeCell ref="L2:M3"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="C5:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="F5:G6"/>
+    <mergeCell ref="I5:J6"/>
+    <mergeCell ref="L5:M6"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="C2:D3"/>
+    <mergeCell ref="L8:M9"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="C11:D12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="F11:G12"/>
+    <mergeCell ref="I11:J12"/>
+    <mergeCell ref="L11:M12"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="C8:D9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="F8:G9"/>
+    <mergeCell ref="I8:J9"/>
     <mergeCell ref="L14:M15"/>
     <mergeCell ref="K16:M16"/>
     <mergeCell ref="H16:J16"/>
@@ -3741,45 +3772,14 @@
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="F14:G15"/>
     <mergeCell ref="I14:J15"/>
-    <mergeCell ref="L8:M9"/>
-    <mergeCell ref="K10:M10"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="C11:D12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="F11:G12"/>
-    <mergeCell ref="I11:J12"/>
-    <mergeCell ref="L11:M12"/>
-    <mergeCell ref="K13:M13"/>
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="C8:D9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="F8:G9"/>
-    <mergeCell ref="I8:J9"/>
-    <mergeCell ref="I2:J3"/>
-    <mergeCell ref="L2:M3"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="C5:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="F5:G6"/>
-    <mergeCell ref="I5:J6"/>
-    <mergeCell ref="L5:M6"/>
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="C2:D3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="F2:G3"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="L20:M21"/>
+    <mergeCell ref="K22:M22"/>
+    <mergeCell ref="H22:J22"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="C20:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="F20:G21"/>
+    <mergeCell ref="I20:J21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -3808,7 +3808,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="219" t="s">
+      <c r="A1" s="213" t="s">
         <v>14</v>
       </c>
       <c r="B1" s="87" t="s">
@@ -3850,7 +3850,7 @@
       <c r="N1" s="42"/>
     </row>
     <row r="2" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="220"/>
+      <c r="A2" s="214"/>
       <c r="B2" s="20" t="s">
         <v>0</v>
       </c>
@@ -3898,63 +3898,63 @@
       <c r="N2" s="31"/>
     </row>
     <row r="3" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="212">
+      <c r="A3" s="215">
         <v>44571</v>
       </c>
       <c r="B3" s="10">
         <v>0.33333333333333331</v>
       </c>
-      <c r="C3" s="215" t="s">
+      <c r="C3" s="218" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="143"/>
+      <c r="D3" s="156"/>
       <c r="E3" s="11">
         <v>0.33333333333333331</v>
       </c>
-      <c r="F3" s="216" t="s">
+      <c r="F3" s="219" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="150"/>
+      <c r="G3" s="149"/>
       <c r="H3" s="12">
         <v>0.33333333333333331</v>
       </c>
-      <c r="I3" s="217" t="s">
+      <c r="I3" s="220" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="139"/>
+      <c r="J3" s="145"/>
       <c r="K3" s="33">
         <v>0.33333333333333331</v>
       </c>
-      <c r="L3" s="218" t="s">
+      <c r="L3" s="212" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="161"/>
+      <c r="M3" s="137"/>
     </row>
     <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="213"/>
+      <c r="A4" s="216"/>
       <c r="B4" s="14">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C4" s="144"/>
-      <c r="D4" s="145"/>
+      <c r="C4" s="157"/>
+      <c r="D4" s="158"/>
       <c r="E4" s="15">
         <v>0.41666666666666669</v>
       </c>
-      <c r="F4" s="151"/>
-      <c r="G4" s="152"/>
+      <c r="F4" s="150"/>
+      <c r="G4" s="151"/>
       <c r="H4" s="16">
         <v>0.41666666666666669</v>
       </c>
-      <c r="I4" s="140"/>
-      <c r="J4" s="141"/>
+      <c r="I4" s="146"/>
+      <c r="J4" s="147"/>
       <c r="K4" s="39">
         <v>0.41666666666666669</v>
       </c>
-      <c r="L4" s="162"/>
-      <c r="M4" s="163"/>
+      <c r="L4" s="138"/>
+      <c r="M4" s="139"/>
     </row>
     <row r="5" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="214"/>
+      <c r="A5" s="217"/>
       <c r="B5" s="48">
         <f>B4-B3</f>
         <v>8.333333333333337E-2</v>
@@ -3981,63 +3981,63 @@
       <c r="M5" s="53"/>
     </row>
     <row r="6" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="212">
+      <c r="A6" s="215">
         <v>44583</v>
       </c>
       <c r="B6" s="10">
         <v>0.79166666666666663</v>
       </c>
-      <c r="C6" s="215" t="s">
+      <c r="C6" s="218" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="143"/>
+      <c r="D6" s="156"/>
       <c r="E6" s="11">
         <v>0.82291666666666663</v>
       </c>
-      <c r="F6" s="216" t="s">
+      <c r="F6" s="219" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="150"/>
+      <c r="G6" s="149"/>
       <c r="H6" s="12">
         <v>0.79166666666666663</v>
       </c>
-      <c r="I6" s="217" t="s">
+      <c r="I6" s="220" t="s">
         <v>19</v>
       </c>
-      <c r="J6" s="139"/>
+      <c r="J6" s="145"/>
       <c r="K6" s="13">
         <v>0.79166666666666663</v>
       </c>
-      <c r="L6" s="218" t="s">
+      <c r="L6" s="212" t="s">
         <v>19</v>
       </c>
-      <c r="M6" s="161"/>
+      <c r="M6" s="137"/>
     </row>
     <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="213"/>
+      <c r="A7" s="216"/>
       <c r="B7" s="14">
         <v>0.8979166666666667</v>
       </c>
-      <c r="C7" s="144"/>
-      <c r="D7" s="145"/>
+      <c r="C7" s="157"/>
+      <c r="D7" s="158"/>
       <c r="E7" s="15">
         <v>0.8979166666666667</v>
       </c>
-      <c r="F7" s="151"/>
-      <c r="G7" s="152"/>
+      <c r="F7" s="150"/>
+      <c r="G7" s="151"/>
       <c r="H7" s="16">
         <v>0.89583333333333337</v>
       </c>
-      <c r="I7" s="140"/>
-      <c r="J7" s="141"/>
+      <c r="I7" s="146"/>
+      <c r="J7" s="147"/>
       <c r="K7" s="39">
         <v>0.8979166666666667</v>
       </c>
-      <c r="L7" s="162"/>
-      <c r="M7" s="163"/>
+      <c r="L7" s="138"/>
+      <c r="M7" s="139"/>
     </row>
     <row r="8" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="214"/>
+      <c r="A8" s="217"/>
       <c r="B8" s="48">
         <f>B7-B6</f>
         <v>0.10625000000000007</v>
@@ -4064,63 +4064,63 @@
       <c r="M8" s="24"/>
     </row>
     <row r="9" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="212">
+      <c r="A9" s="215">
         <v>44584</v>
       </c>
       <c r="B9" s="10">
         <v>0.75694444444444453</v>
       </c>
-      <c r="C9" s="215" t="s">
+      <c r="C9" s="218" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="143"/>
+      <c r="D9" s="156"/>
       <c r="E9" s="11">
         <v>0.75694444444444453</v>
       </c>
-      <c r="F9" s="216" t="s">
+      <c r="F9" s="219" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="150"/>
+      <c r="G9" s="149"/>
       <c r="H9" s="12">
         <v>0.75694444444444453</v>
       </c>
-      <c r="I9" s="217" t="s">
+      <c r="I9" s="220" t="s">
         <v>20</v>
       </c>
-      <c r="J9" s="139"/>
+      <c r="J9" s="145"/>
       <c r="K9" s="40">
         <v>0.75694444444444453</v>
       </c>
-      <c r="L9" s="218" t="s">
+      <c r="L9" s="212" t="s">
         <v>20</v>
       </c>
-      <c r="M9" s="161"/>
+      <c r="M9" s="137"/>
     </row>
     <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="213"/>
+      <c r="A10" s="216"/>
       <c r="B10" s="14">
         <v>0.8354166666666667</v>
       </c>
-      <c r="C10" s="144"/>
-      <c r="D10" s="145"/>
+      <c r="C10" s="157"/>
+      <c r="D10" s="158"/>
       <c r="E10" s="15">
         <v>0.8354166666666667</v>
       </c>
-      <c r="F10" s="151"/>
-      <c r="G10" s="152"/>
+      <c r="F10" s="150"/>
+      <c r="G10" s="151"/>
       <c r="H10" s="16">
         <v>0.8354166666666667</v>
       </c>
-      <c r="I10" s="140"/>
-      <c r="J10" s="141"/>
+      <c r="I10" s="146"/>
+      <c r="J10" s="147"/>
       <c r="K10" s="39">
         <v>0.8354166666666667</v>
       </c>
-      <c r="L10" s="162"/>
-      <c r="M10" s="163"/>
+      <c r="L10" s="138"/>
+      <c r="M10" s="139"/>
     </row>
     <row r="11" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="214"/>
+      <c r="A11" s="217"/>
       <c r="B11" s="48">
         <f>(B10-B9)</f>
         <v>7.8472222222222165E-2</v>
@@ -4147,45 +4147,45 @@
       <c r="M11" s="24"/>
     </row>
     <row r="12" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="212"/>
+      <c r="A12" s="215"/>
       <c r="B12" s="10"/>
-      <c r="C12" s="215" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="143"/>
+      <c r="C12" s="218" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="156"/>
       <c r="E12" s="11"/>
-      <c r="F12" s="216" t="s">
-        <v>4</v>
-      </c>
-      <c r="G12" s="150"/>
+      <c r="F12" s="219" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="149"/>
       <c r="H12" s="12"/>
-      <c r="I12" s="217" t="s">
-        <v>4</v>
-      </c>
-      <c r="J12" s="139"/>
+      <c r="I12" s="220" t="s">
+        <v>4</v>
+      </c>
+      <c r="J12" s="145"/>
       <c r="K12" s="40"/>
-      <c r="L12" s="218" t="s">
-        <v>4</v>
-      </c>
-      <c r="M12" s="161"/>
+      <c r="L12" s="212" t="s">
+        <v>4</v>
+      </c>
+      <c r="M12" s="137"/>
     </row>
     <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="213"/>
+      <c r="A13" s="216"/>
       <c r="B13" s="14"/>
-      <c r="C13" s="144"/>
-      <c r="D13" s="145"/>
+      <c r="C13" s="157"/>
+      <c r="D13" s="158"/>
       <c r="E13" s="15"/>
-      <c r="F13" s="151"/>
-      <c r="G13" s="152"/>
+      <c r="F13" s="150"/>
+      <c r="G13" s="151"/>
       <c r="H13" s="16"/>
-      <c r="I13" s="140"/>
-      <c r="J13" s="141"/>
+      <c r="I13" s="146"/>
+      <c r="J13" s="147"/>
       <c r="K13" s="34"/>
-      <c r="L13" s="162"/>
-      <c r="M13" s="163"/>
+      <c r="L13" s="138"/>
+      <c r="M13" s="139"/>
     </row>
     <row r="14" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="214"/>
+      <c r="A14" s="217"/>
       <c r="B14" s="48">
         <f>(B13-B12)</f>
         <v>0</v>
@@ -4212,45 +4212,45 @@
       <c r="M14" s="55"/>
     </row>
     <row r="15" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="212"/>
+      <c r="A15" s="215"/>
       <c r="B15" s="10"/>
-      <c r="C15" s="215" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" s="143"/>
+      <c r="C15" s="218" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="156"/>
       <c r="E15" s="11"/>
-      <c r="F15" s="216" t="s">
-        <v>4</v>
-      </c>
-      <c r="G15" s="150"/>
+      <c r="F15" s="219" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" s="149"/>
       <c r="H15" s="12"/>
-      <c r="I15" s="217" t="s">
-        <v>4</v>
-      </c>
-      <c r="J15" s="139"/>
+      <c r="I15" s="220" t="s">
+        <v>4</v>
+      </c>
+      <c r="J15" s="145"/>
       <c r="K15" s="33"/>
-      <c r="L15" s="218" t="s">
-        <v>4</v>
-      </c>
-      <c r="M15" s="161"/>
+      <c r="L15" s="212" t="s">
+        <v>4</v>
+      </c>
+      <c r="M15" s="137"/>
     </row>
     <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="213"/>
+      <c r="A16" s="216"/>
       <c r="B16" s="14"/>
-      <c r="C16" s="144"/>
-      <c r="D16" s="145"/>
+      <c r="C16" s="157"/>
+      <c r="D16" s="158"/>
       <c r="E16" s="15"/>
-      <c r="F16" s="151"/>
-      <c r="G16" s="152"/>
+      <c r="F16" s="150"/>
+      <c r="G16" s="151"/>
       <c r="H16" s="16"/>
-      <c r="I16" s="140"/>
-      <c r="J16" s="141"/>
+      <c r="I16" s="146"/>
+      <c r="J16" s="147"/>
       <c r="K16" s="39"/>
-      <c r="L16" s="162"/>
-      <c r="M16" s="163"/>
+      <c r="L16" s="138"/>
+      <c r="M16" s="139"/>
     </row>
     <row r="17" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="214"/>
+      <c r="A17" s="217"/>
       <c r="B17" s="48">
         <f>(B16-B15)</f>
         <v>0</v>
@@ -4277,45 +4277,45 @@
       <c r="M17" s="24"/>
     </row>
     <row r="18" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="212"/>
+      <c r="A18" s="215"/>
       <c r="B18" s="10"/>
-      <c r="C18" s="215" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="143"/>
+      <c r="C18" s="218" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="156"/>
       <c r="E18" s="11"/>
-      <c r="F18" s="216" t="s">
-        <v>4</v>
-      </c>
-      <c r="G18" s="150"/>
+      <c r="F18" s="219" t="s">
+        <v>4</v>
+      </c>
+      <c r="G18" s="149"/>
       <c r="H18" s="12"/>
-      <c r="I18" s="217" t="s">
-        <v>4</v>
-      </c>
-      <c r="J18" s="139"/>
+      <c r="I18" s="220" t="s">
+        <v>4</v>
+      </c>
+      <c r="J18" s="145"/>
       <c r="K18" s="40"/>
-      <c r="L18" s="218" t="s">
-        <v>4</v>
-      </c>
-      <c r="M18" s="161"/>
+      <c r="L18" s="212" t="s">
+        <v>4</v>
+      </c>
+      <c r="M18" s="137"/>
     </row>
     <row r="19" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="213"/>
+      <c r="A19" s="216"/>
       <c r="B19" s="14"/>
-      <c r="C19" s="144"/>
-      <c r="D19" s="145"/>
+      <c r="C19" s="157"/>
+      <c r="D19" s="158"/>
       <c r="E19" s="15"/>
-      <c r="F19" s="151"/>
-      <c r="G19" s="152"/>
+      <c r="F19" s="150"/>
+      <c r="G19" s="151"/>
       <c r="H19" s="16"/>
-      <c r="I19" s="140"/>
-      <c r="J19" s="141"/>
+      <c r="I19" s="146"/>
+      <c r="J19" s="147"/>
       <c r="K19" s="39"/>
-      <c r="L19" s="162"/>
-      <c r="M19" s="163"/>
+      <c r="L19" s="138"/>
+      <c r="M19" s="139"/>
     </row>
     <row r="20" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="214"/>
+      <c r="A20" s="217"/>
       <c r="B20" s="48">
         <f>(B19-B18)</f>
         <v>0</v>
@@ -4342,45 +4342,45 @@
       <c r="M20" s="24"/>
     </row>
     <row r="21" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="212"/>
+      <c r="A21" s="215"/>
       <c r="B21" s="10"/>
-      <c r="C21" s="215" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" s="143"/>
+      <c r="C21" s="218" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="156"/>
       <c r="E21" s="11"/>
-      <c r="F21" s="216" t="s">
-        <v>4</v>
-      </c>
-      <c r="G21" s="150"/>
+      <c r="F21" s="219" t="s">
+        <v>4</v>
+      </c>
+      <c r="G21" s="149"/>
       <c r="H21" s="12"/>
-      <c r="I21" s="217" t="s">
-        <v>4</v>
-      </c>
-      <c r="J21" s="139"/>
+      <c r="I21" s="220" t="s">
+        <v>4</v>
+      </c>
+      <c r="J21" s="145"/>
       <c r="K21" s="33"/>
-      <c r="L21" s="218" t="s">
-        <v>4</v>
-      </c>
-      <c r="M21" s="161"/>
+      <c r="L21" s="212" t="s">
+        <v>4</v>
+      </c>
+      <c r="M21" s="137"/>
     </row>
     <row r="22" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="213"/>
+      <c r="A22" s="216"/>
       <c r="B22" s="14"/>
-      <c r="C22" s="144"/>
-      <c r="D22" s="145"/>
+      <c r="C22" s="157"/>
+      <c r="D22" s="158"/>
       <c r="E22" s="15"/>
-      <c r="F22" s="151"/>
-      <c r="G22" s="152"/>
+      <c r="F22" s="150"/>
+      <c r="G22" s="151"/>
       <c r="H22" s="16"/>
-      <c r="I22" s="140"/>
-      <c r="J22" s="141"/>
+      <c r="I22" s="146"/>
+      <c r="J22" s="147"/>
       <c r="K22" s="34"/>
-      <c r="L22" s="162"/>
-      <c r="M22" s="163"/>
+      <c r="L22" s="138"/>
+      <c r="M22" s="139"/>
     </row>
     <row r="23" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="214"/>
+      <c r="A23" s="217"/>
       <c r="B23" s="48">
         <f>(B22-B21)</f>
         <v>0</v>
@@ -4427,42 +4427,42 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="C18:D19"/>
+    <mergeCell ref="F18:G19"/>
+    <mergeCell ref="I18:J19"/>
+    <mergeCell ref="L18:M19"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="C21:D22"/>
+    <mergeCell ref="F21:G22"/>
+    <mergeCell ref="I21:J22"/>
+    <mergeCell ref="L21:M22"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="C12:D13"/>
+    <mergeCell ref="F12:G13"/>
+    <mergeCell ref="I12:J13"/>
+    <mergeCell ref="L12:M13"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="C15:D16"/>
+    <mergeCell ref="F15:G16"/>
+    <mergeCell ref="I15:J16"/>
+    <mergeCell ref="L15:M16"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="C6:D7"/>
+    <mergeCell ref="F6:G7"/>
+    <mergeCell ref="I6:J7"/>
+    <mergeCell ref="L6:M7"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="C9:D10"/>
+    <mergeCell ref="F9:G10"/>
+    <mergeCell ref="I9:J10"/>
+    <mergeCell ref="L9:M10"/>
     <mergeCell ref="L3:M4"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="C3:D4"/>
     <mergeCell ref="F3:G4"/>
     <mergeCell ref="I3:J4"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="C9:D10"/>
-    <mergeCell ref="F9:G10"/>
-    <mergeCell ref="I9:J10"/>
-    <mergeCell ref="L9:M10"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="C6:D7"/>
-    <mergeCell ref="F6:G7"/>
-    <mergeCell ref="I6:J7"/>
-    <mergeCell ref="L6:M7"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="C15:D16"/>
-    <mergeCell ref="F15:G16"/>
-    <mergeCell ref="I15:J16"/>
-    <mergeCell ref="L15:M16"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="C12:D13"/>
-    <mergeCell ref="F12:G13"/>
-    <mergeCell ref="I12:J13"/>
-    <mergeCell ref="L12:M13"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="C21:D22"/>
-    <mergeCell ref="F21:G22"/>
-    <mergeCell ref="I21:J22"/>
-    <mergeCell ref="L21:M22"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="C18:D19"/>
-    <mergeCell ref="F18:G19"/>
-    <mergeCell ref="I18:J19"/>
-    <mergeCell ref="L18:M19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4474,7 +4474,7 @@
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4491,7 +4491,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="154" t="s">
+      <c r="A1" s="153" t="s">
         <v>14</v>
       </c>
       <c r="B1" s="116" t="s">
@@ -4533,17 +4533,17 @@
       <c r="N1" s="42"/>
     </row>
     <row r="2" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="155"/>
+      <c r="A2" s="154"/>
       <c r="B2" s="124" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="125" cm="1">
         <f t="array" ref="C2">SUM(B5:B23*(MOD(ROW(B5:B23)-2,3)=0))</f>
-        <v>0.13541666666666663</v>
+        <v>0.21875</v>
       </c>
       <c r="D2" s="126">
         <f>C2+Sprint_3!D2</f>
-        <v>1.4993055555555563</v>
+        <v>1.5826388888888898</v>
       </c>
       <c r="E2" s="127" t="s">
         <v>1</v>
@@ -4581,63 +4581,63 @@
       <c r="N2" s="31"/>
     </row>
     <row r="3" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="212">
+      <c r="A3" s="215">
         <v>44585</v>
       </c>
       <c r="B3" s="10">
         <v>0.33333333333333331</v>
       </c>
-      <c r="C3" s="142" t="s">
+      <c r="C3" s="155" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="143"/>
+      <c r="D3" s="156"/>
       <c r="E3" s="11">
         <v>0.33333333333333331</v>
       </c>
-      <c r="F3" s="149" t="s">
+      <c r="F3" s="152" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="150"/>
+      <c r="G3" s="149"/>
       <c r="H3" s="12">
         <v>0.33333333333333331</v>
       </c>
-      <c r="I3" s="138" t="s">
+      <c r="I3" s="144" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="139"/>
+      <c r="J3" s="145"/>
       <c r="K3" s="33">
         <v>0.33333333333333331</v>
       </c>
-      <c r="L3" s="160" t="s">
+      <c r="L3" s="136" t="s">
         <v>26</v>
       </c>
-      <c r="M3" s="161"/>
+      <c r="M3" s="137"/>
     </row>
     <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="213"/>
+      <c r="A4" s="216"/>
       <c r="B4" s="14">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C4" s="144"/>
-      <c r="D4" s="145"/>
+      <c r="C4" s="157"/>
+      <c r="D4" s="158"/>
       <c r="E4" s="15">
         <v>0.41666666666666669</v>
       </c>
-      <c r="F4" s="151"/>
-      <c r="G4" s="152"/>
+      <c r="F4" s="150"/>
+      <c r="G4" s="151"/>
       <c r="H4" s="16">
         <v>0.41666666666666669</v>
       </c>
-      <c r="I4" s="140"/>
-      <c r="J4" s="141"/>
+      <c r="I4" s="146"/>
+      <c r="J4" s="147"/>
       <c r="K4" s="39">
         <v>0.41666666666666669</v>
       </c>
-      <c r="L4" s="162"/>
-      <c r="M4" s="163"/>
+      <c r="L4" s="138"/>
+      <c r="M4" s="139"/>
     </row>
     <row r="5" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="214"/>
+      <c r="A5" s="217"/>
       <c r="B5" s="68">
         <f>B4-B3</f>
         <v>8.333333333333337E-2</v>
@@ -4664,63 +4664,63 @@
       <c r="M5" s="76"/>
     </row>
     <row r="6" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="212">
+      <c r="A6" s="215">
         <v>44585</v>
       </c>
       <c r="B6" s="10">
         <v>0.6875</v>
       </c>
-      <c r="C6" s="142" t="s">
+      <c r="C6" s="155" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="157"/>
+      <c r="D6" s="160"/>
       <c r="E6" s="11">
         <v>0.6875</v>
       </c>
-      <c r="F6" s="153" t="s">
+      <c r="F6" s="148" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="150"/>
+      <c r="G6" s="149"/>
       <c r="H6" s="12">
         <v>0.6875</v>
       </c>
-      <c r="I6" s="138" t="s">
+      <c r="I6" s="144" t="s">
         <v>29</v>
       </c>
-      <c r="J6" s="139"/>
+      <c r="J6" s="145"/>
       <c r="K6" s="13">
         <v>0.6875</v>
       </c>
-      <c r="L6" s="164" t="s">
+      <c r="L6" s="140" t="s">
         <v>30</v>
       </c>
-      <c r="M6" s="161"/>
+      <c r="M6" s="137"/>
     </row>
     <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="213"/>
+      <c r="A7" s="216"/>
       <c r="B7" s="14">
         <v>0.71875</v>
       </c>
-      <c r="C7" s="158"/>
-      <c r="D7" s="159"/>
+      <c r="C7" s="161"/>
+      <c r="D7" s="162"/>
       <c r="E7" s="15">
         <v>0.71875</v>
       </c>
-      <c r="F7" s="151"/>
-      <c r="G7" s="152"/>
+      <c r="F7" s="150"/>
+      <c r="G7" s="151"/>
       <c r="H7" s="16">
         <v>0.71875</v>
       </c>
-      <c r="I7" s="140"/>
-      <c r="J7" s="141"/>
+      <c r="I7" s="146"/>
+      <c r="J7" s="147"/>
       <c r="K7" s="39">
         <v>0.71875</v>
       </c>
-      <c r="L7" s="162"/>
-      <c r="M7" s="163"/>
+      <c r="L7" s="138"/>
+      <c r="M7" s="139"/>
     </row>
     <row r="8" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="214"/>
+      <c r="A8" s="217"/>
       <c r="B8" s="68">
         <f>B7-B6</f>
         <v>3.125E-2</v>
@@ -4747,54 +4747,54 @@
       <c r="M8" s="82"/>
     </row>
     <row r="9" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="212">
+      <c r="A9" s="215">
         <v>44586</v>
       </c>
       <c r="B9" s="10">
         <v>0.58333333333333337</v>
       </c>
-      <c r="C9" s="156" t="s">
+      <c r="C9" s="159" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="143"/>
+      <c r="D9" s="156"/>
       <c r="E9" s="11"/>
-      <c r="F9" s="153" t="s">
+      <c r="F9" s="148" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="150"/>
+      <c r="G9" s="149"/>
       <c r="H9" s="12"/>
-      <c r="I9" s="138" t="s">
+      <c r="I9" s="144" t="s">
         <v>24</v>
       </c>
-      <c r="J9" s="139"/>
+      <c r="J9" s="145"/>
       <c r="K9" s="40"/>
-      <c r="L9" s="160" t="s">
+      <c r="L9" s="136" t="s">
         <v>24</v>
       </c>
-      <c r="M9" s="161"/>
+      <c r="M9" s="137"/>
     </row>
     <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="213"/>
+      <c r="A10" s="216"/>
       <c r="B10" s="14">
-        <v>0.60416666666666663</v>
-      </c>
-      <c r="C10" s="144"/>
-      <c r="D10" s="145"/>
+        <v>0.6875</v>
+      </c>
+      <c r="C10" s="157"/>
+      <c r="D10" s="158"/>
       <c r="E10" s="15"/>
-      <c r="F10" s="151"/>
-      <c r="G10" s="152"/>
+      <c r="F10" s="150"/>
+      <c r="G10" s="151"/>
       <c r="H10" s="16"/>
-      <c r="I10" s="140"/>
-      <c r="J10" s="141"/>
+      <c r="I10" s="146"/>
+      <c r="J10" s="147"/>
       <c r="K10" s="39"/>
-      <c r="L10" s="162"/>
-      <c r="M10" s="163"/>
+      <c r="L10" s="138"/>
+      <c r="M10" s="139"/>
     </row>
     <row r="11" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="214"/>
+      <c r="A11" s="217"/>
       <c r="B11" s="68">
         <f>(B10-B9)</f>
-        <v>2.0833333333333259E-2</v>
+        <v>0.10416666666666663</v>
       </c>
       <c r="C11" s="69"/>
       <c r="D11" s="70"/>
@@ -4818,45 +4818,45 @@
       <c r="M11" s="82"/>
     </row>
     <row r="12" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="212"/>
+      <c r="A12" s="215"/>
       <c r="B12" s="10"/>
-      <c r="C12" s="142" t="s">
+      <c r="C12" s="155" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="143"/>
+      <c r="D12" s="156"/>
       <c r="E12" s="11"/>
-      <c r="F12" s="149" t="s">
+      <c r="F12" s="152" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="150"/>
+      <c r="G12" s="149"/>
       <c r="H12" s="12"/>
-      <c r="I12" s="138" t="s">
+      <c r="I12" s="144" t="s">
         <v>24</v>
       </c>
-      <c r="J12" s="139"/>
+      <c r="J12" s="145"/>
       <c r="K12" s="40"/>
-      <c r="L12" s="160" t="s">
+      <c r="L12" s="136" t="s">
         <v>24</v>
       </c>
-      <c r="M12" s="161"/>
+      <c r="M12" s="137"/>
     </row>
     <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="213"/>
+      <c r="A13" s="216"/>
       <c r="B13" s="14"/>
-      <c r="C13" s="144"/>
-      <c r="D13" s="145"/>
+      <c r="C13" s="157"/>
+      <c r="D13" s="158"/>
       <c r="E13" s="15"/>
-      <c r="F13" s="151"/>
-      <c r="G13" s="152"/>
+      <c r="F13" s="150"/>
+      <c r="G13" s="151"/>
       <c r="H13" s="16"/>
-      <c r="I13" s="140"/>
-      <c r="J13" s="141"/>
+      <c r="I13" s="146"/>
+      <c r="J13" s="147"/>
       <c r="K13" s="34"/>
-      <c r="L13" s="162"/>
-      <c r="M13" s="163"/>
+      <c r="L13" s="138"/>
+      <c r="M13" s="139"/>
     </row>
     <row r="14" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="214"/>
+      <c r="A14" s="217"/>
       <c r="B14" s="68">
         <f>(B13-B12)</f>
         <v>0</v>
@@ -4883,45 +4883,45 @@
       <c r="M14" s="84"/>
     </row>
     <row r="15" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="212"/>
+      <c r="A15" s="215"/>
       <c r="B15" s="10"/>
-      <c r="C15" s="142" t="s">
+      <c r="C15" s="155" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="143"/>
+      <c r="D15" s="156"/>
       <c r="E15" s="11"/>
-      <c r="F15" s="149" t="s">
+      <c r="F15" s="152" t="s">
         <v>24</v>
       </c>
-      <c r="G15" s="150"/>
+      <c r="G15" s="149"/>
       <c r="H15" s="12"/>
-      <c r="I15" s="138" t="s">
+      <c r="I15" s="144" t="s">
         <v>24</v>
       </c>
-      <c r="J15" s="139"/>
+      <c r="J15" s="145"/>
       <c r="K15" s="33"/>
-      <c r="L15" s="160" t="s">
+      <c r="L15" s="136" t="s">
         <v>24</v>
       </c>
-      <c r="M15" s="161"/>
+      <c r="M15" s="137"/>
     </row>
     <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="213"/>
+      <c r="A16" s="216"/>
       <c r="B16" s="14"/>
-      <c r="C16" s="144"/>
-      <c r="D16" s="145"/>
+      <c r="C16" s="157"/>
+      <c r="D16" s="158"/>
       <c r="E16" s="15"/>
-      <c r="F16" s="151"/>
-      <c r="G16" s="152"/>
+      <c r="F16" s="150"/>
+      <c r="G16" s="151"/>
       <c r="H16" s="16"/>
-      <c r="I16" s="140"/>
-      <c r="J16" s="141"/>
+      <c r="I16" s="146"/>
+      <c r="J16" s="147"/>
       <c r="K16" s="39"/>
-      <c r="L16" s="162"/>
-      <c r="M16" s="163"/>
+      <c r="L16" s="138"/>
+      <c r="M16" s="139"/>
     </row>
     <row r="17" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="214"/>
+      <c r="A17" s="217"/>
       <c r="B17" s="68">
         <f>(B16-B15)</f>
         <v>0</v>
@@ -4948,45 +4948,45 @@
       <c r="M17" s="82"/>
     </row>
     <row r="18" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="212"/>
+      <c r="A18" s="215"/>
       <c r="B18" s="10"/>
-      <c r="C18" s="142" t="s">
+      <c r="C18" s="155" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="143"/>
+      <c r="D18" s="156"/>
       <c r="E18" s="11"/>
-      <c r="F18" s="149" t="s">
+      <c r="F18" s="152" t="s">
         <v>24</v>
       </c>
-      <c r="G18" s="150"/>
+      <c r="G18" s="149"/>
       <c r="H18" s="12"/>
-      <c r="I18" s="138" t="s">
+      <c r="I18" s="144" t="s">
         <v>24</v>
       </c>
-      <c r="J18" s="139"/>
+      <c r="J18" s="145"/>
       <c r="K18" s="40"/>
-      <c r="L18" s="160" t="s">
+      <c r="L18" s="136" t="s">
         <v>24</v>
       </c>
-      <c r="M18" s="161"/>
+      <c r="M18" s="137"/>
     </row>
     <row r="19" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="213"/>
+      <c r="A19" s="216"/>
       <c r="B19" s="14"/>
-      <c r="C19" s="144"/>
-      <c r="D19" s="145"/>
+      <c r="C19" s="157"/>
+      <c r="D19" s="158"/>
       <c r="E19" s="15"/>
-      <c r="F19" s="151"/>
-      <c r="G19" s="152"/>
+      <c r="F19" s="150"/>
+      <c r="G19" s="151"/>
       <c r="H19" s="16"/>
-      <c r="I19" s="140"/>
-      <c r="J19" s="141"/>
+      <c r="I19" s="146"/>
+      <c r="J19" s="147"/>
       <c r="K19" s="39"/>
-      <c r="L19" s="162"/>
-      <c r="M19" s="163"/>
+      <c r="L19" s="138"/>
+      <c r="M19" s="139"/>
     </row>
     <row r="20" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="214"/>
+      <c r="A20" s="217"/>
       <c r="B20" s="68">
         <f>(B19-B18)</f>
         <v>0</v>
@@ -5013,45 +5013,45 @@
       <c r="M20" s="82"/>
     </row>
     <row r="21" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="212"/>
+      <c r="A21" s="215"/>
       <c r="B21" s="10"/>
-      <c r="C21" s="142" t="s">
+      <c r="C21" s="155" t="s">
         <v>23</v>
       </c>
-      <c r="D21" s="143"/>
+      <c r="D21" s="156"/>
       <c r="E21" s="11"/>
-      <c r="F21" s="149" t="s">
+      <c r="F21" s="152" t="s">
         <v>24</v>
       </c>
-      <c r="G21" s="150"/>
+      <c r="G21" s="149"/>
       <c r="H21" s="12"/>
-      <c r="I21" s="138" t="s">
+      <c r="I21" s="144" t="s">
         <v>24</v>
       </c>
-      <c r="J21" s="139"/>
+      <c r="J21" s="145"/>
       <c r="K21" s="33"/>
-      <c r="L21" s="160" t="s">
+      <c r="L21" s="136" t="s">
         <v>24</v>
       </c>
-      <c r="M21" s="161"/>
+      <c r="M21" s="137"/>
     </row>
     <row r="22" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="213"/>
+      <c r="A22" s="216"/>
       <c r="B22" s="14"/>
-      <c r="C22" s="144"/>
-      <c r="D22" s="145"/>
+      <c r="C22" s="157"/>
+      <c r="D22" s="158"/>
       <c r="E22" s="15"/>
-      <c r="F22" s="151"/>
-      <c r="G22" s="152"/>
+      <c r="F22" s="150"/>
+      <c r="G22" s="151"/>
       <c r="H22" s="16"/>
-      <c r="I22" s="140"/>
-      <c r="J22" s="141"/>
+      <c r="I22" s="146"/>
+      <c r="J22" s="147"/>
       <c r="K22" s="34"/>
-      <c r="L22" s="162"/>
-      <c r="M22" s="163"/>
+      <c r="L22" s="138"/>
+      <c r="M22" s="139"/>
     </row>
     <row r="23" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="214"/>
+      <c r="A23" s="217"/>
       <c r="B23" s="68">
         <f>(B22-B21)</f>
         <v>0</v>
@@ -5079,10 +5079,10 @@
     </row>
     <row r="24" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
     <row r="29" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A29" s="136" t="s">
+      <c r="A29" s="163" t="s">
         <v>21</v>
       </c>
-      <c r="B29" s="137"/>
+      <c r="B29" s="164"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="96" t="s">
@@ -5090,7 +5090,7 @@
       </c>
       <c r="B30" s="95">
         <f>C2+F2+I2+L2</f>
-        <v>0.47916666666666674</v>
+        <v>0.56250000000000011</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.35">
@@ -5099,48 +5099,48 @@
       </c>
       <c r="B31" s="95">
         <f>D2+G2+J2+M2</f>
-        <v>5.44722222222223</v>
+        <v>5.5305555555555621</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="C18:D19"/>
+    <mergeCell ref="F18:G19"/>
+    <mergeCell ref="I18:J19"/>
+    <mergeCell ref="L18:M19"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="C21:D22"/>
+    <mergeCell ref="F21:G22"/>
+    <mergeCell ref="I21:J22"/>
+    <mergeCell ref="L21:M22"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="C12:D13"/>
+    <mergeCell ref="F12:G13"/>
+    <mergeCell ref="I12:J13"/>
+    <mergeCell ref="L12:M13"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="C15:D16"/>
+    <mergeCell ref="F15:G16"/>
+    <mergeCell ref="I15:J16"/>
+    <mergeCell ref="L15:M16"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="C6:D7"/>
+    <mergeCell ref="F6:G7"/>
+    <mergeCell ref="I6:J7"/>
+    <mergeCell ref="L6:M7"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="C9:D10"/>
+    <mergeCell ref="F9:G10"/>
+    <mergeCell ref="I9:J10"/>
+    <mergeCell ref="L9:M10"/>
     <mergeCell ref="L3:M4"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="C3:D4"/>
     <mergeCell ref="F3:G4"/>
     <mergeCell ref="I3:J4"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="C9:D10"/>
-    <mergeCell ref="F9:G10"/>
-    <mergeCell ref="I9:J10"/>
-    <mergeCell ref="L9:M10"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="C6:D7"/>
-    <mergeCell ref="F6:G7"/>
-    <mergeCell ref="I6:J7"/>
-    <mergeCell ref="L6:M7"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="C15:D16"/>
-    <mergeCell ref="F15:G16"/>
-    <mergeCell ref="I15:J16"/>
-    <mergeCell ref="L15:M16"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="C12:D13"/>
-    <mergeCell ref="F12:G13"/>
-    <mergeCell ref="I12:J13"/>
-    <mergeCell ref="L12:M13"/>
-    <mergeCell ref="L18:M19"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="C21:D22"/>
-    <mergeCell ref="F21:G22"/>
-    <mergeCell ref="I21:J22"/>
-    <mergeCell ref="L21:M22"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="C18:D19"/>
-    <mergeCell ref="F18:G19"/>
-    <mergeCell ref="I18:J19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
added UI Prefab and fixed some bugs and scaling issues
</commit_message>
<xml_diff>
--- a/Zeitaufzeichnung_Ishjarta.xlsx
+++ b/Zeitaufzeichnung_Ishjarta.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danijel\Desktop\ishjarta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73533DB8-503D-4ECF-B60D-15C371455013}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBEA8F29-FE81-4604-A351-4BDE3482F87C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Vorlage" sheetId="8" r:id="rId1"/>
+    <sheet name="Vorlage" sheetId="13" r:id="rId1"/>
     <sheet name="Sprint_1" sheetId="2" r:id="rId2"/>
     <sheet name="Sprint_2" sheetId="3" r:id="rId3"/>
     <sheet name="Sprint_3" sheetId="11" r:id="rId4"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="35">
   <si>
     <t>Balog Danijel</t>
   </si>
@@ -337,6 +337,73 @@
         <family val="2"/>
       </rPr>
       <t>Minimap, auf das neue Unity Input System wechseln.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Aufgabe:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Aufgabe:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Sprint Review</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Aufgabe:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>UI</t>
     </r>
   </si>
 </sst>
@@ -985,7 +1052,7 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="221">
+  <cellXfs count="217">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -1203,63 +1270,6 @@
     <xf numFmtId="0" fontId="2" fillId="17" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="20" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="19" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="13" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="14" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="13" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="3" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="14" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="6" borderId="27" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="6" borderId="9" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="6" borderId="11" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="5" borderId="13" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="5" borderId="3" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="5" borderId="14" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="6" borderId="13" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="6" borderId="3" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="6" borderId="14" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="6" borderId="0" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="6" borderId="20" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="6" borderId="8" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="6" borderId="1" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="22" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1308,6 +1318,63 @@
     <xf numFmtId="165" fontId="1" fillId="32" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="13" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="14" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="13" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="3" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="14" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="6" borderId="27" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="6" borderId="9" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="6" borderId="11" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="5" borderId="13" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="5" borderId="3" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="5" borderId="14" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="6" borderId="13" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="6" borderId="3" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="6" borderId="14" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="6" borderId="0" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="6" borderId="20" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="6" borderId="8" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="6" borderId="1" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="10" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1323,15 +1390,6 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="10" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="2" borderId="20" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="10" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1390,9 +1448,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="21" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="1" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1953,11 +2008,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEF2C4FC-2591-492C-A44E-E008E6F36699}">
-  <dimension ref="A1:N31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{488E87CB-D840-4426-829B-D8209C98EC03}">
+  <dimension ref="A1:O42"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1971,638 +2026,1050 @@
     <col min="9" max="10" width="13.6328125" customWidth="1"/>
     <col min="11" max="11" width="15.08984375" customWidth="1"/>
     <col min="12" max="13" width="13.6328125" customWidth="1"/>
+    <col min="14" max="14" width="19.6328125" customWidth="1"/>
+    <col min="15" max="15" width="17.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="153" t="s">
+    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="150" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="116" t="s">
+      <c r="B1" s="97" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="117" t="s">
+      <c r="C1" s="98" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="116" t="s">
+      <c r="D1" s="97" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="118" t="s">
+      <c r="E1" s="99" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="119" t="s">
+      <c r="F1" s="100" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="118" t="s">
+      <c r="G1" s="99" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="120" t="s">
+      <c r="H1" s="101" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="121" t="s">
+      <c r="I1" s="102" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="120" t="s">
+      <c r="J1" s="101" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="122" t="s">
+      <c r="K1" s="103" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="122" t="s">
+      <c r="L1" s="103" t="s">
         <v>15</v>
       </c>
-      <c r="M1" s="123" t="s">
+      <c r="M1" s="104" t="s">
         <v>16</v>
       </c>
-      <c r="N1" s="42"/>
-    </row>
-    <row r="2" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="154"/>
-      <c r="B2" s="124" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="125" cm="1">
-        <f t="array" ref="C2">SUM(B5:B23*(MOD(ROW(B5:B23)-2,3)=0))</f>
+      <c r="N1" s="160" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" s="160"/>
+    </row>
+    <row r="2" spans="1:15" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="151"/>
+      <c r="B2" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="106" cm="1">
+        <f t="array" ref="C2">SUM(B5:B41*(MOD(ROW(B5:B41)-2,3)=0))</f>
         <v>8.333333333333337E-2</v>
       </c>
-      <c r="D2" s="126">
-        <f>C2+Sprint_2!D2</f>
+      <c r="D2" s="107">
+        <f>C2+Sprint_3!D2</f>
+        <v>1.4472222222222233</v>
+      </c>
+      <c r="E2" s="108" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="109" cm="1">
+        <f t="array" ref="F2">SUM(E5:E41*(MOD(ROW(E5:E41)-2,3)=0))</f>
         <v>8.333333333333337E-2</v>
       </c>
-      <c r="E2" s="127" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="128" cm="1">
-        <f t="array" ref="F2">SUM(E5:E23*(MOD(ROW(E5:E23)-2,3)=0))</f>
+      <c r="G2" s="110">
+        <f>F2+Sprint_3!G2</f>
+        <v>1.257638888888891</v>
+      </c>
+      <c r="H2" s="111" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="112" cm="1">
+        <f t="array" ref="I2">SUM(H5:H41*(MOD(ROW(H5:H41)-2,3)=0))</f>
         <v>8.333333333333337E-2</v>
       </c>
-      <c r="G2" s="129">
-        <f>F2+Sprint_2!G2</f>
+      <c r="J2" s="113">
+        <f>I2+Sprint_3!J2</f>
+        <v>1.1826388888888908</v>
+      </c>
+      <c r="K2" s="114" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" s="115" cm="1">
+        <f t="array" ref="L2">SUM(K5:K41*(MOD(ROW(K5:K41)-2,3)=0))</f>
         <v>8.333333333333337E-2</v>
       </c>
-      <c r="H2" s="130" t="s">
-        <v>2</v>
-      </c>
-      <c r="I2" s="131" cm="1">
-        <f t="array" ref="I2">SUM(H5:H23*(MOD(ROW(H5:H23)-2,3)=0))</f>
-        <v>8.333333333333337E-2</v>
-      </c>
-      <c r="J2" s="132">
-        <f>I2+Sprint_2!J2</f>
-        <v>8.333333333333337E-2</v>
-      </c>
-      <c r="K2" s="133" t="s">
-        <v>3</v>
-      </c>
-      <c r="L2" s="134" cm="1">
-        <f t="array" ref="L2">SUM(K5:K23*(MOD(ROW(K5:K23)-2,3)=0))</f>
-        <v>8.333333333333337E-2</v>
-      </c>
-      <c r="M2" s="135">
-        <f>L2+Sprint_2!M2</f>
-        <v>8.333333333333337E-2</v>
-      </c>
-      <c r="N2" s="31"/>
-    </row>
-    <row r="3" spans="1:14" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="141">
-        <v>44571</v>
-      </c>
+      <c r="M2" s="116">
+        <f>L2+Sprint_3!M2</f>
+        <v>1.413888888888891</v>
+      </c>
+      <c r="N2" s="96" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" s="95">
+        <f>C2+F2+I2+L2</f>
+        <v>0.33333333333333348</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="211"/>
       <c r="B3" s="10">
         <v>0.33333333333333331</v>
       </c>
-      <c r="C3" s="155" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="156"/>
+      <c r="C3" s="152" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="153"/>
       <c r="E3" s="11">
         <v>0.33333333333333331</v>
       </c>
-      <c r="F3" s="152" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" s="149"/>
+      <c r="F3" s="149" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="146"/>
       <c r="H3" s="12">
         <v>0.33333333333333331</v>
       </c>
-      <c r="I3" s="144" t="s">
-        <v>26</v>
-      </c>
-      <c r="J3" s="145"/>
+      <c r="I3" s="141" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="142"/>
       <c r="K3" s="33">
         <v>0.33333333333333331</v>
       </c>
       <c r="L3" s="136" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="M3" s="137"/>
-    </row>
-    <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="142"/>
+      <c r="N3" s="96" t="s">
+        <v>18</v>
+      </c>
+      <c r="O3" s="95">
+        <f>D2+G2+J2+M2</f>
+        <v>5.301388888888896</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="212"/>
       <c r="B4" s="14">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C4" s="157"/>
-      <c r="D4" s="158"/>
+      <c r="C4" s="154"/>
+      <c r="D4" s="155"/>
       <c r="E4" s="15">
         <v>0.41666666666666669</v>
       </c>
-      <c r="F4" s="150"/>
-      <c r="G4" s="151"/>
+      <c r="F4" s="147"/>
+      <c r="G4" s="148"/>
       <c r="H4" s="16">
         <v>0.41666666666666669</v>
       </c>
-      <c r="I4" s="146"/>
-      <c r="J4" s="147"/>
+      <c r="I4" s="143"/>
+      <c r="J4" s="144"/>
       <c r="K4" s="39">
         <v>0.41666666666666669</v>
       </c>
       <c r="L4" s="138"/>
       <c r="M4" s="139"/>
     </row>
-    <row r="5" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="143"/>
-      <c r="B5" s="97">
+    <row r="5" spans="1:15" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="213"/>
+      <c r="B5" s="117">
         <f>B4-B3</f>
         <v>8.333333333333337E-2</v>
       </c>
-      <c r="C5" s="98"/>
-      <c r="D5" s="99"/>
-      <c r="E5" s="100">
+      <c r="C5" s="118"/>
+      <c r="D5" s="119"/>
+      <c r="E5" s="120">
         <f>E4-E3</f>
         <v>8.333333333333337E-2</v>
       </c>
-      <c r="F5" s="101"/>
-      <c r="G5" s="102"/>
-      <c r="H5" s="106">
+      <c r="F5" s="121"/>
+      <c r="G5" s="122"/>
+      <c r="H5" s="126">
         <f>H4-H3</f>
         <v>8.333333333333337E-2</v>
       </c>
-      <c r="I5" s="107"/>
-      <c r="J5" s="108"/>
-      <c r="K5" s="103">
+      <c r="I5" s="127"/>
+      <c r="J5" s="128"/>
+      <c r="K5" s="123">
         <f>K4-K3</f>
         <v>8.333333333333337E-2</v>
       </c>
-      <c r="L5" s="104"/>
-      <c r="M5" s="105"/>
-    </row>
-    <row r="6" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="141"/>
+      <c r="L5" s="124"/>
+      <c r="M5" s="125"/>
+    </row>
+    <row r="6" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="211"/>
       <c r="B6" s="10"/>
-      <c r="C6" s="155" t="s">
+      <c r="C6" s="152" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="160"/>
+      <c r="D6" s="157"/>
       <c r="E6" s="11"/>
-      <c r="F6" s="148" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="149"/>
+      <c r="F6" s="145" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="146"/>
       <c r="H6" s="12"/>
-      <c r="I6" s="144" t="s">
-        <v>24</v>
-      </c>
-      <c r="J6" s="145"/>
+      <c r="I6" s="141" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" s="142"/>
       <c r="K6" s="13"/>
       <c r="L6" s="140" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="M6" s="137"/>
     </row>
-    <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="142"/>
+    <row r="7" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="212"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="161"/>
-      <c r="D7" s="162"/>
+      <c r="C7" s="158"/>
+      <c r="D7" s="159"/>
       <c r="E7" s="15"/>
-      <c r="F7" s="150"/>
-      <c r="G7" s="151"/>
+      <c r="F7" s="147"/>
+      <c r="G7" s="148"/>
       <c r="H7" s="16"/>
-      <c r="I7" s="146"/>
-      <c r="J7" s="147"/>
+      <c r="I7" s="143"/>
+      <c r="J7" s="144"/>
       <c r="K7" s="39"/>
       <c r="L7" s="138"/>
       <c r="M7" s="139"/>
     </row>
-    <row r="8" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="143"/>
-      <c r="B8" s="97">
+    <row r="8" spans="1:15" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="213"/>
+      <c r="B8" s="117">
         <f>B7-B6</f>
         <v>0</v>
       </c>
-      <c r="C8" s="98"/>
-      <c r="D8" s="99"/>
-      <c r="E8" s="100">
+      <c r="C8" s="118"/>
+      <c r="D8" s="119"/>
+      <c r="E8" s="120">
         <f>E7-E6</f>
         <v>0</v>
       </c>
-      <c r="F8" s="101"/>
-      <c r="G8" s="102"/>
-      <c r="H8" s="106">
+      <c r="F8" s="121"/>
+      <c r="G8" s="122"/>
+      <c r="H8" s="126">
         <f>H7-H6</f>
         <v>0</v>
       </c>
-      <c r="I8" s="107"/>
-      <c r="J8" s="108"/>
-      <c r="K8" s="109">
+      <c r="I8" s="127"/>
+      <c r="J8" s="128"/>
+      <c r="K8" s="129">
         <f>K7-K6</f>
         <v>0</v>
       </c>
-      <c r="L8" s="110"/>
-      <c r="M8" s="111"/>
-    </row>
-    <row r="9" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="141"/>
+      <c r="L8" s="130"/>
+      <c r="M8" s="131"/>
+    </row>
+    <row r="9" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="211"/>
       <c r="B9" s="10"/>
-      <c r="C9" s="159" t="s">
+      <c r="C9" s="156" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="153"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="145" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="156"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="148" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="149"/>
+      <c r="G9" s="146"/>
       <c r="H9" s="12"/>
-      <c r="I9" s="144" t="s">
-        <v>24</v>
-      </c>
-      <c r="J9" s="145"/>
+      <c r="I9" s="141" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" s="142"/>
       <c r="K9" s="40"/>
       <c r="L9" s="136" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M9" s="137"/>
     </row>
-    <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="142"/>
+    <row r="10" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="212"/>
       <c r="B10" s="14"/>
-      <c r="C10" s="157"/>
-      <c r="D10" s="158"/>
+      <c r="C10" s="154"/>
+      <c r="D10" s="155"/>
       <c r="E10" s="15"/>
-      <c r="F10" s="150"/>
-      <c r="G10" s="151"/>
+      <c r="F10" s="147"/>
+      <c r="G10" s="148"/>
       <c r="H10" s="16"/>
-      <c r="I10" s="146"/>
-      <c r="J10" s="147"/>
+      <c r="I10" s="143"/>
+      <c r="J10" s="144"/>
       <c r="K10" s="39"/>
       <c r="L10" s="138"/>
       <c r="M10" s="139"/>
     </row>
-    <row r="11" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="143"/>
-      <c r="B11" s="97">
+    <row r="11" spans="1:15" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="213"/>
+      <c r="B11" s="117">
         <f>(B10-B9)</f>
         <v>0</v>
       </c>
-      <c r="C11" s="98"/>
-      <c r="D11" s="99"/>
-      <c r="E11" s="100">
+      <c r="C11" s="118"/>
+      <c r="D11" s="119"/>
+      <c r="E11" s="120">
         <f>E10-E9</f>
         <v>0</v>
       </c>
-      <c r="F11" s="101"/>
-      <c r="G11" s="102"/>
-      <c r="H11" s="106">
+      <c r="F11" s="121"/>
+      <c r="G11" s="122"/>
+      <c r="H11" s="126">
         <f>H10-H9</f>
         <v>0</v>
       </c>
-      <c r="I11" s="107"/>
-      <c r="J11" s="108"/>
-      <c r="K11" s="109">
+      <c r="I11" s="127"/>
+      <c r="J11" s="128"/>
+      <c r="K11" s="129">
         <f>K10-K9</f>
         <v>0</v>
       </c>
-      <c r="L11" s="110"/>
-      <c r="M11" s="111"/>
-    </row>
-    <row r="12" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="141"/>
+      <c r="L11" s="130"/>
+      <c r="M11" s="131"/>
+    </row>
+    <row r="12" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="211"/>
       <c r="B12" s="10"/>
-      <c r="C12" s="155" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="156"/>
+      <c r="C12" s="152" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="153"/>
       <c r="E12" s="11"/>
-      <c r="F12" s="152" t="s">
-        <v>24</v>
-      </c>
-      <c r="G12" s="149"/>
+      <c r="F12" s="149" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="146"/>
       <c r="H12" s="12"/>
-      <c r="I12" s="144" t="s">
-        <v>24</v>
-      </c>
-      <c r="J12" s="145"/>
+      <c r="I12" s="141" t="s">
+        <v>23</v>
+      </c>
+      <c r="J12" s="142"/>
       <c r="K12" s="40"/>
       <c r="L12" s="136" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M12" s="137"/>
     </row>
-    <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="142"/>
+    <row r="13" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="212"/>
       <c r="B13" s="14"/>
-      <c r="C13" s="157"/>
-      <c r="D13" s="158"/>
+      <c r="C13" s="154"/>
+      <c r="D13" s="155"/>
       <c r="E13" s="15"/>
-      <c r="F13" s="150"/>
-      <c r="G13" s="151"/>
+      <c r="F13" s="147"/>
+      <c r="G13" s="148"/>
       <c r="H13" s="16"/>
-      <c r="I13" s="146"/>
-      <c r="J13" s="147"/>
+      <c r="I13" s="143"/>
+      <c r="J13" s="144"/>
       <c r="K13" s="34"/>
       <c r="L13" s="138"/>
       <c r="M13" s="139"/>
     </row>
-    <row r="14" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="143"/>
-      <c r="B14" s="97">
+    <row r="14" spans="1:15" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="213"/>
+      <c r="B14" s="117">
         <f>(B13-B12)</f>
         <v>0</v>
       </c>
-      <c r="C14" s="98"/>
-      <c r="D14" s="99"/>
-      <c r="E14" s="100">
+      <c r="C14" s="118"/>
+      <c r="D14" s="119"/>
+      <c r="E14" s="120">
         <f>E13-E12</f>
         <v>0</v>
       </c>
-      <c r="F14" s="101"/>
-      <c r="G14" s="102"/>
-      <c r="H14" s="106">
+      <c r="F14" s="121"/>
+      <c r="G14" s="122"/>
+      <c r="H14" s="126">
         <f>H13-H12</f>
         <v>0</v>
       </c>
-      <c r="I14" s="107"/>
-      <c r="J14" s="108"/>
-      <c r="K14" s="112">
+      <c r="I14" s="127"/>
+      <c r="J14" s="128"/>
+      <c r="K14" s="132">
         <f>K13-K12</f>
         <v>0</v>
       </c>
-      <c r="L14" s="112"/>
-      <c r="M14" s="113"/>
-    </row>
-    <row r="15" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="141"/>
+      <c r="L14" s="132"/>
+      <c r="M14" s="133"/>
+    </row>
+    <row r="15" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="211"/>
       <c r="B15" s="10"/>
-      <c r="C15" s="155" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="156"/>
+      <c r="C15" s="152" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="153"/>
       <c r="E15" s="11"/>
-      <c r="F15" s="152" t="s">
-        <v>24</v>
-      </c>
-      <c r="G15" s="149"/>
+      <c r="F15" s="149" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" s="146"/>
       <c r="H15" s="12"/>
-      <c r="I15" s="144" t="s">
-        <v>24</v>
-      </c>
-      <c r="J15" s="145"/>
+      <c r="I15" s="141" t="s">
+        <v>23</v>
+      </c>
+      <c r="J15" s="142"/>
       <c r="K15" s="33"/>
       <c r="L15" s="136" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M15" s="137"/>
     </row>
-    <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="142"/>
+    <row r="16" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="212"/>
       <c r="B16" s="14"/>
-      <c r="C16" s="157"/>
-      <c r="D16" s="158"/>
+      <c r="C16" s="154"/>
+      <c r="D16" s="155"/>
       <c r="E16" s="15"/>
-      <c r="F16" s="150"/>
-      <c r="G16" s="151"/>
+      <c r="F16" s="147"/>
+      <c r="G16" s="148"/>
       <c r="H16" s="16"/>
-      <c r="I16" s="146"/>
-      <c r="J16" s="147"/>
+      <c r="I16" s="143"/>
+      <c r="J16" s="144"/>
       <c r="K16" s="39"/>
       <c r="L16" s="138"/>
       <c r="M16" s="139"/>
     </row>
     <row r="17" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="143"/>
-      <c r="B17" s="97">
+      <c r="A17" s="213"/>
+      <c r="B17" s="117">
         <f>(B16-B15)</f>
         <v>0</v>
       </c>
-      <c r="C17" s="98"/>
-      <c r="D17" s="99"/>
-      <c r="E17" s="100">
+      <c r="C17" s="118"/>
+      <c r="D17" s="119"/>
+      <c r="E17" s="120">
         <f>E16-E15</f>
         <v>0</v>
       </c>
-      <c r="F17" s="101"/>
-      <c r="G17" s="102"/>
-      <c r="H17" s="106">
+      <c r="F17" s="121"/>
+      <c r="G17" s="122"/>
+      <c r="H17" s="126">
         <f>H16-H15</f>
         <v>0</v>
       </c>
-      <c r="I17" s="107"/>
-      <c r="J17" s="108"/>
-      <c r="K17" s="109">
+      <c r="I17" s="127"/>
+      <c r="J17" s="128"/>
+      <c r="K17" s="129">
         <f>K16-K15</f>
         <v>0</v>
       </c>
-      <c r="L17" s="110"/>
-      <c r="M17" s="111"/>
+      <c r="L17" s="130"/>
+      <c r="M17" s="131"/>
     </row>
     <row r="18" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="141"/>
+      <c r="A18" s="211"/>
       <c r="B18" s="10"/>
-      <c r="C18" s="155" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" s="156"/>
+      <c r="C18" s="152" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="153"/>
       <c r="E18" s="11"/>
-      <c r="F18" s="152" t="s">
-        <v>24</v>
-      </c>
-      <c r="G18" s="149"/>
+      <c r="F18" s="149" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" s="146"/>
       <c r="H18" s="12"/>
-      <c r="I18" s="144" t="s">
-        <v>24</v>
-      </c>
-      <c r="J18" s="145"/>
+      <c r="I18" s="141" t="s">
+        <v>23</v>
+      </c>
+      <c r="J18" s="142"/>
       <c r="K18" s="40"/>
       <c r="L18" s="136" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M18" s="137"/>
     </row>
     <row r="19" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="142"/>
+      <c r="A19" s="212"/>
       <c r="B19" s="14"/>
-      <c r="C19" s="157"/>
-      <c r="D19" s="158"/>
+      <c r="C19" s="154"/>
+      <c r="D19" s="155"/>
       <c r="E19" s="15"/>
-      <c r="F19" s="150"/>
-      <c r="G19" s="151"/>
+      <c r="F19" s="147"/>
+      <c r="G19" s="148"/>
       <c r="H19" s="16"/>
-      <c r="I19" s="146"/>
-      <c r="J19" s="147"/>
+      <c r="I19" s="143"/>
+      <c r="J19" s="144"/>
       <c r="K19" s="39"/>
       <c r="L19" s="138"/>
       <c r="M19" s="139"/>
     </row>
     <row r="20" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="143"/>
-      <c r="B20" s="97">
+      <c r="A20" s="213"/>
+      <c r="B20" s="117">
         <f>(B19-B18)</f>
         <v>0</v>
       </c>
-      <c r="C20" s="98"/>
-      <c r="D20" s="99"/>
-      <c r="E20" s="100">
+      <c r="C20" s="118"/>
+      <c r="D20" s="119"/>
+      <c r="E20" s="120">
         <f>E19-E18</f>
         <v>0</v>
       </c>
-      <c r="F20" s="101"/>
-      <c r="G20" s="102"/>
-      <c r="H20" s="106">
+      <c r="F20" s="121"/>
+      <c r="G20" s="122"/>
+      <c r="H20" s="126">
         <f>H19-H18</f>
         <v>0</v>
       </c>
-      <c r="I20" s="107"/>
-      <c r="J20" s="108"/>
-      <c r="K20" s="109">
+      <c r="I20" s="127"/>
+      <c r="J20" s="128"/>
+      <c r="K20" s="129">
         <f>K19-K18</f>
         <v>0</v>
       </c>
-      <c r="L20" s="110"/>
-      <c r="M20" s="111"/>
+      <c r="L20" s="130"/>
+      <c r="M20" s="131"/>
     </row>
     <row r="21" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="141"/>
+      <c r="A21" s="211"/>
       <c r="B21" s="10"/>
-      <c r="C21" s="155" t="s">
-        <v>23</v>
-      </c>
-      <c r="D21" s="156"/>
+      <c r="C21" s="152" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="153"/>
       <c r="E21" s="11"/>
-      <c r="F21" s="152" t="s">
-        <v>24</v>
-      </c>
-      <c r="G21" s="149"/>
+      <c r="F21" s="149" t="s">
+        <v>23</v>
+      </c>
+      <c r="G21" s="146"/>
       <c r="H21" s="12"/>
-      <c r="I21" s="144" t="s">
-        <v>24</v>
-      </c>
-      <c r="J21" s="145"/>
+      <c r="I21" s="141" t="s">
+        <v>23</v>
+      </c>
+      <c r="J21" s="142"/>
       <c r="K21" s="33"/>
       <c r="L21" s="136" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M21" s="137"/>
     </row>
     <row r="22" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="142"/>
+      <c r="A22" s="212"/>
       <c r="B22" s="14"/>
-      <c r="C22" s="157"/>
-      <c r="D22" s="158"/>
+      <c r="C22" s="154"/>
+      <c r="D22" s="155"/>
       <c r="E22" s="15"/>
-      <c r="F22" s="150"/>
-      <c r="G22" s="151"/>
+      <c r="F22" s="147"/>
+      <c r="G22" s="148"/>
       <c r="H22" s="16"/>
-      <c r="I22" s="146"/>
-      <c r="J22" s="147"/>
+      <c r="I22" s="143"/>
+      <c r="J22" s="144"/>
       <c r="K22" s="34"/>
       <c r="L22" s="138"/>
       <c r="M22" s="139"/>
     </row>
     <row r="23" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="143"/>
-      <c r="B23" s="97">
+      <c r="A23" s="213"/>
+      <c r="B23" s="117">
         <f>(B22-B21)</f>
         <v>0</v>
       </c>
-      <c r="C23" s="98"/>
-      <c r="D23" s="99"/>
-      <c r="E23" s="100">
+      <c r="C23" s="118"/>
+      <c r="D23" s="119"/>
+      <c r="E23" s="120">
         <f>E22-E21</f>
         <v>0</v>
       </c>
-      <c r="F23" s="101"/>
-      <c r="G23" s="102"/>
-      <c r="H23" s="106">
+      <c r="F23" s="121"/>
+      <c r="G23" s="122"/>
+      <c r="H23" s="126">
         <f>H22-H21</f>
         <v>0</v>
       </c>
-      <c r="I23" s="107"/>
-      <c r="J23" s="108"/>
-      <c r="K23" s="114">
+      <c r="I23" s="127"/>
+      <c r="J23" s="128"/>
+      <c r="K23" s="134">
         <f>K22-K21</f>
         <v>0</v>
       </c>
-      <c r="L23" s="114"/>
-      <c r="M23" s="115"/>
-    </row>
-    <row r="24" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A29" s="163" t="s">
-        <v>21</v>
-      </c>
-      <c r="B29" s="164"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A30" s="96" t="s">
-        <v>15</v>
-      </c>
-      <c r="B30" s="95">
-        <f>C2+F2+I2+L2</f>
-        <v>0.33333333333333348</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A31" s="96" t="s">
-        <v>18</v>
-      </c>
-      <c r="B31" s="95">
-        <f>D2+G2+J2+M2</f>
-        <v>0.33333333333333348</v>
-      </c>
-    </row>
+      <c r="L23" s="134"/>
+      <c r="M23" s="135"/>
+    </row>
+    <row r="24" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="211"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="152" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="153"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="149" t="s">
+        <v>23</v>
+      </c>
+      <c r="G24" s="146"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="141" t="s">
+        <v>23</v>
+      </c>
+      <c r="J24" s="142"/>
+      <c r="K24" s="33"/>
+      <c r="L24" s="136" t="s">
+        <v>23</v>
+      </c>
+      <c r="M24" s="137"/>
+    </row>
+    <row r="25" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="212"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="154"/>
+      <c r="D25" s="155"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="147"/>
+      <c r="G25" s="148"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="143"/>
+      <c r="J25" s="144"/>
+      <c r="K25" s="39"/>
+      <c r="L25" s="138"/>
+      <c r="M25" s="139"/>
+    </row>
+    <row r="26" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="213"/>
+      <c r="B26" s="117">
+        <f>(B25-B24)</f>
+        <v>0</v>
+      </c>
+      <c r="C26" s="118"/>
+      <c r="D26" s="119"/>
+      <c r="E26" s="120">
+        <f>E25-E24</f>
+        <v>0</v>
+      </c>
+      <c r="F26" s="121"/>
+      <c r="G26" s="122"/>
+      <c r="H26" s="126">
+        <f>H25-H24</f>
+        <v>0</v>
+      </c>
+      <c r="I26" s="127"/>
+      <c r="J26" s="128"/>
+      <c r="K26" s="129">
+        <f>K25-K24</f>
+        <v>0</v>
+      </c>
+      <c r="L26" s="130"/>
+      <c r="M26" s="131"/>
+    </row>
+    <row r="27" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="211"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="152" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" s="153"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="149" t="s">
+        <v>23</v>
+      </c>
+      <c r="G27" s="146"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="141" t="s">
+        <v>23</v>
+      </c>
+      <c r="J27" s="142"/>
+      <c r="K27" s="40"/>
+      <c r="L27" s="136" t="s">
+        <v>23</v>
+      </c>
+      <c r="M27" s="137"/>
+    </row>
+    <row r="28" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="212"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="154"/>
+      <c r="D28" s="155"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="147"/>
+      <c r="G28" s="148"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="143"/>
+      <c r="J28" s="144"/>
+      <c r="K28" s="39"/>
+      <c r="L28" s="138"/>
+      <c r="M28" s="139"/>
+    </row>
+    <row r="29" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="213"/>
+      <c r="B29" s="117">
+        <f>(B28-B27)</f>
+        <v>0</v>
+      </c>
+      <c r="C29" s="118"/>
+      <c r="D29" s="119"/>
+      <c r="E29" s="120">
+        <f>E28-E27</f>
+        <v>0</v>
+      </c>
+      <c r="F29" s="121"/>
+      <c r="G29" s="122"/>
+      <c r="H29" s="126">
+        <f>H28-H27</f>
+        <v>0</v>
+      </c>
+      <c r="I29" s="127"/>
+      <c r="J29" s="128"/>
+      <c r="K29" s="129">
+        <f>K28-K27</f>
+        <v>0</v>
+      </c>
+      <c r="L29" s="130"/>
+      <c r="M29" s="131"/>
+    </row>
+    <row r="30" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="211"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="152" t="s">
+        <v>23</v>
+      </c>
+      <c r="D30" s="153"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="149" t="s">
+        <v>23</v>
+      </c>
+      <c r="G30" s="146"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="141" t="s">
+        <v>23</v>
+      </c>
+      <c r="J30" s="142"/>
+      <c r="K30" s="33"/>
+      <c r="L30" s="136" t="s">
+        <v>23</v>
+      </c>
+      <c r="M30" s="137"/>
+    </row>
+    <row r="31" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="212"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="154"/>
+      <c r="D31" s="155"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="147"/>
+      <c r="G31" s="148"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="143"/>
+      <c r="J31" s="144"/>
+      <c r="K31" s="34"/>
+      <c r="L31" s="138"/>
+      <c r="M31" s="139"/>
+    </row>
+    <row r="32" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="213"/>
+      <c r="B32" s="117">
+        <f>(B31-B30)</f>
+        <v>0</v>
+      </c>
+      <c r="C32" s="118"/>
+      <c r="D32" s="119"/>
+      <c r="E32" s="120">
+        <f>E31-E30</f>
+        <v>0</v>
+      </c>
+      <c r="F32" s="121"/>
+      <c r="G32" s="122"/>
+      <c r="H32" s="126">
+        <f>H31-H30</f>
+        <v>0</v>
+      </c>
+      <c r="I32" s="127"/>
+      <c r="J32" s="128"/>
+      <c r="K32" s="134">
+        <f>K31-K30</f>
+        <v>0</v>
+      </c>
+      <c r="L32" s="134"/>
+      <c r="M32" s="135"/>
+    </row>
+    <row r="33" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="211"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="152" t="s">
+        <v>23</v>
+      </c>
+      <c r="D33" s="153"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="149" t="s">
+        <v>23</v>
+      </c>
+      <c r="G33" s="146"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="141" t="s">
+        <v>23</v>
+      </c>
+      <c r="J33" s="142"/>
+      <c r="K33" s="33"/>
+      <c r="L33" s="136" t="s">
+        <v>23</v>
+      </c>
+      <c r="M33" s="137"/>
+    </row>
+    <row r="34" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="212"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="154"/>
+      <c r="D34" s="155"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="147"/>
+      <c r="G34" s="148"/>
+      <c r="H34" s="16"/>
+      <c r="I34" s="143"/>
+      <c r="J34" s="144"/>
+      <c r="K34" s="39"/>
+      <c r="L34" s="138"/>
+      <c r="M34" s="139"/>
+    </row>
+    <row r="35" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="213"/>
+      <c r="B35" s="117">
+        <f>(B34-B33)</f>
+        <v>0</v>
+      </c>
+      <c r="C35" s="118"/>
+      <c r="D35" s="119"/>
+      <c r="E35" s="120">
+        <f>E34-E33</f>
+        <v>0</v>
+      </c>
+      <c r="F35" s="121"/>
+      <c r="G35" s="122"/>
+      <c r="H35" s="126">
+        <f>H34-H33</f>
+        <v>0</v>
+      </c>
+      <c r="I35" s="127"/>
+      <c r="J35" s="128"/>
+      <c r="K35" s="129">
+        <f>K34-K33</f>
+        <v>0</v>
+      </c>
+      <c r="L35" s="130"/>
+      <c r="M35" s="131"/>
+    </row>
+    <row r="36" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="211"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="152" t="s">
+        <v>23</v>
+      </c>
+      <c r="D36" s="153"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="149" t="s">
+        <v>23</v>
+      </c>
+      <c r="G36" s="146"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="141" t="s">
+        <v>23</v>
+      </c>
+      <c r="J36" s="142"/>
+      <c r="K36" s="40"/>
+      <c r="L36" s="136" t="s">
+        <v>23</v>
+      </c>
+      <c r="M36" s="137"/>
+    </row>
+    <row r="37" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="212"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="154"/>
+      <c r="D37" s="155"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="147"/>
+      <c r="G37" s="148"/>
+      <c r="H37" s="16"/>
+      <c r="I37" s="143"/>
+      <c r="J37" s="144"/>
+      <c r="K37" s="39"/>
+      <c r="L37" s="138"/>
+      <c r="M37" s="139"/>
+    </row>
+    <row r="38" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="213"/>
+      <c r="B38" s="117">
+        <f>(B37-B36)</f>
+        <v>0</v>
+      </c>
+      <c r="C38" s="118"/>
+      <c r="D38" s="119"/>
+      <c r="E38" s="120">
+        <f>E37-E36</f>
+        <v>0</v>
+      </c>
+      <c r="F38" s="121"/>
+      <c r="G38" s="122"/>
+      <c r="H38" s="126">
+        <f>H37-H36</f>
+        <v>0</v>
+      </c>
+      <c r="I38" s="127"/>
+      <c r="J38" s="128"/>
+      <c r="K38" s="129">
+        <f>K37-K36</f>
+        <v>0</v>
+      </c>
+      <c r="L38" s="130"/>
+      <c r="M38" s="131"/>
+    </row>
+    <row r="39" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="211"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="152" t="s">
+        <v>23</v>
+      </c>
+      <c r="D39" s="153"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="149" t="s">
+        <v>23</v>
+      </c>
+      <c r="G39" s="146"/>
+      <c r="H39" s="12"/>
+      <c r="I39" s="141" t="s">
+        <v>23</v>
+      </c>
+      <c r="J39" s="142"/>
+      <c r="K39" s="33"/>
+      <c r="L39" s="136" t="s">
+        <v>23</v>
+      </c>
+      <c r="M39" s="137"/>
+    </row>
+    <row r="40" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A40" s="212"/>
+      <c r="B40" s="14"/>
+      <c r="C40" s="154"/>
+      <c r="D40" s="155"/>
+      <c r="E40" s="15"/>
+      <c r="F40" s="147"/>
+      <c r="G40" s="148"/>
+      <c r="H40" s="16"/>
+      <c r="I40" s="143"/>
+      <c r="J40" s="144"/>
+      <c r="K40" s="34"/>
+      <c r="L40" s="138"/>
+      <c r="M40" s="139"/>
+    </row>
+    <row r="41" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A41" s="213"/>
+      <c r="B41" s="117">
+        <f>(B40-B39)</f>
+        <v>0</v>
+      </c>
+      <c r="C41" s="118"/>
+      <c r="D41" s="119"/>
+      <c r="E41" s="120">
+        <f>E40-E39</f>
+        <v>0</v>
+      </c>
+      <c r="F41" s="121"/>
+      <c r="G41" s="122"/>
+      <c r="H41" s="126">
+        <f>H40-H39</f>
+        <v>0</v>
+      </c>
+      <c r="I41" s="127"/>
+      <c r="J41" s="128"/>
+      <c r="K41" s="134">
+        <f>K40-K39</f>
+        <v>0</v>
+      </c>
+      <c r="L41" s="134"/>
+      <c r="M41" s="135"/>
+    </row>
+    <row r="42" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
-  <mergeCells count="37">
-    <mergeCell ref="A29:B29"/>
+  <mergeCells count="67">
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="C36:D37"/>
+    <mergeCell ref="F36:G37"/>
+    <mergeCell ref="I36:J37"/>
+    <mergeCell ref="L36:M37"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="C39:D40"/>
+    <mergeCell ref="F39:G40"/>
+    <mergeCell ref="I39:J40"/>
+    <mergeCell ref="L39:M40"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="C30:D31"/>
+    <mergeCell ref="F30:G31"/>
+    <mergeCell ref="I30:J31"/>
+    <mergeCell ref="L30:M31"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="C33:D34"/>
+    <mergeCell ref="F33:G34"/>
+    <mergeCell ref="I33:J34"/>
+    <mergeCell ref="L33:M34"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="C24:D25"/>
+    <mergeCell ref="F24:G25"/>
+    <mergeCell ref="I24:J25"/>
+    <mergeCell ref="L24:M25"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="C27:D28"/>
+    <mergeCell ref="F27:G28"/>
+    <mergeCell ref="I27:J28"/>
+    <mergeCell ref="L27:M28"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="C18:D19"/>
+    <mergeCell ref="F18:G19"/>
+    <mergeCell ref="I18:J19"/>
+    <mergeCell ref="L18:M19"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="C21:D22"/>
+    <mergeCell ref="F21:G22"/>
     <mergeCell ref="I21:J22"/>
-    <mergeCell ref="I18:J19"/>
+    <mergeCell ref="L21:M22"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="C12:D13"/>
+    <mergeCell ref="F12:G13"/>
+    <mergeCell ref="I12:J13"/>
+    <mergeCell ref="L12:M13"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="C15:D16"/>
+    <mergeCell ref="F15:G16"/>
     <mergeCell ref="I15:J16"/>
-    <mergeCell ref="I12:J13"/>
-    <mergeCell ref="C21:D22"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="F21:G22"/>
-    <mergeCell ref="F18:G19"/>
-    <mergeCell ref="F15:G16"/>
-    <mergeCell ref="F12:G13"/>
+    <mergeCell ref="L15:M16"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="C6:D7"/>
+    <mergeCell ref="F6:G7"/>
+    <mergeCell ref="I6:J7"/>
+    <mergeCell ref="L6:M7"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="C9:D10"/>
+    <mergeCell ref="F9:G10"/>
+    <mergeCell ref="I9:J10"/>
+    <mergeCell ref="L9:M10"/>
     <mergeCell ref="A1:A2"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="A3:A5"/>
     <mergeCell ref="C3:D4"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="C18:D19"/>
-    <mergeCell ref="C15:D16"/>
-    <mergeCell ref="C12:D13"/>
-    <mergeCell ref="C9:D10"/>
-    <mergeCell ref="C6:D7"/>
-    <mergeCell ref="L21:M22"/>
-    <mergeCell ref="L18:M19"/>
-    <mergeCell ref="L15:M16"/>
-    <mergeCell ref="L12:M13"/>
-    <mergeCell ref="L9:M10"/>
+    <mergeCell ref="F3:G4"/>
+    <mergeCell ref="I3:J4"/>
     <mergeCell ref="L3:M4"/>
-    <mergeCell ref="L6:M7"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="I3:J4"/>
-    <mergeCell ref="F6:G7"/>
-    <mergeCell ref="F3:G4"/>
-    <mergeCell ref="I6:J7"/>
-    <mergeCell ref="I9:J10"/>
-    <mergeCell ref="F9:G10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2652,407 +3119,407 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="165">
+      <c r="A2" s="161">
         <v>44535</v>
       </c>
       <c r="B2" s="18">
         <v>0.83333333333333304</v>
       </c>
-      <c r="C2" s="166"/>
+      <c r="C2" s="162"/>
       <c r="D2" s="11">
         <v>0.83333333333333304</v>
       </c>
-      <c r="E2" s="167" t="s">
+      <c r="E2" s="163" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="12">
         <v>0.83333333333333304</v>
       </c>
-      <c r="G2" s="168" t="s">
+      <c r="G2" s="164" t="s">
         <v>4</v>
       </c>
       <c r="H2" s="13">
         <v>0.83333333333333304</v>
       </c>
-      <c r="I2" s="169" t="s">
+      <c r="I2" s="165" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="165"/>
+      <c r="A3" s="161"/>
       <c r="B3" s="14">
         <v>1</v>
       </c>
-      <c r="C3" s="166"/>
+      <c r="C3" s="162"/>
       <c r="D3" s="15">
         <v>1</v>
       </c>
-      <c r="E3" s="167"/>
+      <c r="E3" s="163"/>
       <c r="F3" s="16">
         <v>1</v>
       </c>
-      <c r="G3" s="168"/>
+      <c r="G3" s="164"/>
       <c r="H3" s="17">
         <v>1</v>
       </c>
-      <c r="I3" s="169"/>
+      <c r="I3" s="165"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="165"/>
-      <c r="B4" s="170">
+      <c r="A4" s="161"/>
+      <c r="B4" s="166">
         <f>B3-B2</f>
         <v>0.16666666666666696</v>
       </c>
-      <c r="C4" s="170"/>
-      <c r="D4" s="171">
+      <c r="C4" s="166"/>
+      <c r="D4" s="167">
         <f>D3-D2</f>
         <v>0.16666666666666696</v>
       </c>
-      <c r="E4" s="171"/>
-      <c r="F4" s="172">
+      <c r="E4" s="167"/>
+      <c r="F4" s="168">
         <f>F3-F2</f>
         <v>0.16666666666666696</v>
       </c>
-      <c r="G4" s="172"/>
-      <c r="H4" s="173">
+      <c r="G4" s="168"/>
+      <c r="H4" s="169">
         <f>H3-H2</f>
         <v>0.16666666666666696</v>
       </c>
-      <c r="I4" s="173"/>
+      <c r="I4" s="169"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="165">
+      <c r="A5" s="161">
         <v>44542</v>
       </c>
       <c r="B5" s="18">
         <v>0.83333333333333304</v>
       </c>
-      <c r="C5" s="166"/>
+      <c r="C5" s="162"/>
       <c r="D5" s="11">
         <v>0.83333333333333304</v>
       </c>
-      <c r="E5" s="167" t="s">
+      <c r="E5" s="163" t="s">
         <v>4</v>
       </c>
       <c r="F5" s="12">
         <v>0.83333333333333304</v>
       </c>
-      <c r="G5" s="168" t="s">
+      <c r="G5" s="164" t="s">
         <v>4</v>
       </c>
       <c r="H5" s="13">
         <v>0.83333333333333304</v>
       </c>
-      <c r="I5" s="169" t="s">
+      <c r="I5" s="165" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="165"/>
+      <c r="A6" s="161"/>
       <c r="B6" s="14">
         <v>1</v>
       </c>
-      <c r="C6" s="166"/>
+      <c r="C6" s="162"/>
       <c r="D6" s="15">
         <v>1</v>
       </c>
-      <c r="E6" s="167"/>
+      <c r="E6" s="163"/>
       <c r="F6" s="16">
         <v>1</v>
       </c>
-      <c r="G6" s="168"/>
+      <c r="G6" s="164"/>
       <c r="H6" s="17">
         <v>1</v>
       </c>
-      <c r="I6" s="169"/>
+      <c r="I6" s="165"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="165"/>
-      <c r="B7" s="170">
+      <c r="A7" s="161"/>
+      <c r="B7" s="166">
         <f>B6-B5</f>
         <v>0.16666666666666696</v>
       </c>
-      <c r="C7" s="170"/>
-      <c r="D7" s="171">
+      <c r="C7" s="166"/>
+      <c r="D7" s="167">
         <f>D6-D5</f>
         <v>0.16666666666666696</v>
       </c>
-      <c r="E7" s="171"/>
-      <c r="F7" s="172">
+      <c r="E7" s="167"/>
+      <c r="F7" s="168">
         <f>F6-F5</f>
         <v>0.16666666666666696</v>
       </c>
-      <c r="G7" s="172"/>
-      <c r="H7" s="173">
+      <c r="G7" s="168"/>
+      <c r="H7" s="169">
         <f>H6-H5</f>
         <v>0.16666666666666696</v>
       </c>
-      <c r="I7" s="173"/>
+      <c r="I7" s="169"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="165"/>
+      <c r="A8" s="161"/>
       <c r="B8" s="10"/>
-      <c r="C8" s="166" t="s">
+      <c r="C8" s="162" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="11"/>
-      <c r="E8" s="167" t="s">
+      <c r="E8" s="163" t="s">
         <v>4</v>
       </c>
       <c r="F8" s="12"/>
-      <c r="G8" s="168" t="s">
+      <c r="G8" s="164" t="s">
         <v>4</v>
       </c>
       <c r="H8" s="13"/>
-      <c r="I8" s="169" t="s">
+      <c r="I8" s="165" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="165"/>
+      <c r="A9" s="161"/>
       <c r="B9" s="14"/>
-      <c r="C9" s="166"/>
+      <c r="C9" s="162"/>
       <c r="D9" s="15"/>
-      <c r="E9" s="167"/>
+      <c r="E9" s="163"/>
       <c r="F9" s="16"/>
-      <c r="G9" s="168"/>
+      <c r="G9" s="164"/>
       <c r="H9" s="17"/>
-      <c r="I9" s="169"/>
+      <c r="I9" s="165"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="165"/>
-      <c r="B10" s="170">
+      <c r="A10" s="161"/>
+      <c r="B10" s="166">
         <f>(B9-B8)</f>
         <v>0</v>
       </c>
-      <c r="C10" s="170"/>
-      <c r="D10" s="171">
+      <c r="C10" s="166"/>
+      <c r="D10" s="167">
         <f>D9-D8</f>
         <v>0</v>
       </c>
-      <c r="E10" s="171"/>
-      <c r="F10" s="172">
+      <c r="E10" s="167"/>
+      <c r="F10" s="168">
         <f>F9-F8</f>
         <v>0</v>
       </c>
-      <c r="G10" s="172"/>
-      <c r="H10" s="173">
+      <c r="G10" s="168"/>
+      <c r="H10" s="169">
         <f>H9-H8</f>
         <v>0</v>
       </c>
-      <c r="I10" s="173"/>
+      <c r="I10" s="169"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="165"/>
+      <c r="A11" s="161"/>
       <c r="B11" s="10"/>
-      <c r="C11" s="166" t="s">
+      <c r="C11" s="162" t="s">
         <v>4</v>
       </c>
       <c r="D11" s="11"/>
-      <c r="E11" s="167" t="s">
+      <c r="E11" s="163" t="s">
         <v>4</v>
       </c>
       <c r="F11" s="12"/>
-      <c r="G11" s="168" t="s">
+      <c r="G11" s="164" t="s">
         <v>4</v>
       </c>
       <c r="H11" s="13"/>
-      <c r="I11" s="169" t="s">
+      <c r="I11" s="165" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="165"/>
+      <c r="A12" s="161"/>
       <c r="B12" s="14"/>
-      <c r="C12" s="166"/>
+      <c r="C12" s="162"/>
       <c r="D12" s="15"/>
-      <c r="E12" s="167"/>
+      <c r="E12" s="163"/>
       <c r="F12" s="16"/>
-      <c r="G12" s="168"/>
+      <c r="G12" s="164"/>
       <c r="H12" s="17"/>
-      <c r="I12" s="169"/>
+      <c r="I12" s="165"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" s="165"/>
-      <c r="B13" s="170">
+      <c r="A13" s="161"/>
+      <c r="B13" s="166">
         <f>(B12-B11)</f>
         <v>0</v>
       </c>
-      <c r="C13" s="170"/>
-      <c r="D13" s="171">
+      <c r="C13" s="166"/>
+      <c r="D13" s="167">
         <f>D12-D11</f>
         <v>0</v>
       </c>
-      <c r="E13" s="171"/>
-      <c r="F13" s="172">
+      <c r="E13" s="167"/>
+      <c r="F13" s="168">
         <f>F12-F11</f>
         <v>0</v>
       </c>
-      <c r="G13" s="172"/>
-      <c r="H13" s="173">
+      <c r="G13" s="168"/>
+      <c r="H13" s="169">
         <f>H12-H11</f>
         <v>0</v>
       </c>
-      <c r="I13" s="173"/>
+      <c r="I13" s="169"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" s="165"/>
+      <c r="A14" s="161"/>
       <c r="B14" s="10"/>
-      <c r="C14" s="166" t="s">
+      <c r="C14" s="162" t="s">
         <v>4</v>
       </c>
       <c r="D14" s="11"/>
-      <c r="E14" s="167" t="s">
+      <c r="E14" s="163" t="s">
         <v>4</v>
       </c>
       <c r="F14" s="12"/>
-      <c r="G14" s="168" t="s">
+      <c r="G14" s="164" t="s">
         <v>4</v>
       </c>
       <c r="H14" s="13"/>
-      <c r="I14" s="169" t="s">
+      <c r="I14" s="165" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" s="165"/>
+      <c r="A15" s="161"/>
       <c r="B15" s="14"/>
-      <c r="C15" s="166"/>
+      <c r="C15" s="162"/>
       <c r="D15" s="15"/>
-      <c r="E15" s="167"/>
+      <c r="E15" s="163"/>
       <c r="F15" s="16"/>
-      <c r="G15" s="168"/>
+      <c r="G15" s="164"/>
       <c r="H15" s="17"/>
-      <c r="I15" s="169"/>
+      <c r="I15" s="165"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" s="165"/>
-      <c r="B16" s="170">
+      <c r="A16" s="161"/>
+      <c r="B16" s="166">
         <f>(B15-B14)</f>
         <v>0</v>
       </c>
-      <c r="C16" s="170"/>
-      <c r="D16" s="171">
+      <c r="C16" s="166"/>
+      <c r="D16" s="167">
         <f>D15-D14</f>
         <v>0</v>
       </c>
-      <c r="E16" s="171"/>
-      <c r="F16" s="172">
+      <c r="E16" s="167"/>
+      <c r="F16" s="168">
         <f>F15-F14</f>
         <v>0</v>
       </c>
-      <c r="G16" s="172"/>
-      <c r="H16" s="173">
+      <c r="G16" s="168"/>
+      <c r="H16" s="169">
         <f>H15-H14</f>
         <v>0</v>
       </c>
-      <c r="I16" s="173"/>
+      <c r="I16" s="169"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17" s="165"/>
+      <c r="A17" s="161"/>
       <c r="B17" s="10"/>
-      <c r="C17" s="166" t="s">
+      <c r="C17" s="162" t="s">
         <v>4</v>
       </c>
       <c r="D17" s="11"/>
-      <c r="E17" s="167" t="s">
+      <c r="E17" s="163" t="s">
         <v>4</v>
       </c>
       <c r="F17" s="12"/>
-      <c r="G17" s="168" t="s">
+      <c r="G17" s="164" t="s">
         <v>4</v>
       </c>
       <c r="H17" s="13"/>
-      <c r="I17" s="169" t="s">
+      <c r="I17" s="165" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" s="165"/>
+      <c r="A18" s="161"/>
       <c r="B18" s="14"/>
-      <c r="C18" s="166"/>
+      <c r="C18" s="162"/>
       <c r="D18" s="15"/>
-      <c r="E18" s="167"/>
+      <c r="E18" s="163"/>
       <c r="F18" s="16"/>
-      <c r="G18" s="168"/>
+      <c r="G18" s="164"/>
       <c r="H18" s="17"/>
-      <c r="I18" s="169"/>
+      <c r="I18" s="165"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A19" s="165"/>
-      <c r="B19" s="170">
+      <c r="A19" s="161"/>
+      <c r="B19" s="166">
         <f>(B18-B17)</f>
         <v>0</v>
       </c>
-      <c r="C19" s="170"/>
-      <c r="D19" s="171">
+      <c r="C19" s="166"/>
+      <c r="D19" s="167">
         <f>D18-D17</f>
         <v>0</v>
       </c>
-      <c r="E19" s="171"/>
-      <c r="F19" s="172">
+      <c r="E19" s="167"/>
+      <c r="F19" s="168">
         <f>F18-F17</f>
         <v>0</v>
       </c>
-      <c r="G19" s="172"/>
-      <c r="H19" s="173">
+      <c r="G19" s="168"/>
+      <c r="H19" s="169">
         <f>H18-H17</f>
         <v>0</v>
       </c>
-      <c r="I19" s="173"/>
+      <c r="I19" s="169"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A20" s="165"/>
+      <c r="A20" s="161"/>
       <c r="B20" s="10"/>
-      <c r="C20" s="166" t="s">
+      <c r="C20" s="162" t="s">
         <v>4</v>
       </c>
       <c r="D20" s="11"/>
-      <c r="E20" s="167" t="s">
+      <c r="E20" s="163" t="s">
         <v>4</v>
       </c>
       <c r="F20" s="12"/>
-      <c r="G20" s="168" t="s">
+      <c r="G20" s="164" t="s">
         <v>4</v>
       </c>
       <c r="H20" s="13"/>
-      <c r="I20" s="169" t="s">
+      <c r="I20" s="165" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21" s="165"/>
+      <c r="A21" s="161"/>
       <c r="B21" s="14"/>
-      <c r="C21" s="166"/>
+      <c r="C21" s="162"/>
       <c r="D21" s="15"/>
-      <c r="E21" s="167"/>
+      <c r="E21" s="163"/>
       <c r="F21" s="16"/>
-      <c r="G21" s="168"/>
+      <c r="G21" s="164"/>
       <c r="H21" s="17"/>
-      <c r="I21" s="169"/>
+      <c r="I21" s="165"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A22" s="165"/>
-      <c r="B22" s="170">
+      <c r="A22" s="161"/>
+      <c r="B22" s="166">
         <f>(B21-B20)</f>
         <v>0</v>
       </c>
-      <c r="C22" s="170"/>
-      <c r="D22" s="171">
+      <c r="C22" s="166"/>
+      <c r="D22" s="167">
         <f>D21-D20</f>
         <v>0</v>
       </c>
-      <c r="E22" s="171"/>
-      <c r="F22" s="172">
+      <c r="E22" s="167"/>
+      <c r="F22" s="168">
         <f>F21-F20</f>
         <v>0</v>
       </c>
-      <c r="G22" s="172"/>
-      <c r="H22" s="173">
+      <c r="G22" s="168"/>
+      <c r="H22" s="169">
         <f>H21-H20</f>
         <v>0</v>
       </c>
-      <c r="I22" s="173"/>
+      <c r="I22" s="169"/>
     </row>
   </sheetData>
   <mergeCells count="63">
@@ -3195,524 +3662,524 @@
       <c r="N1" s="42"/>
     </row>
     <row r="2" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="165">
+      <c r="A2" s="161">
         <v>44543</v>
       </c>
       <c r="B2" s="10">
         <v>0.33333333333333298</v>
       </c>
-      <c r="C2" s="183" t="s">
+      <c r="C2" s="179" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="184"/>
+      <c r="D2" s="180"/>
       <c r="E2" s="11">
         <v>0.33333333333333298</v>
       </c>
-      <c r="F2" s="190" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="191"/>
+      <c r="F2" s="186" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="187"/>
       <c r="H2" s="12">
         <v>0.33333333333333298</v>
       </c>
-      <c r="I2" s="194" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2" s="205"/>
+      <c r="I2" s="190" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="201"/>
       <c r="K2" s="33">
         <v>0.33333333333333298</v>
       </c>
-      <c r="L2" s="174" t="s">
-        <v>4</v>
-      </c>
-      <c r="M2" s="175"/>
+      <c r="L2" s="170" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" s="171"/>
       <c r="N2" s="31"/>
     </row>
     <row r="3" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="165"/>
+      <c r="A3" s="161"/>
       <c r="B3" s="14">
         <v>0.49166666666666697</v>
       </c>
-      <c r="C3" s="185"/>
-      <c r="D3" s="186"/>
+      <c r="C3" s="181"/>
+      <c r="D3" s="182"/>
       <c r="E3" s="15">
         <v>0.41666666666666702</v>
       </c>
-      <c r="F3" s="192"/>
-      <c r="G3" s="193"/>
+      <c r="F3" s="188"/>
+      <c r="G3" s="189"/>
       <c r="H3" s="16">
         <v>0.41666666666666702</v>
       </c>
-      <c r="I3" s="196"/>
-      <c r="J3" s="197"/>
+      <c r="I3" s="192"/>
+      <c r="J3" s="193"/>
       <c r="K3" s="39">
         <v>0.41666666666666702</v>
       </c>
-      <c r="L3" s="198"/>
-      <c r="M3" s="199"/>
+      <c r="L3" s="194"/>
+      <c r="M3" s="195"/>
     </row>
     <row r="4" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="165"/>
-      <c r="B4" s="187">
+      <c r="A4" s="161"/>
+      <c r="B4" s="183">
         <f>B3-B2</f>
         <v>0.15833333333333399</v>
       </c>
-      <c r="C4" s="188"/>
-      <c r="D4" s="189"/>
-      <c r="E4" s="209">
+      <c r="C4" s="184"/>
+      <c r="D4" s="185"/>
+      <c r="E4" s="205">
         <f>E3-E2</f>
         <v>8.3333333333334036E-2</v>
       </c>
-      <c r="F4" s="210"/>
-      <c r="G4" s="211"/>
-      <c r="H4" s="180">
+      <c r="F4" s="206"/>
+      <c r="G4" s="207"/>
+      <c r="H4" s="176">
         <f>H3-H2</f>
         <v>8.3333333333334036E-2</v>
       </c>
-      <c r="I4" s="181"/>
-      <c r="J4" s="182"/>
-      <c r="K4" s="206">
+      <c r="I4" s="177"/>
+      <c r="J4" s="178"/>
+      <c r="K4" s="202">
         <f>K3-K2</f>
         <v>8.3333333333334036E-2</v>
       </c>
-      <c r="L4" s="207"/>
-      <c r="M4" s="208"/>
+      <c r="L4" s="203"/>
+      <c r="M4" s="204"/>
     </row>
     <row r="5" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="165">
+      <c r="A5" s="161">
         <v>44568</v>
       </c>
       <c r="B5" s="10"/>
-      <c r="C5" s="183" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="184"/>
+      <c r="C5" s="179" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="180"/>
       <c r="E5" s="11">
         <v>0.89583333333333304</v>
       </c>
-      <c r="F5" s="190" t="s">
+      <c r="F5" s="186" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="191"/>
+      <c r="G5" s="187"/>
       <c r="H5" s="12"/>
-      <c r="I5" s="194" t="s">
-        <v>4</v>
-      </c>
-      <c r="J5" s="195"/>
+      <c r="I5" s="190" t="s">
+        <v>4</v>
+      </c>
+      <c r="J5" s="191"/>
       <c r="K5" s="13">
         <v>0.33333333333333298</v>
       </c>
-      <c r="L5" s="174" t="s">
+      <c r="L5" s="170" t="s">
         <v>7</v>
       </c>
-      <c r="M5" s="175"/>
+      <c r="M5" s="171"/>
     </row>
     <row r="6" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="165"/>
+      <c r="A6" s="161"/>
       <c r="B6" s="14"/>
-      <c r="C6" s="185"/>
-      <c r="D6" s="186"/>
+      <c r="C6" s="181"/>
+      <c r="D6" s="182"/>
       <c r="E6" s="15">
         <v>0.97916666666666696</v>
       </c>
-      <c r="F6" s="192"/>
-      <c r="G6" s="193"/>
+      <c r="F6" s="188"/>
+      <c r="G6" s="189"/>
       <c r="H6" s="16"/>
-      <c r="I6" s="196"/>
-      <c r="J6" s="197"/>
+      <c r="I6" s="192"/>
+      <c r="J6" s="193"/>
       <c r="K6" s="39">
         <v>0.625</v>
       </c>
-      <c r="L6" s="176"/>
-      <c r="M6" s="177"/>
+      <c r="L6" s="172"/>
+      <c r="M6" s="173"/>
     </row>
     <row r="7" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="165"/>
-      <c r="B7" s="187">
+      <c r="A7" s="161"/>
+      <c r="B7" s="183">
         <f>B6-B5</f>
         <v>0</v>
       </c>
-      <c r="C7" s="188"/>
-      <c r="D7" s="189"/>
-      <c r="E7" s="209">
+      <c r="C7" s="184"/>
+      <c r="D7" s="185"/>
+      <c r="E7" s="205">
         <f>E6-E5</f>
         <v>8.3333333333333925E-2</v>
       </c>
-      <c r="F7" s="210"/>
-      <c r="G7" s="211"/>
-      <c r="H7" s="180">
+      <c r="F7" s="206"/>
+      <c r="G7" s="207"/>
+      <c r="H7" s="176">
         <f>H6-H5</f>
         <v>0</v>
       </c>
-      <c r="I7" s="181"/>
-      <c r="J7" s="182"/>
-      <c r="K7" s="200">
+      <c r="I7" s="177"/>
+      <c r="J7" s="178"/>
+      <c r="K7" s="196">
         <f>K6-K5</f>
         <v>0.29166666666666702</v>
       </c>
-      <c r="L7" s="201"/>
-      <c r="M7" s="202"/>
+      <c r="L7" s="197"/>
+      <c r="M7" s="198"/>
     </row>
     <row r="8" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="165">
+      <c r="A8" s="161">
         <v>44569</v>
       </c>
       <c r="B8" s="10">
         <v>0.72916666666666696</v>
       </c>
-      <c r="C8" s="183" t="s">
+      <c r="C8" s="179" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="184"/>
+      <c r="D8" s="180"/>
       <c r="E8" s="11">
         <v>0.77083333333333304</v>
       </c>
-      <c r="F8" s="190" t="s">
+      <c r="F8" s="186" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="191"/>
+      <c r="G8" s="187"/>
       <c r="H8" s="12">
         <v>0.77083333333333304</v>
       </c>
-      <c r="I8" s="194" t="s">
-        <v>4</v>
-      </c>
-      <c r="J8" s="195"/>
+      <c r="I8" s="190" t="s">
+        <v>4</v>
+      </c>
+      <c r="J8" s="191"/>
       <c r="K8" s="40">
         <v>0.77083333333333304</v>
       </c>
-      <c r="L8" s="198" t="s">
-        <v>4</v>
-      </c>
-      <c r="M8" s="199"/>
+      <c r="L8" s="194" t="s">
+        <v>4</v>
+      </c>
+      <c r="M8" s="195"/>
     </row>
     <row r="9" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="165"/>
+      <c r="A9" s="161"/>
       <c r="B9" s="14">
         <v>1</v>
       </c>
-      <c r="C9" s="185"/>
-      <c r="D9" s="186"/>
+      <c r="C9" s="181"/>
+      <c r="D9" s="182"/>
       <c r="E9" s="15">
         <v>0.91666666666666696</v>
       </c>
-      <c r="F9" s="192"/>
-      <c r="G9" s="193"/>
+      <c r="F9" s="188"/>
+      <c r="G9" s="189"/>
       <c r="H9" s="16">
         <v>0.9375</v>
       </c>
-      <c r="I9" s="196"/>
-      <c r="J9" s="197"/>
+      <c r="I9" s="192"/>
+      <c r="J9" s="193"/>
       <c r="K9" s="39">
         <v>0.91666666666666696</v>
       </c>
-      <c r="L9" s="198"/>
-      <c r="M9" s="199"/>
+      <c r="L9" s="194"/>
+      <c r="M9" s="195"/>
     </row>
     <row r="10" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="165"/>
-      <c r="B10" s="187">
+      <c r="A10" s="161"/>
+      <c r="B10" s="183">
         <f>(B9-B8)</f>
         <v>0.27083333333333304</v>
       </c>
-      <c r="C10" s="188"/>
-      <c r="D10" s="189"/>
-      <c r="E10" s="209">
+      <c r="C10" s="184"/>
+      <c r="D10" s="185"/>
+      <c r="E10" s="205">
         <f>E9-E8</f>
         <v>0.14583333333333393</v>
       </c>
-      <c r="F10" s="210"/>
-      <c r="G10" s="211"/>
-      <c r="H10" s="180">
+      <c r="F10" s="206"/>
+      <c r="G10" s="207"/>
+      <c r="H10" s="176">
         <f>H9-H8</f>
         <v>0.16666666666666696</v>
       </c>
-      <c r="I10" s="181"/>
-      <c r="J10" s="182"/>
-      <c r="K10" s="200">
+      <c r="I10" s="177"/>
+      <c r="J10" s="178"/>
+      <c r="K10" s="196">
         <f>K9-K8</f>
         <v>0.14583333333333393</v>
       </c>
-      <c r="L10" s="201"/>
-      <c r="M10" s="202"/>
+      <c r="L10" s="197"/>
+      <c r="M10" s="198"/>
     </row>
     <row r="11" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="165">
+      <c r="A11" s="161">
         <v>44805</v>
       </c>
       <c r="B11" s="10">
         <v>0.66666666666666696</v>
       </c>
-      <c r="C11" s="183" t="s">
+      <c r="C11" s="179" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="184"/>
+      <c r="D11" s="180"/>
       <c r="E11" s="11">
         <v>0.66666666666666696</v>
       </c>
-      <c r="F11" s="190" t="s">
+      <c r="F11" s="186" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="191"/>
+      <c r="G11" s="187"/>
       <c r="H11" s="12">
         <v>0.75</v>
       </c>
-      <c r="I11" s="194" t="s">
-        <v>4</v>
-      </c>
-      <c r="J11" s="195"/>
+      <c r="I11" s="190" t="s">
+        <v>4</v>
+      </c>
+      <c r="J11" s="191"/>
       <c r="K11" s="40">
         <v>0.75</v>
       </c>
-      <c r="L11" s="198" t="s">
-        <v>4</v>
-      </c>
-      <c r="M11" s="199"/>
+      <c r="L11" s="194" t="s">
+        <v>4</v>
+      </c>
+      <c r="M11" s="195"/>
     </row>
     <row r="12" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="165"/>
+      <c r="A12" s="161"/>
       <c r="B12" s="14">
         <v>1</v>
       </c>
-      <c r="C12" s="185"/>
-      <c r="D12" s="186"/>
+      <c r="C12" s="181"/>
+      <c r="D12" s="182"/>
       <c r="E12" s="15">
         <v>0.95833333333333304</v>
       </c>
-      <c r="F12" s="192"/>
-      <c r="G12" s="193"/>
+      <c r="F12" s="188"/>
+      <c r="G12" s="189"/>
       <c r="H12" s="16">
         <v>1</v>
       </c>
-      <c r="I12" s="196"/>
-      <c r="J12" s="197"/>
+      <c r="I12" s="192"/>
+      <c r="J12" s="193"/>
       <c r="K12" s="34">
         <v>0.95833333333333304</v>
       </c>
-      <c r="L12" s="176"/>
-      <c r="M12" s="177"/>
+      <c r="L12" s="172"/>
+      <c r="M12" s="173"/>
     </row>
     <row r="13" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="165"/>
-      <c r="B13" s="187">
+      <c r="A13" s="161"/>
+      <c r="B13" s="183">
         <f>(B12-B11)</f>
         <v>0.33333333333333304</v>
       </c>
-      <c r="C13" s="188"/>
-      <c r="D13" s="189"/>
-      <c r="E13" s="209">
+      <c r="C13" s="184"/>
+      <c r="D13" s="185"/>
+      <c r="E13" s="205">
         <f>E12-E11</f>
         <v>0.29166666666666607</v>
       </c>
-      <c r="F13" s="210"/>
-      <c r="G13" s="211"/>
-      <c r="H13" s="180">
+      <c r="F13" s="206"/>
+      <c r="G13" s="207"/>
+      <c r="H13" s="176">
         <f>H12-H11</f>
         <v>0.25</v>
       </c>
-      <c r="I13" s="181"/>
-      <c r="J13" s="182"/>
-      <c r="K13" s="203">
+      <c r="I13" s="177"/>
+      <c r="J13" s="178"/>
+      <c r="K13" s="199">
         <f>K12-K11</f>
         <v>0.20833333333333304</v>
       </c>
-      <c r="L13" s="203"/>
-      <c r="M13" s="204"/>
+      <c r="L13" s="199"/>
+      <c r="M13" s="200"/>
     </row>
     <row r="14" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="165"/>
+      <c r="A14" s="161"/>
       <c r="B14" s="10"/>
-      <c r="C14" s="183" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="184"/>
+      <c r="C14" s="179" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="180"/>
       <c r="E14" s="11"/>
-      <c r="F14" s="190" t="s">
-        <v>4</v>
-      </c>
-      <c r="G14" s="191"/>
+      <c r="F14" s="186" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14" s="187"/>
       <c r="H14" s="12"/>
-      <c r="I14" s="194" t="s">
-        <v>4</v>
-      </c>
-      <c r="J14" s="195"/>
+      <c r="I14" s="190" t="s">
+        <v>4</v>
+      </c>
+      <c r="J14" s="191"/>
       <c r="K14" s="33"/>
-      <c r="L14" s="174" t="s">
-        <v>4</v>
-      </c>
-      <c r="M14" s="175"/>
+      <c r="L14" s="170" t="s">
+        <v>4</v>
+      </c>
+      <c r="M14" s="171"/>
     </row>
     <row r="15" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="165"/>
+      <c r="A15" s="161"/>
       <c r="B15" s="14"/>
-      <c r="C15" s="185"/>
-      <c r="D15" s="186"/>
+      <c r="C15" s="181"/>
+      <c r="D15" s="182"/>
       <c r="E15" s="15"/>
-      <c r="F15" s="192"/>
-      <c r="G15" s="193"/>
+      <c r="F15" s="188"/>
+      <c r="G15" s="189"/>
       <c r="H15" s="16"/>
-      <c r="I15" s="196"/>
-      <c r="J15" s="197"/>
+      <c r="I15" s="192"/>
+      <c r="J15" s="193"/>
       <c r="K15" s="39"/>
-      <c r="L15" s="198"/>
-      <c r="M15" s="199"/>
+      <c r="L15" s="194"/>
+      <c r="M15" s="195"/>
     </row>
     <row r="16" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="165"/>
-      <c r="B16" s="187">
+      <c r="A16" s="161"/>
+      <c r="B16" s="183">
         <f>(B15-B14)</f>
         <v>0</v>
       </c>
-      <c r="C16" s="188"/>
-      <c r="D16" s="189"/>
-      <c r="E16" s="209">
+      <c r="C16" s="184"/>
+      <c r="D16" s="185"/>
+      <c r="E16" s="205">
         <f>E15-E14</f>
         <v>0</v>
       </c>
-      <c r="F16" s="210"/>
-      <c r="G16" s="211"/>
-      <c r="H16" s="180">
+      <c r="F16" s="206"/>
+      <c r="G16" s="207"/>
+      <c r="H16" s="176">
         <f>H15-H14</f>
         <v>0</v>
       </c>
-      <c r="I16" s="181"/>
-      <c r="J16" s="182"/>
-      <c r="K16" s="200">
+      <c r="I16" s="177"/>
+      <c r="J16" s="178"/>
+      <c r="K16" s="196">
         <f>K15-K14</f>
         <v>0</v>
       </c>
-      <c r="L16" s="201"/>
-      <c r="M16" s="202"/>
+      <c r="L16" s="197"/>
+      <c r="M16" s="198"/>
     </row>
     <row r="17" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="165"/>
+      <c r="A17" s="161"/>
       <c r="B17" s="10"/>
-      <c r="C17" s="183" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" s="184"/>
+      <c r="C17" s="179" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="180"/>
       <c r="E17" s="11"/>
-      <c r="F17" s="190" t="s">
-        <v>4</v>
-      </c>
-      <c r="G17" s="191"/>
+      <c r="F17" s="186" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" s="187"/>
       <c r="H17" s="12"/>
-      <c r="I17" s="194" t="s">
-        <v>4</v>
-      </c>
-      <c r="J17" s="195"/>
+      <c r="I17" s="190" t="s">
+        <v>4</v>
+      </c>
+      <c r="J17" s="191"/>
       <c r="K17" s="40"/>
-      <c r="L17" s="198" t="s">
-        <v>4</v>
-      </c>
-      <c r="M17" s="199"/>
+      <c r="L17" s="194" t="s">
+        <v>4</v>
+      </c>
+      <c r="M17" s="195"/>
     </row>
     <row r="18" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="165"/>
+      <c r="A18" s="161"/>
       <c r="B18" s="14"/>
-      <c r="C18" s="185"/>
-      <c r="D18" s="186"/>
+      <c r="C18" s="181"/>
+      <c r="D18" s="182"/>
       <c r="E18" s="15"/>
-      <c r="F18" s="192"/>
-      <c r="G18" s="193"/>
+      <c r="F18" s="188"/>
+      <c r="G18" s="189"/>
       <c r="H18" s="16"/>
-      <c r="I18" s="196"/>
-      <c r="J18" s="197"/>
+      <c r="I18" s="192"/>
+      <c r="J18" s="193"/>
       <c r="K18" s="39"/>
-      <c r="L18" s="198"/>
-      <c r="M18" s="199"/>
+      <c r="L18" s="194"/>
+      <c r="M18" s="195"/>
     </row>
     <row r="19" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="165"/>
-      <c r="B19" s="187">
+      <c r="A19" s="161"/>
+      <c r="B19" s="183">
         <f>(B18-B17)</f>
         <v>0</v>
       </c>
-      <c r="C19" s="188"/>
-      <c r="D19" s="189"/>
-      <c r="E19" s="209">
+      <c r="C19" s="184"/>
+      <c r="D19" s="185"/>
+      <c r="E19" s="205">
         <f>E18-E17</f>
         <v>0</v>
       </c>
-      <c r="F19" s="210"/>
-      <c r="G19" s="211"/>
-      <c r="H19" s="180">
+      <c r="F19" s="206"/>
+      <c r="G19" s="207"/>
+      <c r="H19" s="176">
         <f>H18-H17</f>
         <v>0</v>
       </c>
-      <c r="I19" s="181"/>
-      <c r="J19" s="182"/>
-      <c r="K19" s="200">
+      <c r="I19" s="177"/>
+      <c r="J19" s="178"/>
+      <c r="K19" s="196">
         <f>K18-K17</f>
         <v>0</v>
       </c>
-      <c r="L19" s="201"/>
-      <c r="M19" s="202"/>
+      <c r="L19" s="197"/>
+      <c r="M19" s="198"/>
     </row>
     <row r="20" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="165"/>
+      <c r="A20" s="161"/>
       <c r="B20" s="10"/>
-      <c r="C20" s="183" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" s="184"/>
+      <c r="C20" s="179" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="180"/>
       <c r="E20" s="11"/>
-      <c r="F20" s="190" t="s">
-        <v>4</v>
-      </c>
-      <c r="G20" s="191"/>
+      <c r="F20" s="186" t="s">
+        <v>4</v>
+      </c>
+      <c r="G20" s="187"/>
       <c r="H20" s="12"/>
-      <c r="I20" s="194" t="s">
-        <v>4</v>
-      </c>
-      <c r="J20" s="195"/>
+      <c r="I20" s="190" t="s">
+        <v>4</v>
+      </c>
+      <c r="J20" s="191"/>
       <c r="K20" s="33"/>
-      <c r="L20" s="174" t="s">
-        <v>4</v>
-      </c>
-      <c r="M20" s="175"/>
+      <c r="L20" s="170" t="s">
+        <v>4</v>
+      </c>
+      <c r="M20" s="171"/>
     </row>
     <row r="21" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="165"/>
+      <c r="A21" s="161"/>
       <c r="B21" s="14"/>
-      <c r="C21" s="185"/>
-      <c r="D21" s="186"/>
+      <c r="C21" s="181"/>
+      <c r="D21" s="182"/>
       <c r="E21" s="15"/>
-      <c r="F21" s="192"/>
-      <c r="G21" s="193"/>
+      <c r="F21" s="188"/>
+      <c r="G21" s="189"/>
       <c r="H21" s="16"/>
-      <c r="I21" s="196"/>
-      <c r="J21" s="197"/>
+      <c r="I21" s="192"/>
+      <c r="J21" s="193"/>
       <c r="K21" s="34"/>
-      <c r="L21" s="176"/>
-      <c r="M21" s="177"/>
+      <c r="L21" s="172"/>
+      <c r="M21" s="173"/>
     </row>
     <row r="22" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="165"/>
-      <c r="B22" s="187">
+      <c r="A22" s="161"/>
+      <c r="B22" s="183">
         <f>(B21-B20)</f>
         <v>0</v>
       </c>
-      <c r="C22" s="188"/>
-      <c r="D22" s="189"/>
-      <c r="E22" s="209">
+      <c r="C22" s="184"/>
+      <c r="D22" s="185"/>
+      <c r="E22" s="205">
         <f>E21-E20</f>
         <v>0</v>
       </c>
-      <c r="F22" s="210"/>
-      <c r="G22" s="211"/>
-      <c r="H22" s="180">
+      <c r="F22" s="206"/>
+      <c r="G22" s="207"/>
+      <c r="H22" s="176">
         <f>H21-H20</f>
         <v>0</v>
       </c>
-      <c r="I22" s="181"/>
-      <c r="J22" s="182"/>
-      <c r="K22" s="178">
+      <c r="I22" s="177"/>
+      <c r="J22" s="178"/>
+      <c r="K22" s="174">
         <f>K21-K20</f>
         <v>0</v>
       </c>
-      <c r="L22" s="178"/>
-      <c r="M22" s="179"/>
+      <c r="L22" s="174"/>
+      <c r="M22" s="175"/>
     </row>
     <row r="23" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
@@ -3808,7 +4275,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="213" t="s">
+      <c r="A1" s="209" t="s">
         <v>14</v>
       </c>
       <c r="B1" s="87" t="s">
@@ -3850,7 +4317,7 @@
       <c r="N1" s="42"/>
     </row>
     <row r="2" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="214"/>
+      <c r="A2" s="210"/>
       <c r="B2" s="20" t="s">
         <v>0</v>
       </c>
@@ -3898,55 +4365,55 @@
       <c r="N2" s="31"/>
     </row>
     <row r="3" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="215">
+      <c r="A3" s="211">
         <v>44571</v>
       </c>
       <c r="B3" s="10">
         <v>0.33333333333333331</v>
       </c>
-      <c r="C3" s="218" t="s">
+      <c r="C3" s="214" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="156"/>
+      <c r="D3" s="153"/>
       <c r="E3" s="11">
         <v>0.33333333333333331</v>
       </c>
-      <c r="F3" s="219" t="s">
+      <c r="F3" s="215" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="149"/>
+      <c r="G3" s="146"/>
       <c r="H3" s="12">
         <v>0.33333333333333331</v>
       </c>
-      <c r="I3" s="220" t="s">
+      <c r="I3" s="216" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="145"/>
+      <c r="J3" s="142"/>
       <c r="K3" s="33">
         <v>0.33333333333333331</v>
       </c>
-      <c r="L3" s="212" t="s">
+      <c r="L3" s="208" t="s">
         <v>12</v>
       </c>
       <c r="M3" s="137"/>
     </row>
     <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="216"/>
+      <c r="A4" s="212"/>
       <c r="B4" s="14">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C4" s="157"/>
-      <c r="D4" s="158"/>
+      <c r="C4" s="154"/>
+      <c r="D4" s="155"/>
       <c r="E4" s="15">
         <v>0.41666666666666669</v>
       </c>
-      <c r="F4" s="150"/>
-      <c r="G4" s="151"/>
+      <c r="F4" s="147"/>
+      <c r="G4" s="148"/>
       <c r="H4" s="16">
         <v>0.41666666666666669</v>
       </c>
-      <c r="I4" s="146"/>
-      <c r="J4" s="147"/>
+      <c r="I4" s="143"/>
+      <c r="J4" s="144"/>
       <c r="K4" s="39">
         <v>0.41666666666666669</v>
       </c>
@@ -3954,7 +4421,7 @@
       <c r="M4" s="139"/>
     </row>
     <row r="5" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="217"/>
+      <c r="A5" s="213"/>
       <c r="B5" s="48">
         <f>B4-B3</f>
         <v>8.333333333333337E-2</v>
@@ -3981,55 +4448,55 @@
       <c r="M5" s="53"/>
     </row>
     <row r="6" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="215">
+      <c r="A6" s="211">
         <v>44583</v>
       </c>
       <c r="B6" s="10">
         <v>0.79166666666666663</v>
       </c>
-      <c r="C6" s="218" t="s">
+      <c r="C6" s="214" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="156"/>
+      <c r="D6" s="153"/>
       <c r="E6" s="11">
         <v>0.82291666666666663</v>
       </c>
-      <c r="F6" s="219" t="s">
+      <c r="F6" s="215" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="149"/>
+      <c r="G6" s="146"/>
       <c r="H6" s="12">
         <v>0.79166666666666663</v>
       </c>
-      <c r="I6" s="220" t="s">
+      <c r="I6" s="216" t="s">
         <v>19</v>
       </c>
-      <c r="J6" s="145"/>
+      <c r="J6" s="142"/>
       <c r="K6" s="13">
         <v>0.79166666666666663</v>
       </c>
-      <c r="L6" s="212" t="s">
+      <c r="L6" s="208" t="s">
         <v>19</v>
       </c>
       <c r="M6" s="137"/>
     </row>
     <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="216"/>
+      <c r="A7" s="212"/>
       <c r="B7" s="14">
         <v>0.8979166666666667</v>
       </c>
-      <c r="C7" s="157"/>
-      <c r="D7" s="158"/>
+      <c r="C7" s="154"/>
+      <c r="D7" s="155"/>
       <c r="E7" s="15">
         <v>0.8979166666666667</v>
       </c>
-      <c r="F7" s="150"/>
-      <c r="G7" s="151"/>
+      <c r="F7" s="147"/>
+      <c r="G7" s="148"/>
       <c r="H7" s="16">
         <v>0.89583333333333337</v>
       </c>
-      <c r="I7" s="146"/>
-      <c r="J7" s="147"/>
+      <c r="I7" s="143"/>
+      <c r="J7" s="144"/>
       <c r="K7" s="39">
         <v>0.8979166666666667</v>
       </c>
@@ -4037,7 +4504,7 @@
       <c r="M7" s="139"/>
     </row>
     <row r="8" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="217"/>
+      <c r="A8" s="213"/>
       <c r="B8" s="48">
         <f>B7-B6</f>
         <v>0.10625000000000007</v>
@@ -4064,55 +4531,55 @@
       <c r="M8" s="24"/>
     </row>
     <row r="9" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="215">
+      <c r="A9" s="211">
         <v>44584</v>
       </c>
       <c r="B9" s="10">
         <v>0.75694444444444453</v>
       </c>
-      <c r="C9" s="218" t="s">
+      <c r="C9" s="214" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="156"/>
+      <c r="D9" s="153"/>
       <c r="E9" s="11">
         <v>0.75694444444444453</v>
       </c>
-      <c r="F9" s="219" t="s">
+      <c r="F9" s="215" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="149"/>
+      <c r="G9" s="146"/>
       <c r="H9" s="12">
         <v>0.75694444444444453</v>
       </c>
-      <c r="I9" s="220" t="s">
+      <c r="I9" s="216" t="s">
         <v>20</v>
       </c>
-      <c r="J9" s="145"/>
+      <c r="J9" s="142"/>
       <c r="K9" s="40">
         <v>0.75694444444444453</v>
       </c>
-      <c r="L9" s="212" t="s">
+      <c r="L9" s="208" t="s">
         <v>20</v>
       </c>
       <c r="M9" s="137"/>
     </row>
     <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="216"/>
+      <c r="A10" s="212"/>
       <c r="B10" s="14">
         <v>0.8354166666666667</v>
       </c>
-      <c r="C10" s="157"/>
-      <c r="D10" s="158"/>
+      <c r="C10" s="154"/>
+      <c r="D10" s="155"/>
       <c r="E10" s="15">
         <v>0.8354166666666667</v>
       </c>
-      <c r="F10" s="150"/>
-      <c r="G10" s="151"/>
+      <c r="F10" s="147"/>
+      <c r="G10" s="148"/>
       <c r="H10" s="16">
         <v>0.8354166666666667</v>
       </c>
-      <c r="I10" s="146"/>
-      <c r="J10" s="147"/>
+      <c r="I10" s="143"/>
+      <c r="J10" s="144"/>
       <c r="K10" s="39">
         <v>0.8354166666666667</v>
       </c>
@@ -4120,7 +4587,7 @@
       <c r="M10" s="139"/>
     </row>
     <row r="11" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="217"/>
+      <c r="A11" s="213"/>
       <c r="B11" s="48">
         <f>(B10-B9)</f>
         <v>7.8472222222222165E-2</v>
@@ -4147,45 +4614,45 @@
       <c r="M11" s="24"/>
     </row>
     <row r="12" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="215"/>
+      <c r="A12" s="211"/>
       <c r="B12" s="10"/>
-      <c r="C12" s="218" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="156"/>
+      <c r="C12" s="214" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="153"/>
       <c r="E12" s="11"/>
-      <c r="F12" s="219" t="s">
-        <v>4</v>
-      </c>
-      <c r="G12" s="149"/>
+      <c r="F12" s="215" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="146"/>
       <c r="H12" s="12"/>
-      <c r="I12" s="220" t="s">
-        <v>4</v>
-      </c>
-      <c r="J12" s="145"/>
+      <c r="I12" s="216" t="s">
+        <v>4</v>
+      </c>
+      <c r="J12" s="142"/>
       <c r="K12" s="40"/>
-      <c r="L12" s="212" t="s">
+      <c r="L12" s="208" t="s">
         <v>4</v>
       </c>
       <c r="M12" s="137"/>
     </row>
     <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="216"/>
+      <c r="A13" s="212"/>
       <c r="B13" s="14"/>
-      <c r="C13" s="157"/>
-      <c r="D13" s="158"/>
+      <c r="C13" s="154"/>
+      <c r="D13" s="155"/>
       <c r="E13" s="15"/>
-      <c r="F13" s="150"/>
-      <c r="G13" s="151"/>
+      <c r="F13" s="147"/>
+      <c r="G13" s="148"/>
       <c r="H13" s="16"/>
-      <c r="I13" s="146"/>
-      <c r="J13" s="147"/>
+      <c r="I13" s="143"/>
+      <c r="J13" s="144"/>
       <c r="K13" s="34"/>
       <c r="L13" s="138"/>
       <c r="M13" s="139"/>
     </row>
     <row r="14" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="217"/>
+      <c r="A14" s="213"/>
       <c r="B14" s="48">
         <f>(B13-B12)</f>
         <v>0</v>
@@ -4212,45 +4679,45 @@
       <c r="M14" s="55"/>
     </row>
     <row r="15" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="215"/>
+      <c r="A15" s="211"/>
       <c r="B15" s="10"/>
-      <c r="C15" s="218" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" s="156"/>
+      <c r="C15" s="214" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="153"/>
       <c r="E15" s="11"/>
-      <c r="F15" s="219" t="s">
-        <v>4</v>
-      </c>
-      <c r="G15" s="149"/>
+      <c r="F15" s="215" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" s="146"/>
       <c r="H15" s="12"/>
-      <c r="I15" s="220" t="s">
-        <v>4</v>
-      </c>
-      <c r="J15" s="145"/>
+      <c r="I15" s="216" t="s">
+        <v>4</v>
+      </c>
+      <c r="J15" s="142"/>
       <c r="K15" s="33"/>
-      <c r="L15" s="212" t="s">
+      <c r="L15" s="208" t="s">
         <v>4</v>
       </c>
       <c r="M15" s="137"/>
     </row>
     <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="216"/>
+      <c r="A16" s="212"/>
       <c r="B16" s="14"/>
-      <c r="C16" s="157"/>
-      <c r="D16" s="158"/>
+      <c r="C16" s="154"/>
+      <c r="D16" s="155"/>
       <c r="E16" s="15"/>
-      <c r="F16" s="150"/>
-      <c r="G16" s="151"/>
+      <c r="F16" s="147"/>
+      <c r="G16" s="148"/>
       <c r="H16" s="16"/>
-      <c r="I16" s="146"/>
-      <c r="J16" s="147"/>
+      <c r="I16" s="143"/>
+      <c r="J16" s="144"/>
       <c r="K16" s="39"/>
       <c r="L16" s="138"/>
       <c r="M16" s="139"/>
     </row>
     <row r="17" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="217"/>
+      <c r="A17" s="213"/>
       <c r="B17" s="48">
         <f>(B16-B15)</f>
         <v>0</v>
@@ -4277,45 +4744,45 @@
       <c r="M17" s="24"/>
     </row>
     <row r="18" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="215"/>
+      <c r="A18" s="211"/>
       <c r="B18" s="10"/>
-      <c r="C18" s="218" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="156"/>
+      <c r="C18" s="214" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="153"/>
       <c r="E18" s="11"/>
-      <c r="F18" s="219" t="s">
-        <v>4</v>
-      </c>
-      <c r="G18" s="149"/>
+      <c r="F18" s="215" t="s">
+        <v>4</v>
+      </c>
+      <c r="G18" s="146"/>
       <c r="H18" s="12"/>
-      <c r="I18" s="220" t="s">
-        <v>4</v>
-      </c>
-      <c r="J18" s="145"/>
+      <c r="I18" s="216" t="s">
+        <v>4</v>
+      </c>
+      <c r="J18" s="142"/>
       <c r="K18" s="40"/>
-      <c r="L18" s="212" t="s">
+      <c r="L18" s="208" t="s">
         <v>4</v>
       </c>
       <c r="M18" s="137"/>
     </row>
     <row r="19" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="216"/>
+      <c r="A19" s="212"/>
       <c r="B19" s="14"/>
-      <c r="C19" s="157"/>
-      <c r="D19" s="158"/>
+      <c r="C19" s="154"/>
+      <c r="D19" s="155"/>
       <c r="E19" s="15"/>
-      <c r="F19" s="150"/>
-      <c r="G19" s="151"/>
+      <c r="F19" s="147"/>
+      <c r="G19" s="148"/>
       <c r="H19" s="16"/>
-      <c r="I19" s="146"/>
-      <c r="J19" s="147"/>
+      <c r="I19" s="143"/>
+      <c r="J19" s="144"/>
       <c r="K19" s="39"/>
       <c r="L19" s="138"/>
       <c r="M19" s="139"/>
     </row>
     <row r="20" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="217"/>
+      <c r="A20" s="213"/>
       <c r="B20" s="48">
         <f>(B19-B18)</f>
         <v>0</v>
@@ -4342,45 +4809,45 @@
       <c r="M20" s="24"/>
     </row>
     <row r="21" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="215"/>
+      <c r="A21" s="211"/>
       <c r="B21" s="10"/>
-      <c r="C21" s="218" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" s="156"/>
+      <c r="C21" s="214" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="153"/>
       <c r="E21" s="11"/>
-      <c r="F21" s="219" t="s">
-        <v>4</v>
-      </c>
-      <c r="G21" s="149"/>
+      <c r="F21" s="215" t="s">
+        <v>4</v>
+      </c>
+      <c r="G21" s="146"/>
       <c r="H21" s="12"/>
-      <c r="I21" s="220" t="s">
-        <v>4</v>
-      </c>
-      <c r="J21" s="145"/>
+      <c r="I21" s="216" t="s">
+        <v>4</v>
+      </c>
+      <c r="J21" s="142"/>
       <c r="K21" s="33"/>
-      <c r="L21" s="212" t="s">
+      <c r="L21" s="208" t="s">
         <v>4</v>
       </c>
       <c r="M21" s="137"/>
     </row>
     <row r="22" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="216"/>
+      <c r="A22" s="212"/>
       <c r="B22" s="14"/>
-      <c r="C22" s="157"/>
-      <c r="D22" s="158"/>
+      <c r="C22" s="154"/>
+      <c r="D22" s="155"/>
       <c r="E22" s="15"/>
-      <c r="F22" s="150"/>
-      <c r="G22" s="151"/>
+      <c r="F22" s="147"/>
+      <c r="G22" s="148"/>
       <c r="H22" s="16"/>
-      <c r="I22" s="146"/>
-      <c r="J22" s="147"/>
+      <c r="I22" s="143"/>
+      <c r="J22" s="144"/>
       <c r="K22" s="34"/>
       <c r="L22" s="138"/>
       <c r="M22" s="139"/>
     </row>
     <row r="23" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="217"/>
+      <c r="A23" s="213"/>
       <c r="B23" s="48">
         <f>(B22-B21)</f>
         <v>0</v>
@@ -4471,10 +4938,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6268C972-D036-425F-A827-D7932DAA225B}">
-  <dimension ref="A1:N31"/>
+  <dimension ref="A1:O42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4488,123 +4955,134 @@
     <col min="9" max="10" width="13.6328125" customWidth="1"/>
     <col min="11" max="11" width="15.08984375" customWidth="1"/>
     <col min="12" max="13" width="13.6328125" customWidth="1"/>
+    <col min="14" max="14" width="19.6328125" customWidth="1"/>
+    <col min="15" max="15" width="17.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="153" t="s">
+    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="150" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="116" t="s">
+      <c r="B1" s="97" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="117" t="s">
+      <c r="C1" s="98" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="116" t="s">
+      <c r="D1" s="97" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="118" t="s">
+      <c r="E1" s="99" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="119" t="s">
+      <c r="F1" s="100" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="118" t="s">
+      <c r="G1" s="99" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="120" t="s">
+      <c r="H1" s="101" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="121" t="s">
+      <c r="I1" s="102" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="120" t="s">
+      <c r="J1" s="101" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="122" t="s">
+      <c r="K1" s="103" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="122" t="s">
+      <c r="L1" s="103" t="s">
         <v>15</v>
       </c>
-      <c r="M1" s="123" t="s">
+      <c r="M1" s="104" t="s">
         <v>16</v>
       </c>
-      <c r="N1" s="42"/>
-    </row>
-    <row r="2" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="154"/>
-      <c r="B2" s="124" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="125" cm="1">
-        <f t="array" ref="C2">SUM(B5:B23*(MOD(ROW(B5:B23)-2,3)=0))</f>
-        <v>0.21875</v>
-      </c>
-      <c r="D2" s="126">
+      <c r="N1" s="160" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" s="160"/>
+    </row>
+    <row r="2" spans="1:15" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="151"/>
+      <c r="B2" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="106" cm="1">
+        <f t="array" ref="C2">SUM(B5:B41*(MOD(ROW(B5:B41)-2,3)=0))</f>
+        <v>0.26041666666666674</v>
+      </c>
+      <c r="D2" s="107">
         <f>C2+Sprint_3!D2</f>
-        <v>1.5826388888888898</v>
-      </c>
-      <c r="E2" s="127" t="s">
+        <v>1.6243055555555566</v>
+      </c>
+      <c r="E2" s="108" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="128" cm="1">
-        <f t="array" ref="F2">SUM(E5:E23*(MOD(ROW(E5:E23)-2,3)=0))</f>
+      <c r="F2" s="109" cm="1">
+        <f t="array" ref="F2">SUM(E5:E41*(MOD(ROW(E5:E41)-2,3)=0))</f>
         <v>0.11458333333333337</v>
       </c>
-      <c r="G2" s="129">
+      <c r="G2" s="110">
         <f>F2+Sprint_3!G2</f>
         <v>1.288888888888891</v>
       </c>
-      <c r="H2" s="130" t="s">
+      <c r="H2" s="111" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="131" cm="1">
-        <f t="array" ref="I2">SUM(H5:H23*(MOD(ROW(H5:H23)-2,3)=0))</f>
+      <c r="I2" s="112" cm="1">
+        <f t="array" ref="I2">SUM(H5:H41*(MOD(ROW(H5:H41)-2,3)=0))</f>
         <v>0.11458333333333337</v>
       </c>
-      <c r="J2" s="132">
+      <c r="J2" s="113">
         <f>I2+Sprint_3!J2</f>
         <v>1.2138888888888908</v>
       </c>
-      <c r="K2" s="133" t="s">
+      <c r="K2" s="114" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="134" cm="1">
-        <f t="array" ref="L2">SUM(K5:K23*(MOD(ROW(K5:K23)-2,3)=0))</f>
+      <c r="L2" s="115" cm="1">
+        <f t="array" ref="L2">SUM(K5:K41*(MOD(ROW(K5:K41)-2,3)=0))</f>
         <v>0.11458333333333337</v>
       </c>
-      <c r="M2" s="135">
+      <c r="M2" s="116">
         <f>L2+Sprint_3!M2</f>
         <v>1.445138888888891</v>
       </c>
-      <c r="N2" s="31"/>
-    </row>
-    <row r="3" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="215">
+      <c r="N2" s="96" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" s="95">
+        <f>C2+F2+I2+L2</f>
+        <v>0.60416666666666685</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="211">
         <v>44585</v>
       </c>
       <c r="B3" s="10">
         <v>0.33333333333333331</v>
       </c>
-      <c r="C3" s="155" t="s">
+      <c r="C3" s="152" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="156"/>
+      <c r="D3" s="153"/>
       <c r="E3" s="11">
         <v>0.33333333333333331</v>
       </c>
-      <c r="F3" s="152" t="s">
+      <c r="F3" s="149" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="149"/>
+      <c r="G3" s="146"/>
       <c r="H3" s="12">
         <v>0.33333333333333331</v>
       </c>
-      <c r="I3" s="144" t="s">
+      <c r="I3" s="141" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="145"/>
+      <c r="J3" s="142"/>
       <c r="K3" s="33">
         <v>0.33333333333333331</v>
       </c>
@@ -4612,32 +5090,39 @@
         <v>26</v>
       </c>
       <c r="M3" s="137"/>
-    </row>
-    <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="216"/>
+      <c r="N3" s="96" t="s">
+        <v>18</v>
+      </c>
+      <c r="O3" s="95">
+        <f>D2+G2+J2+M2</f>
+        <v>5.57222222222223</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="212"/>
       <c r="B4" s="14">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C4" s="157"/>
-      <c r="D4" s="158"/>
+      <c r="C4" s="154"/>
+      <c r="D4" s="155"/>
       <c r="E4" s="15">
         <v>0.41666666666666669</v>
       </c>
-      <c r="F4" s="150"/>
-      <c r="G4" s="151"/>
+      <c r="F4" s="147"/>
+      <c r="G4" s="148"/>
       <c r="H4" s="16">
         <v>0.41666666666666669</v>
       </c>
-      <c r="I4" s="146"/>
-      <c r="J4" s="147"/>
+      <c r="I4" s="143"/>
+      <c r="J4" s="144"/>
       <c r="K4" s="39">
         <v>0.41666666666666669</v>
       </c>
       <c r="L4" s="138"/>
       <c r="M4" s="139"/>
     </row>
-    <row r="5" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="217"/>
+    <row r="5" spans="1:15" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="213"/>
       <c r="B5" s="68">
         <f>B4-B3</f>
         <v>8.333333333333337E-2</v>
@@ -4663,31 +5148,31 @@
       <c r="L5" s="75"/>
       <c r="M5" s="76"/>
     </row>
-    <row r="6" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="215">
+    <row r="6" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="211">
         <v>44585</v>
       </c>
       <c r="B6" s="10">
         <v>0.6875</v>
       </c>
-      <c r="C6" s="155" t="s">
+      <c r="C6" s="152" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="160"/>
+      <c r="D6" s="157"/>
       <c r="E6" s="11">
         <v>0.6875</v>
       </c>
-      <c r="F6" s="148" t="s">
+      <c r="F6" s="145" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="149"/>
+      <c r="G6" s="146"/>
       <c r="H6" s="12">
         <v>0.6875</v>
       </c>
-      <c r="I6" s="144" t="s">
+      <c r="I6" s="141" t="s">
         <v>29</v>
       </c>
-      <c r="J6" s="145"/>
+      <c r="J6" s="142"/>
       <c r="K6" s="13">
         <v>0.6875</v>
       </c>
@@ -4696,31 +5181,31 @@
       </c>
       <c r="M6" s="137"/>
     </row>
-    <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="216"/>
+    <row r="7" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="212"/>
       <c r="B7" s="14">
         <v>0.71875</v>
       </c>
-      <c r="C7" s="161"/>
-      <c r="D7" s="162"/>
+      <c r="C7" s="158"/>
+      <c r="D7" s="159"/>
       <c r="E7" s="15">
         <v>0.71875</v>
       </c>
-      <c r="F7" s="150"/>
-      <c r="G7" s="151"/>
+      <c r="F7" s="147"/>
+      <c r="G7" s="148"/>
       <c r="H7" s="16">
         <v>0.71875</v>
       </c>
-      <c r="I7" s="146"/>
-      <c r="J7" s="147"/>
+      <c r="I7" s="143"/>
+      <c r="J7" s="144"/>
       <c r="K7" s="39">
         <v>0.71875</v>
       </c>
       <c r="L7" s="138"/>
       <c r="M7" s="139"/>
     </row>
-    <row r="8" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="217"/>
+    <row r="8" spans="1:15" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="213"/>
       <c r="B8" s="68">
         <f>B7-B6</f>
         <v>3.125E-2</v>
@@ -4746,52 +5231,52 @@
       <c r="L8" s="81"/>
       <c r="M8" s="82"/>
     </row>
-    <row r="9" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="215">
+    <row r="9" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="211">
         <v>44586</v>
       </c>
       <c r="B9" s="10">
         <v>0.58333333333333337</v>
       </c>
-      <c r="C9" s="159" t="s">
+      <c r="C9" s="156" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="156"/>
+      <c r="D9" s="153"/>
       <c r="E9" s="11"/>
-      <c r="F9" s="148" t="s">
+      <c r="F9" s="145" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="149"/>
+      <c r="G9" s="146"/>
       <c r="H9" s="12"/>
-      <c r="I9" s="144" t="s">
+      <c r="I9" s="141" t="s">
         <v>24</v>
       </c>
-      <c r="J9" s="145"/>
+      <c r="J9" s="142"/>
       <c r="K9" s="40"/>
       <c r="L9" s="136" t="s">
         <v>24</v>
       </c>
       <c r="M9" s="137"/>
     </row>
-    <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="216"/>
+    <row r="10" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="212"/>
       <c r="B10" s="14">
         <v>0.6875</v>
       </c>
-      <c r="C10" s="157"/>
-      <c r="D10" s="158"/>
+      <c r="C10" s="154"/>
+      <c r="D10" s="155"/>
       <c r="E10" s="15"/>
-      <c r="F10" s="150"/>
-      <c r="G10" s="151"/>
+      <c r="F10" s="147"/>
+      <c r="G10" s="148"/>
       <c r="H10" s="16"/>
-      <c r="I10" s="146"/>
-      <c r="J10" s="147"/>
+      <c r="I10" s="143"/>
+      <c r="J10" s="144"/>
       <c r="K10" s="39"/>
       <c r="L10" s="138"/>
       <c r="M10" s="139"/>
     </row>
-    <row r="11" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="217"/>
+    <row r="11" spans="1:15" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="213"/>
       <c r="B11" s="68">
         <f>(B10-B9)</f>
         <v>0.10416666666666663</v>
@@ -4817,49 +5302,55 @@
       <c r="L11" s="81"/>
       <c r="M11" s="82"/>
     </row>
-    <row r="12" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="215"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="155" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="156"/>
+    <row r="12" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="211">
+        <v>44588</v>
+      </c>
+      <c r="B12" s="10">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="C12" s="152" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="153"/>
       <c r="E12" s="11"/>
-      <c r="F12" s="152" t="s">
+      <c r="F12" s="149" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="149"/>
+      <c r="G12" s="146"/>
       <c r="H12" s="12"/>
-      <c r="I12" s="144" t="s">
+      <c r="I12" s="141" t="s">
         <v>24</v>
       </c>
-      <c r="J12" s="145"/>
+      <c r="J12" s="142"/>
       <c r="K12" s="40"/>
       <c r="L12" s="136" t="s">
         <v>24</v>
       </c>
       <c r="M12" s="137"/>
     </row>
-    <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="216"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="157"/>
-      <c r="D13" s="158"/>
+    <row r="13" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="212"/>
+      <c r="B13" s="14">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="C13" s="154"/>
+      <c r="D13" s="155"/>
       <c r="E13" s="15"/>
-      <c r="F13" s="150"/>
-      <c r="G13" s="151"/>
+      <c r="F13" s="147"/>
+      <c r="G13" s="148"/>
       <c r="H13" s="16"/>
-      <c r="I13" s="146"/>
-      <c r="J13" s="147"/>
+      <c r="I13" s="143"/>
+      <c r="J13" s="144"/>
       <c r="K13" s="34"/>
       <c r="L13" s="138"/>
       <c r="M13" s="139"/>
     </row>
-    <row r="14" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="217"/>
+    <row r="14" spans="1:15" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="213"/>
       <c r="B14" s="68">
         <f>(B13-B12)</f>
-        <v>0</v>
+        <v>4.1666666666666741E-2</v>
       </c>
       <c r="C14" s="69"/>
       <c r="D14" s="70"/>
@@ -4882,46 +5373,46 @@
       <c r="L14" s="83"/>
       <c r="M14" s="84"/>
     </row>
-    <row r="15" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="215"/>
+    <row r="15" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="211"/>
       <c r="B15" s="10"/>
-      <c r="C15" s="155" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="156"/>
+      <c r="C15" s="152" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="153"/>
       <c r="E15" s="11"/>
-      <c r="F15" s="152" t="s">
+      <c r="F15" s="149" t="s">
         <v>24</v>
       </c>
-      <c r="G15" s="149"/>
+      <c r="G15" s="146"/>
       <c r="H15" s="12"/>
-      <c r="I15" s="144" t="s">
+      <c r="I15" s="141" t="s">
         <v>24</v>
       </c>
-      <c r="J15" s="145"/>
+      <c r="J15" s="142"/>
       <c r="K15" s="33"/>
       <c r="L15" s="136" t="s">
         <v>24</v>
       </c>
       <c r="M15" s="137"/>
     </row>
-    <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="216"/>
+    <row r="16" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="212"/>
       <c r="B16" s="14"/>
-      <c r="C16" s="157"/>
-      <c r="D16" s="158"/>
+      <c r="C16" s="154"/>
+      <c r="D16" s="155"/>
       <c r="E16" s="15"/>
-      <c r="F16" s="150"/>
-      <c r="G16" s="151"/>
+      <c r="F16" s="147"/>
+      <c r="G16" s="148"/>
       <c r="H16" s="16"/>
-      <c r="I16" s="146"/>
-      <c r="J16" s="147"/>
+      <c r="I16" s="143"/>
+      <c r="J16" s="144"/>
       <c r="K16" s="39"/>
       <c r="L16" s="138"/>
       <c r="M16" s="139"/>
     </row>
     <row r="17" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="217"/>
+      <c r="A17" s="213"/>
       <c r="B17" s="68">
         <f>(B16-B15)</f>
         <v>0</v>
@@ -4948,22 +5439,22 @@
       <c r="M17" s="82"/>
     </row>
     <row r="18" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="215"/>
+      <c r="A18" s="211"/>
       <c r="B18" s="10"/>
-      <c r="C18" s="155" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" s="156"/>
+      <c r="C18" s="152" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="153"/>
       <c r="E18" s="11"/>
-      <c r="F18" s="152" t="s">
+      <c r="F18" s="149" t="s">
         <v>24</v>
       </c>
-      <c r="G18" s="149"/>
+      <c r="G18" s="146"/>
       <c r="H18" s="12"/>
-      <c r="I18" s="144" t="s">
+      <c r="I18" s="141" t="s">
         <v>24</v>
       </c>
-      <c r="J18" s="145"/>
+      <c r="J18" s="142"/>
       <c r="K18" s="40"/>
       <c r="L18" s="136" t="s">
         <v>24</v>
@@ -4971,22 +5462,22 @@
       <c r="M18" s="137"/>
     </row>
     <row r="19" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="216"/>
+      <c r="A19" s="212"/>
       <c r="B19" s="14"/>
-      <c r="C19" s="157"/>
-      <c r="D19" s="158"/>
+      <c r="C19" s="154"/>
+      <c r="D19" s="155"/>
       <c r="E19" s="15"/>
-      <c r="F19" s="150"/>
-      <c r="G19" s="151"/>
+      <c r="F19" s="147"/>
+      <c r="G19" s="148"/>
       <c r="H19" s="16"/>
-      <c r="I19" s="146"/>
-      <c r="J19" s="147"/>
+      <c r="I19" s="143"/>
+      <c r="J19" s="144"/>
       <c r="K19" s="39"/>
       <c r="L19" s="138"/>
       <c r="M19" s="139"/>
     </row>
     <row r="20" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="217"/>
+      <c r="A20" s="213"/>
       <c r="B20" s="68">
         <f>(B19-B18)</f>
         <v>0</v>
@@ -5013,22 +5504,22 @@
       <c r="M20" s="82"/>
     </row>
     <row r="21" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="215"/>
+      <c r="A21" s="211"/>
       <c r="B21" s="10"/>
-      <c r="C21" s="155" t="s">
-        <v>23</v>
-      </c>
-      <c r="D21" s="156"/>
+      <c r="C21" s="152" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="153"/>
       <c r="E21" s="11"/>
-      <c r="F21" s="152" t="s">
+      <c r="F21" s="149" t="s">
         <v>24</v>
       </c>
-      <c r="G21" s="149"/>
+      <c r="G21" s="146"/>
       <c r="H21" s="12"/>
-      <c r="I21" s="144" t="s">
+      <c r="I21" s="141" t="s">
         <v>24</v>
       </c>
-      <c r="J21" s="145"/>
+      <c r="J21" s="142"/>
       <c r="K21" s="33"/>
       <c r="L21" s="136" t="s">
         <v>24</v>
@@ -5036,22 +5527,22 @@
       <c r="M21" s="137"/>
     </row>
     <row r="22" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="216"/>
+      <c r="A22" s="212"/>
       <c r="B22" s="14"/>
-      <c r="C22" s="157"/>
-      <c r="D22" s="158"/>
+      <c r="C22" s="154"/>
+      <c r="D22" s="155"/>
       <c r="E22" s="15"/>
-      <c r="F22" s="150"/>
-      <c r="G22" s="151"/>
+      <c r="F22" s="147"/>
+      <c r="G22" s="148"/>
       <c r="H22" s="16"/>
-      <c r="I22" s="146"/>
-      <c r="J22" s="147"/>
+      <c r="I22" s="143"/>
+      <c r="J22" s="144"/>
       <c r="K22" s="34"/>
       <c r="L22" s="138"/>
       <c r="M22" s="139"/>
     </row>
     <row r="23" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="217"/>
+      <c r="A23" s="213"/>
       <c r="B23" s="68">
         <f>(B22-B21)</f>
         <v>0</v>
@@ -5077,38 +5568,434 @@
       <c r="L23" s="85"/>
       <c r="M23" s="86"/>
     </row>
-    <row r="24" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A29" s="163" t="s">
-        <v>21</v>
-      </c>
-      <c r="B29" s="164"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A30" s="96" t="s">
-        <v>15</v>
-      </c>
-      <c r="B30" s="95">
-        <f>C2+F2+I2+L2</f>
-        <v>0.56250000000000011</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A31" s="96" t="s">
-        <v>18</v>
-      </c>
-      <c r="B31" s="95">
-        <f>D2+G2+J2+M2</f>
-        <v>5.5305555555555621</v>
-      </c>
-    </row>
+    <row r="24" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="211"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="152" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="153"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="149" t="s">
+        <v>23</v>
+      </c>
+      <c r="G24" s="146"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="141" t="s">
+        <v>23</v>
+      </c>
+      <c r="J24" s="142"/>
+      <c r="K24" s="33"/>
+      <c r="L24" s="136" t="s">
+        <v>23</v>
+      </c>
+      <c r="M24" s="137"/>
+    </row>
+    <row r="25" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="212"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="154"/>
+      <c r="D25" s="155"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="147"/>
+      <c r="G25" s="148"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="143"/>
+      <c r="J25" s="144"/>
+      <c r="K25" s="39"/>
+      <c r="L25" s="138"/>
+      <c r="M25" s="139"/>
+    </row>
+    <row r="26" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="213"/>
+      <c r="B26" s="117">
+        <f>(B25-B24)</f>
+        <v>0</v>
+      </c>
+      <c r="C26" s="118"/>
+      <c r="D26" s="119"/>
+      <c r="E26" s="120">
+        <f>E25-E24</f>
+        <v>0</v>
+      </c>
+      <c r="F26" s="121"/>
+      <c r="G26" s="122"/>
+      <c r="H26" s="126">
+        <f>H25-H24</f>
+        <v>0</v>
+      </c>
+      <c r="I26" s="127"/>
+      <c r="J26" s="128"/>
+      <c r="K26" s="129">
+        <f>K25-K24</f>
+        <v>0</v>
+      </c>
+      <c r="L26" s="130"/>
+      <c r="M26" s="131"/>
+    </row>
+    <row r="27" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="211"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="152" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" s="153"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="149" t="s">
+        <v>23</v>
+      </c>
+      <c r="G27" s="146"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="141" t="s">
+        <v>23</v>
+      </c>
+      <c r="J27" s="142"/>
+      <c r="K27" s="40"/>
+      <c r="L27" s="136" t="s">
+        <v>23</v>
+      </c>
+      <c r="M27" s="137"/>
+    </row>
+    <row r="28" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="212"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="154"/>
+      <c r="D28" s="155"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="147"/>
+      <c r="G28" s="148"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="143"/>
+      <c r="J28" s="144"/>
+      <c r="K28" s="39"/>
+      <c r="L28" s="138"/>
+      <c r="M28" s="139"/>
+    </row>
+    <row r="29" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="213"/>
+      <c r="B29" s="117">
+        <f>(B28-B27)</f>
+        <v>0</v>
+      </c>
+      <c r="C29" s="118"/>
+      <c r="D29" s="119"/>
+      <c r="E29" s="120">
+        <f>E28-E27</f>
+        <v>0</v>
+      </c>
+      <c r="F29" s="121"/>
+      <c r="G29" s="122"/>
+      <c r="H29" s="126">
+        <f>H28-H27</f>
+        <v>0</v>
+      </c>
+      <c r="I29" s="127"/>
+      <c r="J29" s="128"/>
+      <c r="K29" s="129">
+        <f>K28-K27</f>
+        <v>0</v>
+      </c>
+      <c r="L29" s="130"/>
+      <c r="M29" s="131"/>
+    </row>
+    <row r="30" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="211"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="152" t="s">
+        <v>23</v>
+      </c>
+      <c r="D30" s="153"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="149" t="s">
+        <v>23</v>
+      </c>
+      <c r="G30" s="146"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="141" t="s">
+        <v>23</v>
+      </c>
+      <c r="J30" s="142"/>
+      <c r="K30" s="33"/>
+      <c r="L30" s="136" t="s">
+        <v>23</v>
+      </c>
+      <c r="M30" s="137"/>
+    </row>
+    <row r="31" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="212"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="154"/>
+      <c r="D31" s="155"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="147"/>
+      <c r="G31" s="148"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="143"/>
+      <c r="J31" s="144"/>
+      <c r="K31" s="34"/>
+      <c r="L31" s="138"/>
+      <c r="M31" s="139"/>
+    </row>
+    <row r="32" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="213"/>
+      <c r="B32" s="117">
+        <f>(B31-B30)</f>
+        <v>0</v>
+      </c>
+      <c r="C32" s="118"/>
+      <c r="D32" s="119"/>
+      <c r="E32" s="120">
+        <f>E31-E30</f>
+        <v>0</v>
+      </c>
+      <c r="F32" s="121"/>
+      <c r="G32" s="122"/>
+      <c r="H32" s="126">
+        <f>H31-H30</f>
+        <v>0</v>
+      </c>
+      <c r="I32" s="127"/>
+      <c r="J32" s="128"/>
+      <c r="K32" s="134">
+        <f>K31-K30</f>
+        <v>0</v>
+      </c>
+      <c r="L32" s="134"/>
+      <c r="M32" s="135"/>
+    </row>
+    <row r="33" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="211"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="152" t="s">
+        <v>23</v>
+      </c>
+      <c r="D33" s="153"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="149" t="s">
+        <v>23</v>
+      </c>
+      <c r="G33" s="146"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="141" t="s">
+        <v>23</v>
+      </c>
+      <c r="J33" s="142"/>
+      <c r="K33" s="33"/>
+      <c r="L33" s="136" t="s">
+        <v>23</v>
+      </c>
+      <c r="M33" s="137"/>
+    </row>
+    <row r="34" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="212"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="154"/>
+      <c r="D34" s="155"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="147"/>
+      <c r="G34" s="148"/>
+      <c r="H34" s="16"/>
+      <c r="I34" s="143"/>
+      <c r="J34" s="144"/>
+      <c r="K34" s="39"/>
+      <c r="L34" s="138"/>
+      <c r="M34" s="139"/>
+    </row>
+    <row r="35" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="213"/>
+      <c r="B35" s="117">
+        <f>(B34-B33)</f>
+        <v>0</v>
+      </c>
+      <c r="C35" s="118"/>
+      <c r="D35" s="119"/>
+      <c r="E35" s="120">
+        <f>E34-E33</f>
+        <v>0</v>
+      </c>
+      <c r="F35" s="121"/>
+      <c r="G35" s="122"/>
+      <c r="H35" s="126">
+        <f>H34-H33</f>
+        <v>0</v>
+      </c>
+      <c r="I35" s="127"/>
+      <c r="J35" s="128"/>
+      <c r="K35" s="129">
+        <f>K34-K33</f>
+        <v>0</v>
+      </c>
+      <c r="L35" s="130"/>
+      <c r="M35" s="131"/>
+    </row>
+    <row r="36" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="211"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="152" t="s">
+        <v>23</v>
+      </c>
+      <c r="D36" s="153"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="149" t="s">
+        <v>23</v>
+      </c>
+      <c r="G36" s="146"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="141" t="s">
+        <v>23</v>
+      </c>
+      <c r="J36" s="142"/>
+      <c r="K36" s="40"/>
+      <c r="L36" s="136" t="s">
+        <v>23</v>
+      </c>
+      <c r="M36" s="137"/>
+    </row>
+    <row r="37" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="212"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="154"/>
+      <c r="D37" s="155"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="147"/>
+      <c r="G37" s="148"/>
+      <c r="H37" s="16"/>
+      <c r="I37" s="143"/>
+      <c r="J37" s="144"/>
+      <c r="K37" s="39"/>
+      <c r="L37" s="138"/>
+      <c r="M37" s="139"/>
+    </row>
+    <row r="38" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="213"/>
+      <c r="B38" s="117">
+        <f>(B37-B36)</f>
+        <v>0</v>
+      </c>
+      <c r="C38" s="118"/>
+      <c r="D38" s="119"/>
+      <c r="E38" s="120">
+        <f>E37-E36</f>
+        <v>0</v>
+      </c>
+      <c r="F38" s="121"/>
+      <c r="G38" s="122"/>
+      <c r="H38" s="126">
+        <f>H37-H36</f>
+        <v>0</v>
+      </c>
+      <c r="I38" s="127"/>
+      <c r="J38" s="128"/>
+      <c r="K38" s="129">
+        <f>K37-K36</f>
+        <v>0</v>
+      </c>
+      <c r="L38" s="130"/>
+      <c r="M38" s="131"/>
+    </row>
+    <row r="39" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="211"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="152" t="s">
+        <v>23</v>
+      </c>
+      <c r="D39" s="153"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="149" t="s">
+        <v>23</v>
+      </c>
+      <c r="G39" s="146"/>
+      <c r="H39" s="12"/>
+      <c r="I39" s="141" t="s">
+        <v>23</v>
+      </c>
+      <c r="J39" s="142"/>
+      <c r="K39" s="33"/>
+      <c r="L39" s="136" t="s">
+        <v>23</v>
+      </c>
+      <c r="M39" s="137"/>
+    </row>
+    <row r="40" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A40" s="212"/>
+      <c r="B40" s="14"/>
+      <c r="C40" s="154"/>
+      <c r="D40" s="155"/>
+      <c r="E40" s="15"/>
+      <c r="F40" s="147"/>
+      <c r="G40" s="148"/>
+      <c r="H40" s="16"/>
+      <c r="I40" s="143"/>
+      <c r="J40" s="144"/>
+      <c r="K40" s="34"/>
+      <c r="L40" s="138"/>
+      <c r="M40" s="139"/>
+    </row>
+    <row r="41" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A41" s="213"/>
+      <c r="B41" s="117">
+        <f>(B40-B39)</f>
+        <v>0</v>
+      </c>
+      <c r="C41" s="118"/>
+      <c r="D41" s="119"/>
+      <c r="E41" s="120">
+        <f>E40-E39</f>
+        <v>0</v>
+      </c>
+      <c r="F41" s="121"/>
+      <c r="G41" s="122"/>
+      <c r="H41" s="126">
+        <f>H40-H39</f>
+        <v>0</v>
+      </c>
+      <c r="I41" s="127"/>
+      <c r="J41" s="128"/>
+      <c r="K41" s="134">
+        <f>K40-K39</f>
+        <v>0</v>
+      </c>
+      <c r="L41" s="134"/>
+      <c r="M41" s="135"/>
+    </row>
+    <row r="42" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
-  <mergeCells count="37">
-    <mergeCell ref="A29:B29"/>
+  <mergeCells count="67">
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="C39:D40"/>
+    <mergeCell ref="F39:G40"/>
+    <mergeCell ref="I39:J40"/>
+    <mergeCell ref="L39:M40"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="C36:D37"/>
+    <mergeCell ref="F36:G37"/>
+    <mergeCell ref="I36:J37"/>
+    <mergeCell ref="L36:M37"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="C33:D34"/>
+    <mergeCell ref="F33:G34"/>
+    <mergeCell ref="I33:J34"/>
+    <mergeCell ref="L33:M34"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="C30:D31"/>
+    <mergeCell ref="F30:G31"/>
+    <mergeCell ref="I30:J31"/>
+    <mergeCell ref="L30:M31"/>
+    <mergeCell ref="L24:M25"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="C27:D28"/>
+    <mergeCell ref="F27:G28"/>
+    <mergeCell ref="I27:J28"/>
+    <mergeCell ref="L27:M28"/>
     <mergeCell ref="A18:A20"/>
     <mergeCell ref="C18:D19"/>
     <mergeCell ref="F18:G19"/>
     <mergeCell ref="I18:J19"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="C24:D25"/>
+    <mergeCell ref="F24:G25"/>
+    <mergeCell ref="I24:J25"/>
     <mergeCell ref="L18:M19"/>
     <mergeCell ref="A21:A23"/>
     <mergeCell ref="C21:D22"/>

</xml_diff>

<commit_message>
added new Ranged enemy Type
</commit_message>
<xml_diff>
--- a/Zeitaufzeichnung_Ishjarta.xlsx
+++ b/Zeitaufzeichnung_Ishjarta.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fragon\Documents\GitHub\ishjarta\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danijel\Desktop\ishjarta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF082128-9771-4486-B6A1-1495DBC9CDED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E3D51D-0929-4B2F-A52E-EDA25A52F54B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vorlage" sheetId="1" r:id="rId1"/>
@@ -1187,27 +1187,27 @@
     <xf numFmtId="165" fontId="2" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="6" borderId="10" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="12" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="12" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="12" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="12" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="6" borderId="10" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="12" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="12" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="12" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="12" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="167" fontId="2" fillId="6" borderId="17" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1244,41 +1244,41 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="5" borderId="1" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="32" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="30" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="5" borderId="31" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="32" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="33" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="165" fontId="2" fillId="5" borderId="23" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="5" borderId="1" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="165" fontId="2" fillId="5" borderId="31" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -1677,23 +1677,23 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.765625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="15.21875" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" customWidth="1"/>
-    <col min="3" max="4" width="13.6640625" customWidth="1"/>
-    <col min="5" max="5" width="16.109375" customWidth="1"/>
-    <col min="6" max="7" width="13.6640625" customWidth="1"/>
-    <col min="8" max="8" width="15.109375" customWidth="1"/>
-    <col min="9" max="10" width="13.6640625" customWidth="1"/>
-    <col min="11" max="11" width="15.109375" customWidth="1"/>
-    <col min="12" max="13" width="13.6640625" customWidth="1"/>
-    <col min="14" max="14" width="19.6640625" customWidth="1"/>
-    <col min="15" max="15" width="17.88671875" customWidth="1"/>
+    <col min="1" max="1" width="15.23046875" customWidth="1"/>
+    <col min="2" max="2" width="15.07421875" customWidth="1"/>
+    <col min="3" max="4" width="13.69140625" customWidth="1"/>
+    <col min="5" max="5" width="16.07421875" customWidth="1"/>
+    <col min="6" max="7" width="13.69140625" customWidth="1"/>
+    <col min="8" max="8" width="15.07421875" customWidth="1"/>
+    <col min="9" max="10" width="13.69140625" customWidth="1"/>
+    <col min="11" max="11" width="15.07421875" customWidth="1"/>
+    <col min="12" max="13" width="13.69140625" customWidth="1"/>
+    <col min="14" max="14" width="19.69140625" customWidth="1"/>
+    <col min="15" max="15" width="17.84375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="98" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A1" s="103" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1732,13 +1732,13 @@
       <c r="M1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="99" t="s">
+      <c r="N1" s="104" t="s">
         <v>4</v>
       </c>
-      <c r="O1" s="99"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="98"/>
+      <c r="O1" s="104"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A2" s="103"/>
       <c r="B2" s="9" t="s">
         <v>5</v>
       </c>
@@ -1791,36 +1791,36 @@
         <v>0.33333333333333615</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="100"/>
+    <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="98"/>
       <c r="B3" s="23">
         <v>0.33333333333333298</v>
       </c>
-      <c r="C3" s="101" t="s">
+      <c r="C3" s="99" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="101"/>
+      <c r="D3" s="99"/>
       <c r="E3" s="24">
         <v>0.33333333333333298</v>
       </c>
-      <c r="F3" s="102" t="s">
+      <c r="F3" s="100" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="102"/>
+      <c r="G3" s="100"/>
       <c r="H3" s="25">
         <v>0.33333333333333298</v>
       </c>
-      <c r="I3" s="103" t="s">
+      <c r="I3" s="101" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="103"/>
+      <c r="J3" s="101"/>
       <c r="K3" s="26">
         <v>0.33333333333333298</v>
       </c>
-      <c r="L3" s="104" t="s">
+      <c r="L3" s="102" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="104"/>
+      <c r="M3" s="102"/>
       <c r="N3" s="21" t="s">
         <v>10</v>
       </c>
@@ -1829,31 +1829,31 @@
         <v>5.3013888888889031</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="100"/>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A4" s="98"/>
       <c r="B4" s="27">
         <v>0.41666666666666702</v>
       </c>
-      <c r="C4" s="101"/>
-      <c r="D4" s="101"/>
+      <c r="C4" s="99"/>
+      <c r="D4" s="99"/>
       <c r="E4" s="28">
         <v>0.41666666666666702</v>
       </c>
-      <c r="F4" s="102"/>
-      <c r="G4" s="102"/>
+      <c r="F4" s="100"/>
+      <c r="G4" s="100"/>
       <c r="H4" s="29">
         <v>0.41666666666666702</v>
       </c>
-      <c r="I4" s="103"/>
-      <c r="J4" s="103"/>
+      <c r="I4" s="101"/>
+      <c r="J4" s="101"/>
       <c r="K4" s="30">
         <v>0.41666666666666702</v>
       </c>
-      <c r="L4" s="104"/>
-      <c r="M4" s="104"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="100"/>
+      <c r="L4" s="102"/>
+      <c r="M4" s="102"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A5" s="98"/>
       <c r="B5" s="31">
         <f>B4-B3</f>
         <v>8.3333333333334036E-2</v>
@@ -1879,46 +1879,46 @@
       <c r="L5" s="41"/>
       <c r="M5" s="42"/>
     </row>
-    <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="100"/>
+    <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="98"/>
       <c r="B6" s="23"/>
-      <c r="C6" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="101"/>
+      <c r="C6" s="99" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="99"/>
       <c r="E6" s="24"/>
-      <c r="F6" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="102"/>
+      <c r="F6" s="100" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="100"/>
       <c r="H6" s="25"/>
-      <c r="I6" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="J6" s="103"/>
+      <c r="I6" s="101" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="101"/>
       <c r="K6" s="43"/>
-      <c r="L6" s="104" t="s">
-        <v>12</v>
-      </c>
-      <c r="M6" s="104"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="100"/>
+      <c r="L6" s="102" t="s">
+        <v>12</v>
+      </c>
+      <c r="M6" s="102"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A7" s="98"/>
       <c r="B7" s="27"/>
-      <c r="C7" s="101"/>
-      <c r="D7" s="101"/>
+      <c r="C7" s="99"/>
+      <c r="D7" s="99"/>
       <c r="E7" s="28"/>
-      <c r="F7" s="102"/>
-      <c r="G7" s="102"/>
+      <c r="F7" s="100"/>
+      <c r="G7" s="100"/>
       <c r="H7" s="29"/>
-      <c r="I7" s="103"/>
-      <c r="J7" s="103"/>
+      <c r="I7" s="101"/>
+      <c r="J7" s="101"/>
       <c r="K7" s="30"/>
-      <c r="L7" s="104"/>
-      <c r="M7" s="104"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="100"/>
+      <c r="L7" s="102"/>
+      <c r="M7" s="102"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A8" s="98"/>
       <c r="B8" s="31">
         <f>B7-B6</f>
         <v>0</v>
@@ -1944,46 +1944,46 @@
       <c r="L8" s="45"/>
       <c r="M8" s="46"/>
     </row>
-    <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="100"/>
+    <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="98"/>
       <c r="B9" s="23"/>
-      <c r="C9" s="101" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="101"/>
+      <c r="C9" s="99" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="99"/>
       <c r="E9" s="24"/>
-      <c r="F9" s="102" t="s">
+      <c r="F9" s="100" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="102"/>
+      <c r="G9" s="100"/>
       <c r="H9" s="25"/>
-      <c r="I9" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="J9" s="103"/>
+      <c r="I9" s="101" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" s="101"/>
       <c r="K9" s="47"/>
-      <c r="L9" s="104" t="s">
-        <v>11</v>
-      </c>
-      <c r="M9" s="104"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="100"/>
+      <c r="L9" s="102" t="s">
+        <v>11</v>
+      </c>
+      <c r="M9" s="102"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A10" s="98"/>
       <c r="B10" s="27"/>
-      <c r="C10" s="101"/>
-      <c r="D10" s="101"/>
+      <c r="C10" s="99"/>
+      <c r="D10" s="99"/>
       <c r="E10" s="28"/>
-      <c r="F10" s="102"/>
-      <c r="G10" s="102"/>
+      <c r="F10" s="100"/>
+      <c r="G10" s="100"/>
       <c r="H10" s="29"/>
-      <c r="I10" s="103"/>
-      <c r="J10" s="103"/>
+      <c r="I10" s="101"/>
+      <c r="J10" s="101"/>
       <c r="K10" s="30"/>
-      <c r="L10" s="104"/>
-      <c r="M10" s="104"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="100"/>
+      <c r="L10" s="102"/>
+      <c r="M10" s="102"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A11" s="98"/>
       <c r="B11" s="31">
         <f>(B10-B9)</f>
         <v>0</v>
@@ -2009,46 +2009,46 @@
       <c r="L11" s="45"/>
       <c r="M11" s="46"/>
     </row>
-    <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="100"/>
+    <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="98"/>
       <c r="B12" s="23"/>
-      <c r="C12" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="101"/>
+      <c r="C12" s="99" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="99"/>
       <c r="E12" s="24"/>
-      <c r="F12" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" s="102"/>
+      <c r="F12" s="100" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="100"/>
       <c r="H12" s="25"/>
-      <c r="I12" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="J12" s="103"/>
+      <c r="I12" s="101" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" s="101"/>
       <c r="K12" s="47"/>
-      <c r="L12" s="104" t="s">
-        <v>11</v>
-      </c>
-      <c r="M12" s="104"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="100"/>
+      <c r="L12" s="102" t="s">
+        <v>11</v>
+      </c>
+      <c r="M12" s="102"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A13" s="98"/>
       <c r="B13" s="27"/>
-      <c r="C13" s="101"/>
-      <c r="D13" s="101"/>
+      <c r="C13" s="99"/>
+      <c r="D13" s="99"/>
       <c r="E13" s="28"/>
-      <c r="F13" s="102"/>
-      <c r="G13" s="102"/>
+      <c r="F13" s="100"/>
+      <c r="G13" s="100"/>
       <c r="H13" s="29"/>
-      <c r="I13" s="103"/>
-      <c r="J13" s="103"/>
+      <c r="I13" s="101"/>
+      <c r="J13" s="101"/>
       <c r="K13" s="48"/>
-      <c r="L13" s="104"/>
-      <c r="M13" s="104"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="100"/>
+      <c r="L13" s="102"/>
+      <c r="M13" s="102"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A14" s="98"/>
       <c r="B14" s="31">
         <f>(B13-B12)</f>
         <v>0</v>
@@ -2074,46 +2074,46 @@
       <c r="L14" s="49"/>
       <c r="M14" s="50"/>
     </row>
-    <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="100"/>
+    <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="98"/>
       <c r="B15" s="23"/>
-      <c r="C15" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="101"/>
+      <c r="C15" s="99" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="99"/>
       <c r="E15" s="24"/>
-      <c r="F15" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="G15" s="102"/>
+      <c r="F15" s="100" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="100"/>
       <c r="H15" s="25"/>
-      <c r="I15" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="J15" s="103"/>
+      <c r="I15" s="101" t="s">
+        <v>11</v>
+      </c>
+      <c r="J15" s="101"/>
       <c r="K15" s="26"/>
-      <c r="L15" s="104" t="s">
-        <v>11</v>
-      </c>
-      <c r="M15" s="104"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" s="100"/>
+      <c r="L15" s="102" t="s">
+        <v>11</v>
+      </c>
+      <c r="M15" s="102"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A16" s="98"/>
       <c r="B16" s="27"/>
-      <c r="C16" s="101"/>
-      <c r="D16" s="101"/>
+      <c r="C16" s="99"/>
+      <c r="D16" s="99"/>
       <c r="E16" s="28"/>
-      <c r="F16" s="102"/>
-      <c r="G16" s="102"/>
+      <c r="F16" s="100"/>
+      <c r="G16" s="100"/>
       <c r="H16" s="29"/>
-      <c r="I16" s="103"/>
-      <c r="J16" s="103"/>
+      <c r="I16" s="101"/>
+      <c r="J16" s="101"/>
       <c r="K16" s="30"/>
-      <c r="L16" s="104"/>
-      <c r="M16" s="104"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17" s="100"/>
+      <c r="L16" s="102"/>
+      <c r="M16" s="102"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A17" s="98"/>
       <c r="B17" s="31">
         <f>(B16-B15)</f>
         <v>0</v>
@@ -2139,46 +2139,46 @@
       <c r="L17" s="45"/>
       <c r="M17" s="46"/>
     </row>
-    <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="100"/>
+    <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="98"/>
       <c r="B18" s="23"/>
-      <c r="C18" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="101"/>
+      <c r="C18" s="99" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="99"/>
       <c r="E18" s="24"/>
-      <c r="F18" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="G18" s="102"/>
+      <c r="F18" s="100" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" s="100"/>
       <c r="H18" s="25"/>
-      <c r="I18" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="J18" s="103"/>
+      <c r="I18" s="101" t="s">
+        <v>11</v>
+      </c>
+      <c r="J18" s="101"/>
       <c r="K18" s="47"/>
-      <c r="L18" s="104" t="s">
-        <v>11</v>
-      </c>
-      <c r="M18" s="104"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="100"/>
+      <c r="L18" s="102" t="s">
+        <v>11</v>
+      </c>
+      <c r="M18" s="102"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A19" s="98"/>
       <c r="B19" s="27"/>
-      <c r="C19" s="101"/>
-      <c r="D19" s="101"/>
+      <c r="C19" s="99"/>
+      <c r="D19" s="99"/>
       <c r="E19" s="28"/>
-      <c r="F19" s="102"/>
-      <c r="G19" s="102"/>
+      <c r="F19" s="100"/>
+      <c r="G19" s="100"/>
       <c r="H19" s="29"/>
-      <c r="I19" s="103"/>
-      <c r="J19" s="103"/>
+      <c r="I19" s="101"/>
+      <c r="J19" s="101"/>
       <c r="K19" s="30"/>
-      <c r="L19" s="104"/>
-      <c r="M19" s="104"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" s="100"/>
+      <c r="L19" s="102"/>
+      <c r="M19" s="102"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A20" s="98"/>
       <c r="B20" s="31">
         <f>(B19-B18)</f>
         <v>0</v>
@@ -2204,46 +2204,46 @@
       <c r="L20" s="45"/>
       <c r="M20" s="46"/>
     </row>
-    <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="100"/>
+    <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="98"/>
       <c r="B21" s="23"/>
-      <c r="C21" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" s="101"/>
+      <c r="C21" s="99" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="99"/>
       <c r="E21" s="24"/>
-      <c r="F21" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="G21" s="102"/>
+      <c r="F21" s="100" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" s="100"/>
       <c r="H21" s="25"/>
-      <c r="I21" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="J21" s="103"/>
+      <c r="I21" s="101" t="s">
+        <v>11</v>
+      </c>
+      <c r="J21" s="101"/>
       <c r="K21" s="26"/>
-      <c r="L21" s="104" t="s">
-        <v>11</v>
-      </c>
-      <c r="M21" s="104"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" s="100"/>
+      <c r="L21" s="102" t="s">
+        <v>11</v>
+      </c>
+      <c r="M21" s="102"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A22" s="98"/>
       <c r="B22" s="27"/>
-      <c r="C22" s="101"/>
-      <c r="D22" s="101"/>
+      <c r="C22" s="99"/>
+      <c r="D22" s="99"/>
       <c r="E22" s="28"/>
-      <c r="F22" s="102"/>
-      <c r="G22" s="102"/>
+      <c r="F22" s="100"/>
+      <c r="G22" s="100"/>
       <c r="H22" s="29"/>
-      <c r="I22" s="103"/>
-      <c r="J22" s="103"/>
+      <c r="I22" s="101"/>
+      <c r="J22" s="101"/>
       <c r="K22" s="48"/>
-      <c r="L22" s="104"/>
-      <c r="M22" s="104"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23" s="100"/>
+      <c r="L22" s="102"/>
+      <c r="M22" s="102"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A23" s="98"/>
       <c r="B23" s="31">
         <f>(B22-B21)</f>
         <v>0</v>
@@ -2269,46 +2269,46 @@
       <c r="L23" s="51"/>
       <c r="M23" s="52"/>
     </row>
-    <row r="24" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="100"/>
+    <row r="24" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="98"/>
       <c r="B24" s="23"/>
-      <c r="C24" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" s="101"/>
+      <c r="C24" s="99" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="99"/>
       <c r="E24" s="24"/>
-      <c r="F24" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="G24" s="102"/>
+      <c r="F24" s="100" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" s="100"/>
       <c r="H24" s="25"/>
-      <c r="I24" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="J24" s="103"/>
+      <c r="I24" s="101" t="s">
+        <v>11</v>
+      </c>
+      <c r="J24" s="101"/>
       <c r="K24" s="26"/>
-      <c r="L24" s="104" t="s">
-        <v>11</v>
-      </c>
-      <c r="M24" s="104"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25" s="100"/>
+      <c r="L24" s="102" t="s">
+        <v>11</v>
+      </c>
+      <c r="M24" s="102"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A25" s="98"/>
       <c r="B25" s="27"/>
-      <c r="C25" s="101"/>
-      <c r="D25" s="101"/>
+      <c r="C25" s="99"/>
+      <c r="D25" s="99"/>
       <c r="E25" s="28"/>
-      <c r="F25" s="102"/>
-      <c r="G25" s="102"/>
+      <c r="F25" s="100"/>
+      <c r="G25" s="100"/>
       <c r="H25" s="29"/>
-      <c r="I25" s="103"/>
-      <c r="J25" s="103"/>
+      <c r="I25" s="101"/>
+      <c r="J25" s="101"/>
       <c r="K25" s="30"/>
-      <c r="L25" s="104"/>
-      <c r="M25" s="104"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26" s="100"/>
+      <c r="L25" s="102"/>
+      <c r="M25" s="102"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A26" s="98"/>
       <c r="B26" s="31">
         <f>(B25-B24)</f>
         <v>0</v>
@@ -2334,46 +2334,46 @@
       <c r="L26" s="45"/>
       <c r="M26" s="46"/>
     </row>
-    <row r="27" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="100"/>
+    <row r="27" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="98"/>
       <c r="B27" s="23"/>
-      <c r="C27" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="D27" s="101"/>
+      <c r="C27" s="99" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="99"/>
       <c r="E27" s="24"/>
-      <c r="F27" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="G27" s="102"/>
+      <c r="F27" s="100" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" s="100"/>
       <c r="H27" s="25"/>
-      <c r="I27" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="J27" s="103"/>
+      <c r="I27" s="101" t="s">
+        <v>11</v>
+      </c>
+      <c r="J27" s="101"/>
       <c r="K27" s="47"/>
-      <c r="L27" s="104" t="s">
-        <v>11</v>
-      </c>
-      <c r="M27" s="104"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28" s="100"/>
+      <c r="L27" s="102" t="s">
+        <v>11</v>
+      </c>
+      <c r="M27" s="102"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A28" s="98"/>
       <c r="B28" s="27"/>
-      <c r="C28" s="101"/>
-      <c r="D28" s="101"/>
+      <c r="C28" s="99"/>
+      <c r="D28" s="99"/>
       <c r="E28" s="28"/>
-      <c r="F28" s="102"/>
-      <c r="G28" s="102"/>
+      <c r="F28" s="100"/>
+      <c r="G28" s="100"/>
       <c r="H28" s="29"/>
-      <c r="I28" s="103"/>
-      <c r="J28" s="103"/>
+      <c r="I28" s="101"/>
+      <c r="J28" s="101"/>
       <c r="K28" s="30"/>
-      <c r="L28" s="104"/>
-      <c r="M28" s="104"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A29" s="100"/>
+      <c r="L28" s="102"/>
+      <c r="M28" s="102"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A29" s="98"/>
       <c r="B29" s="31">
         <f>(B28-B27)</f>
         <v>0</v>
@@ -2399,46 +2399,46 @@
       <c r="L29" s="45"/>
       <c r="M29" s="46"/>
     </row>
-    <row r="30" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="100"/>
+    <row r="30" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="98"/>
       <c r="B30" s="23"/>
-      <c r="C30" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="D30" s="101"/>
+      <c r="C30" s="99" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" s="99"/>
       <c r="E30" s="24"/>
-      <c r="F30" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="G30" s="102"/>
+      <c r="F30" s="100" t="s">
+        <v>11</v>
+      </c>
+      <c r="G30" s="100"/>
       <c r="H30" s="25"/>
-      <c r="I30" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="J30" s="103"/>
+      <c r="I30" s="101" t="s">
+        <v>11</v>
+      </c>
+      <c r="J30" s="101"/>
       <c r="K30" s="26"/>
-      <c r="L30" s="104" t="s">
-        <v>11</v>
-      </c>
-      <c r="M30" s="104"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A31" s="100"/>
+      <c r="L30" s="102" t="s">
+        <v>11</v>
+      </c>
+      <c r="M30" s="102"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A31" s="98"/>
       <c r="B31" s="27"/>
-      <c r="C31" s="101"/>
-      <c r="D31" s="101"/>
+      <c r="C31" s="99"/>
+      <c r="D31" s="99"/>
       <c r="E31" s="28"/>
-      <c r="F31" s="102"/>
-      <c r="G31" s="102"/>
+      <c r="F31" s="100"/>
+      <c r="G31" s="100"/>
       <c r="H31" s="29"/>
-      <c r="I31" s="103"/>
-      <c r="J31" s="103"/>
+      <c r="I31" s="101"/>
+      <c r="J31" s="101"/>
       <c r="K31" s="48"/>
-      <c r="L31" s="104"/>
-      <c r="M31" s="104"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A32" s="100"/>
+      <c r="L31" s="102"/>
+      <c r="M31" s="102"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A32" s="98"/>
       <c r="B32" s="31">
         <f>(B31-B30)</f>
         <v>0</v>
@@ -2464,46 +2464,46 @@
       <c r="L32" s="51"/>
       <c r="M32" s="52"/>
     </row>
-    <row r="33" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="100"/>
+    <row r="33" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="98"/>
       <c r="B33" s="23"/>
-      <c r="C33" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="D33" s="101"/>
+      <c r="C33" s="99" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="99"/>
       <c r="E33" s="24"/>
-      <c r="F33" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="G33" s="102"/>
+      <c r="F33" s="100" t="s">
+        <v>11</v>
+      </c>
+      <c r="G33" s="100"/>
       <c r="H33" s="25"/>
-      <c r="I33" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="J33" s="103"/>
+      <c r="I33" s="101" t="s">
+        <v>11</v>
+      </c>
+      <c r="J33" s="101"/>
       <c r="K33" s="26"/>
-      <c r="L33" s="104" t="s">
-        <v>11</v>
-      </c>
-      <c r="M33" s="104"/>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A34" s="100"/>
+      <c r="L33" s="102" t="s">
+        <v>11</v>
+      </c>
+      <c r="M33" s="102"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A34" s="98"/>
       <c r="B34" s="27"/>
-      <c r="C34" s="101"/>
-      <c r="D34" s="101"/>
+      <c r="C34" s="99"/>
+      <c r="D34" s="99"/>
       <c r="E34" s="28"/>
-      <c r="F34" s="102"/>
-      <c r="G34" s="102"/>
+      <c r="F34" s="100"/>
+      <c r="G34" s="100"/>
       <c r="H34" s="29"/>
-      <c r="I34" s="103"/>
-      <c r="J34" s="103"/>
+      <c r="I34" s="101"/>
+      <c r="J34" s="101"/>
       <c r="K34" s="30"/>
-      <c r="L34" s="104"/>
-      <c r="M34" s="104"/>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A35" s="100"/>
+      <c r="L34" s="102"/>
+      <c r="M34" s="102"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A35" s="98"/>
       <c r="B35" s="31">
         <f>(B34-B33)</f>
         <v>0</v>
@@ -2529,46 +2529,46 @@
       <c r="L35" s="45"/>
       <c r="M35" s="46"/>
     </row>
-    <row r="36" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="100"/>
+    <row r="36" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="98"/>
       <c r="B36" s="23"/>
-      <c r="C36" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="D36" s="101"/>
+      <c r="C36" s="99" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" s="99"/>
       <c r="E36" s="24"/>
-      <c r="F36" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="G36" s="102"/>
+      <c r="F36" s="100" t="s">
+        <v>11</v>
+      </c>
+      <c r="G36" s="100"/>
       <c r="H36" s="25"/>
-      <c r="I36" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="J36" s="103"/>
+      <c r="I36" s="101" t="s">
+        <v>11</v>
+      </c>
+      <c r="J36" s="101"/>
       <c r="K36" s="47"/>
-      <c r="L36" s="104" t="s">
-        <v>11</v>
-      </c>
-      <c r="M36" s="104"/>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A37" s="100"/>
+      <c r="L36" s="102" t="s">
+        <v>11</v>
+      </c>
+      <c r="M36" s="102"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A37" s="98"/>
       <c r="B37" s="27"/>
-      <c r="C37" s="101"/>
-      <c r="D37" s="101"/>
+      <c r="C37" s="99"/>
+      <c r="D37" s="99"/>
       <c r="E37" s="28"/>
-      <c r="F37" s="102"/>
-      <c r="G37" s="102"/>
+      <c r="F37" s="100"/>
+      <c r="G37" s="100"/>
       <c r="H37" s="29"/>
-      <c r="I37" s="103"/>
-      <c r="J37" s="103"/>
+      <c r="I37" s="101"/>
+      <c r="J37" s="101"/>
       <c r="K37" s="30"/>
-      <c r="L37" s="104"/>
-      <c r="M37" s="104"/>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A38" s="100"/>
+      <c r="L37" s="102"/>
+      <c r="M37" s="102"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A38" s="98"/>
       <c r="B38" s="31">
         <f>(B37-B36)</f>
         <v>0</v>
@@ -2594,46 +2594,46 @@
       <c r="L38" s="45"/>
       <c r="M38" s="46"/>
     </row>
-    <row r="39" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="100"/>
+    <row r="39" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="98"/>
       <c r="B39" s="23"/>
-      <c r="C39" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="D39" s="101"/>
+      <c r="C39" s="99" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" s="99"/>
       <c r="E39" s="24"/>
-      <c r="F39" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="G39" s="102"/>
+      <c r="F39" s="100" t="s">
+        <v>11</v>
+      </c>
+      <c r="G39" s="100"/>
       <c r="H39" s="25"/>
-      <c r="I39" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="J39" s="103"/>
+      <c r="I39" s="101" t="s">
+        <v>11</v>
+      </c>
+      <c r="J39" s="101"/>
       <c r="K39" s="26"/>
-      <c r="L39" s="104" t="s">
-        <v>11</v>
-      </c>
-      <c r="M39" s="104"/>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A40" s="100"/>
+      <c r="L39" s="102" t="s">
+        <v>11</v>
+      </c>
+      <c r="M39" s="102"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A40" s="98"/>
       <c r="B40" s="27"/>
-      <c r="C40" s="101"/>
-      <c r="D40" s="101"/>
+      <c r="C40" s="99"/>
+      <c r="D40" s="99"/>
       <c r="E40" s="28"/>
-      <c r="F40" s="102"/>
-      <c r="G40" s="102"/>
+      <c r="F40" s="100"/>
+      <c r="G40" s="100"/>
       <c r="H40" s="29"/>
-      <c r="I40" s="103"/>
-      <c r="J40" s="103"/>
+      <c r="I40" s="101"/>
+      <c r="J40" s="101"/>
       <c r="K40" s="48"/>
-      <c r="L40" s="104"/>
-      <c r="M40" s="104"/>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A41" s="100"/>
+      <c r="L40" s="102"/>
+      <c r="M40" s="102"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A41" s="98"/>
       <c r="B41" s="31">
         <f>(B40-B39)</f>
         <v>0</v>
@@ -2661,66 +2661,6 @@
     </row>
   </sheetData>
   <mergeCells count="67">
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="C39:D40"/>
-    <mergeCell ref="F39:G40"/>
-    <mergeCell ref="I39:J40"/>
-    <mergeCell ref="L39:M40"/>
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="C36:D37"/>
-    <mergeCell ref="F36:G37"/>
-    <mergeCell ref="I36:J37"/>
-    <mergeCell ref="L36:M37"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="C33:D34"/>
-    <mergeCell ref="F33:G34"/>
-    <mergeCell ref="I33:J34"/>
-    <mergeCell ref="L33:M34"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="C30:D31"/>
-    <mergeCell ref="F30:G31"/>
-    <mergeCell ref="I30:J31"/>
-    <mergeCell ref="L30:M31"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="C27:D28"/>
-    <mergeCell ref="F27:G28"/>
-    <mergeCell ref="I27:J28"/>
-    <mergeCell ref="L27:M28"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="C24:D25"/>
-    <mergeCell ref="F24:G25"/>
-    <mergeCell ref="I24:J25"/>
-    <mergeCell ref="L24:M25"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="C21:D22"/>
-    <mergeCell ref="F21:G22"/>
-    <mergeCell ref="I21:J22"/>
-    <mergeCell ref="L21:M22"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="C18:D19"/>
-    <mergeCell ref="F18:G19"/>
-    <mergeCell ref="I18:J19"/>
-    <mergeCell ref="L18:M19"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="C15:D16"/>
-    <mergeCell ref="F15:G16"/>
-    <mergeCell ref="I15:J16"/>
-    <mergeCell ref="L15:M16"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="C12:D13"/>
-    <mergeCell ref="F12:G13"/>
-    <mergeCell ref="I12:J13"/>
-    <mergeCell ref="L12:M13"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="C9:D10"/>
-    <mergeCell ref="F9:G10"/>
-    <mergeCell ref="I9:J10"/>
-    <mergeCell ref="L9:M10"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="C6:D7"/>
-    <mergeCell ref="F6:G7"/>
-    <mergeCell ref="I6:J7"/>
-    <mergeCell ref="L6:M7"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="A3:A5"/>
@@ -2728,6 +2668,66 @@
     <mergeCell ref="F3:G4"/>
     <mergeCell ref="I3:J4"/>
     <mergeCell ref="L3:M4"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="C6:D7"/>
+    <mergeCell ref="F6:G7"/>
+    <mergeCell ref="I6:J7"/>
+    <mergeCell ref="L6:M7"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="C9:D10"/>
+    <mergeCell ref="F9:G10"/>
+    <mergeCell ref="I9:J10"/>
+    <mergeCell ref="L9:M10"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="C12:D13"/>
+    <mergeCell ref="F12:G13"/>
+    <mergeCell ref="I12:J13"/>
+    <mergeCell ref="L12:M13"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="C15:D16"/>
+    <mergeCell ref="F15:G16"/>
+    <mergeCell ref="I15:J16"/>
+    <mergeCell ref="L15:M16"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="C18:D19"/>
+    <mergeCell ref="F18:G19"/>
+    <mergeCell ref="I18:J19"/>
+    <mergeCell ref="L18:M19"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="C21:D22"/>
+    <mergeCell ref="F21:G22"/>
+    <mergeCell ref="I21:J22"/>
+    <mergeCell ref="L21:M22"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="C24:D25"/>
+    <mergeCell ref="F24:G25"/>
+    <mergeCell ref="I24:J25"/>
+    <mergeCell ref="L24:M25"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="C27:D28"/>
+    <mergeCell ref="F27:G28"/>
+    <mergeCell ref="I27:J28"/>
+    <mergeCell ref="L27:M28"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="C30:D31"/>
+    <mergeCell ref="F30:G31"/>
+    <mergeCell ref="I30:J31"/>
+    <mergeCell ref="L30:M31"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="C33:D34"/>
+    <mergeCell ref="F33:G34"/>
+    <mergeCell ref="I33:J34"/>
+    <mergeCell ref="L33:M34"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="C36:D37"/>
+    <mergeCell ref="F36:G37"/>
+    <mergeCell ref="I36:J37"/>
+    <mergeCell ref="L36:M37"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="C39:D40"/>
+    <mergeCell ref="F39:G40"/>
+    <mergeCell ref="I39:J40"/>
+    <mergeCell ref="L39:M40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2742,13 +2742,13 @@
       <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.765625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="15.21875" customWidth="1"/>
-    <col min="2" max="9" width="17.21875" customWidth="1"/>
+    <col min="1" max="1" width="15.23046875" customWidth="1"/>
+    <col min="2" max="9" width="17.23046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A1" s="53"/>
       <c r="B1" s="54" t="s">
         <v>5</v>
@@ -2779,7 +2779,7 @@
         <v>0.33333333333333393</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A2" s="105">
         <v>44535</v>
       </c>
@@ -2806,7 +2806,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A3" s="105"/>
       <c r="B3" s="27">
         <v>1</v>
@@ -2825,7 +2825,7 @@
       </c>
       <c r="I3" s="109"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A4" s="105"/>
       <c r="B4" s="110">
         <f>B3-B2</f>
@@ -2848,7 +2848,7 @@
       </c>
       <c r="I4" s="113"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A5" s="105">
         <v>44542</v>
       </c>
@@ -2875,7 +2875,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A6" s="105"/>
       <c r="B6" s="27">
         <v>1</v>
@@ -2894,7 +2894,7 @@
       </c>
       <c r="I6" s="109"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A7" s="105"/>
       <c r="B7" s="110">
         <f>B6-B5</f>
@@ -2917,7 +2917,7 @@
       </c>
       <c r="I7" s="113"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A8" s="105"/>
       <c r="B8" s="23"/>
       <c r="C8" s="106" t="s">
@@ -2936,7 +2936,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A9" s="105"/>
       <c r="B9" s="27"/>
       <c r="C9" s="106"/>
@@ -2947,7 +2947,7 @@
       <c r="H9" s="63"/>
       <c r="I9" s="109"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A10" s="105"/>
       <c r="B10" s="110">
         <f>(B9-B8)</f>
@@ -2970,7 +2970,7 @@
       </c>
       <c r="I10" s="113"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A11" s="105"/>
       <c r="B11" s="23"/>
       <c r="C11" s="106" t="s">
@@ -2989,7 +2989,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A12" s="105"/>
       <c r="B12" s="27"/>
       <c r="C12" s="106"/>
@@ -3000,7 +3000,7 @@
       <c r="H12" s="63"/>
       <c r="I12" s="109"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A13" s="105"/>
       <c r="B13" s="110">
         <f>(B12-B11)</f>
@@ -3023,7 +3023,7 @@
       </c>
       <c r="I13" s="113"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A14" s="105"/>
       <c r="B14" s="23"/>
       <c r="C14" s="106" t="s">
@@ -3042,7 +3042,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A15" s="105"/>
       <c r="B15" s="27"/>
       <c r="C15" s="106"/>
@@ -3053,7 +3053,7 @@
       <c r="H15" s="63"/>
       <c r="I15" s="109"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A16" s="105"/>
       <c r="B16" s="110">
         <f>(B15-B14)</f>
@@ -3076,7 +3076,7 @@
       </c>
       <c r="I16" s="113"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A17" s="105"/>
       <c r="B17" s="23"/>
       <c r="C17" s="106" t="s">
@@ -3095,7 +3095,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A18" s="105"/>
       <c r="B18" s="27"/>
       <c r="C18" s="106"/>
@@ -3106,7 +3106,7 @@
       <c r="H18" s="63"/>
       <c r="I18" s="109"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A19" s="105"/>
       <c r="B19" s="110">
         <f>(B18-B17)</f>
@@ -3129,7 +3129,7 @@
       </c>
       <c r="I19" s="113"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A20" s="105"/>
       <c r="B20" s="23"/>
       <c r="C20" s="106" t="s">
@@ -3148,7 +3148,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A21" s="105"/>
       <c r="B21" s="27"/>
       <c r="C21" s="106"/>
@@ -3159,7 +3159,7 @@
       <c r="H21" s="63"/>
       <c r="I21" s="109"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A22" s="105"/>
       <c r="B22" s="110">
         <f>(B21-B20)</f>
@@ -3184,6 +3184,60 @@
     </row>
   </sheetData>
   <mergeCells count="63">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H19:I19"/>
     <mergeCell ref="A20:A22"/>
     <mergeCell ref="C20:C21"/>
     <mergeCell ref="E20:E21"/>
@@ -3193,60 +3247,6 @@
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="F22:G22"/>
     <mergeCell ref="H22:I22"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -3261,20 +3261,20 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.765625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="15.21875" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" customWidth="1"/>
-    <col min="3" max="4" width="13.6640625" customWidth="1"/>
-    <col min="5" max="5" width="16.109375" customWidth="1"/>
-    <col min="6" max="7" width="13.6640625" customWidth="1"/>
-    <col min="8" max="8" width="15.109375" customWidth="1"/>
-    <col min="9" max="10" width="13.6640625" customWidth="1"/>
-    <col min="11" max="11" width="15.109375" customWidth="1"/>
-    <col min="12" max="13" width="13.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.23046875" customWidth="1"/>
+    <col min="2" max="2" width="15.07421875" customWidth="1"/>
+    <col min="3" max="4" width="13.69140625" customWidth="1"/>
+    <col min="5" max="5" width="16.07421875" customWidth="1"/>
+    <col min="6" max="7" width="13.69140625" customWidth="1"/>
+    <col min="8" max="8" width="15.07421875" customWidth="1"/>
+    <col min="9" max="10" width="13.69140625" customWidth="1"/>
+    <col min="11" max="11" width="15.07421875" customWidth="1"/>
+    <col min="12" max="13" width="13.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A1" s="53"/>
       <c r="B1" s="64" t="s">
         <v>5</v>
@@ -3322,7 +3322,7 @@
       </c>
       <c r="N1" s="76"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A2" s="105">
         <v>44543</v>
       </c>
@@ -3350,13 +3350,13 @@
       <c r="K2" s="26">
         <v>0.33333333333333298</v>
       </c>
-      <c r="L2" s="117" t="s">
-        <v>12</v>
-      </c>
-      <c r="M2" s="117"/>
+      <c r="L2" s="120" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="120"/>
       <c r="N2" s="77"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A3" s="105"/>
       <c r="B3" s="27">
         <v>0.49166666666666697</v>
@@ -3376,10 +3376,10 @@
       <c r="K3" s="30">
         <v>0.41666666666666702</v>
       </c>
-      <c r="L3" s="117"/>
-      <c r="M3" s="117"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L3" s="120"/>
+      <c r="M3" s="120"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A4" s="105"/>
       <c r="B4" s="110">
         <f>B3-B2</f>
@@ -3399,14 +3399,14 @@
       </c>
       <c r="I4" s="112"/>
       <c r="J4" s="112"/>
-      <c r="K4" s="118">
+      <c r="K4" s="123">
         <f>K3-K2</f>
         <v>8.3333333333334036E-2</v>
       </c>
-      <c r="L4" s="118"/>
-      <c r="M4" s="118"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L4" s="123"/>
+      <c r="M4" s="123"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A5" s="105">
         <v>44568</v>
       </c>
@@ -3430,12 +3430,12 @@
       <c r="K5" s="43">
         <v>0.33333333333333298</v>
       </c>
-      <c r="L5" s="119" t="s">
+      <c r="L5" s="117" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="119"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M5" s="117"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A6" s="105"/>
       <c r="B6" s="27"/>
       <c r="C6" s="114"/>
@@ -3451,10 +3451,10 @@
       <c r="K6" s="30">
         <v>0.625</v>
       </c>
-      <c r="L6" s="119"/>
-      <c r="M6" s="119"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L6" s="117"/>
+      <c r="M6" s="117"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A7" s="105"/>
       <c r="B7" s="110">
         <f>B6-B5</f>
@@ -3481,7 +3481,7 @@
       <c r="L7" s="113"/>
       <c r="M7" s="113"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A8" s="105">
         <v>44569</v>
       </c>
@@ -3509,12 +3509,12 @@
       <c r="K8" s="47">
         <v>0.77083333333333304</v>
       </c>
-      <c r="L8" s="120" t="s">
-        <v>12</v>
-      </c>
-      <c r="M8" s="120"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L8" s="119" t="s">
+        <v>12</v>
+      </c>
+      <c r="M8" s="119"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A9" s="105"/>
       <c r="B9" s="27">
         <v>1</v>
@@ -3534,10 +3534,10 @@
       <c r="K9" s="30">
         <v>0.91666666666666696</v>
       </c>
-      <c r="L9" s="120"/>
-      <c r="M9" s="120"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L9" s="119"/>
+      <c r="M9" s="119"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A10" s="105"/>
       <c r="B10" s="110">
         <f>(B9-B8)</f>
@@ -3564,7 +3564,7 @@
       <c r="L10" s="113"/>
       <c r="M10" s="113"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A11" s="105">
         <v>44805</v>
       </c>
@@ -3597,7 +3597,7 @@
       </c>
       <c r="M11" s="121"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A12" s="105"/>
       <c r="B12" s="27">
         <v>1</v>
@@ -3620,7 +3620,7 @@
       <c r="L12" s="121"/>
       <c r="M12" s="121"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A13" s="105"/>
       <c r="B13" s="110">
         <f>(B12-B11)</f>
@@ -3647,7 +3647,7 @@
       <c r="L13" s="122"/>
       <c r="M13" s="122"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A14" s="105"/>
       <c r="B14" s="23"/>
       <c r="C14" s="114" t="s">
@@ -3665,12 +3665,12 @@
       </c>
       <c r="J14" s="116"/>
       <c r="K14" s="26"/>
-      <c r="L14" s="117" t="s">
-        <v>12</v>
-      </c>
-      <c r="M14" s="117"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L14" s="120" t="s">
+        <v>12</v>
+      </c>
+      <c r="M14" s="120"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A15" s="105"/>
       <c r="B15" s="27"/>
       <c r="C15" s="114"/>
@@ -3682,10 +3682,10 @@
       <c r="I15" s="116"/>
       <c r="J15" s="116"/>
       <c r="K15" s="30"/>
-      <c r="L15" s="117"/>
-      <c r="M15" s="117"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L15" s="120"/>
+      <c r="M15" s="120"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A16" s="105"/>
       <c r="B16" s="110">
         <f>(B15-B14)</f>
@@ -3712,7 +3712,7 @@
       <c r="L16" s="113"/>
       <c r="M16" s="113"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A17" s="105"/>
       <c r="B17" s="23"/>
       <c r="C17" s="114" t="s">
@@ -3730,12 +3730,12 @@
       </c>
       <c r="J17" s="116"/>
       <c r="K17" s="47"/>
-      <c r="L17" s="120" t="s">
-        <v>12</v>
-      </c>
-      <c r="M17" s="120"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L17" s="119" t="s">
+        <v>12</v>
+      </c>
+      <c r="M17" s="119"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A18" s="105"/>
       <c r="B18" s="27"/>
       <c r="C18" s="114"/>
@@ -3747,10 +3747,10 @@
       <c r="I18" s="116"/>
       <c r="J18" s="116"/>
       <c r="K18" s="30"/>
-      <c r="L18" s="120"/>
-      <c r="M18" s="120"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L18" s="119"/>
+      <c r="M18" s="119"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A19" s="105"/>
       <c r="B19" s="110">
         <f>(B18-B17)</f>
@@ -3777,7 +3777,7 @@
       <c r="L19" s="113"/>
       <c r="M19" s="113"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A20" s="105"/>
       <c r="B20" s="23"/>
       <c r="C20" s="114" t="s">
@@ -3795,12 +3795,12 @@
       </c>
       <c r="J20" s="116"/>
       <c r="K20" s="26"/>
-      <c r="L20" s="119" t="s">
-        <v>12</v>
-      </c>
-      <c r="M20" s="119"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L20" s="117" t="s">
+        <v>12</v>
+      </c>
+      <c r="M20" s="117"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A21" s="105"/>
       <c r="B21" s="27"/>
       <c r="C21" s="114"/>
@@ -3812,10 +3812,10 @@
       <c r="I21" s="116"/>
       <c r="J21" s="116"/>
       <c r="K21" s="48"/>
-      <c r="L21" s="119"/>
-      <c r="M21" s="119"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L21" s="117"/>
+      <c r="M21" s="117"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A22" s="105"/>
       <c r="B22" s="110">
         <f>(B21-B20)</f>
@@ -3835,15 +3835,69 @@
       </c>
       <c r="I22" s="112"/>
       <c r="J22" s="112"/>
-      <c r="K22" s="123">
+      <c r="K22" s="118">
         <f>K21-K20</f>
         <v>0</v>
       </c>
-      <c r="L22" s="123"/>
-      <c r="M22" s="123"/>
+      <c r="L22" s="118"/>
+      <c r="M22" s="118"/>
     </row>
   </sheetData>
   <mergeCells count="63">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="C2:D3"/>
+    <mergeCell ref="F2:G3"/>
+    <mergeCell ref="I2:J3"/>
+    <mergeCell ref="L2:M3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="C5:D6"/>
+    <mergeCell ref="F5:G6"/>
+    <mergeCell ref="I5:J6"/>
+    <mergeCell ref="L5:M6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="C8:D9"/>
+    <mergeCell ref="F8:G9"/>
+    <mergeCell ref="I8:J9"/>
+    <mergeCell ref="L8:M9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="C11:D12"/>
+    <mergeCell ref="F11:G12"/>
+    <mergeCell ref="I11:J12"/>
+    <mergeCell ref="L11:M12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="C14:D15"/>
+    <mergeCell ref="F14:G15"/>
+    <mergeCell ref="I14:J15"/>
+    <mergeCell ref="L14:M15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="C17:D18"/>
+    <mergeCell ref="F17:G18"/>
+    <mergeCell ref="I17:J18"/>
+    <mergeCell ref="L17:M18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="K19:M19"/>
     <mergeCell ref="A20:A22"/>
     <mergeCell ref="C20:D21"/>
     <mergeCell ref="F20:G21"/>
@@ -3853,60 +3907,6 @@
     <mergeCell ref="E22:G22"/>
     <mergeCell ref="H22:J22"/>
     <mergeCell ref="K22:M22"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="C17:D18"/>
-    <mergeCell ref="F17:G18"/>
-    <mergeCell ref="I17:J18"/>
-    <mergeCell ref="L17:M18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="K19:M19"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="C14:D15"/>
-    <mergeCell ref="F14:G15"/>
-    <mergeCell ref="I14:J15"/>
-    <mergeCell ref="L14:M15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="K16:M16"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="C11:D12"/>
-    <mergeCell ref="F11:G12"/>
-    <mergeCell ref="I11:J12"/>
-    <mergeCell ref="L11:M12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="K13:M13"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="C8:D9"/>
-    <mergeCell ref="F8:G9"/>
-    <mergeCell ref="I8:J9"/>
-    <mergeCell ref="L8:M9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="K10:M10"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="C5:D6"/>
-    <mergeCell ref="F5:G6"/>
-    <mergeCell ref="I5:J6"/>
-    <mergeCell ref="L5:M6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="C2:D3"/>
-    <mergeCell ref="F2:G3"/>
-    <mergeCell ref="I2:J3"/>
-    <mergeCell ref="L2:M3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:M4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -3921,21 +3921,21 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.765625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="15.21875" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" customWidth="1"/>
-    <col min="3" max="4" width="13.6640625" customWidth="1"/>
-    <col min="5" max="5" width="16.109375" customWidth="1"/>
-    <col min="6" max="7" width="13.6640625" customWidth="1"/>
-    <col min="8" max="8" width="15.109375" customWidth="1"/>
-    <col min="9" max="10" width="13.6640625" customWidth="1"/>
-    <col min="11" max="11" width="15.109375" customWidth="1"/>
-    <col min="12" max="13" width="13.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.23046875" customWidth="1"/>
+    <col min="2" max="2" width="15.07421875" customWidth="1"/>
+    <col min="3" max="4" width="13.69140625" customWidth="1"/>
+    <col min="5" max="5" width="16.07421875" customWidth="1"/>
+    <col min="6" max="7" width="13.69140625" customWidth="1"/>
+    <col min="8" max="8" width="15.07421875" customWidth="1"/>
+    <col min="9" max="10" width="13.69140625" customWidth="1"/>
+    <col min="11" max="11" width="15.07421875" customWidth="1"/>
+    <col min="12" max="13" width="13.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="124" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A1" s="128" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="78" t="s">
@@ -3976,8 +3976,8 @@
       </c>
       <c r="N1" s="76"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="124"/>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A2" s="128"/>
       <c r="B2" s="86" t="s">
         <v>5</v>
       </c>
@@ -4024,64 +4024,64 @@
       </c>
       <c r="N2" s="77"/>
     </row>
-    <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="100">
+    <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="98">
         <v>44571</v>
       </c>
       <c r="B3" s="23">
         <v>0.33333333333333298</v>
       </c>
-      <c r="C3" s="125" t="s">
+      <c r="C3" s="124" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="125"/>
+      <c r="D3" s="124"/>
       <c r="E3" s="24">
         <v>0.33333333333333298</v>
       </c>
-      <c r="F3" s="126" t="s">
+      <c r="F3" s="125" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="126"/>
+      <c r="G3" s="125"/>
       <c r="H3" s="25">
         <v>0.33333333333333298</v>
       </c>
-      <c r="I3" s="127" t="s">
+      <c r="I3" s="126" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="127"/>
+      <c r="J3" s="126"/>
       <c r="K3" s="26">
         <v>0.33333333333333298</v>
       </c>
-      <c r="L3" s="128" t="s">
+      <c r="L3" s="127" t="s">
         <v>21</v>
       </c>
-      <c r="M3" s="128"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="100"/>
+      <c r="M3" s="127"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A4" s="98"/>
       <c r="B4" s="27">
         <v>0.41666666666666702</v>
       </c>
-      <c r="C4" s="125"/>
-      <c r="D4" s="125"/>
+      <c r="C4" s="124"/>
+      <c r="D4" s="124"/>
       <c r="E4" s="28">
         <v>0.41666666666666702</v>
       </c>
-      <c r="F4" s="126"/>
-      <c r="G4" s="126"/>
+      <c r="F4" s="125"/>
+      <c r="G4" s="125"/>
       <c r="H4" s="29">
         <v>0.41666666666666702</v>
       </c>
-      <c r="I4" s="127"/>
-      <c r="J4" s="127"/>
+      <c r="I4" s="126"/>
+      <c r="J4" s="126"/>
       <c r="K4" s="30">
         <v>0.41666666666666702</v>
       </c>
-      <c r="L4" s="128"/>
-      <c r="M4" s="128"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="100"/>
+      <c r="L4" s="127"/>
+      <c r="M4" s="127"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A5" s="98"/>
       <c r="B5" s="31">
         <f>B4-B3</f>
         <v>8.3333333333334036E-2</v>
@@ -4107,64 +4107,64 @@
       <c r="L5" s="41"/>
       <c r="M5" s="42"/>
     </row>
-    <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="100">
+    <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="98">
         <v>44583</v>
       </c>
       <c r="B6" s="23">
         <v>0.79166666666666696</v>
       </c>
-      <c r="C6" s="125" t="s">
+      <c r="C6" s="124" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="125"/>
+      <c r="D6" s="124"/>
       <c r="E6" s="24">
         <v>0.82291666666666696</v>
       </c>
-      <c r="F6" s="126" t="s">
+      <c r="F6" s="125" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="126"/>
+      <c r="G6" s="125"/>
       <c r="H6" s="25">
         <v>0.79166666666666696</v>
       </c>
-      <c r="I6" s="127" t="s">
+      <c r="I6" s="126" t="s">
         <v>22</v>
       </c>
-      <c r="J6" s="127"/>
+      <c r="J6" s="126"/>
       <c r="K6" s="43">
         <v>0.79166666666666696</v>
       </c>
-      <c r="L6" s="128" t="s">
+      <c r="L6" s="127" t="s">
         <v>22</v>
       </c>
-      <c r="M6" s="128"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="100"/>
+      <c r="M6" s="127"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A7" s="98"/>
       <c r="B7" s="27">
         <v>0.89791666666666703</v>
       </c>
-      <c r="C7" s="125"/>
-      <c r="D7" s="125"/>
+      <c r="C7" s="124"/>
+      <c r="D7" s="124"/>
       <c r="E7" s="28">
         <v>0.89791666666666703</v>
       </c>
-      <c r="F7" s="126"/>
-      <c r="G7" s="126"/>
+      <c r="F7" s="125"/>
+      <c r="G7" s="125"/>
       <c r="H7" s="29">
         <v>0.89583333333333304</v>
       </c>
-      <c r="I7" s="127"/>
-      <c r="J7" s="127"/>
+      <c r="I7" s="126"/>
+      <c r="J7" s="126"/>
       <c r="K7" s="30">
         <v>0.89791666666666703</v>
       </c>
-      <c r="L7" s="128"/>
-      <c r="M7" s="128"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="100"/>
+      <c r="L7" s="127"/>
+      <c r="M7" s="127"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A8" s="98"/>
       <c r="B8" s="31">
         <f>B7-B6</f>
         <v>0.10625000000000007</v>
@@ -4190,64 +4190,64 @@
       <c r="L8" s="45"/>
       <c r="M8" s="46"/>
     </row>
-    <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="100">
+    <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="98">
         <v>44584</v>
       </c>
       <c r="B9" s="23">
         <v>0.75694444444444398</v>
       </c>
-      <c r="C9" s="125" t="s">
+      <c r="C9" s="124" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="125"/>
+      <c r="D9" s="124"/>
       <c r="E9" s="24">
         <v>0.75694444444444398</v>
       </c>
-      <c r="F9" s="126" t="s">
+      <c r="F9" s="125" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="126"/>
+      <c r="G9" s="125"/>
       <c r="H9" s="25">
         <v>0.75694444444444398</v>
       </c>
-      <c r="I9" s="127" t="s">
+      <c r="I9" s="126" t="s">
         <v>23</v>
       </c>
-      <c r="J9" s="127"/>
+      <c r="J9" s="126"/>
       <c r="K9" s="47">
         <v>0.75694444444444398</v>
       </c>
-      <c r="L9" s="128" t="s">
+      <c r="L9" s="127" t="s">
         <v>23</v>
       </c>
-      <c r="M9" s="128"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="100"/>
+      <c r="M9" s="127"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A10" s="98"/>
       <c r="B10" s="27">
         <v>0.83541666666666703</v>
       </c>
-      <c r="C10" s="125"/>
-      <c r="D10" s="125"/>
+      <c r="C10" s="124"/>
+      <c r="D10" s="124"/>
       <c r="E10" s="28">
         <v>0.83541666666666703</v>
       </c>
-      <c r="F10" s="126"/>
-      <c r="G10" s="126"/>
+      <c r="F10" s="125"/>
+      <c r="G10" s="125"/>
       <c r="H10" s="29">
         <v>0.83541666666666703</v>
       </c>
-      <c r="I10" s="127"/>
-      <c r="J10" s="127"/>
+      <c r="I10" s="126"/>
+      <c r="J10" s="126"/>
       <c r="K10" s="30">
         <v>0.83541666666666703</v>
       </c>
-      <c r="L10" s="128"/>
-      <c r="M10" s="128"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="100"/>
+      <c r="L10" s="127"/>
+      <c r="M10" s="127"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A11" s="98"/>
       <c r="B11" s="31">
         <f>(B10-B9)</f>
         <v>7.8472222222223054E-2</v>
@@ -4273,46 +4273,46 @@
       <c r="L11" s="45"/>
       <c r="M11" s="46"/>
     </row>
-    <row r="12" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="100"/>
+    <row r="12" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="98"/>
       <c r="B12" s="23"/>
-      <c r="C12" s="125" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="125"/>
+      <c r="C12" s="124" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="124"/>
       <c r="E12" s="24"/>
-      <c r="F12" s="126" t="s">
-        <v>12</v>
-      </c>
-      <c r="G12" s="126"/>
+      <c r="F12" s="125" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="125"/>
       <c r="H12" s="25"/>
-      <c r="I12" s="127" t="s">
-        <v>12</v>
-      </c>
-      <c r="J12" s="127"/>
+      <c r="I12" s="126" t="s">
+        <v>12</v>
+      </c>
+      <c r="J12" s="126"/>
       <c r="K12" s="47"/>
-      <c r="L12" s="128" t="s">
-        <v>12</v>
-      </c>
-      <c r="M12" s="128"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="100"/>
+      <c r="L12" s="127" t="s">
+        <v>12</v>
+      </c>
+      <c r="M12" s="127"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A13" s="98"/>
       <c r="B13" s="27"/>
-      <c r="C13" s="125"/>
-      <c r="D13" s="125"/>
+      <c r="C13" s="124"/>
+      <c r="D13" s="124"/>
       <c r="E13" s="28"/>
-      <c r="F13" s="126"/>
-      <c r="G13" s="126"/>
+      <c r="F13" s="125"/>
+      <c r="G13" s="125"/>
       <c r="H13" s="29"/>
-      <c r="I13" s="127"/>
-      <c r="J13" s="127"/>
+      <c r="I13" s="126"/>
+      <c r="J13" s="126"/>
       <c r="K13" s="48"/>
-      <c r="L13" s="128"/>
-      <c r="M13" s="128"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" s="100"/>
+      <c r="L13" s="127"/>
+      <c r="M13" s="127"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A14" s="98"/>
       <c r="B14" s="31">
         <f>(B13-B12)</f>
         <v>0</v>
@@ -4338,46 +4338,46 @@
       <c r="L14" s="49"/>
       <c r="M14" s="50"/>
     </row>
-    <row r="15" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="100"/>
+    <row r="15" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="98"/>
       <c r="B15" s="23"/>
-      <c r="C15" s="125" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" s="125"/>
+      <c r="C15" s="124" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="124"/>
       <c r="E15" s="24"/>
-      <c r="F15" s="126" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" s="126"/>
+      <c r="F15" s="125" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="125"/>
       <c r="H15" s="25"/>
-      <c r="I15" s="127" t="s">
-        <v>12</v>
-      </c>
-      <c r="J15" s="127"/>
+      <c r="I15" s="126" t="s">
+        <v>12</v>
+      </c>
+      <c r="J15" s="126"/>
       <c r="K15" s="26"/>
-      <c r="L15" s="128" t="s">
-        <v>12</v>
-      </c>
-      <c r="M15" s="128"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" s="100"/>
+      <c r="L15" s="127" t="s">
+        <v>12</v>
+      </c>
+      <c r="M15" s="127"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A16" s="98"/>
       <c r="B16" s="27"/>
-      <c r="C16" s="125"/>
-      <c r="D16" s="125"/>
+      <c r="C16" s="124"/>
+      <c r="D16" s="124"/>
       <c r="E16" s="28"/>
-      <c r="F16" s="126"/>
-      <c r="G16" s="126"/>
+      <c r="F16" s="125"/>
+      <c r="G16" s="125"/>
       <c r="H16" s="29"/>
-      <c r="I16" s="127"/>
-      <c r="J16" s="127"/>
+      <c r="I16" s="126"/>
+      <c r="J16" s="126"/>
       <c r="K16" s="30"/>
-      <c r="L16" s="128"/>
-      <c r="M16" s="128"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17" s="100"/>
+      <c r="L16" s="127"/>
+      <c r="M16" s="127"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A17" s="98"/>
       <c r="B17" s="31">
         <f>(B16-B15)</f>
         <v>0</v>
@@ -4403,46 +4403,46 @@
       <c r="L17" s="45"/>
       <c r="M17" s="46"/>
     </row>
-    <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="100"/>
+    <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="98"/>
       <c r="B18" s="23"/>
-      <c r="C18" s="125" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" s="125"/>
+      <c r="C18" s="124" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="124"/>
       <c r="E18" s="24"/>
-      <c r="F18" s="126" t="s">
-        <v>12</v>
-      </c>
-      <c r="G18" s="126"/>
+      <c r="F18" s="125" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="125"/>
       <c r="H18" s="25"/>
-      <c r="I18" s="127" t="s">
-        <v>12</v>
-      </c>
-      <c r="J18" s="127"/>
+      <c r="I18" s="126" t="s">
+        <v>12</v>
+      </c>
+      <c r="J18" s="126"/>
       <c r="K18" s="47"/>
-      <c r="L18" s="128" t="s">
-        <v>12</v>
-      </c>
-      <c r="M18" s="128"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="100"/>
+      <c r="L18" s="127" t="s">
+        <v>12</v>
+      </c>
+      <c r="M18" s="127"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A19" s="98"/>
       <c r="B19" s="27"/>
-      <c r="C19" s="125"/>
-      <c r="D19" s="125"/>
+      <c r="C19" s="124"/>
+      <c r="D19" s="124"/>
       <c r="E19" s="28"/>
-      <c r="F19" s="126"/>
-      <c r="G19" s="126"/>
+      <c r="F19" s="125"/>
+      <c r="G19" s="125"/>
       <c r="H19" s="29"/>
-      <c r="I19" s="127"/>
-      <c r="J19" s="127"/>
+      <c r="I19" s="126"/>
+      <c r="J19" s="126"/>
       <c r="K19" s="30"/>
-      <c r="L19" s="128"/>
-      <c r="M19" s="128"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" s="100"/>
+      <c r="L19" s="127"/>
+      <c r="M19" s="127"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A20" s="98"/>
       <c r="B20" s="31">
         <f>(B19-B18)</f>
         <v>0</v>
@@ -4468,46 +4468,46 @@
       <c r="L20" s="45"/>
       <c r="M20" s="46"/>
     </row>
-    <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="100"/>
+    <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="98"/>
       <c r="B21" s="23"/>
-      <c r="C21" s="125" t="s">
-        <v>12</v>
-      </c>
-      <c r="D21" s="125"/>
+      <c r="C21" s="124" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="124"/>
       <c r="E21" s="24"/>
-      <c r="F21" s="126" t="s">
-        <v>12</v>
-      </c>
-      <c r="G21" s="126"/>
+      <c r="F21" s="125" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" s="125"/>
       <c r="H21" s="25"/>
-      <c r="I21" s="127" t="s">
-        <v>12</v>
-      </c>
-      <c r="J21" s="127"/>
+      <c r="I21" s="126" t="s">
+        <v>12</v>
+      </c>
+      <c r="J21" s="126"/>
       <c r="K21" s="26"/>
-      <c r="L21" s="128" t="s">
-        <v>12</v>
-      </c>
-      <c r="M21" s="128"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" s="100"/>
+      <c r="L21" s="127" t="s">
+        <v>12</v>
+      </c>
+      <c r="M21" s="127"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A22" s="98"/>
       <c r="B22" s="27"/>
-      <c r="C22" s="125"/>
-      <c r="D22" s="125"/>
+      <c r="C22" s="124"/>
+      <c r="D22" s="124"/>
       <c r="E22" s="28"/>
-      <c r="F22" s="126"/>
-      <c r="G22" s="126"/>
+      <c r="F22" s="125"/>
+      <c r="G22" s="125"/>
       <c r="H22" s="29"/>
-      <c r="I22" s="127"/>
-      <c r="J22" s="127"/>
+      <c r="I22" s="126"/>
+      <c r="J22" s="126"/>
       <c r="K22" s="48"/>
-      <c r="L22" s="128"/>
-      <c r="M22" s="128"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23" s="100"/>
+      <c r="L22" s="127"/>
+      <c r="M22" s="127"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A23" s="98"/>
       <c r="B23" s="31">
         <f>(B22-B21)</f>
         <v>0</v>
@@ -4533,7 +4533,7 @@
       <c r="L23" s="51"/>
       <c r="M23" s="52"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A30" s="21" t="s">
         <v>2</v>
       </c>
@@ -4542,7 +4542,7 @@
         <v>1.0388888888888945</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A31" s="21" t="s">
         <v>10</v>
       </c>
@@ -4553,42 +4553,42 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="C21:D22"/>
-    <mergeCell ref="F21:G22"/>
-    <mergeCell ref="I21:J22"/>
-    <mergeCell ref="L21:M22"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="C18:D19"/>
-    <mergeCell ref="F18:G19"/>
-    <mergeCell ref="I18:J19"/>
-    <mergeCell ref="L18:M19"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="C15:D16"/>
-    <mergeCell ref="F15:G16"/>
-    <mergeCell ref="I15:J16"/>
-    <mergeCell ref="L15:M16"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="C12:D13"/>
-    <mergeCell ref="F12:G13"/>
-    <mergeCell ref="I12:J13"/>
-    <mergeCell ref="L12:M13"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="C9:D10"/>
-    <mergeCell ref="F9:G10"/>
-    <mergeCell ref="I9:J10"/>
-    <mergeCell ref="L9:M10"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="C3:D4"/>
+    <mergeCell ref="F3:G4"/>
+    <mergeCell ref="I3:J4"/>
     <mergeCell ref="L3:M4"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="C6:D7"/>
     <mergeCell ref="F6:G7"/>
     <mergeCell ref="I6:J7"/>
     <mergeCell ref="L6:M7"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="C3:D4"/>
-    <mergeCell ref="F3:G4"/>
-    <mergeCell ref="I3:J4"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="C9:D10"/>
+    <mergeCell ref="F9:G10"/>
+    <mergeCell ref="I9:J10"/>
+    <mergeCell ref="L9:M10"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="C12:D13"/>
+    <mergeCell ref="F12:G13"/>
+    <mergeCell ref="I12:J13"/>
+    <mergeCell ref="L12:M13"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="C15:D16"/>
+    <mergeCell ref="F15:G16"/>
+    <mergeCell ref="I15:J16"/>
+    <mergeCell ref="L15:M16"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="C18:D19"/>
+    <mergeCell ref="F18:G19"/>
+    <mergeCell ref="I18:J19"/>
+    <mergeCell ref="L18:M19"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="C21:D22"/>
+    <mergeCell ref="F21:G22"/>
+    <mergeCell ref="I21:J22"/>
+    <mergeCell ref="L21:M22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -4599,27 +4599,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:O41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L30" sqref="L30:M31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.765625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="15.21875" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" customWidth="1"/>
-    <col min="3" max="4" width="13.6640625" customWidth="1"/>
-    <col min="5" max="5" width="16.109375" customWidth="1"/>
-    <col min="6" max="7" width="13.6640625" customWidth="1"/>
-    <col min="8" max="8" width="15.109375" customWidth="1"/>
-    <col min="9" max="10" width="13.6640625" customWidth="1"/>
-    <col min="11" max="11" width="15.109375" customWidth="1"/>
-    <col min="12" max="13" width="13.6640625" customWidth="1"/>
-    <col min="14" max="14" width="19.6640625" customWidth="1"/>
-    <col min="15" max="15" width="17.88671875" customWidth="1"/>
+    <col min="1" max="1" width="15.23046875" customWidth="1"/>
+    <col min="2" max="2" width="15.07421875" customWidth="1"/>
+    <col min="3" max="4" width="13.69140625" customWidth="1"/>
+    <col min="5" max="5" width="16.07421875" customWidth="1"/>
+    <col min="6" max="7" width="13.69140625" customWidth="1"/>
+    <col min="8" max="8" width="15.07421875" customWidth="1"/>
+    <col min="9" max="10" width="13.69140625" customWidth="1"/>
+    <col min="11" max="11" width="15.07421875" customWidth="1"/>
+    <col min="12" max="13" width="13.69140625" customWidth="1"/>
+    <col min="14" max="14" width="19.69140625" customWidth="1"/>
+    <col min="15" max="15" width="17.84375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="98" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A1" s="103" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -4658,130 +4658,130 @@
       <c r="M1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="99" t="s">
+      <c r="N1" s="104" t="s">
         <v>4</v>
       </c>
-      <c r="O1" s="99"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="98"/>
+      <c r="O1" s="104"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A2" s="103"/>
       <c r="B2" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="10">
         <f t="array" ref="C2">SUM(B5:B41*(MOD(ROW(B5:B41)-2,3)=0))</f>
-        <v>0.6770833333333337</v>
+        <v>0.84375000000000033</v>
       </c>
       <c r="D2" s="11">
         <f>C2+Sprint_3!D2</f>
-        <v>2.0409722222222246</v>
+        <v>2.2076388888888916</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="13">
         <f t="array" ref="F2">SUM(E5:E41*(MOD(ROW(E5:E41)-2,3)=0))</f>
-        <v>0.53125000000000067</v>
+        <v>0.6979166666666673</v>
       </c>
       <c r="G2" s="14">
         <f>F2+Sprint_3!G2</f>
-        <v>1.7055555555555597</v>
+        <v>1.8722222222222262</v>
       </c>
       <c r="H2" s="15" t="s">
         <v>7</v>
       </c>
       <c r="I2" s="16">
         <f t="array" ref="I2">SUM(H5:H41*(MOD(ROW(H5:H41)-2,3)=0))</f>
-        <v>0.60069444444444509</v>
+        <v>0.76736111111111172</v>
       </c>
       <c r="J2" s="17">
         <f>I2+Sprint_3!J2</f>
-        <v>1.7000000000000033</v>
+        <v>1.8666666666666698</v>
       </c>
       <c r="K2" s="18" t="s">
         <v>8</v>
       </c>
       <c r="L2" s="19">
         <f t="array" ref="L2">SUM(K5:K41*(MOD(ROW(K5:K41)-2,3)=0))</f>
-        <v>0.61458333333333481</v>
+        <v>0.78125000000000144</v>
       </c>
       <c r="M2" s="20">
         <f>L2+Sprint_3!M2</f>
-        <v>1.9451388888888941</v>
+        <v>2.1118055555555606</v>
       </c>
       <c r="N2" s="21" t="s">
         <v>2</v>
       </c>
       <c r="O2" s="22">
         <f>C2+F2+I2+L2</f>
-        <v>2.4236111111111143</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="100">
+        <v>3.0902777777777808</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="98">
         <v>44585</v>
       </c>
       <c r="B3" s="23">
         <v>0.33333333333333298</v>
       </c>
-      <c r="C3" s="101" t="s">
+      <c r="C3" s="99" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="101"/>
+      <c r="D3" s="99"/>
       <c r="E3" s="24">
         <v>0.33333333333333298</v>
       </c>
-      <c r="F3" s="102" t="s">
+      <c r="F3" s="100" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="102"/>
+      <c r="G3" s="100"/>
       <c r="H3" s="25">
         <v>0.33333333333333298</v>
       </c>
-      <c r="I3" s="103" t="s">
+      <c r="I3" s="101" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="103"/>
+      <c r="J3" s="101"/>
       <c r="K3" s="26">
         <v>0.33333333333333298</v>
       </c>
-      <c r="L3" s="104" t="s">
+      <c r="L3" s="102" t="s">
         <v>24</v>
       </c>
-      <c r="M3" s="104"/>
+      <c r="M3" s="102"/>
       <c r="N3" s="21" t="s">
         <v>10</v>
       </c>
       <c r="O3" s="22">
         <f>D2+G2+J2+M2</f>
-        <v>7.3916666666666817</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="100"/>
+        <v>8.0583333333333478</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A4" s="98"/>
       <c r="B4" s="27">
         <v>0.41666666666666702</v>
       </c>
-      <c r="C4" s="101"/>
-      <c r="D4" s="101"/>
+      <c r="C4" s="99"/>
+      <c r="D4" s="99"/>
       <c r="E4" s="28">
         <v>0.41666666666666702</v>
       </c>
-      <c r="F4" s="102"/>
-      <c r="G4" s="102"/>
+      <c r="F4" s="100"/>
+      <c r="G4" s="100"/>
       <c r="H4" s="29">
         <v>0.41666666666666702</v>
       </c>
-      <c r="I4" s="103"/>
-      <c r="J4" s="103"/>
+      <c r="I4" s="101"/>
+      <c r="J4" s="101"/>
       <c r="K4" s="30">
         <v>0.41666666666666702</v>
       </c>
-      <c r="L4" s="104"/>
-      <c r="M4" s="104"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="100"/>
+      <c r="L4" s="102"/>
+      <c r="M4" s="102"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A5" s="98"/>
       <c r="B5" s="31">
         <f>B4-B3</f>
         <v>8.3333333333334036E-2</v>
@@ -4807,64 +4807,64 @@
       <c r="L5" s="41"/>
       <c r="M5" s="42"/>
     </row>
-    <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="100">
+    <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="98">
         <v>44585</v>
       </c>
       <c r="B6" s="23">
         <v>0.6875</v>
       </c>
-      <c r="C6" s="101" t="s">
+      <c r="C6" s="99" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="101"/>
+      <c r="D6" s="99"/>
       <c r="E6" s="24">
         <v>0.6875</v>
       </c>
-      <c r="F6" s="102" t="s">
+      <c r="F6" s="100" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="102"/>
+      <c r="G6" s="100"/>
       <c r="H6" s="25">
         <v>0.6875</v>
       </c>
-      <c r="I6" s="103" t="s">
+      <c r="I6" s="101" t="s">
         <v>25</v>
       </c>
-      <c r="J6" s="103"/>
+      <c r="J6" s="101"/>
       <c r="K6" s="43">
         <v>0.6875</v>
       </c>
-      <c r="L6" s="104" t="s">
+      <c r="L6" s="102" t="s">
         <v>26</v>
       </c>
-      <c r="M6" s="104"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="100"/>
+      <c r="M6" s="102"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A7" s="98"/>
       <c r="B7" s="27">
         <v>0.71875</v>
       </c>
-      <c r="C7" s="101"/>
-      <c r="D7" s="101"/>
+      <c r="C7" s="99"/>
+      <c r="D7" s="99"/>
       <c r="E7" s="28">
         <v>0.71875</v>
       </c>
-      <c r="F7" s="102"/>
-      <c r="G7" s="102"/>
+      <c r="F7" s="100"/>
+      <c r="G7" s="100"/>
       <c r="H7" s="29">
         <v>0.71875</v>
       </c>
-      <c r="I7" s="103"/>
-      <c r="J7" s="103"/>
+      <c r="I7" s="101"/>
+      <c r="J7" s="101"/>
       <c r="K7" s="30">
         <v>0.71875</v>
       </c>
-      <c r="L7" s="104"/>
-      <c r="M7" s="104"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="100"/>
+      <c r="L7" s="102"/>
+      <c r="M7" s="102"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A8" s="98"/>
       <c r="B8" s="31">
         <f>B7-B6</f>
         <v>3.125E-2</v>
@@ -4890,52 +4890,52 @@
       <c r="L8" s="45"/>
       <c r="M8" s="46"/>
     </row>
-    <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="100">
+    <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="98">
         <v>44586</v>
       </c>
       <c r="B9" s="23">
         <v>0.58333333333333304</v>
       </c>
-      <c r="C9" s="101" t="s">
+      <c r="C9" s="99" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="101"/>
+      <c r="D9" s="99"/>
       <c r="E9" s="24"/>
-      <c r="F9" s="102" t="s">
+      <c r="F9" s="100" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="102"/>
+      <c r="G9" s="100"/>
       <c r="H9" s="25"/>
-      <c r="I9" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="J9" s="103"/>
+      <c r="I9" s="101" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" s="101"/>
       <c r="K9" s="47"/>
-      <c r="L9" s="104" t="s">
-        <v>11</v>
-      </c>
-      <c r="M9" s="104"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="100"/>
+      <c r="L9" s="102" t="s">
+        <v>11</v>
+      </c>
+      <c r="M9" s="102"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A10" s="98"/>
       <c r="B10" s="27">
         <v>0.6875</v>
       </c>
-      <c r="C10" s="101"/>
-      <c r="D10" s="101"/>
+      <c r="C10" s="99"/>
+      <c r="D10" s="99"/>
       <c r="E10" s="28"/>
-      <c r="F10" s="102"/>
-      <c r="G10" s="102"/>
+      <c r="F10" s="100"/>
+      <c r="G10" s="100"/>
       <c r="H10" s="29"/>
-      <c r="I10" s="103"/>
-      <c r="J10" s="103"/>
+      <c r="I10" s="101"/>
+      <c r="J10" s="101"/>
       <c r="K10" s="30"/>
-      <c r="L10" s="104"/>
-      <c r="M10" s="104"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="100"/>
+      <c r="L10" s="102"/>
+      <c r="M10" s="102"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A11" s="98"/>
       <c r="B11" s="31">
         <f>(B10-B9)</f>
         <v>0.10416666666666696</v>
@@ -4961,52 +4961,52 @@
       <c r="L11" s="45"/>
       <c r="M11" s="46"/>
     </row>
-    <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="100">
+    <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="98">
         <v>44588</v>
       </c>
       <c r="B12" s="23">
         <v>0.85416666666666696</v>
       </c>
-      <c r="C12" s="101" t="s">
+      <c r="C12" s="99" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="101"/>
+      <c r="D12" s="99"/>
       <c r="E12" s="24"/>
-      <c r="F12" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" s="102"/>
+      <c r="F12" s="100" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="100"/>
       <c r="H12" s="25"/>
-      <c r="I12" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="J12" s="103"/>
+      <c r="I12" s="101" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" s="101"/>
       <c r="K12" s="47"/>
-      <c r="L12" s="104" t="s">
-        <v>11</v>
-      </c>
-      <c r="M12" s="104"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="100"/>
+      <c r="L12" s="102" t="s">
+        <v>11</v>
+      </c>
+      <c r="M12" s="102"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A13" s="98"/>
       <c r="B13" s="27">
         <v>0.89583333333333304</v>
       </c>
-      <c r="C13" s="101"/>
-      <c r="D13" s="101"/>
+      <c r="C13" s="99"/>
+      <c r="D13" s="99"/>
       <c r="E13" s="28"/>
-      <c r="F13" s="102"/>
-      <c r="G13" s="102"/>
+      <c r="F13" s="100"/>
+      <c r="G13" s="100"/>
       <c r="H13" s="29"/>
-      <c r="I13" s="103"/>
-      <c r="J13" s="103"/>
+      <c r="I13" s="101"/>
+      <c r="J13" s="101"/>
       <c r="K13" s="48"/>
-      <c r="L13" s="104"/>
-      <c r="M13" s="104"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="100"/>
+      <c r="L13" s="102"/>
+      <c r="M13" s="102"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A14" s="98"/>
       <c r="B14" s="31">
         <f>(B13-B12)</f>
         <v>4.1666666666666075E-2</v>
@@ -5032,52 +5032,52 @@
       <c r="L14" s="49"/>
       <c r="M14" s="50"/>
     </row>
-    <row r="15" spans="1:15" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="100">
+    <row r="15" spans="1:15" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="98">
         <v>44591</v>
       </c>
       <c r="B15" s="23"/>
-      <c r="C15" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="101"/>
+      <c r="C15" s="99" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="99"/>
       <c r="E15" s="24"/>
-      <c r="F15" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="G15" s="102"/>
+      <c r="F15" s="100" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="100"/>
       <c r="H15" s="25"/>
-      <c r="I15" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="J15" s="103"/>
+      <c r="I15" s="101" t="s">
+        <v>11</v>
+      </c>
+      <c r="J15" s="101"/>
       <c r="K15" s="26">
         <v>0.33333333333333298</v>
       </c>
-      <c r="L15" s="104" t="s">
+      <c r="L15" s="102" t="s">
         <v>28</v>
       </c>
-      <c r="M15" s="104"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" s="100"/>
+      <c r="M15" s="102"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A16" s="98"/>
       <c r="B16" s="27"/>
-      <c r="C16" s="101"/>
-      <c r="D16" s="101"/>
+      <c r="C16" s="99"/>
+      <c r="D16" s="99"/>
       <c r="E16" s="28"/>
-      <c r="F16" s="102"/>
-      <c r="G16" s="102"/>
+      <c r="F16" s="100"/>
+      <c r="G16" s="100"/>
       <c r="H16" s="29"/>
-      <c r="I16" s="103"/>
-      <c r="J16" s="103"/>
+      <c r="I16" s="101"/>
+      <c r="J16" s="101"/>
       <c r="K16" s="30">
         <v>0.41666666666666702</v>
       </c>
-      <c r="L16" s="104"/>
-      <c r="M16" s="104"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17" s="100"/>
+      <c r="L16" s="102"/>
+      <c r="M16" s="102"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A17" s="98"/>
       <c r="B17" s="31">
         <f>(B16-B15)</f>
         <v>0</v>
@@ -5103,64 +5103,64 @@
       <c r="L17" s="45"/>
       <c r="M17" s="46"/>
     </row>
-    <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="100">
+    <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="98">
         <v>44591</v>
       </c>
       <c r="B18" s="23">
         <v>0.70833333333333337</v>
       </c>
-      <c r="C18" s="101" t="s">
+      <c r="C18" s="99" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="101"/>
+      <c r="D18" s="99"/>
       <c r="E18" s="24">
         <v>0.70833333333333337</v>
       </c>
-      <c r="F18" s="102" t="s">
+      <c r="F18" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="G18" s="102"/>
+      <c r="G18" s="100"/>
       <c r="H18" s="25">
         <v>0.61805555555555558</v>
       </c>
-      <c r="I18" s="103" t="s">
+      <c r="I18" s="101" t="s">
         <v>32</v>
       </c>
-      <c r="J18" s="103"/>
+      <c r="J18" s="101"/>
       <c r="K18" s="47">
         <v>0.70833333333333337</v>
       </c>
-      <c r="L18" s="104" t="s">
+      <c r="L18" s="102" t="s">
         <v>30</v>
       </c>
-      <c r="M18" s="104"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="100"/>
+      <c r="M18" s="102"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A19" s="98"/>
       <c r="B19" s="27">
         <v>0.92708333333333337</v>
       </c>
-      <c r="C19" s="101"/>
-      <c r="D19" s="101"/>
+      <c r="C19" s="99"/>
+      <c r="D19" s="99"/>
       <c r="E19" s="28">
         <v>0.92708333333333337</v>
       </c>
-      <c r="F19" s="102"/>
-      <c r="G19" s="102"/>
+      <c r="F19" s="100"/>
+      <c r="G19" s="100"/>
       <c r="H19" s="29">
         <v>0.92708333333333337</v>
       </c>
-      <c r="I19" s="103"/>
-      <c r="J19" s="103"/>
+      <c r="I19" s="101"/>
+      <c r="J19" s="101"/>
       <c r="K19" s="30">
         <v>0.92708333333333337</v>
       </c>
-      <c r="L19" s="104"/>
-      <c r="M19" s="104"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" s="100"/>
+      <c r="L19" s="102"/>
+      <c r="M19" s="102"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A20" s="98"/>
       <c r="B20" s="31">
         <f>(B19-B18)</f>
         <v>0.21875</v>
@@ -5186,64 +5186,64 @@
       <c r="L20" s="45"/>
       <c r="M20" s="46"/>
     </row>
-    <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="100">
+    <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="98">
         <v>44592</v>
       </c>
       <c r="B21" s="23">
         <v>0.375</v>
       </c>
-      <c r="C21" s="101" t="s">
+      <c r="C21" s="99" t="s">
         <v>30</v>
       </c>
-      <c r="D21" s="101"/>
+      <c r="D21" s="99"/>
       <c r="E21" s="24">
         <v>0.375</v>
       </c>
-      <c r="F21" s="102" t="s">
+      <c r="F21" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="G21" s="102"/>
+      <c r="G21" s="100"/>
       <c r="H21" s="25">
         <v>0.375</v>
       </c>
-      <c r="I21" s="103" t="s">
+      <c r="I21" s="101" t="s">
         <v>32</v>
       </c>
-      <c r="J21" s="103"/>
+      <c r="J21" s="101"/>
       <c r="K21" s="26">
         <v>0.375</v>
       </c>
-      <c r="L21" s="104" t="s">
+      <c r="L21" s="102" t="s">
         <v>30</v>
       </c>
-      <c r="M21" s="104"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" s="100"/>
+      <c r="M21" s="102"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A22" s="98"/>
       <c r="B22" s="27">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C22" s="101"/>
-      <c r="D22" s="101"/>
+      <c r="C22" s="99"/>
+      <c r="D22" s="99"/>
       <c r="E22" s="28">
         <v>0.41666666666666669</v>
       </c>
-      <c r="F22" s="102"/>
-      <c r="G22" s="102"/>
+      <c r="F22" s="100"/>
+      <c r="G22" s="100"/>
       <c r="H22" s="29">
         <v>0.41666666666666669</v>
       </c>
-      <c r="I22" s="103"/>
-      <c r="J22" s="103"/>
+      <c r="I22" s="101"/>
+      <c r="J22" s="101"/>
       <c r="K22" s="48">
         <v>0.41666666666666669</v>
       </c>
-      <c r="L22" s="104"/>
-      <c r="M22" s="104"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23" s="100"/>
+      <c r="L22" s="102"/>
+      <c r="M22" s="102"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A23" s="98"/>
       <c r="B23" s="31">
         <f>(B22-B21)</f>
         <v>4.1666666666666685E-2</v>
@@ -5269,64 +5269,64 @@
       <c r="L23" s="51"/>
       <c r="M23" s="52"/>
     </row>
-    <row r="24" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="100">
+    <row r="24" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="98">
         <v>44592</v>
       </c>
       <c r="B24" s="23">
         <v>0.625</v>
       </c>
-      <c r="C24" s="101" t="s">
+      <c r="C24" s="99" t="s">
         <v>30</v>
       </c>
-      <c r="D24" s="101"/>
+      <c r="D24" s="99"/>
       <c r="E24" s="24">
         <v>0.625</v>
       </c>
-      <c r="F24" s="102" t="s">
+      <c r="F24" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="G24" s="102"/>
+      <c r="G24" s="100"/>
       <c r="H24" s="25">
         <v>0.625</v>
       </c>
-      <c r="I24" s="103" t="s">
+      <c r="I24" s="101" t="s">
         <v>33</v>
       </c>
-      <c r="J24" s="103"/>
+      <c r="J24" s="101"/>
       <c r="K24" s="26">
         <v>0.625</v>
       </c>
-      <c r="L24" s="104" t="s">
+      <c r="L24" s="102" t="s">
         <v>34</v>
       </c>
-      <c r="M24" s="104"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25" s="100"/>
+      <c r="M24" s="102"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A25" s="98"/>
       <c r="B25" s="27">
         <v>0.75</v>
       </c>
-      <c r="C25" s="101"/>
-      <c r="D25" s="101"/>
+      <c r="C25" s="99"/>
+      <c r="D25" s="99"/>
       <c r="E25" s="28">
         <v>0.75</v>
       </c>
-      <c r="F25" s="102"/>
-      <c r="G25" s="102"/>
+      <c r="F25" s="100"/>
+      <c r="G25" s="100"/>
       <c r="H25" s="29">
         <v>0.72916666666666663</v>
       </c>
-      <c r="I25" s="103"/>
-      <c r="J25" s="103"/>
+      <c r="I25" s="101"/>
+      <c r="J25" s="101"/>
       <c r="K25" s="30">
         <v>0.75</v>
       </c>
-      <c r="L25" s="104"/>
-      <c r="M25" s="104"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26" s="100"/>
+      <c r="L25" s="102"/>
+      <c r="M25" s="102"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A26" s="98"/>
       <c r="B26" s="31">
         <f>(B25-B24)</f>
         <v>0.125</v>
@@ -5352,64 +5352,64 @@
       <c r="L26" s="45"/>
       <c r="M26" s="46"/>
     </row>
-    <row r="27" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="100">
+    <row r="27" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="98">
         <v>44594</v>
       </c>
       <c r="B27" s="23">
         <v>0.5</v>
       </c>
-      <c r="C27" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="D27" s="101"/>
+      <c r="C27" s="99" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="99"/>
       <c r="E27" s="24">
         <v>0.5</v>
       </c>
-      <c r="F27" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="G27" s="102"/>
+      <c r="F27" s="100" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" s="100"/>
       <c r="H27" s="25">
         <v>0.5</v>
       </c>
-      <c r="I27" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="J27" s="103"/>
+      <c r="I27" s="101" t="s">
+        <v>11</v>
+      </c>
+      <c r="J27" s="101"/>
       <c r="K27" s="47">
         <v>0.5</v>
       </c>
-      <c r="L27" s="104" t="s">
-        <v>11</v>
-      </c>
-      <c r="M27" s="104"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28" s="100"/>
+      <c r="L27" s="102" t="s">
+        <v>11</v>
+      </c>
+      <c r="M27" s="102"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A28" s="98"/>
       <c r="B28" s="27">
         <v>0.53125</v>
       </c>
-      <c r="C28" s="101"/>
-      <c r="D28" s="101"/>
+      <c r="C28" s="99"/>
+      <c r="D28" s="99"/>
       <c r="E28" s="28">
         <v>0.53125</v>
       </c>
-      <c r="F28" s="102"/>
-      <c r="G28" s="102"/>
+      <c r="F28" s="100"/>
+      <c r="G28" s="100"/>
       <c r="H28" s="29">
         <v>0.53125</v>
       </c>
-      <c r="I28" s="103"/>
-      <c r="J28" s="103"/>
+      <c r="I28" s="101"/>
+      <c r="J28" s="101"/>
       <c r="K28" s="30">
         <v>0.53125</v>
       </c>
-      <c r="L28" s="104"/>
-      <c r="M28" s="104"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A29" s="100"/>
+      <c r="L28" s="102"/>
+      <c r="M28" s="102"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A29" s="98"/>
       <c r="B29" s="31">
         <f>(B28-B27)</f>
         <v>3.125E-2</v>
@@ -5435,111 +5435,129 @@
       <c r="L29" s="45"/>
       <c r="M29" s="46"/>
     </row>
-    <row r="30" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="100"/>
-      <c r="B30" s="23"/>
-      <c r="C30" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="D30" s="101"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="G30" s="102"/>
-      <c r="H30" s="25"/>
-      <c r="I30" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="J30" s="103"/>
-      <c r="K30" s="26"/>
-      <c r="L30" s="104" t="s">
-        <v>11</v>
-      </c>
-      <c r="M30" s="104"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A31" s="100"/>
-      <c r="B31" s="27"/>
-      <c r="C31" s="101"/>
-      <c r="D31" s="101"/>
-      <c r="E31" s="28"/>
-      <c r="F31" s="102"/>
-      <c r="G31" s="102"/>
-      <c r="H31" s="29"/>
-      <c r="I31" s="103"/>
-      <c r="J31" s="103"/>
-      <c r="K31" s="48"/>
-      <c r="L31" s="104"/>
-      <c r="M31" s="104"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A32" s="100"/>
+    <row r="30" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="98">
+        <v>44597</v>
+      </c>
+      <c r="B30" s="23">
+        <v>0.75</v>
+      </c>
+      <c r="C30" s="99" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" s="99"/>
+      <c r="E30" s="24">
+        <v>0.75</v>
+      </c>
+      <c r="F30" s="100" t="s">
+        <v>11</v>
+      </c>
+      <c r="G30" s="100"/>
+      <c r="H30" s="25">
+        <v>0.75</v>
+      </c>
+      <c r="I30" s="101" t="s">
+        <v>11</v>
+      </c>
+      <c r="J30" s="101"/>
+      <c r="K30" s="26">
+        <v>0.75</v>
+      </c>
+      <c r="L30" s="102" t="s">
+        <v>11</v>
+      </c>
+      <c r="M30" s="102"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A31" s="98"/>
+      <c r="B31" s="27">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="C31" s="99"/>
+      <c r="D31" s="99"/>
+      <c r="E31" s="28">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="F31" s="100"/>
+      <c r="G31" s="100"/>
+      <c r="H31" s="29">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="I31" s="101"/>
+      <c r="J31" s="101"/>
+      <c r="K31" s="48">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="L31" s="102"/>
+      <c r="M31" s="102"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A32" s="98"/>
       <c r="B32" s="31">
         <f>(B31-B30)</f>
-        <v>0</v>
+        <v>0.16666666666666663</v>
       </c>
       <c r="C32" s="32"/>
       <c r="D32" s="33"/>
       <c r="E32" s="34">
         <f>E31-E30</f>
-        <v>0</v>
+        <v>0.16666666666666663</v>
       </c>
       <c r="F32" s="35"/>
       <c r="G32" s="36"/>
       <c r="H32" s="37">
         <f>H31-H30</f>
-        <v>0</v>
+        <v>0.16666666666666663</v>
       </c>
       <c r="I32" s="38"/>
       <c r="J32" s="39"/>
       <c r="K32" s="51">
         <f>K31-K30</f>
-        <v>0</v>
+        <v>0.16666666666666663</v>
       </c>
       <c r="L32" s="51"/>
       <c r="M32" s="52"/>
     </row>
-    <row r="33" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="100"/>
+    <row r="33" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="98"/>
       <c r="B33" s="23"/>
-      <c r="C33" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="D33" s="101"/>
+      <c r="C33" s="99" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="99"/>
       <c r="E33" s="24"/>
-      <c r="F33" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="G33" s="102"/>
+      <c r="F33" s="100" t="s">
+        <v>11</v>
+      </c>
+      <c r="G33" s="100"/>
       <c r="H33" s="25"/>
-      <c r="I33" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="J33" s="103"/>
+      <c r="I33" s="101" t="s">
+        <v>11</v>
+      </c>
+      <c r="J33" s="101"/>
       <c r="K33" s="26"/>
-      <c r="L33" s="104" t="s">
-        <v>11</v>
-      </c>
-      <c r="M33" s="104"/>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A34" s="100"/>
+      <c r="L33" s="102" t="s">
+        <v>11</v>
+      </c>
+      <c r="M33" s="102"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A34" s="98"/>
       <c r="B34" s="27"/>
-      <c r="C34" s="101"/>
-      <c r="D34" s="101"/>
+      <c r="C34" s="99"/>
+      <c r="D34" s="99"/>
       <c r="E34" s="28"/>
-      <c r="F34" s="102"/>
-      <c r="G34" s="102"/>
+      <c r="F34" s="100"/>
+      <c r="G34" s="100"/>
       <c r="H34" s="29"/>
-      <c r="I34" s="103"/>
-      <c r="J34" s="103"/>
+      <c r="I34" s="101"/>
+      <c r="J34" s="101"/>
       <c r="K34" s="30"/>
-      <c r="L34" s="104"/>
-      <c r="M34" s="104"/>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A35" s="100"/>
+      <c r="L34" s="102"/>
+      <c r="M34" s="102"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A35" s="98"/>
       <c r="B35" s="31">
         <f>(B34-B33)</f>
         <v>0</v>
@@ -5565,46 +5583,46 @@
       <c r="L35" s="45"/>
       <c r="M35" s="46"/>
     </row>
-    <row r="36" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="100"/>
+    <row r="36" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="98"/>
       <c r="B36" s="23"/>
-      <c r="C36" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="D36" s="101"/>
+      <c r="C36" s="99" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" s="99"/>
       <c r="E36" s="24"/>
-      <c r="F36" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="G36" s="102"/>
+      <c r="F36" s="100" t="s">
+        <v>11</v>
+      </c>
+      <c r="G36" s="100"/>
       <c r="H36" s="25"/>
-      <c r="I36" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="J36" s="103"/>
+      <c r="I36" s="101" t="s">
+        <v>11</v>
+      </c>
+      <c r="J36" s="101"/>
       <c r="K36" s="47"/>
-      <c r="L36" s="104" t="s">
-        <v>11</v>
-      </c>
-      <c r="M36" s="104"/>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A37" s="100"/>
+      <c r="L36" s="102" t="s">
+        <v>11</v>
+      </c>
+      <c r="M36" s="102"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A37" s="98"/>
       <c r="B37" s="27"/>
-      <c r="C37" s="101"/>
-      <c r="D37" s="101"/>
+      <c r="C37" s="99"/>
+      <c r="D37" s="99"/>
       <c r="E37" s="28"/>
-      <c r="F37" s="102"/>
-      <c r="G37" s="102"/>
+      <c r="F37" s="100"/>
+      <c r="G37" s="100"/>
       <c r="H37" s="29"/>
-      <c r="I37" s="103"/>
-      <c r="J37" s="103"/>
+      <c r="I37" s="101"/>
+      <c r="J37" s="101"/>
       <c r="K37" s="30"/>
-      <c r="L37" s="104"/>
-      <c r="M37" s="104"/>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A38" s="100"/>
+      <c r="L37" s="102"/>
+      <c r="M37" s="102"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A38" s="98"/>
       <c r="B38" s="31">
         <f>(B37-B36)</f>
         <v>0</v>
@@ -5630,46 +5648,46 @@
       <c r="L38" s="45"/>
       <c r="M38" s="46"/>
     </row>
-    <row r="39" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="100"/>
+    <row r="39" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="98"/>
       <c r="B39" s="23"/>
-      <c r="C39" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="D39" s="101"/>
+      <c r="C39" s="99" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" s="99"/>
       <c r="E39" s="24"/>
-      <c r="F39" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="G39" s="102"/>
+      <c r="F39" s="100" t="s">
+        <v>11</v>
+      </c>
+      <c r="G39" s="100"/>
       <c r="H39" s="25"/>
-      <c r="I39" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="J39" s="103"/>
+      <c r="I39" s="101" t="s">
+        <v>11</v>
+      </c>
+      <c r="J39" s="101"/>
       <c r="K39" s="26"/>
-      <c r="L39" s="104" t="s">
-        <v>11</v>
-      </c>
-      <c r="M39" s="104"/>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A40" s="100"/>
+      <c r="L39" s="102" t="s">
+        <v>11</v>
+      </c>
+      <c r="M39" s="102"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A40" s="98"/>
       <c r="B40" s="27"/>
-      <c r="C40" s="101"/>
-      <c r="D40" s="101"/>
+      <c r="C40" s="99"/>
+      <c r="D40" s="99"/>
       <c r="E40" s="28"/>
-      <c r="F40" s="102"/>
-      <c r="G40" s="102"/>
+      <c r="F40" s="100"/>
+      <c r="G40" s="100"/>
       <c r="H40" s="29"/>
-      <c r="I40" s="103"/>
-      <c r="J40" s="103"/>
+      <c r="I40" s="101"/>
+      <c r="J40" s="101"/>
       <c r="K40" s="48"/>
-      <c r="L40" s="104"/>
-      <c r="M40" s="104"/>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A41" s="100"/>
+      <c r="L40" s="102"/>
+      <c r="M40" s="102"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A41" s="98"/>
       <c r="B41" s="31">
         <f>(B40-B39)</f>
         <v>0</v>
@@ -5697,66 +5715,6 @@
     </row>
   </sheetData>
   <mergeCells count="67">
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="C39:D40"/>
-    <mergeCell ref="F39:G40"/>
-    <mergeCell ref="I39:J40"/>
-    <mergeCell ref="L39:M40"/>
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="C36:D37"/>
-    <mergeCell ref="F36:G37"/>
-    <mergeCell ref="I36:J37"/>
-    <mergeCell ref="L36:M37"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="C33:D34"/>
-    <mergeCell ref="F33:G34"/>
-    <mergeCell ref="I33:J34"/>
-    <mergeCell ref="L33:M34"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="C30:D31"/>
-    <mergeCell ref="F30:G31"/>
-    <mergeCell ref="I30:J31"/>
-    <mergeCell ref="L30:M31"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="C27:D28"/>
-    <mergeCell ref="F27:G28"/>
-    <mergeCell ref="I27:J28"/>
-    <mergeCell ref="L27:M28"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="C24:D25"/>
-    <mergeCell ref="F24:G25"/>
-    <mergeCell ref="I24:J25"/>
-    <mergeCell ref="L24:M25"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="C21:D22"/>
-    <mergeCell ref="F21:G22"/>
-    <mergeCell ref="I21:J22"/>
-    <mergeCell ref="L21:M22"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="C18:D19"/>
-    <mergeCell ref="F18:G19"/>
-    <mergeCell ref="I18:J19"/>
-    <mergeCell ref="L18:M19"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="C15:D16"/>
-    <mergeCell ref="F15:G16"/>
-    <mergeCell ref="I15:J16"/>
-    <mergeCell ref="L15:M16"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="C12:D13"/>
-    <mergeCell ref="F12:G13"/>
-    <mergeCell ref="I12:J13"/>
-    <mergeCell ref="L12:M13"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="C9:D10"/>
-    <mergeCell ref="F9:G10"/>
-    <mergeCell ref="I9:J10"/>
-    <mergeCell ref="L9:M10"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="C6:D7"/>
-    <mergeCell ref="F6:G7"/>
-    <mergeCell ref="I6:J7"/>
-    <mergeCell ref="L6:M7"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="A3:A5"/>
@@ -5764,6 +5722,66 @@
     <mergeCell ref="F3:G4"/>
     <mergeCell ref="I3:J4"/>
     <mergeCell ref="L3:M4"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="C6:D7"/>
+    <mergeCell ref="F6:G7"/>
+    <mergeCell ref="I6:J7"/>
+    <mergeCell ref="L6:M7"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="C9:D10"/>
+    <mergeCell ref="F9:G10"/>
+    <mergeCell ref="I9:J10"/>
+    <mergeCell ref="L9:M10"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="C12:D13"/>
+    <mergeCell ref="F12:G13"/>
+    <mergeCell ref="I12:J13"/>
+    <mergeCell ref="L12:M13"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="C15:D16"/>
+    <mergeCell ref="F15:G16"/>
+    <mergeCell ref="I15:J16"/>
+    <mergeCell ref="L15:M16"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="C18:D19"/>
+    <mergeCell ref="F18:G19"/>
+    <mergeCell ref="I18:J19"/>
+    <mergeCell ref="L18:M19"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="C21:D22"/>
+    <mergeCell ref="F21:G22"/>
+    <mergeCell ref="I21:J22"/>
+    <mergeCell ref="L21:M22"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="C24:D25"/>
+    <mergeCell ref="F24:G25"/>
+    <mergeCell ref="I24:J25"/>
+    <mergeCell ref="L24:M25"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="C27:D28"/>
+    <mergeCell ref="F27:G28"/>
+    <mergeCell ref="I27:J28"/>
+    <mergeCell ref="L27:M28"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="C30:D31"/>
+    <mergeCell ref="F30:G31"/>
+    <mergeCell ref="I30:J31"/>
+    <mergeCell ref="L30:M31"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="C33:D34"/>
+    <mergeCell ref="F33:G34"/>
+    <mergeCell ref="I33:J34"/>
+    <mergeCell ref="L33:M34"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="C36:D37"/>
+    <mergeCell ref="F36:G37"/>
+    <mergeCell ref="I36:J37"/>
+    <mergeCell ref="L36:M37"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="C39:D40"/>
+    <mergeCell ref="F39:G40"/>
+    <mergeCell ref="I39:J40"/>
+    <mergeCell ref="L39:M40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
added some new UI stuff
</commit_message>
<xml_diff>
--- a/Zeitaufzeichnung_Ishjarta.xlsx
+++ b/Zeitaufzeichnung_Ishjarta.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SYP\ishjarta\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danijel\Desktop\ishjarta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{03AE51D4-701F-4097-A369-481DD58A9989}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C32653BC-F7B5-4858-B467-E72C1D3D41B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4457" yWindow="4457" windowWidth="24686" windowHeight="13140" tabRatio="500" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vorlage" sheetId="1" r:id="rId1"/>
@@ -390,7 +390,7 @@
     <numFmt numFmtId="167" formatCode="m/d/yyyy"/>
     <numFmt numFmtId="168" formatCode="hh:mm&quot; Uhr&quot;"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1192,27 +1192,27 @@
     <xf numFmtId="165" fontId="2" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="6" borderId="10" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="12" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="12" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="12" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="12" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="6" borderId="10" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="12" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="12" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="12" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="12" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="167" fontId="2" fillId="6" borderId="17" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1249,41 +1249,41 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="5" borderId="1" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="32" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="30" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="5" borderId="31" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="32" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="33" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="165" fontId="2" fillId="5" borderId="23" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="5" borderId="1" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="165" fontId="2" fillId="5" borderId="31" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -1380,7 +1380,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1682,23 +1682,23 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.69140625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" customWidth="1"/>
-    <col min="3" max="4" width="13.7109375" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="6" max="7" width="13.7109375" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" customWidth="1"/>
-    <col min="9" max="10" width="13.7109375" customWidth="1"/>
-    <col min="11" max="11" width="15.140625" customWidth="1"/>
-    <col min="12" max="13" width="13.7109375" customWidth="1"/>
-    <col min="14" max="14" width="19.7109375" customWidth="1"/>
-    <col min="15" max="15" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="15.3046875" customWidth="1"/>
+    <col min="2" max="2" width="15.15234375" customWidth="1"/>
+    <col min="3" max="4" width="13.69140625" customWidth="1"/>
+    <col min="5" max="5" width="16.15234375" customWidth="1"/>
+    <col min="6" max="7" width="13.69140625" customWidth="1"/>
+    <col min="8" max="8" width="15.15234375" customWidth="1"/>
+    <col min="9" max="10" width="13.69140625" customWidth="1"/>
+    <col min="11" max="11" width="15.15234375" customWidth="1"/>
+    <col min="12" max="13" width="13.69140625" customWidth="1"/>
+    <col min="14" max="14" width="19.69140625" customWidth="1"/>
+    <col min="15" max="15" width="17.84375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
-      <c r="A1" s="97" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A1" s="102" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1737,13 +1737,13 @@
       <c r="M1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="98" t="s">
+      <c r="N1" s="103" t="s">
         <v>4</v>
       </c>
-      <c r="O1" s="98"/>
-    </row>
-    <row r="2" spans="1:15">
-      <c r="A2" s="97"/>
+      <c r="O1" s="103"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A2" s="102"/>
       <c r="B2" s="9" t="s">
         <v>5</v>
       </c>
@@ -1796,36 +1796,36 @@
         <v>0.33333333333333615</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15" customHeight="1">
-      <c r="A3" s="99"/>
+    <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="97"/>
       <c r="B3" s="23">
         <v>0.33333333333333298</v>
       </c>
-      <c r="C3" s="100" t="s">
+      <c r="C3" s="98" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="100"/>
+      <c r="D3" s="98"/>
       <c r="E3" s="24">
         <v>0.33333333333333298</v>
       </c>
-      <c r="F3" s="101" t="s">
+      <c r="F3" s="99" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="101"/>
+      <c r="G3" s="99"/>
       <c r="H3" s="25">
         <v>0.33333333333333298</v>
       </c>
-      <c r="I3" s="102" t="s">
+      <c r="I3" s="100" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="102"/>
+      <c r="J3" s="100"/>
       <c r="K3" s="26">
         <v>0.33333333333333298</v>
       </c>
-      <c r="L3" s="103" t="s">
+      <c r="L3" s="101" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="103"/>
+      <c r="M3" s="101"/>
       <c r="N3" s="21" t="s">
         <v>10</v>
       </c>
@@ -1834,31 +1834,31 @@
         <v>5.3013888888889031</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
-      <c r="A4" s="99"/>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A4" s="97"/>
       <c r="B4" s="27">
         <v>0.41666666666666702</v>
       </c>
-      <c r="C4" s="100"/>
-      <c r="D4" s="100"/>
+      <c r="C4" s="98"/>
+      <c r="D4" s="98"/>
       <c r="E4" s="28">
         <v>0.41666666666666702</v>
       </c>
-      <c r="F4" s="101"/>
-      <c r="G4" s="101"/>
+      <c r="F4" s="99"/>
+      <c r="G4" s="99"/>
       <c r="H4" s="29">
         <v>0.41666666666666702</v>
       </c>
-      <c r="I4" s="102"/>
-      <c r="J4" s="102"/>
+      <c r="I4" s="100"/>
+      <c r="J4" s="100"/>
       <c r="K4" s="30">
         <v>0.41666666666666702</v>
       </c>
-      <c r="L4" s="103"/>
-      <c r="M4" s="103"/>
-    </row>
-    <row r="5" spans="1:15">
-      <c r="A5" s="99"/>
+      <c r="L4" s="101"/>
+      <c r="M4" s="101"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A5" s="97"/>
       <c r="B5" s="31">
         <f>B4-B3</f>
         <v>8.3333333333334036E-2</v>
@@ -1884,46 +1884,46 @@
       <c r="L5" s="41"/>
       <c r="M5" s="42"/>
     </row>
-    <row r="6" spans="1:15" ht="15" customHeight="1">
-      <c r="A6" s="99"/>
+    <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="97"/>
       <c r="B6" s="23"/>
-      <c r="C6" s="100" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="100"/>
+      <c r="C6" s="98" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="98"/>
       <c r="E6" s="24"/>
-      <c r="F6" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="101"/>
+      <c r="F6" s="99" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="99"/>
       <c r="H6" s="25"/>
-      <c r="I6" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="J6" s="102"/>
+      <c r="I6" s="100" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="100"/>
       <c r="K6" s="43"/>
-      <c r="L6" s="103" t="s">
-        <v>12</v>
-      </c>
-      <c r="M6" s="103"/>
-    </row>
-    <row r="7" spans="1:15">
-      <c r="A7" s="99"/>
+      <c r="L6" s="101" t="s">
+        <v>12</v>
+      </c>
+      <c r="M6" s="101"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A7" s="97"/>
       <c r="B7" s="27"/>
-      <c r="C7" s="100"/>
-      <c r="D7" s="100"/>
+      <c r="C7" s="98"/>
+      <c r="D7" s="98"/>
       <c r="E7" s="28"/>
-      <c r="F7" s="101"/>
-      <c r="G7" s="101"/>
+      <c r="F7" s="99"/>
+      <c r="G7" s="99"/>
       <c r="H7" s="29"/>
-      <c r="I7" s="102"/>
-      <c r="J7" s="102"/>
+      <c r="I7" s="100"/>
+      <c r="J7" s="100"/>
       <c r="K7" s="30"/>
-      <c r="L7" s="103"/>
-      <c r="M7" s="103"/>
-    </row>
-    <row r="8" spans="1:15">
-      <c r="A8" s="99"/>
+      <c r="L7" s="101"/>
+      <c r="M7" s="101"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A8" s="97"/>
       <c r="B8" s="31">
         <f>B7-B6</f>
         <v>0</v>
@@ -1949,46 +1949,46 @@
       <c r="L8" s="45"/>
       <c r="M8" s="46"/>
     </row>
-    <row r="9" spans="1:15" ht="15" customHeight="1">
-      <c r="A9" s="99"/>
+    <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="97"/>
       <c r="B9" s="23"/>
-      <c r="C9" s="100" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="100"/>
+      <c r="C9" s="98" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="98"/>
       <c r="E9" s="24"/>
-      <c r="F9" s="101" t="s">
+      <c r="F9" s="99" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="101"/>
+      <c r="G9" s="99"/>
       <c r="H9" s="25"/>
-      <c r="I9" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="J9" s="102"/>
+      <c r="I9" s="100" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" s="100"/>
       <c r="K9" s="47"/>
-      <c r="L9" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="M9" s="103"/>
-    </row>
-    <row r="10" spans="1:15">
-      <c r="A10" s="99"/>
+      <c r="L9" s="101" t="s">
+        <v>11</v>
+      </c>
+      <c r="M9" s="101"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A10" s="97"/>
       <c r="B10" s="27"/>
-      <c r="C10" s="100"/>
-      <c r="D10" s="100"/>
+      <c r="C10" s="98"/>
+      <c r="D10" s="98"/>
       <c r="E10" s="28"/>
-      <c r="F10" s="101"/>
-      <c r="G10" s="101"/>
+      <c r="F10" s="99"/>
+      <c r="G10" s="99"/>
       <c r="H10" s="29"/>
-      <c r="I10" s="102"/>
-      <c r="J10" s="102"/>
+      <c r="I10" s="100"/>
+      <c r="J10" s="100"/>
       <c r="K10" s="30"/>
-      <c r="L10" s="103"/>
-      <c r="M10" s="103"/>
-    </row>
-    <row r="11" spans="1:15">
-      <c r="A11" s="99"/>
+      <c r="L10" s="101"/>
+      <c r="M10" s="101"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A11" s="97"/>
       <c r="B11" s="31">
         <f>(B10-B9)</f>
         <v>0</v>
@@ -2014,46 +2014,46 @@
       <c r="L11" s="45"/>
       <c r="M11" s="46"/>
     </row>
-    <row r="12" spans="1:15" ht="15" customHeight="1">
-      <c r="A12" s="99"/>
+    <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="97"/>
       <c r="B12" s="23"/>
-      <c r="C12" s="100" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="100"/>
+      <c r="C12" s="98" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="98"/>
       <c r="E12" s="24"/>
-      <c r="F12" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" s="101"/>
+      <c r="F12" s="99" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="99"/>
       <c r="H12" s="25"/>
-      <c r="I12" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="J12" s="102"/>
+      <c r="I12" s="100" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" s="100"/>
       <c r="K12" s="47"/>
-      <c r="L12" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="M12" s="103"/>
-    </row>
-    <row r="13" spans="1:15">
-      <c r="A13" s="99"/>
+      <c r="L12" s="101" t="s">
+        <v>11</v>
+      </c>
+      <c r="M12" s="101"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A13" s="97"/>
       <c r="B13" s="27"/>
-      <c r="C13" s="100"/>
-      <c r="D13" s="100"/>
+      <c r="C13" s="98"/>
+      <c r="D13" s="98"/>
       <c r="E13" s="28"/>
-      <c r="F13" s="101"/>
-      <c r="G13" s="101"/>
+      <c r="F13" s="99"/>
+      <c r="G13" s="99"/>
       <c r="H13" s="29"/>
-      <c r="I13" s="102"/>
-      <c r="J13" s="102"/>
+      <c r="I13" s="100"/>
+      <c r="J13" s="100"/>
       <c r="K13" s="48"/>
-      <c r="L13" s="103"/>
-      <c r="M13" s="103"/>
-    </row>
-    <row r="14" spans="1:15">
-      <c r="A14" s="99"/>
+      <c r="L13" s="101"/>
+      <c r="M13" s="101"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A14" s="97"/>
       <c r="B14" s="31">
         <f>(B13-B12)</f>
         <v>0</v>
@@ -2079,46 +2079,46 @@
       <c r="L14" s="49"/>
       <c r="M14" s="50"/>
     </row>
-    <row r="15" spans="1:15" ht="15" customHeight="1">
-      <c r="A15" s="99"/>
+    <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="97"/>
       <c r="B15" s="23"/>
-      <c r="C15" s="100" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="100"/>
+      <c r="C15" s="98" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="98"/>
       <c r="E15" s="24"/>
-      <c r="F15" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="G15" s="101"/>
+      <c r="F15" s="99" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="99"/>
       <c r="H15" s="25"/>
-      <c r="I15" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="J15" s="102"/>
+      <c r="I15" s="100" t="s">
+        <v>11</v>
+      </c>
+      <c r="J15" s="100"/>
       <c r="K15" s="26"/>
-      <c r="L15" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="M15" s="103"/>
-    </row>
-    <row r="16" spans="1:15">
-      <c r="A16" s="99"/>
+      <c r="L15" s="101" t="s">
+        <v>11</v>
+      </c>
+      <c r="M15" s="101"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A16" s="97"/>
       <c r="B16" s="27"/>
-      <c r="C16" s="100"/>
-      <c r="D16" s="100"/>
+      <c r="C16" s="98"/>
+      <c r="D16" s="98"/>
       <c r="E16" s="28"/>
-      <c r="F16" s="101"/>
-      <c r="G16" s="101"/>
+      <c r="F16" s="99"/>
+      <c r="G16" s="99"/>
       <c r="H16" s="29"/>
-      <c r="I16" s="102"/>
-      <c r="J16" s="102"/>
+      <c r="I16" s="100"/>
+      <c r="J16" s="100"/>
       <c r="K16" s="30"/>
-      <c r="L16" s="103"/>
-      <c r="M16" s="103"/>
-    </row>
-    <row r="17" spans="1:13">
-      <c r="A17" s="99"/>
+      <c r="L16" s="101"/>
+      <c r="M16" s="101"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A17" s="97"/>
       <c r="B17" s="31">
         <f>(B16-B15)</f>
         <v>0</v>
@@ -2144,46 +2144,46 @@
       <c r="L17" s="45"/>
       <c r="M17" s="46"/>
     </row>
-    <row r="18" spans="1:13" ht="15" customHeight="1">
-      <c r="A18" s="99"/>
+    <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="97"/>
       <c r="B18" s="23"/>
-      <c r="C18" s="100" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="100"/>
+      <c r="C18" s="98" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="98"/>
       <c r="E18" s="24"/>
-      <c r="F18" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="G18" s="101"/>
+      <c r="F18" s="99" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" s="99"/>
       <c r="H18" s="25"/>
-      <c r="I18" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="J18" s="102"/>
+      <c r="I18" s="100" t="s">
+        <v>11</v>
+      </c>
+      <c r="J18" s="100"/>
       <c r="K18" s="47"/>
-      <c r="L18" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="M18" s="103"/>
-    </row>
-    <row r="19" spans="1:13">
-      <c r="A19" s="99"/>
+      <c r="L18" s="101" t="s">
+        <v>11</v>
+      </c>
+      <c r="M18" s="101"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A19" s="97"/>
       <c r="B19" s="27"/>
-      <c r="C19" s="100"/>
-      <c r="D19" s="100"/>
+      <c r="C19" s="98"/>
+      <c r="D19" s="98"/>
       <c r="E19" s="28"/>
-      <c r="F19" s="101"/>
-      <c r="G19" s="101"/>
+      <c r="F19" s="99"/>
+      <c r="G19" s="99"/>
       <c r="H19" s="29"/>
-      <c r="I19" s="102"/>
-      <c r="J19" s="102"/>
+      <c r="I19" s="100"/>
+      <c r="J19" s="100"/>
       <c r="K19" s="30"/>
-      <c r="L19" s="103"/>
-      <c r="M19" s="103"/>
-    </row>
-    <row r="20" spans="1:13">
-      <c r="A20" s="99"/>
+      <c r="L19" s="101"/>
+      <c r="M19" s="101"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A20" s="97"/>
       <c r="B20" s="31">
         <f>(B19-B18)</f>
         <v>0</v>
@@ -2209,46 +2209,46 @@
       <c r="L20" s="45"/>
       <c r="M20" s="46"/>
     </row>
-    <row r="21" spans="1:13" ht="15" customHeight="1">
-      <c r="A21" s="99"/>
+    <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="97"/>
       <c r="B21" s="23"/>
-      <c r="C21" s="100" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" s="100"/>
+      <c r="C21" s="98" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="98"/>
       <c r="E21" s="24"/>
-      <c r="F21" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="G21" s="101"/>
+      <c r="F21" s="99" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" s="99"/>
       <c r="H21" s="25"/>
-      <c r="I21" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="J21" s="102"/>
+      <c r="I21" s="100" t="s">
+        <v>11</v>
+      </c>
+      <c r="J21" s="100"/>
       <c r="K21" s="26"/>
-      <c r="L21" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="M21" s="103"/>
-    </row>
-    <row r="22" spans="1:13">
-      <c r="A22" s="99"/>
+      <c r="L21" s="101" t="s">
+        <v>11</v>
+      </c>
+      <c r="M21" s="101"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A22" s="97"/>
       <c r="B22" s="27"/>
-      <c r="C22" s="100"/>
-      <c r="D22" s="100"/>
+      <c r="C22" s="98"/>
+      <c r="D22" s="98"/>
       <c r="E22" s="28"/>
-      <c r="F22" s="101"/>
-      <c r="G22" s="101"/>
+      <c r="F22" s="99"/>
+      <c r="G22" s="99"/>
       <c r="H22" s="29"/>
-      <c r="I22" s="102"/>
-      <c r="J22" s="102"/>
+      <c r="I22" s="100"/>
+      <c r="J22" s="100"/>
       <c r="K22" s="48"/>
-      <c r="L22" s="103"/>
-      <c r="M22" s="103"/>
-    </row>
-    <row r="23" spans="1:13">
-      <c r="A23" s="99"/>
+      <c r="L22" s="101"/>
+      <c r="M22" s="101"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A23" s="97"/>
       <c r="B23" s="31">
         <f>(B22-B21)</f>
         <v>0</v>
@@ -2274,46 +2274,46 @@
       <c r="L23" s="51"/>
       <c r="M23" s="52"/>
     </row>
-    <row r="24" spans="1:13" ht="15" customHeight="1">
-      <c r="A24" s="99"/>
+    <row r="24" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="97"/>
       <c r="B24" s="23"/>
-      <c r="C24" s="100" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" s="100"/>
+      <c r="C24" s="98" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="98"/>
       <c r="E24" s="24"/>
-      <c r="F24" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="G24" s="101"/>
+      <c r="F24" s="99" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" s="99"/>
       <c r="H24" s="25"/>
-      <c r="I24" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="J24" s="102"/>
+      <c r="I24" s="100" t="s">
+        <v>11</v>
+      </c>
+      <c r="J24" s="100"/>
       <c r="K24" s="26"/>
-      <c r="L24" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="M24" s="103"/>
-    </row>
-    <row r="25" spans="1:13">
-      <c r="A25" s="99"/>
+      <c r="L24" s="101" t="s">
+        <v>11</v>
+      </c>
+      <c r="M24" s="101"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A25" s="97"/>
       <c r="B25" s="27"/>
-      <c r="C25" s="100"/>
-      <c r="D25" s="100"/>
+      <c r="C25" s="98"/>
+      <c r="D25" s="98"/>
       <c r="E25" s="28"/>
-      <c r="F25" s="101"/>
-      <c r="G25" s="101"/>
+      <c r="F25" s="99"/>
+      <c r="G25" s="99"/>
       <c r="H25" s="29"/>
-      <c r="I25" s="102"/>
-      <c r="J25" s="102"/>
+      <c r="I25" s="100"/>
+      <c r="J25" s="100"/>
       <c r="K25" s="30"/>
-      <c r="L25" s="103"/>
-      <c r="M25" s="103"/>
-    </row>
-    <row r="26" spans="1:13">
-      <c r="A26" s="99"/>
+      <c r="L25" s="101"/>
+      <c r="M25" s="101"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A26" s="97"/>
       <c r="B26" s="31">
         <f>(B25-B24)</f>
         <v>0</v>
@@ -2339,46 +2339,46 @@
       <c r="L26" s="45"/>
       <c r="M26" s="46"/>
     </row>
-    <row r="27" spans="1:13" ht="15" customHeight="1">
-      <c r="A27" s="99"/>
+    <row r="27" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="97"/>
       <c r="B27" s="23"/>
-      <c r="C27" s="100" t="s">
-        <v>11</v>
-      </c>
-      <c r="D27" s="100"/>
+      <c r="C27" s="98" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="98"/>
       <c r="E27" s="24"/>
-      <c r="F27" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="G27" s="101"/>
+      <c r="F27" s="99" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" s="99"/>
       <c r="H27" s="25"/>
-      <c r="I27" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="J27" s="102"/>
+      <c r="I27" s="100" t="s">
+        <v>11</v>
+      </c>
+      <c r="J27" s="100"/>
       <c r="K27" s="47"/>
-      <c r="L27" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="M27" s="103"/>
-    </row>
-    <row r="28" spans="1:13">
-      <c r="A28" s="99"/>
+      <c r="L27" s="101" t="s">
+        <v>11</v>
+      </c>
+      <c r="M27" s="101"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A28" s="97"/>
       <c r="B28" s="27"/>
-      <c r="C28" s="100"/>
-      <c r="D28" s="100"/>
+      <c r="C28" s="98"/>
+      <c r="D28" s="98"/>
       <c r="E28" s="28"/>
-      <c r="F28" s="101"/>
-      <c r="G28" s="101"/>
+      <c r="F28" s="99"/>
+      <c r="G28" s="99"/>
       <c r="H28" s="29"/>
-      <c r="I28" s="102"/>
-      <c r="J28" s="102"/>
+      <c r="I28" s="100"/>
+      <c r="J28" s="100"/>
       <c r="K28" s="30"/>
-      <c r="L28" s="103"/>
-      <c r="M28" s="103"/>
-    </row>
-    <row r="29" spans="1:13">
-      <c r="A29" s="99"/>
+      <c r="L28" s="101"/>
+      <c r="M28" s="101"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A29" s="97"/>
       <c r="B29" s="31">
         <f>(B28-B27)</f>
         <v>0</v>
@@ -2404,46 +2404,46 @@
       <c r="L29" s="45"/>
       <c r="M29" s="46"/>
     </row>
-    <row r="30" spans="1:13" ht="15" customHeight="1">
-      <c r="A30" s="99"/>
+    <row r="30" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="97"/>
       <c r="B30" s="23"/>
-      <c r="C30" s="100" t="s">
-        <v>11</v>
-      </c>
-      <c r="D30" s="100"/>
+      <c r="C30" s="98" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" s="98"/>
       <c r="E30" s="24"/>
-      <c r="F30" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="G30" s="101"/>
+      <c r="F30" s="99" t="s">
+        <v>11</v>
+      </c>
+      <c r="G30" s="99"/>
       <c r="H30" s="25"/>
-      <c r="I30" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="J30" s="102"/>
+      <c r="I30" s="100" t="s">
+        <v>11</v>
+      </c>
+      <c r="J30" s="100"/>
       <c r="K30" s="26"/>
-      <c r="L30" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="M30" s="103"/>
-    </row>
-    <row r="31" spans="1:13">
-      <c r="A31" s="99"/>
+      <c r="L30" s="101" t="s">
+        <v>11</v>
+      </c>
+      <c r="M30" s="101"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A31" s="97"/>
       <c r="B31" s="27"/>
-      <c r="C31" s="100"/>
-      <c r="D31" s="100"/>
+      <c r="C31" s="98"/>
+      <c r="D31" s="98"/>
       <c r="E31" s="28"/>
-      <c r="F31" s="101"/>
-      <c r="G31" s="101"/>
+      <c r="F31" s="99"/>
+      <c r="G31" s="99"/>
       <c r="H31" s="29"/>
-      <c r="I31" s="102"/>
-      <c r="J31" s="102"/>
+      <c r="I31" s="100"/>
+      <c r="J31" s="100"/>
       <c r="K31" s="48"/>
-      <c r="L31" s="103"/>
-      <c r="M31" s="103"/>
-    </row>
-    <row r="32" spans="1:13">
-      <c r="A32" s="99"/>
+      <c r="L31" s="101"/>
+      <c r="M31" s="101"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A32" s="97"/>
       <c r="B32" s="31">
         <f>(B31-B30)</f>
         <v>0</v>
@@ -2469,46 +2469,46 @@
       <c r="L32" s="51"/>
       <c r="M32" s="52"/>
     </row>
-    <row r="33" spans="1:13" ht="15" customHeight="1">
-      <c r="A33" s="99"/>
+    <row r="33" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="97"/>
       <c r="B33" s="23"/>
-      <c r="C33" s="100" t="s">
-        <v>11</v>
-      </c>
-      <c r="D33" s="100"/>
+      <c r="C33" s="98" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="98"/>
       <c r="E33" s="24"/>
-      <c r="F33" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="G33" s="101"/>
+      <c r="F33" s="99" t="s">
+        <v>11</v>
+      </c>
+      <c r="G33" s="99"/>
       <c r="H33" s="25"/>
-      <c r="I33" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="J33" s="102"/>
+      <c r="I33" s="100" t="s">
+        <v>11</v>
+      </c>
+      <c r="J33" s="100"/>
       <c r="K33" s="26"/>
-      <c r="L33" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="M33" s="103"/>
-    </row>
-    <row r="34" spans="1:13">
-      <c r="A34" s="99"/>
+      <c r="L33" s="101" t="s">
+        <v>11</v>
+      </c>
+      <c r="M33" s="101"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A34" s="97"/>
       <c r="B34" s="27"/>
-      <c r="C34" s="100"/>
-      <c r="D34" s="100"/>
+      <c r="C34" s="98"/>
+      <c r="D34" s="98"/>
       <c r="E34" s="28"/>
-      <c r="F34" s="101"/>
-      <c r="G34" s="101"/>
+      <c r="F34" s="99"/>
+      <c r="G34" s="99"/>
       <c r="H34" s="29"/>
-      <c r="I34" s="102"/>
-      <c r="J34" s="102"/>
+      <c r="I34" s="100"/>
+      <c r="J34" s="100"/>
       <c r="K34" s="30"/>
-      <c r="L34" s="103"/>
-      <c r="M34" s="103"/>
-    </row>
-    <row r="35" spans="1:13">
-      <c r="A35" s="99"/>
+      <c r="L34" s="101"/>
+      <c r="M34" s="101"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A35" s="97"/>
       <c r="B35" s="31">
         <f>(B34-B33)</f>
         <v>0</v>
@@ -2534,46 +2534,46 @@
       <c r="L35" s="45"/>
       <c r="M35" s="46"/>
     </row>
-    <row r="36" spans="1:13" ht="15" customHeight="1">
-      <c r="A36" s="99"/>
+    <row r="36" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="97"/>
       <c r="B36" s="23"/>
-      <c r="C36" s="100" t="s">
-        <v>11</v>
-      </c>
-      <c r="D36" s="100"/>
+      <c r="C36" s="98" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" s="98"/>
       <c r="E36" s="24"/>
-      <c r="F36" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="G36" s="101"/>
+      <c r="F36" s="99" t="s">
+        <v>11</v>
+      </c>
+      <c r="G36" s="99"/>
       <c r="H36" s="25"/>
-      <c r="I36" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="J36" s="102"/>
+      <c r="I36" s="100" t="s">
+        <v>11</v>
+      </c>
+      <c r="J36" s="100"/>
       <c r="K36" s="47"/>
-      <c r="L36" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="M36" s="103"/>
-    </row>
-    <row r="37" spans="1:13">
-      <c r="A37" s="99"/>
+      <c r="L36" s="101" t="s">
+        <v>11</v>
+      </c>
+      <c r="M36" s="101"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A37" s="97"/>
       <c r="B37" s="27"/>
-      <c r="C37" s="100"/>
-      <c r="D37" s="100"/>
+      <c r="C37" s="98"/>
+      <c r="D37" s="98"/>
       <c r="E37" s="28"/>
-      <c r="F37" s="101"/>
-      <c r="G37" s="101"/>
+      <c r="F37" s="99"/>
+      <c r="G37" s="99"/>
       <c r="H37" s="29"/>
-      <c r="I37" s="102"/>
-      <c r="J37" s="102"/>
+      <c r="I37" s="100"/>
+      <c r="J37" s="100"/>
       <c r="K37" s="30"/>
-      <c r="L37" s="103"/>
-      <c r="M37" s="103"/>
-    </row>
-    <row r="38" spans="1:13">
-      <c r="A38" s="99"/>
+      <c r="L37" s="101"/>
+      <c r="M37" s="101"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A38" s="97"/>
       <c r="B38" s="31">
         <f>(B37-B36)</f>
         <v>0</v>
@@ -2599,46 +2599,46 @@
       <c r="L38" s="45"/>
       <c r="M38" s="46"/>
     </row>
-    <row r="39" spans="1:13" ht="15" customHeight="1">
-      <c r="A39" s="99"/>
+    <row r="39" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="97"/>
       <c r="B39" s="23"/>
-      <c r="C39" s="100" t="s">
-        <v>11</v>
-      </c>
-      <c r="D39" s="100"/>
+      <c r="C39" s="98" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" s="98"/>
       <c r="E39" s="24"/>
-      <c r="F39" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="G39" s="101"/>
+      <c r="F39" s="99" t="s">
+        <v>11</v>
+      </c>
+      <c r="G39" s="99"/>
       <c r="H39" s="25"/>
-      <c r="I39" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="J39" s="102"/>
+      <c r="I39" s="100" t="s">
+        <v>11</v>
+      </c>
+      <c r="J39" s="100"/>
       <c r="K39" s="26"/>
-      <c r="L39" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="M39" s="103"/>
-    </row>
-    <row r="40" spans="1:13">
-      <c r="A40" s="99"/>
+      <c r="L39" s="101" t="s">
+        <v>11</v>
+      </c>
+      <c r="M39" s="101"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A40" s="97"/>
       <c r="B40" s="27"/>
-      <c r="C40" s="100"/>
-      <c r="D40" s="100"/>
+      <c r="C40" s="98"/>
+      <c r="D40" s="98"/>
       <c r="E40" s="28"/>
-      <c r="F40" s="101"/>
-      <c r="G40" s="101"/>
+      <c r="F40" s="99"/>
+      <c r="G40" s="99"/>
       <c r="H40" s="29"/>
-      <c r="I40" s="102"/>
-      <c r="J40" s="102"/>
+      <c r="I40" s="100"/>
+      <c r="J40" s="100"/>
       <c r="K40" s="48"/>
-      <c r="L40" s="103"/>
-      <c r="M40" s="103"/>
-    </row>
-    <row r="41" spans="1:13">
-      <c r="A41" s="99"/>
+      <c r="L40" s="101"/>
+      <c r="M40" s="101"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A41" s="97"/>
       <c r="B41" s="31">
         <f>(B40-B39)</f>
         <v>0</v>
@@ -2666,66 +2666,6 @@
     </row>
   </sheetData>
   <mergeCells count="67">
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="C39:D40"/>
-    <mergeCell ref="F39:G40"/>
-    <mergeCell ref="I39:J40"/>
-    <mergeCell ref="L39:M40"/>
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="C36:D37"/>
-    <mergeCell ref="F36:G37"/>
-    <mergeCell ref="I36:J37"/>
-    <mergeCell ref="L36:M37"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="C33:D34"/>
-    <mergeCell ref="F33:G34"/>
-    <mergeCell ref="I33:J34"/>
-    <mergeCell ref="L33:M34"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="C30:D31"/>
-    <mergeCell ref="F30:G31"/>
-    <mergeCell ref="I30:J31"/>
-    <mergeCell ref="L30:M31"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="C27:D28"/>
-    <mergeCell ref="F27:G28"/>
-    <mergeCell ref="I27:J28"/>
-    <mergeCell ref="L27:M28"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="C24:D25"/>
-    <mergeCell ref="F24:G25"/>
-    <mergeCell ref="I24:J25"/>
-    <mergeCell ref="L24:M25"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="C21:D22"/>
-    <mergeCell ref="F21:G22"/>
-    <mergeCell ref="I21:J22"/>
-    <mergeCell ref="L21:M22"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="C18:D19"/>
-    <mergeCell ref="F18:G19"/>
-    <mergeCell ref="I18:J19"/>
-    <mergeCell ref="L18:M19"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="C15:D16"/>
-    <mergeCell ref="F15:G16"/>
-    <mergeCell ref="I15:J16"/>
-    <mergeCell ref="L15:M16"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="C12:D13"/>
-    <mergeCell ref="F12:G13"/>
-    <mergeCell ref="I12:J13"/>
-    <mergeCell ref="L12:M13"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="C9:D10"/>
-    <mergeCell ref="F9:G10"/>
-    <mergeCell ref="I9:J10"/>
-    <mergeCell ref="L9:M10"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="C6:D7"/>
-    <mergeCell ref="F6:G7"/>
-    <mergeCell ref="I6:J7"/>
-    <mergeCell ref="L6:M7"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="A3:A5"/>
@@ -2733,6 +2673,66 @@
     <mergeCell ref="F3:G4"/>
     <mergeCell ref="I3:J4"/>
     <mergeCell ref="L3:M4"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="C6:D7"/>
+    <mergeCell ref="F6:G7"/>
+    <mergeCell ref="I6:J7"/>
+    <mergeCell ref="L6:M7"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="C9:D10"/>
+    <mergeCell ref="F9:G10"/>
+    <mergeCell ref="I9:J10"/>
+    <mergeCell ref="L9:M10"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="C12:D13"/>
+    <mergeCell ref="F12:G13"/>
+    <mergeCell ref="I12:J13"/>
+    <mergeCell ref="L12:M13"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="C15:D16"/>
+    <mergeCell ref="F15:G16"/>
+    <mergeCell ref="I15:J16"/>
+    <mergeCell ref="L15:M16"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="C18:D19"/>
+    <mergeCell ref="F18:G19"/>
+    <mergeCell ref="I18:J19"/>
+    <mergeCell ref="L18:M19"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="C21:D22"/>
+    <mergeCell ref="F21:G22"/>
+    <mergeCell ref="I21:J22"/>
+    <mergeCell ref="L21:M22"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="C24:D25"/>
+    <mergeCell ref="F24:G25"/>
+    <mergeCell ref="I24:J25"/>
+    <mergeCell ref="L24:M25"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="C27:D28"/>
+    <mergeCell ref="F27:G28"/>
+    <mergeCell ref="I27:J28"/>
+    <mergeCell ref="L27:M28"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="C30:D31"/>
+    <mergeCell ref="F30:G31"/>
+    <mergeCell ref="I30:J31"/>
+    <mergeCell ref="L30:M31"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="C33:D34"/>
+    <mergeCell ref="F33:G34"/>
+    <mergeCell ref="I33:J34"/>
+    <mergeCell ref="L33:M34"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="C36:D37"/>
+    <mergeCell ref="F36:G37"/>
+    <mergeCell ref="I36:J37"/>
+    <mergeCell ref="L36:M37"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="C39:D40"/>
+    <mergeCell ref="F39:G40"/>
+    <mergeCell ref="I39:J40"/>
+    <mergeCell ref="L39:M40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2747,13 +2747,13 @@
       <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.69140625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
-    <col min="2" max="9" width="17.28515625" customWidth="1"/>
+    <col min="1" max="1" width="15.3046875" customWidth="1"/>
+    <col min="2" max="9" width="17.3046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A1" s="53"/>
       <c r="B1" s="54" t="s">
         <v>5</v>
@@ -2784,7 +2784,7 @@
         <v>0.33333333333333393</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A2" s="104">
         <v>44535</v>
       </c>
@@ -2811,7 +2811,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A3" s="104"/>
       <c r="B3" s="27">
         <v>1</v>
@@ -2830,7 +2830,7 @@
       </c>
       <c r="I3" s="108"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A4" s="104"/>
       <c r="B4" s="109">
         <f>B3-B2</f>
@@ -2853,7 +2853,7 @@
       </c>
       <c r="I4" s="112"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A5" s="104">
         <v>44542</v>
       </c>
@@ -2880,7 +2880,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A6" s="104"/>
       <c r="B6" s="27">
         <v>1</v>
@@ -2899,7 +2899,7 @@
       </c>
       <c r="I6" s="108"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A7" s="104"/>
       <c r="B7" s="109">
         <f>B6-B5</f>
@@ -2922,7 +2922,7 @@
       </c>
       <c r="I7" s="112"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A8" s="104"/>
       <c r="B8" s="23"/>
       <c r="C8" s="105" t="s">
@@ -2941,7 +2941,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A9" s="104"/>
       <c r="B9" s="27"/>
       <c r="C9" s="105"/>
@@ -2952,7 +2952,7 @@
       <c r="H9" s="63"/>
       <c r="I9" s="108"/>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A10" s="104"/>
       <c r="B10" s="109">
         <f>(B9-B8)</f>
@@ -2975,7 +2975,7 @@
       </c>
       <c r="I10" s="112"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A11" s="104"/>
       <c r="B11" s="23"/>
       <c r="C11" s="105" t="s">
@@ -2994,7 +2994,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A12" s="104"/>
       <c r="B12" s="27"/>
       <c r="C12" s="105"/>
@@ -3005,7 +3005,7 @@
       <c r="H12" s="63"/>
       <c r="I12" s="108"/>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A13" s="104"/>
       <c r="B13" s="109">
         <f>(B12-B11)</f>
@@ -3028,7 +3028,7 @@
       </c>
       <c r="I13" s="112"/>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A14" s="104"/>
       <c r="B14" s="23"/>
       <c r="C14" s="105" t="s">
@@ -3047,7 +3047,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A15" s="104"/>
       <c r="B15" s="27"/>
       <c r="C15" s="105"/>
@@ -3058,7 +3058,7 @@
       <c r="H15" s="63"/>
       <c r="I15" s="108"/>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A16" s="104"/>
       <c r="B16" s="109">
         <f>(B15-B14)</f>
@@ -3081,7 +3081,7 @@
       </c>
       <c r="I16" s="112"/>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A17" s="104"/>
       <c r="B17" s="23"/>
       <c r="C17" s="105" t="s">
@@ -3100,7 +3100,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A18" s="104"/>
       <c r="B18" s="27"/>
       <c r="C18" s="105"/>
@@ -3111,7 +3111,7 @@
       <c r="H18" s="63"/>
       <c r="I18" s="108"/>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A19" s="104"/>
       <c r="B19" s="109">
         <f>(B18-B17)</f>
@@ -3134,7 +3134,7 @@
       </c>
       <c r="I19" s="112"/>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A20" s="104"/>
       <c r="B20" s="23"/>
       <c r="C20" s="105" t="s">
@@ -3153,7 +3153,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A21" s="104"/>
       <c r="B21" s="27"/>
       <c r="C21" s="105"/>
@@ -3164,7 +3164,7 @@
       <c r="H21" s="63"/>
       <c r="I21" s="108"/>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A22" s="104"/>
       <c r="B22" s="109">
         <f>(B21-B20)</f>
@@ -3189,6 +3189,60 @@
     </row>
   </sheetData>
   <mergeCells count="63">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H19:I19"/>
     <mergeCell ref="A20:A22"/>
     <mergeCell ref="C20:C21"/>
     <mergeCell ref="E20:E21"/>
@@ -3198,60 +3252,6 @@
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="F22:G22"/>
     <mergeCell ref="H22:I22"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -3266,20 +3266,20 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.69140625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" customWidth="1"/>
-    <col min="3" max="4" width="13.7109375" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="6" max="7" width="13.7109375" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" customWidth="1"/>
-    <col min="9" max="10" width="13.7109375" customWidth="1"/>
-    <col min="11" max="11" width="15.140625" customWidth="1"/>
-    <col min="12" max="13" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.3046875" customWidth="1"/>
+    <col min="2" max="2" width="15.15234375" customWidth="1"/>
+    <col min="3" max="4" width="13.69140625" customWidth="1"/>
+    <col min="5" max="5" width="16.15234375" customWidth="1"/>
+    <col min="6" max="7" width="13.69140625" customWidth="1"/>
+    <col min="8" max="8" width="15.15234375" customWidth="1"/>
+    <col min="9" max="10" width="13.69140625" customWidth="1"/>
+    <col min="11" max="11" width="15.15234375" customWidth="1"/>
+    <col min="12" max="13" width="13.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A1" s="53"/>
       <c r="B1" s="64" t="s">
         <v>5</v>
@@ -3327,7 +3327,7 @@
       </c>
       <c r="N1" s="76"/>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A2" s="104">
         <v>44543</v>
       </c>
@@ -3355,12 +3355,12 @@
       <c r="K2" s="26">
         <v>0.33333333333333298</v>
       </c>
-      <c r="L2" s="116" t="s">
-        <v>12</v>
-      </c>
-      <c r="M2" s="116"/>
-    </row>
-    <row r="3" spans="1:14">
+      <c r="L2" s="119" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="119"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A3" s="104"/>
       <c r="B3" s="27">
         <v>0.49166666666666697</v>
@@ -3380,10 +3380,10 @@
       <c r="K3" s="30">
         <v>0.41666666666666702</v>
       </c>
-      <c r="L3" s="116"/>
-      <c r="M3" s="116"/>
-    </row>
-    <row r="4" spans="1:14">
+      <c r="L3" s="119"/>
+      <c r="M3" s="119"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A4" s="104"/>
       <c r="B4" s="109">
         <f>B3-B2</f>
@@ -3403,14 +3403,14 @@
       </c>
       <c r="I4" s="111"/>
       <c r="J4" s="111"/>
-      <c r="K4" s="117">
+      <c r="K4" s="122">
         <f>K3-K2</f>
         <v>8.3333333333334036E-2</v>
       </c>
-      <c r="L4" s="117"/>
-      <c r="M4" s="117"/>
-    </row>
-    <row r="5" spans="1:14">
+      <c r="L4" s="122"/>
+      <c r="M4" s="122"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A5" s="104">
         <v>44568</v>
       </c>
@@ -3434,12 +3434,12 @@
       <c r="K5" s="43">
         <v>0.33333333333333298</v>
       </c>
-      <c r="L5" s="118" t="s">
+      <c r="L5" s="116" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="118"/>
-    </row>
-    <row r="6" spans="1:14">
+      <c r="M5" s="116"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A6" s="104"/>
       <c r="B6" s="27"/>
       <c r="C6" s="113"/>
@@ -3455,10 +3455,10 @@
       <c r="K6" s="30">
         <v>0.625</v>
       </c>
-      <c r="L6" s="118"/>
-      <c r="M6" s="118"/>
-    </row>
-    <row r="7" spans="1:14">
+      <c r="L6" s="116"/>
+      <c r="M6" s="116"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A7" s="104"/>
       <c r="B7" s="109">
         <f>B6-B5</f>
@@ -3485,7 +3485,7 @@
       <c r="L7" s="112"/>
       <c r="M7" s="112"/>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A8" s="104">
         <v>44569</v>
       </c>
@@ -3513,12 +3513,12 @@
       <c r="K8" s="47">
         <v>0.77083333333333304</v>
       </c>
-      <c r="L8" s="119" t="s">
-        <v>12</v>
-      </c>
-      <c r="M8" s="119"/>
-    </row>
-    <row r="9" spans="1:14">
+      <c r="L8" s="118" t="s">
+        <v>12</v>
+      </c>
+      <c r="M8" s="118"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A9" s="104"/>
       <c r="B9" s="27">
         <v>1</v>
@@ -3538,10 +3538,10 @@
       <c r="K9" s="30">
         <v>0.91666666666666696</v>
       </c>
-      <c r="L9" s="119"/>
-      <c r="M9" s="119"/>
-    </row>
-    <row r="10" spans="1:14">
+      <c r="L9" s="118"/>
+      <c r="M9" s="118"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A10" s="104"/>
       <c r="B10" s="109">
         <f>(B9-B8)</f>
@@ -3568,7 +3568,7 @@
       <c r="L10" s="112"/>
       <c r="M10" s="112"/>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A11" s="104">
         <v>44805</v>
       </c>
@@ -3601,7 +3601,7 @@
       </c>
       <c r="M11" s="120"/>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A12" s="104"/>
       <c r="B12" s="27">
         <v>1</v>
@@ -3624,7 +3624,7 @@
       <c r="L12" s="120"/>
       <c r="M12" s="120"/>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A13" s="104"/>
       <c r="B13" s="109">
         <f>(B12-B11)</f>
@@ -3651,7 +3651,7 @@
       <c r="L13" s="121"/>
       <c r="M13" s="121"/>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A14" s="104"/>
       <c r="B14" s="23"/>
       <c r="C14" s="113" t="s">
@@ -3669,12 +3669,12 @@
       </c>
       <c r="J14" s="115"/>
       <c r="K14" s="26"/>
-      <c r="L14" s="116" t="s">
-        <v>12</v>
-      </c>
-      <c r="M14" s="116"/>
-    </row>
-    <row r="15" spans="1:14">
+      <c r="L14" s="119" t="s">
+        <v>12</v>
+      </c>
+      <c r="M14" s="119"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A15" s="104"/>
       <c r="B15" s="27"/>
       <c r="C15" s="113"/>
@@ -3686,10 +3686,10 @@
       <c r="I15" s="115"/>
       <c r="J15" s="115"/>
       <c r="K15" s="30"/>
-      <c r="L15" s="116"/>
-      <c r="M15" s="116"/>
-    </row>
-    <row r="16" spans="1:14">
+      <c r="L15" s="119"/>
+      <c r="M15" s="119"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A16" s="104"/>
       <c r="B16" s="109">
         <f>(B15-B14)</f>
@@ -3716,7 +3716,7 @@
       <c r="L16" s="112"/>
       <c r="M16" s="112"/>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A17" s="104"/>
       <c r="B17" s="23"/>
       <c r="C17" s="113" t="s">
@@ -3734,12 +3734,12 @@
       </c>
       <c r="J17" s="115"/>
       <c r="K17" s="47"/>
-      <c r="L17" s="119" t="s">
-        <v>12</v>
-      </c>
-      <c r="M17" s="119"/>
-    </row>
-    <row r="18" spans="1:13">
+      <c r="L17" s="118" t="s">
+        <v>12</v>
+      </c>
+      <c r="M17" s="118"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A18" s="104"/>
       <c r="B18" s="27"/>
       <c r="C18" s="113"/>
@@ -3751,10 +3751,10 @@
       <c r="I18" s="115"/>
       <c r="J18" s="115"/>
       <c r="K18" s="30"/>
-      <c r="L18" s="119"/>
-      <c r="M18" s="119"/>
-    </row>
-    <row r="19" spans="1:13">
+      <c r="L18" s="118"/>
+      <c r="M18" s="118"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A19" s="104"/>
       <c r="B19" s="109">
         <f>(B18-B17)</f>
@@ -3781,7 +3781,7 @@
       <c r="L19" s="112"/>
       <c r="M19" s="112"/>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A20" s="104"/>
       <c r="B20" s="23"/>
       <c r="C20" s="113" t="s">
@@ -3799,12 +3799,12 @@
       </c>
       <c r="J20" s="115"/>
       <c r="K20" s="26"/>
-      <c r="L20" s="118" t="s">
-        <v>12</v>
-      </c>
-      <c r="M20" s="118"/>
-    </row>
-    <row r="21" spans="1:13">
+      <c r="L20" s="116" t="s">
+        <v>12</v>
+      </c>
+      <c r="M20" s="116"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A21" s="104"/>
       <c r="B21" s="27"/>
       <c r="C21" s="113"/>
@@ -3816,10 +3816,10 @@
       <c r="I21" s="115"/>
       <c r="J21" s="115"/>
       <c r="K21" s="48"/>
-      <c r="L21" s="118"/>
-      <c r="M21" s="118"/>
-    </row>
-    <row r="22" spans="1:13">
+      <c r="L21" s="116"/>
+      <c r="M21" s="116"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A22" s="104"/>
       <c r="B22" s="109">
         <f>(B21-B20)</f>
@@ -3839,15 +3839,69 @@
       </c>
       <c r="I22" s="111"/>
       <c r="J22" s="111"/>
-      <c r="K22" s="122">
+      <c r="K22" s="117">
         <f>K21-K20</f>
         <v>0</v>
       </c>
-      <c r="L22" s="122"/>
-      <c r="M22" s="122"/>
+      <c r="L22" s="117"/>
+      <c r="M22" s="117"/>
     </row>
   </sheetData>
   <mergeCells count="63">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="C2:D3"/>
+    <mergeCell ref="F2:G3"/>
+    <mergeCell ref="I2:J3"/>
+    <mergeCell ref="L2:M3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="C5:D6"/>
+    <mergeCell ref="F5:G6"/>
+    <mergeCell ref="I5:J6"/>
+    <mergeCell ref="L5:M6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="C8:D9"/>
+    <mergeCell ref="F8:G9"/>
+    <mergeCell ref="I8:J9"/>
+    <mergeCell ref="L8:M9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="C11:D12"/>
+    <mergeCell ref="F11:G12"/>
+    <mergeCell ref="I11:J12"/>
+    <mergeCell ref="L11:M12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="C14:D15"/>
+    <mergeCell ref="F14:G15"/>
+    <mergeCell ref="I14:J15"/>
+    <mergeCell ref="L14:M15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="C17:D18"/>
+    <mergeCell ref="F17:G18"/>
+    <mergeCell ref="I17:J18"/>
+    <mergeCell ref="L17:M18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="K19:M19"/>
     <mergeCell ref="A20:A22"/>
     <mergeCell ref="C20:D21"/>
     <mergeCell ref="F20:G21"/>
@@ -3857,60 +3911,6 @@
     <mergeCell ref="E22:G22"/>
     <mergeCell ref="H22:J22"/>
     <mergeCell ref="K22:M22"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="C17:D18"/>
-    <mergeCell ref="F17:G18"/>
-    <mergeCell ref="I17:J18"/>
-    <mergeCell ref="L17:M18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="K19:M19"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="C14:D15"/>
-    <mergeCell ref="F14:G15"/>
-    <mergeCell ref="I14:J15"/>
-    <mergeCell ref="L14:M15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="K16:M16"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="C11:D12"/>
-    <mergeCell ref="F11:G12"/>
-    <mergeCell ref="I11:J12"/>
-    <mergeCell ref="L11:M12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="K13:M13"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="C8:D9"/>
-    <mergeCell ref="F8:G9"/>
-    <mergeCell ref="I8:J9"/>
-    <mergeCell ref="L8:M9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="K10:M10"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="C5:D6"/>
-    <mergeCell ref="F5:G6"/>
-    <mergeCell ref="I5:J6"/>
-    <mergeCell ref="L5:M6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="C2:D3"/>
-    <mergeCell ref="F2:G3"/>
-    <mergeCell ref="I2:J3"/>
-    <mergeCell ref="L2:M3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:M4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -3925,21 +3925,21 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.69140625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" customWidth="1"/>
-    <col min="3" max="4" width="13.7109375" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="6" max="7" width="13.7109375" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" customWidth="1"/>
-    <col min="9" max="10" width="13.7109375" customWidth="1"/>
-    <col min="11" max="11" width="15.140625" customWidth="1"/>
-    <col min="12" max="13" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.3046875" customWidth="1"/>
+    <col min="2" max="2" width="15.15234375" customWidth="1"/>
+    <col min="3" max="4" width="13.69140625" customWidth="1"/>
+    <col min="5" max="5" width="16.15234375" customWidth="1"/>
+    <col min="6" max="7" width="13.69140625" customWidth="1"/>
+    <col min="8" max="8" width="15.15234375" customWidth="1"/>
+    <col min="9" max="10" width="13.69140625" customWidth="1"/>
+    <col min="11" max="11" width="15.15234375" customWidth="1"/>
+    <col min="12" max="13" width="13.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
-      <c r="A1" s="123" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A1" s="127" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="77" t="s">
@@ -3980,8 +3980,8 @@
       </c>
       <c r="N1" s="76"/>
     </row>
-    <row r="2" spans="1:14">
-      <c r="A2" s="123"/>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A2" s="127"/>
       <c r="B2" s="85" t="s">
         <v>5</v>
       </c>
@@ -4027,64 +4027,64 @@
         <v>1.3305555555555593</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15" customHeight="1">
-      <c r="A3" s="99">
+    <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="97">
         <v>44571</v>
       </c>
       <c r="B3" s="23">
         <v>0.33333333333333298</v>
       </c>
-      <c r="C3" s="124" t="s">
+      <c r="C3" s="123" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="124"/>
+      <c r="D3" s="123"/>
       <c r="E3" s="24">
         <v>0.33333333333333298</v>
       </c>
-      <c r="F3" s="125" t="s">
+      <c r="F3" s="124" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="125"/>
+      <c r="G3" s="124"/>
       <c r="H3" s="25">
         <v>0.33333333333333298</v>
       </c>
-      <c r="I3" s="126" t="s">
+      <c r="I3" s="125" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="126"/>
+      <c r="J3" s="125"/>
       <c r="K3" s="26">
         <v>0.33333333333333298</v>
       </c>
-      <c r="L3" s="127" t="s">
+      <c r="L3" s="126" t="s">
         <v>21</v>
       </c>
-      <c r="M3" s="127"/>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="A4" s="99"/>
+      <c r="M3" s="126"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A4" s="97"/>
       <c r="B4" s="27">
         <v>0.41666666666666702</v>
       </c>
-      <c r="C4" s="124"/>
-      <c r="D4" s="124"/>
+      <c r="C4" s="123"/>
+      <c r="D4" s="123"/>
       <c r="E4" s="28">
         <v>0.41666666666666702</v>
       </c>
-      <c r="F4" s="125"/>
-      <c r="G4" s="125"/>
+      <c r="F4" s="124"/>
+      <c r="G4" s="124"/>
       <c r="H4" s="29">
         <v>0.41666666666666702</v>
       </c>
-      <c r="I4" s="126"/>
-      <c r="J4" s="126"/>
+      <c r="I4" s="125"/>
+      <c r="J4" s="125"/>
       <c r="K4" s="30">
         <v>0.41666666666666702</v>
       </c>
-      <c r="L4" s="127"/>
-      <c r="M4" s="127"/>
-    </row>
-    <row r="5" spans="1:14">
-      <c r="A5" s="99"/>
+      <c r="L4" s="126"/>
+      <c r="M4" s="126"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A5" s="97"/>
       <c r="B5" s="31">
         <f>B4-B3</f>
         <v>8.3333333333334036E-2</v>
@@ -4110,64 +4110,64 @@
       <c r="L5" s="41"/>
       <c r="M5" s="42"/>
     </row>
-    <row r="6" spans="1:14" ht="15" customHeight="1">
-      <c r="A6" s="99">
+    <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="97">
         <v>44583</v>
       </c>
       <c r="B6" s="23">
         <v>0.79166666666666696</v>
       </c>
-      <c r="C6" s="124" t="s">
+      <c r="C6" s="123" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="124"/>
+      <c r="D6" s="123"/>
       <c r="E6" s="24">
         <v>0.82291666666666696</v>
       </c>
-      <c r="F6" s="125" t="s">
+      <c r="F6" s="124" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="125"/>
+      <c r="G6" s="124"/>
       <c r="H6" s="25">
         <v>0.79166666666666696</v>
       </c>
-      <c r="I6" s="126" t="s">
+      <c r="I6" s="125" t="s">
         <v>22</v>
       </c>
-      <c r="J6" s="126"/>
+      <c r="J6" s="125"/>
       <c r="K6" s="43">
         <v>0.79166666666666696</v>
       </c>
-      <c r="L6" s="127" t="s">
+      <c r="L6" s="126" t="s">
         <v>22</v>
       </c>
-      <c r="M6" s="127"/>
-    </row>
-    <row r="7" spans="1:14">
-      <c r="A7" s="99"/>
+      <c r="M6" s="126"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A7" s="97"/>
       <c r="B7" s="27">
         <v>0.89791666666666703</v>
       </c>
-      <c r="C7" s="124"/>
-      <c r="D7" s="124"/>
+      <c r="C7" s="123"/>
+      <c r="D7" s="123"/>
       <c r="E7" s="28">
         <v>0.89791666666666703</v>
       </c>
-      <c r="F7" s="125"/>
-      <c r="G7" s="125"/>
+      <c r="F7" s="124"/>
+      <c r="G7" s="124"/>
       <c r="H7" s="29">
         <v>0.89583333333333304</v>
       </c>
-      <c r="I7" s="126"/>
-      <c r="J7" s="126"/>
+      <c r="I7" s="125"/>
+      <c r="J7" s="125"/>
       <c r="K7" s="30">
         <v>0.89791666666666703</v>
       </c>
-      <c r="L7" s="127"/>
-      <c r="M7" s="127"/>
-    </row>
-    <row r="8" spans="1:14">
-      <c r="A8" s="99"/>
+      <c r="L7" s="126"/>
+      <c r="M7" s="126"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A8" s="97"/>
       <c r="B8" s="31">
         <f>B7-B6</f>
         <v>0.10625000000000007</v>
@@ -4193,64 +4193,64 @@
       <c r="L8" s="45"/>
       <c r="M8" s="46"/>
     </row>
-    <row r="9" spans="1:14" ht="15" customHeight="1">
-      <c r="A9" s="99">
+    <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="97">
         <v>44584</v>
       </c>
       <c r="B9" s="23">
         <v>0.75694444444444398</v>
       </c>
-      <c r="C9" s="124" t="s">
+      <c r="C9" s="123" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="124"/>
+      <c r="D9" s="123"/>
       <c r="E9" s="24">
         <v>0.75694444444444398</v>
       </c>
-      <c r="F9" s="125" t="s">
+      <c r="F9" s="124" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="125"/>
+      <c r="G9" s="124"/>
       <c r="H9" s="25">
         <v>0.75694444444444398</v>
       </c>
-      <c r="I9" s="126" t="s">
+      <c r="I9" s="125" t="s">
         <v>23</v>
       </c>
-      <c r="J9" s="126"/>
+      <c r="J9" s="125"/>
       <c r="K9" s="47">
         <v>0.75694444444444398</v>
       </c>
-      <c r="L9" s="127" t="s">
+      <c r="L9" s="126" t="s">
         <v>23</v>
       </c>
-      <c r="M9" s="127"/>
-    </row>
-    <row r="10" spans="1:14">
-      <c r="A10" s="99"/>
+      <c r="M9" s="126"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A10" s="97"/>
       <c r="B10" s="27">
         <v>0.83541666666666703</v>
       </c>
-      <c r="C10" s="124"/>
-      <c r="D10" s="124"/>
+      <c r="C10" s="123"/>
+      <c r="D10" s="123"/>
       <c r="E10" s="28">
         <v>0.83541666666666703</v>
       </c>
-      <c r="F10" s="125"/>
-      <c r="G10" s="125"/>
+      <c r="F10" s="124"/>
+      <c r="G10" s="124"/>
       <c r="H10" s="29">
         <v>0.83541666666666703</v>
       </c>
-      <c r="I10" s="126"/>
-      <c r="J10" s="126"/>
+      <c r="I10" s="125"/>
+      <c r="J10" s="125"/>
       <c r="K10" s="30">
         <v>0.83541666666666703</v>
       </c>
-      <c r="L10" s="127"/>
-      <c r="M10" s="127"/>
-    </row>
-    <row r="11" spans="1:14">
-      <c r="A11" s="99"/>
+      <c r="L10" s="126"/>
+      <c r="M10" s="126"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A11" s="97"/>
       <c r="B11" s="31">
         <f>(B10-B9)</f>
         <v>7.8472222222223054E-2</v>
@@ -4276,46 +4276,46 @@
       <c r="L11" s="45"/>
       <c r="M11" s="46"/>
     </row>
-    <row r="12" spans="1:14" ht="15" customHeight="1">
-      <c r="A12" s="99"/>
+    <row r="12" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="97"/>
       <c r="B12" s="23"/>
-      <c r="C12" s="124" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="124"/>
+      <c r="C12" s="123" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="123"/>
       <c r="E12" s="24"/>
-      <c r="F12" s="125" t="s">
-        <v>12</v>
-      </c>
-      <c r="G12" s="125"/>
+      <c r="F12" s="124" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="124"/>
       <c r="H12" s="25"/>
-      <c r="I12" s="126" t="s">
-        <v>12</v>
-      </c>
-      <c r="J12" s="126"/>
+      <c r="I12" s="125" t="s">
+        <v>12</v>
+      </c>
+      <c r="J12" s="125"/>
       <c r="K12" s="47"/>
-      <c r="L12" s="127" t="s">
-        <v>12</v>
-      </c>
-      <c r="M12" s="127"/>
-    </row>
-    <row r="13" spans="1:14">
-      <c r="A13" s="99"/>
+      <c r="L12" s="126" t="s">
+        <v>12</v>
+      </c>
+      <c r="M12" s="126"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A13" s="97"/>
       <c r="B13" s="27"/>
-      <c r="C13" s="124"/>
-      <c r="D13" s="124"/>
+      <c r="C13" s="123"/>
+      <c r="D13" s="123"/>
       <c r="E13" s="28"/>
-      <c r="F13" s="125"/>
-      <c r="G13" s="125"/>
+      <c r="F13" s="124"/>
+      <c r="G13" s="124"/>
       <c r="H13" s="29"/>
-      <c r="I13" s="126"/>
-      <c r="J13" s="126"/>
+      <c r="I13" s="125"/>
+      <c r="J13" s="125"/>
       <c r="K13" s="48"/>
-      <c r="L13" s="127"/>
-      <c r="M13" s="127"/>
-    </row>
-    <row r="14" spans="1:14">
-      <c r="A14" s="99"/>
+      <c r="L13" s="126"/>
+      <c r="M13" s="126"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A14" s="97"/>
       <c r="B14" s="31">
         <f>(B13-B12)</f>
         <v>0</v>
@@ -4341,46 +4341,46 @@
       <c r="L14" s="49"/>
       <c r="M14" s="50"/>
     </row>
-    <row r="15" spans="1:14" ht="15" customHeight="1">
-      <c r="A15" s="99"/>
+    <row r="15" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="97"/>
       <c r="B15" s="23"/>
-      <c r="C15" s="124" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" s="124"/>
+      <c r="C15" s="123" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="123"/>
       <c r="E15" s="24"/>
-      <c r="F15" s="125" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" s="125"/>
+      <c r="F15" s="124" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="124"/>
       <c r="H15" s="25"/>
-      <c r="I15" s="126" t="s">
-        <v>12</v>
-      </c>
-      <c r="J15" s="126"/>
+      <c r="I15" s="125" t="s">
+        <v>12</v>
+      </c>
+      <c r="J15" s="125"/>
       <c r="K15" s="26"/>
-      <c r="L15" s="127" t="s">
-        <v>12</v>
-      </c>
-      <c r="M15" s="127"/>
-    </row>
-    <row r="16" spans="1:14">
-      <c r="A16" s="99"/>
+      <c r="L15" s="126" t="s">
+        <v>12</v>
+      </c>
+      <c r="M15" s="126"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A16" s="97"/>
       <c r="B16" s="27"/>
-      <c r="C16" s="124"/>
-      <c r="D16" s="124"/>
+      <c r="C16" s="123"/>
+      <c r="D16" s="123"/>
       <c r="E16" s="28"/>
-      <c r="F16" s="125"/>
-      <c r="G16" s="125"/>
+      <c r="F16" s="124"/>
+      <c r="G16" s="124"/>
       <c r="H16" s="29"/>
-      <c r="I16" s="126"/>
-      <c r="J16" s="126"/>
+      <c r="I16" s="125"/>
+      <c r="J16" s="125"/>
       <c r="K16" s="30"/>
-      <c r="L16" s="127"/>
-      <c r="M16" s="127"/>
-    </row>
-    <row r="17" spans="1:13">
-      <c r="A17" s="99"/>
+      <c r="L16" s="126"/>
+      <c r="M16" s="126"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A17" s="97"/>
       <c r="B17" s="31">
         <f>(B16-B15)</f>
         <v>0</v>
@@ -4406,46 +4406,46 @@
       <c r="L17" s="45"/>
       <c r="M17" s="46"/>
     </row>
-    <row r="18" spans="1:13" ht="15" customHeight="1">
-      <c r="A18" s="99"/>
+    <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="97"/>
       <c r="B18" s="23"/>
-      <c r="C18" s="124" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" s="124"/>
+      <c r="C18" s="123" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="123"/>
       <c r="E18" s="24"/>
-      <c r="F18" s="125" t="s">
-        <v>12</v>
-      </c>
-      <c r="G18" s="125"/>
+      <c r="F18" s="124" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="124"/>
       <c r="H18" s="25"/>
-      <c r="I18" s="126" t="s">
-        <v>12</v>
-      </c>
-      <c r="J18" s="126"/>
+      <c r="I18" s="125" t="s">
+        <v>12</v>
+      </c>
+      <c r="J18" s="125"/>
       <c r="K18" s="47"/>
-      <c r="L18" s="127" t="s">
-        <v>12</v>
-      </c>
-      <c r="M18" s="127"/>
-    </row>
-    <row r="19" spans="1:13">
-      <c r="A19" s="99"/>
+      <c r="L18" s="126" t="s">
+        <v>12</v>
+      </c>
+      <c r="M18" s="126"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A19" s="97"/>
       <c r="B19" s="27"/>
-      <c r="C19" s="124"/>
-      <c r="D19" s="124"/>
+      <c r="C19" s="123"/>
+      <c r="D19" s="123"/>
       <c r="E19" s="28"/>
-      <c r="F19" s="125"/>
-      <c r="G19" s="125"/>
+      <c r="F19" s="124"/>
+      <c r="G19" s="124"/>
       <c r="H19" s="29"/>
-      <c r="I19" s="126"/>
-      <c r="J19" s="126"/>
+      <c r="I19" s="125"/>
+      <c r="J19" s="125"/>
       <c r="K19" s="30"/>
-      <c r="L19" s="127"/>
-      <c r="M19" s="127"/>
-    </row>
-    <row r="20" spans="1:13">
-      <c r="A20" s="99"/>
+      <c r="L19" s="126"/>
+      <c r="M19" s="126"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A20" s="97"/>
       <c r="B20" s="31">
         <f>(B19-B18)</f>
         <v>0</v>
@@ -4471,46 +4471,46 @@
       <c r="L20" s="45"/>
       <c r="M20" s="46"/>
     </row>
-    <row r="21" spans="1:13" ht="15" customHeight="1">
-      <c r="A21" s="99"/>
+    <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="97"/>
       <c r="B21" s="23"/>
-      <c r="C21" s="124" t="s">
-        <v>12</v>
-      </c>
-      <c r="D21" s="124"/>
+      <c r="C21" s="123" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="123"/>
       <c r="E21" s="24"/>
-      <c r="F21" s="125" t="s">
-        <v>12</v>
-      </c>
-      <c r="G21" s="125"/>
+      <c r="F21" s="124" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" s="124"/>
       <c r="H21" s="25"/>
-      <c r="I21" s="126" t="s">
-        <v>12</v>
-      </c>
-      <c r="J21" s="126"/>
+      <c r="I21" s="125" t="s">
+        <v>12</v>
+      </c>
+      <c r="J21" s="125"/>
       <c r="K21" s="26"/>
-      <c r="L21" s="127" t="s">
-        <v>12</v>
-      </c>
-      <c r="M21" s="127"/>
-    </row>
-    <row r="22" spans="1:13">
-      <c r="A22" s="99"/>
+      <c r="L21" s="126" t="s">
+        <v>12</v>
+      </c>
+      <c r="M21" s="126"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A22" s="97"/>
       <c r="B22" s="27"/>
-      <c r="C22" s="124"/>
-      <c r="D22" s="124"/>
+      <c r="C22" s="123"/>
+      <c r="D22" s="123"/>
       <c r="E22" s="28"/>
-      <c r="F22" s="125"/>
-      <c r="G22" s="125"/>
+      <c r="F22" s="124"/>
+      <c r="G22" s="124"/>
       <c r="H22" s="29"/>
-      <c r="I22" s="126"/>
-      <c r="J22" s="126"/>
+      <c r="I22" s="125"/>
+      <c r="J22" s="125"/>
       <c r="K22" s="48"/>
-      <c r="L22" s="127"/>
-      <c r="M22" s="127"/>
-    </row>
-    <row r="23" spans="1:13">
-      <c r="A23" s="99"/>
+      <c r="L22" s="126"/>
+      <c r="M22" s="126"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A23" s="97"/>
       <c r="B23" s="31">
         <f>(B22-B21)</f>
         <v>0</v>
@@ -4536,7 +4536,7 @@
       <c r="L23" s="51"/>
       <c r="M23" s="52"/>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A30" s="21" t="s">
         <v>2</v>
       </c>
@@ -4545,7 +4545,7 @@
         <v>1.0388888888888945</v>
       </c>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A31" s="21" t="s">
         <v>10</v>
       </c>
@@ -4556,42 +4556,42 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="C21:D22"/>
-    <mergeCell ref="F21:G22"/>
-    <mergeCell ref="I21:J22"/>
-    <mergeCell ref="L21:M22"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="C18:D19"/>
-    <mergeCell ref="F18:G19"/>
-    <mergeCell ref="I18:J19"/>
-    <mergeCell ref="L18:M19"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="C15:D16"/>
-    <mergeCell ref="F15:G16"/>
-    <mergeCell ref="I15:J16"/>
-    <mergeCell ref="L15:M16"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="C12:D13"/>
-    <mergeCell ref="F12:G13"/>
-    <mergeCell ref="I12:J13"/>
-    <mergeCell ref="L12:M13"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="C9:D10"/>
-    <mergeCell ref="F9:G10"/>
-    <mergeCell ref="I9:J10"/>
-    <mergeCell ref="L9:M10"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="C3:D4"/>
+    <mergeCell ref="F3:G4"/>
+    <mergeCell ref="I3:J4"/>
     <mergeCell ref="L3:M4"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="C6:D7"/>
     <mergeCell ref="F6:G7"/>
     <mergeCell ref="I6:J7"/>
     <mergeCell ref="L6:M7"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="C3:D4"/>
-    <mergeCell ref="F3:G4"/>
-    <mergeCell ref="I3:J4"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="C9:D10"/>
+    <mergeCell ref="F9:G10"/>
+    <mergeCell ref="I9:J10"/>
+    <mergeCell ref="L9:M10"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="C12:D13"/>
+    <mergeCell ref="F12:G13"/>
+    <mergeCell ref="I12:J13"/>
+    <mergeCell ref="L12:M13"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="C15:D16"/>
+    <mergeCell ref="F15:G16"/>
+    <mergeCell ref="I15:J16"/>
+    <mergeCell ref="L15:M16"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="C18:D19"/>
+    <mergeCell ref="F18:G19"/>
+    <mergeCell ref="I18:J19"/>
+    <mergeCell ref="L18:M19"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="C21:D22"/>
+    <mergeCell ref="F21:G22"/>
+    <mergeCell ref="I21:J22"/>
+    <mergeCell ref="L21:M22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -4602,27 +4602,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:O41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L33" sqref="L33:M34"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.69140625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" customWidth="1"/>
-    <col min="3" max="4" width="13.7109375" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="6" max="7" width="13.7109375" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" customWidth="1"/>
-    <col min="9" max="10" width="13.7109375" customWidth="1"/>
-    <col min="11" max="11" width="15.140625" customWidth="1"/>
-    <col min="12" max="13" width="13.7109375" customWidth="1"/>
-    <col min="14" max="14" width="19.7109375" customWidth="1"/>
-    <col min="15" max="15" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="15.3046875" customWidth="1"/>
+    <col min="2" max="2" width="15.15234375" customWidth="1"/>
+    <col min="3" max="4" width="13.69140625" customWidth="1"/>
+    <col min="5" max="5" width="16.15234375" customWidth="1"/>
+    <col min="6" max="7" width="13.69140625" customWidth="1"/>
+    <col min="8" max="8" width="15.15234375" customWidth="1"/>
+    <col min="9" max="10" width="13.69140625" customWidth="1"/>
+    <col min="11" max="11" width="15.15234375" customWidth="1"/>
+    <col min="12" max="13" width="13.69140625" customWidth="1"/>
+    <col min="14" max="14" width="19.69140625" customWidth="1"/>
+    <col min="15" max="15" width="17.84375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
-      <c r="A1" s="97" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A1" s="102" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -4661,23 +4661,23 @@
       <c r="M1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="98" t="s">
+      <c r="N1" s="103" t="s">
         <v>4</v>
       </c>
-      <c r="O1" s="98"/>
-    </row>
-    <row r="2" spans="1:15">
-      <c r="A2" s="97"/>
+      <c r="O1" s="103"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A2" s="102"/>
       <c r="B2" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="10">
         <f t="array" ref="C2">SUM(B5:B41*(MOD(ROW(B5:B41)-2,3)=0))</f>
-        <v>0.88541666666666707</v>
+        <v>0.97569444444444486</v>
       </c>
       <c r="D2" s="11">
         <f>C2+Sprint_3!D2</f>
-        <v>2.2493055555555581</v>
+        <v>2.3395833333333362</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>6</v>
@@ -4717,74 +4717,74 @@
       </c>
       <c r="O2" s="22">
         <f>C2+F2+I2+L2</f>
-        <v>3.5486111111111143</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="15" customHeight="1">
-      <c r="A3" s="99">
+        <v>3.6388888888888928</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="97">
         <v>44585</v>
       </c>
       <c r="B3" s="23">
         <v>0.33333333333333298</v>
       </c>
-      <c r="C3" s="100" t="s">
+      <c r="C3" s="98" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="100"/>
+      <c r="D3" s="98"/>
       <c r="E3" s="24">
         <v>0.33333333333333298</v>
       </c>
-      <c r="F3" s="101" t="s">
+      <c r="F3" s="99" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="101"/>
+      <c r="G3" s="99"/>
       <c r="H3" s="25">
         <v>0.33333333333333298</v>
       </c>
-      <c r="I3" s="102" t="s">
+      <c r="I3" s="100" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="102"/>
+      <c r="J3" s="100"/>
       <c r="K3" s="26">
         <v>0.33333333333333298</v>
       </c>
-      <c r="L3" s="103" t="s">
+      <c r="L3" s="101" t="s">
         <v>24</v>
       </c>
-      <c r="M3" s="103"/>
+      <c r="M3" s="101"/>
       <c r="N3" s="21" t="s">
         <v>10</v>
       </c>
       <c r="O3" s="22">
         <f>D2+G2+J2+M2</f>
-        <v>8.5166666666666835</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15">
-      <c r="A4" s="99"/>
+        <v>8.6069444444444603</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A4" s="97"/>
       <c r="B4" s="27">
         <v>0.41666666666666702</v>
       </c>
-      <c r="C4" s="100"/>
-      <c r="D4" s="100"/>
+      <c r="C4" s="98"/>
+      <c r="D4" s="98"/>
       <c r="E4" s="28">
         <v>0.41666666666666702</v>
       </c>
-      <c r="F4" s="101"/>
-      <c r="G4" s="101"/>
+      <c r="F4" s="99"/>
+      <c r="G4" s="99"/>
       <c r="H4" s="29">
         <v>0.41666666666666702</v>
       </c>
-      <c r="I4" s="102"/>
-      <c r="J4" s="102"/>
+      <c r="I4" s="100"/>
+      <c r="J4" s="100"/>
       <c r="K4" s="30">
         <v>0.41666666666666702</v>
       </c>
-      <c r="L4" s="103"/>
-      <c r="M4" s="103"/>
-    </row>
-    <row r="5" spans="1:15">
-      <c r="A5" s="99"/>
+      <c r="L4" s="101"/>
+      <c r="M4" s="101"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A5" s="97"/>
       <c r="B5" s="31">
         <f>B4-B3</f>
         <v>8.3333333333334036E-2</v>
@@ -4810,64 +4810,64 @@
       <c r="L5" s="41"/>
       <c r="M5" s="42"/>
     </row>
-    <row r="6" spans="1:15" ht="15" customHeight="1">
-      <c r="A6" s="99">
+    <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="97">
         <v>44585</v>
       </c>
       <c r="B6" s="23">
         <v>0.6875</v>
       </c>
-      <c r="C6" s="100" t="s">
+      <c r="C6" s="98" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="100"/>
+      <c r="D6" s="98"/>
       <c r="E6" s="24">
         <v>0.6875</v>
       </c>
-      <c r="F6" s="101" t="s">
+      <c r="F6" s="99" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="101"/>
+      <c r="G6" s="99"/>
       <c r="H6" s="25">
         <v>0.6875</v>
       </c>
-      <c r="I6" s="102" t="s">
+      <c r="I6" s="100" t="s">
         <v>25</v>
       </c>
-      <c r="J6" s="102"/>
+      <c r="J6" s="100"/>
       <c r="K6" s="43">
         <v>0.6875</v>
       </c>
-      <c r="L6" s="103" t="s">
+      <c r="L6" s="101" t="s">
         <v>26</v>
       </c>
-      <c r="M6" s="103"/>
-    </row>
-    <row r="7" spans="1:15">
-      <c r="A7" s="99"/>
+      <c r="M6" s="101"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A7" s="97"/>
       <c r="B7" s="27">
         <v>0.71875</v>
       </c>
-      <c r="C7" s="100"/>
-      <c r="D7" s="100"/>
+      <c r="C7" s="98"/>
+      <c r="D7" s="98"/>
       <c r="E7" s="28">
         <v>0.71875</v>
       </c>
-      <c r="F7" s="101"/>
-      <c r="G7" s="101"/>
+      <c r="F7" s="99"/>
+      <c r="G7" s="99"/>
       <c r="H7" s="29">
         <v>0.71875</v>
       </c>
-      <c r="I7" s="102"/>
-      <c r="J7" s="102"/>
+      <c r="I7" s="100"/>
+      <c r="J7" s="100"/>
       <c r="K7" s="30">
         <v>0.71875</v>
       </c>
-      <c r="L7" s="103"/>
-      <c r="M7" s="103"/>
-    </row>
-    <row r="8" spans="1:15">
-      <c r="A8" s="99"/>
+      <c r="L7" s="101"/>
+      <c r="M7" s="101"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A8" s="97"/>
       <c r="B8" s="31">
         <f>B7-B6</f>
         <v>3.125E-2</v>
@@ -4893,52 +4893,52 @@
       <c r="L8" s="45"/>
       <c r="M8" s="46"/>
     </row>
-    <row r="9" spans="1:15" ht="15" customHeight="1">
-      <c r="A9" s="99">
+    <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="97">
         <v>44586</v>
       </c>
       <c r="B9" s="23">
         <v>0.58333333333333304</v>
       </c>
-      <c r="C9" s="100" t="s">
+      <c r="C9" s="98" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="100"/>
+      <c r="D9" s="98"/>
       <c r="E9" s="24"/>
-      <c r="F9" s="101" t="s">
+      <c r="F9" s="99" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="101"/>
+      <c r="G9" s="99"/>
       <c r="H9" s="25"/>
-      <c r="I9" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="J9" s="102"/>
+      <c r="I9" s="100" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" s="100"/>
       <c r="K9" s="47"/>
-      <c r="L9" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="M9" s="103"/>
-    </row>
-    <row r="10" spans="1:15">
-      <c r="A10" s="99"/>
+      <c r="L9" s="101" t="s">
+        <v>11</v>
+      </c>
+      <c r="M9" s="101"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A10" s="97"/>
       <c r="B10" s="27">
         <v>0.6875</v>
       </c>
-      <c r="C10" s="100"/>
-      <c r="D10" s="100"/>
+      <c r="C10" s="98"/>
+      <c r="D10" s="98"/>
       <c r="E10" s="28"/>
-      <c r="F10" s="101"/>
-      <c r="G10" s="101"/>
+      <c r="F10" s="99"/>
+      <c r="G10" s="99"/>
       <c r="H10" s="29"/>
-      <c r="I10" s="102"/>
-      <c r="J10" s="102"/>
+      <c r="I10" s="100"/>
+      <c r="J10" s="100"/>
       <c r="K10" s="30"/>
-      <c r="L10" s="103"/>
-      <c r="M10" s="103"/>
-    </row>
-    <row r="11" spans="1:15">
-      <c r="A11" s="99"/>
+      <c r="L10" s="101"/>
+      <c r="M10" s="101"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A11" s="97"/>
       <c r="B11" s="31">
         <f>(B10-B9)</f>
         <v>0.10416666666666696</v>
@@ -4964,52 +4964,52 @@
       <c r="L11" s="45"/>
       <c r="M11" s="46"/>
     </row>
-    <row r="12" spans="1:15" ht="15" customHeight="1">
-      <c r="A12" s="99">
+    <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="97">
         <v>44588</v>
       </c>
       <c r="B12" s="23">
         <v>0.85416666666666696</v>
       </c>
-      <c r="C12" s="100" t="s">
+      <c r="C12" s="98" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="100"/>
+      <c r="D12" s="98"/>
       <c r="E12" s="24"/>
-      <c r="F12" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" s="101"/>
+      <c r="F12" s="99" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="99"/>
       <c r="H12" s="25"/>
-      <c r="I12" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="J12" s="102"/>
+      <c r="I12" s="100" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" s="100"/>
       <c r="K12" s="47"/>
-      <c r="L12" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="M12" s="103"/>
-    </row>
-    <row r="13" spans="1:15">
-      <c r="A13" s="99"/>
+      <c r="L12" s="101" t="s">
+        <v>11</v>
+      </c>
+      <c r="M12" s="101"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A13" s="97"/>
       <c r="B13" s="27">
         <v>0.89583333333333304</v>
       </c>
-      <c r="C13" s="100"/>
-      <c r="D13" s="100"/>
+      <c r="C13" s="98"/>
+      <c r="D13" s="98"/>
       <c r="E13" s="28"/>
-      <c r="F13" s="101"/>
-      <c r="G13" s="101"/>
+      <c r="F13" s="99"/>
+      <c r="G13" s="99"/>
       <c r="H13" s="29"/>
-      <c r="I13" s="102"/>
-      <c r="J13" s="102"/>
+      <c r="I13" s="100"/>
+      <c r="J13" s="100"/>
       <c r="K13" s="48"/>
-      <c r="L13" s="103"/>
-      <c r="M13" s="103"/>
-    </row>
-    <row r="14" spans="1:15">
-      <c r="A14" s="99"/>
+      <c r="L13" s="101"/>
+      <c r="M13" s="101"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A14" s="97"/>
       <c r="B14" s="31">
         <f>(B13-B12)</f>
         <v>4.1666666666666075E-2</v>
@@ -5035,52 +5035,52 @@
       <c r="L14" s="49"/>
       <c r="M14" s="50"/>
     </row>
-    <row r="15" spans="1:15" ht="13.9" customHeight="1">
-      <c r="A15" s="99">
+    <row r="15" spans="1:15" ht="13.95" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="97">
         <v>44591</v>
       </c>
       <c r="B15" s="23"/>
-      <c r="C15" s="100" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="100"/>
+      <c r="C15" s="98" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="98"/>
       <c r="E15" s="24"/>
-      <c r="F15" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="G15" s="101"/>
+      <c r="F15" s="99" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="99"/>
       <c r="H15" s="25"/>
-      <c r="I15" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="J15" s="102"/>
+      <c r="I15" s="100" t="s">
+        <v>11</v>
+      </c>
+      <c r="J15" s="100"/>
       <c r="K15" s="26">
         <v>0.33333333333333298</v>
       </c>
-      <c r="L15" s="103" t="s">
+      <c r="L15" s="101" t="s">
         <v>29</v>
       </c>
-      <c r="M15" s="103"/>
-    </row>
-    <row r="16" spans="1:15">
-      <c r="A16" s="99"/>
+      <c r="M15" s="101"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A16" s="97"/>
       <c r="B16" s="27"/>
-      <c r="C16" s="100"/>
-      <c r="D16" s="100"/>
+      <c r="C16" s="98"/>
+      <c r="D16" s="98"/>
       <c r="E16" s="28"/>
-      <c r="F16" s="101"/>
-      <c r="G16" s="101"/>
+      <c r="F16" s="99"/>
+      <c r="G16" s="99"/>
       <c r="H16" s="29"/>
-      <c r="I16" s="102"/>
-      <c r="J16" s="102"/>
+      <c r="I16" s="100"/>
+      <c r="J16" s="100"/>
       <c r="K16" s="30">
         <v>0.41666666666666702</v>
       </c>
-      <c r="L16" s="103"/>
-      <c r="M16" s="103"/>
-    </row>
-    <row r="17" spans="1:13">
-      <c r="A17" s="99"/>
+      <c r="L16" s="101"/>
+      <c r="M16" s="101"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A17" s="97"/>
       <c r="B17" s="31">
         <f>(B16-B15)</f>
         <v>0</v>
@@ -5106,64 +5106,64 @@
       <c r="L17" s="45"/>
       <c r="M17" s="46"/>
     </row>
-    <row r="18" spans="1:13" ht="15" customHeight="1">
-      <c r="A18" s="99">
+    <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="97">
         <v>44591</v>
       </c>
       <c r="B18" s="23">
         <v>0.70833333333333337</v>
       </c>
-      <c r="C18" s="100" t="s">
+      <c r="C18" s="98" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="100"/>
+      <c r="D18" s="98"/>
       <c r="E18" s="24">
         <v>0.70833333333333337</v>
       </c>
-      <c r="F18" s="101" t="s">
+      <c r="F18" s="99" t="s">
         <v>31</v>
       </c>
-      <c r="G18" s="101"/>
+      <c r="G18" s="99"/>
       <c r="H18" s="25">
         <v>0.61805555555555558</v>
       </c>
-      <c r="I18" s="102" t="s">
+      <c r="I18" s="100" t="s">
         <v>32</v>
       </c>
-      <c r="J18" s="102"/>
+      <c r="J18" s="100"/>
       <c r="K18" s="47">
         <v>0.70833333333333337</v>
       </c>
-      <c r="L18" s="103" t="s">
+      <c r="L18" s="101" t="s">
         <v>30</v>
       </c>
-      <c r="M18" s="103"/>
-    </row>
-    <row r="19" spans="1:13">
-      <c r="A19" s="99"/>
+      <c r="M18" s="101"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A19" s="97"/>
       <c r="B19" s="27">
         <v>0.92708333333333337</v>
       </c>
-      <c r="C19" s="100"/>
-      <c r="D19" s="100"/>
+      <c r="C19" s="98"/>
+      <c r="D19" s="98"/>
       <c r="E19" s="28">
         <v>0.92708333333333337</v>
       </c>
-      <c r="F19" s="101"/>
-      <c r="G19" s="101"/>
+      <c r="F19" s="99"/>
+      <c r="G19" s="99"/>
       <c r="H19" s="29">
         <v>0.92708333333333337</v>
       </c>
-      <c r="I19" s="102"/>
-      <c r="J19" s="102"/>
+      <c r="I19" s="100"/>
+      <c r="J19" s="100"/>
       <c r="K19" s="30">
         <v>0.92708333333333337</v>
       </c>
-      <c r="L19" s="103"/>
-      <c r="M19" s="103"/>
-    </row>
-    <row r="20" spans="1:13">
-      <c r="A20" s="99"/>
+      <c r="L19" s="101"/>
+      <c r="M19" s="101"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A20" s="97"/>
       <c r="B20" s="31">
         <f>(B19-B18)</f>
         <v>0.21875</v>
@@ -5189,64 +5189,64 @@
       <c r="L20" s="45"/>
       <c r="M20" s="46"/>
     </row>
-    <row r="21" spans="1:13" ht="15" customHeight="1">
-      <c r="A21" s="99">
+    <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="97">
         <v>44592</v>
       </c>
       <c r="B21" s="23">
         <v>0.375</v>
       </c>
-      <c r="C21" s="100" t="s">
+      <c r="C21" s="98" t="s">
         <v>30</v>
       </c>
-      <c r="D21" s="100"/>
+      <c r="D21" s="98"/>
       <c r="E21" s="24">
         <v>0.375</v>
       </c>
-      <c r="F21" s="101" t="s">
+      <c r="F21" s="99" t="s">
         <v>31</v>
       </c>
-      <c r="G21" s="101"/>
+      <c r="G21" s="99"/>
       <c r="H21" s="25">
         <v>0.375</v>
       </c>
-      <c r="I21" s="102" t="s">
+      <c r="I21" s="100" t="s">
         <v>32</v>
       </c>
-      <c r="J21" s="102"/>
+      <c r="J21" s="100"/>
       <c r="K21" s="26">
         <v>0.375</v>
       </c>
-      <c r="L21" s="103" t="s">
+      <c r="L21" s="101" t="s">
         <v>30</v>
       </c>
-      <c r="M21" s="103"/>
-    </row>
-    <row r="22" spans="1:13">
-      <c r="A22" s="99"/>
+      <c r="M21" s="101"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A22" s="97"/>
       <c r="B22" s="27">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C22" s="100"/>
-      <c r="D22" s="100"/>
+      <c r="C22" s="98"/>
+      <c r="D22" s="98"/>
       <c r="E22" s="28">
         <v>0.41666666666666669</v>
       </c>
-      <c r="F22" s="101"/>
-      <c r="G22" s="101"/>
+      <c r="F22" s="99"/>
+      <c r="G22" s="99"/>
       <c r="H22" s="29">
         <v>0.41666666666666669</v>
       </c>
-      <c r="I22" s="102"/>
-      <c r="J22" s="102"/>
+      <c r="I22" s="100"/>
+      <c r="J22" s="100"/>
       <c r="K22" s="48">
         <v>0.41666666666666669</v>
       </c>
-      <c r="L22" s="103"/>
-      <c r="M22" s="103"/>
-    </row>
-    <row r="23" spans="1:13">
-      <c r="A23" s="99"/>
+      <c r="L22" s="101"/>
+      <c r="M22" s="101"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A23" s="97"/>
       <c r="B23" s="31">
         <f>(B22-B21)</f>
         <v>4.1666666666666685E-2</v>
@@ -5272,64 +5272,64 @@
       <c r="L23" s="51"/>
       <c r="M23" s="52"/>
     </row>
-    <row r="24" spans="1:13" ht="15" customHeight="1">
-      <c r="A24" s="99">
+    <row r="24" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="97">
         <v>44592</v>
       </c>
       <c r="B24" s="23">
         <v>0.625</v>
       </c>
-      <c r="C24" s="100" t="s">
+      <c r="C24" s="98" t="s">
         <v>30</v>
       </c>
-      <c r="D24" s="100"/>
+      <c r="D24" s="98"/>
       <c r="E24" s="24">
         <v>0.625</v>
       </c>
-      <c r="F24" s="101" t="s">
+      <c r="F24" s="99" t="s">
         <v>31</v>
       </c>
-      <c r="G24" s="101"/>
+      <c r="G24" s="99"/>
       <c r="H24" s="25">
         <v>0.625</v>
       </c>
-      <c r="I24" s="102" t="s">
+      <c r="I24" s="100" t="s">
         <v>33</v>
       </c>
-      <c r="J24" s="102"/>
+      <c r="J24" s="100"/>
       <c r="K24" s="26">
         <v>0.625</v>
       </c>
-      <c r="L24" s="103" t="s">
+      <c r="L24" s="101" t="s">
         <v>34</v>
       </c>
-      <c r="M24" s="103"/>
-    </row>
-    <row r="25" spans="1:13">
-      <c r="A25" s="99"/>
+      <c r="M24" s="101"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A25" s="97"/>
       <c r="B25" s="27">
         <v>0.75</v>
       </c>
-      <c r="C25" s="100"/>
-      <c r="D25" s="100"/>
+      <c r="C25" s="98"/>
+      <c r="D25" s="98"/>
       <c r="E25" s="28">
         <v>0.75</v>
       </c>
-      <c r="F25" s="101"/>
-      <c r="G25" s="101"/>
+      <c r="F25" s="99"/>
+      <c r="G25" s="99"/>
       <c r="H25" s="29">
         <v>0.70833333333333337</v>
       </c>
-      <c r="I25" s="102"/>
-      <c r="J25" s="102"/>
+      <c r="I25" s="100"/>
+      <c r="J25" s="100"/>
       <c r="K25" s="30">
         <v>0.75</v>
       </c>
-      <c r="L25" s="103"/>
-      <c r="M25" s="103"/>
-    </row>
-    <row r="26" spans="1:13">
-      <c r="A26" s="99"/>
+      <c r="L25" s="101"/>
+      <c r="M25" s="101"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A26" s="97"/>
       <c r="B26" s="31">
         <f>(B25-B24)</f>
         <v>0.125</v>
@@ -5355,64 +5355,64 @@
       <c r="L26" s="45"/>
       <c r="M26" s="46"/>
     </row>
-    <row r="27" spans="1:13" ht="15" customHeight="1">
-      <c r="A27" s="99">
+    <row r="27" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="97">
         <v>44594</v>
       </c>
       <c r="B27" s="23">
         <v>0.5</v>
       </c>
-      <c r="C27" s="100" t="s">
-        <v>11</v>
-      </c>
-      <c r="D27" s="100"/>
+      <c r="C27" s="98" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="98"/>
       <c r="E27" s="24">
         <v>0.5</v>
       </c>
-      <c r="F27" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="G27" s="101"/>
+      <c r="F27" s="99" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" s="99"/>
       <c r="H27" s="25">
         <v>0.5</v>
       </c>
-      <c r="I27" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="J27" s="102"/>
+      <c r="I27" s="100" t="s">
+        <v>11</v>
+      </c>
+      <c r="J27" s="100"/>
       <c r="K27" s="47">
         <v>0.5</v>
       </c>
-      <c r="L27" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="M27" s="103"/>
-    </row>
-    <row r="28" spans="1:13">
-      <c r="A28" s="99"/>
+      <c r="L27" s="101" t="s">
+        <v>11</v>
+      </c>
+      <c r="M27" s="101"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A28" s="97"/>
       <c r="B28" s="27">
         <v>0.53125</v>
       </c>
-      <c r="C28" s="100"/>
-      <c r="D28" s="100"/>
+      <c r="C28" s="98"/>
+      <c r="D28" s="98"/>
       <c r="E28" s="28">
         <v>0.53125</v>
       </c>
-      <c r="F28" s="101"/>
-      <c r="G28" s="101"/>
+      <c r="F28" s="99"/>
+      <c r="G28" s="99"/>
       <c r="H28" s="29">
         <v>0.53125</v>
       </c>
-      <c r="I28" s="102"/>
-      <c r="J28" s="102"/>
+      <c r="I28" s="100"/>
+      <c r="J28" s="100"/>
       <c r="K28" s="30">
         <v>0.53125</v>
       </c>
-      <c r="L28" s="103"/>
-      <c r="M28" s="103"/>
-    </row>
-    <row r="29" spans="1:13">
-      <c r="A29" s="99"/>
+      <c r="L28" s="101"/>
+      <c r="M28" s="101"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A29" s="97"/>
       <c r="B29" s="31">
         <f>(B28-B27)</f>
         <v>3.125E-2</v>
@@ -5438,64 +5438,64 @@
       <c r="L29" s="45"/>
       <c r="M29" s="46"/>
     </row>
-    <row r="30" spans="1:13" ht="15" customHeight="1">
-      <c r="A30" s="99">
+    <row r="30" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="97">
         <v>44597</v>
       </c>
       <c r="B30" s="23">
         <v>0.75</v>
       </c>
-      <c r="C30" s="100" t="s">
-        <v>11</v>
-      </c>
-      <c r="D30" s="100"/>
+      <c r="C30" s="98" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" s="98"/>
       <c r="E30" s="24">
         <v>0.75</v>
       </c>
-      <c r="F30" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="G30" s="101"/>
+      <c r="F30" s="99" t="s">
+        <v>11</v>
+      </c>
+      <c r="G30" s="99"/>
       <c r="H30" s="25">
         <v>0.75</v>
       </c>
-      <c r="I30" s="102" t="s">
+      <c r="I30" s="100" t="s">
         <v>35</v>
       </c>
-      <c r="J30" s="102"/>
+      <c r="J30" s="100"/>
       <c r="K30" s="26">
         <v>0.75</v>
       </c>
-      <c r="L30" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="M30" s="103"/>
-    </row>
-    <row r="31" spans="1:13">
-      <c r="A31" s="99"/>
+      <c r="L30" s="101" t="s">
+        <v>11</v>
+      </c>
+      <c r="M30" s="101"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A31" s="97"/>
       <c r="B31" s="27">
         <v>0.95833333333333337</v>
       </c>
-      <c r="C31" s="100"/>
-      <c r="D31" s="100"/>
+      <c r="C31" s="98"/>
+      <c r="D31" s="98"/>
       <c r="E31" s="28">
         <v>0.95833333333333337</v>
       </c>
-      <c r="F31" s="101"/>
-      <c r="G31" s="101"/>
+      <c r="F31" s="99"/>
+      <c r="G31" s="99"/>
       <c r="H31" s="29">
         <v>0.9375</v>
       </c>
-      <c r="I31" s="102"/>
-      <c r="J31" s="102"/>
+      <c r="I31" s="100"/>
+      <c r="J31" s="100"/>
       <c r="K31" s="48">
         <v>0.95833333333333337</v>
       </c>
-      <c r="L31" s="103"/>
-      <c r="M31" s="103"/>
-    </row>
-    <row r="32" spans="1:13">
-      <c r="A32" s="99"/>
+      <c r="L31" s="101"/>
+      <c r="M31" s="101"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A32" s="97"/>
       <c r="B32" s="31">
         <f>(B31-B30)</f>
         <v>0.20833333333333337</v>
@@ -5521,55 +5521,59 @@
       <c r="L32" s="51"/>
       <c r="M32" s="52"/>
     </row>
-    <row r="33" spans="1:13" ht="15" customHeight="1">
-      <c r="A33" s="99">
+    <row r="33" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="97">
         <v>44598</v>
       </c>
-      <c r="B33" s="23"/>
-      <c r="C33" s="100" t="s">
-        <v>11</v>
-      </c>
-      <c r="D33" s="100"/>
+      <c r="B33" s="23">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="C33" s="98" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="98"/>
       <c r="E33" s="24"/>
-      <c r="F33" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="G33" s="101"/>
+      <c r="F33" s="99" t="s">
+        <v>11</v>
+      </c>
+      <c r="G33" s="99"/>
       <c r="H33" s="25"/>
-      <c r="I33" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="J33" s="102"/>
+      <c r="I33" s="100" t="s">
+        <v>11</v>
+      </c>
+      <c r="J33" s="100"/>
       <c r="K33" s="26">
         <v>0.41666666666666669</v>
       </c>
-      <c r="L33" s="103" t="s">
+      <c r="L33" s="101" t="s">
         <v>36</v>
       </c>
-      <c r="M33" s="103"/>
-    </row>
-    <row r="34" spans="1:13">
-      <c r="A34" s="99"/>
-      <c r="B34" s="27"/>
-      <c r="C34" s="100"/>
-      <c r="D34" s="100"/>
+      <c r="M33" s="101"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A34" s="97"/>
+      <c r="B34" s="27">
+        <v>0.98611111111111116</v>
+      </c>
+      <c r="C34" s="98"/>
+      <c r="D34" s="98"/>
       <c r="E34" s="28"/>
-      <c r="F34" s="101"/>
-      <c r="G34" s="101"/>
+      <c r="F34" s="99"/>
+      <c r="G34" s="99"/>
       <c r="H34" s="29"/>
-      <c r="I34" s="102"/>
-      <c r="J34" s="102"/>
+      <c r="I34" s="100"/>
+      <c r="J34" s="100"/>
       <c r="K34" s="30">
         <v>0.75</v>
       </c>
-      <c r="L34" s="103"/>
-      <c r="M34" s="103"/>
-    </row>
-    <row r="35" spans="1:13">
-      <c r="A35" s="99"/>
+      <c r="L34" s="101"/>
+      <c r="M34" s="101"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A35" s="97"/>
       <c r="B35" s="31">
         <f>(B34-B33)</f>
-        <v>0</v>
+        <v>9.027777777777779E-2</v>
       </c>
       <c r="C35" s="32"/>
       <c r="D35" s="33"/>
@@ -5592,46 +5596,46 @@
       <c r="L35" s="45"/>
       <c r="M35" s="46"/>
     </row>
-    <row r="36" spans="1:13" ht="15" customHeight="1">
-      <c r="A36" s="99"/>
+    <row r="36" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="97"/>
       <c r="B36" s="23"/>
-      <c r="C36" s="100" t="s">
-        <v>11</v>
-      </c>
-      <c r="D36" s="100"/>
+      <c r="C36" s="98" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" s="98"/>
       <c r="E36" s="24"/>
-      <c r="F36" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="G36" s="101"/>
+      <c r="F36" s="99" t="s">
+        <v>11</v>
+      </c>
+      <c r="G36" s="99"/>
       <c r="H36" s="25"/>
-      <c r="I36" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="J36" s="102"/>
+      <c r="I36" s="100" t="s">
+        <v>11</v>
+      </c>
+      <c r="J36" s="100"/>
       <c r="K36" s="47"/>
-      <c r="L36" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="M36" s="103"/>
-    </row>
-    <row r="37" spans="1:13">
-      <c r="A37" s="99"/>
+      <c r="L36" s="101" t="s">
+        <v>11</v>
+      </c>
+      <c r="M36" s="101"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A37" s="97"/>
       <c r="B37" s="27"/>
-      <c r="C37" s="100"/>
-      <c r="D37" s="100"/>
+      <c r="C37" s="98"/>
+      <c r="D37" s="98"/>
       <c r="E37" s="28"/>
-      <c r="F37" s="101"/>
-      <c r="G37" s="101"/>
+      <c r="F37" s="99"/>
+      <c r="G37" s="99"/>
       <c r="H37" s="29"/>
-      <c r="I37" s="102"/>
-      <c r="J37" s="102"/>
+      <c r="I37" s="100"/>
+      <c r="J37" s="100"/>
       <c r="K37" s="30"/>
-      <c r="L37" s="103"/>
-      <c r="M37" s="103"/>
-    </row>
-    <row r="38" spans="1:13">
-      <c r="A38" s="99"/>
+      <c r="L37" s="101"/>
+      <c r="M37" s="101"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A38" s="97"/>
       <c r="B38" s="31">
         <f>(B37-B36)</f>
         <v>0</v>
@@ -5657,46 +5661,46 @@
       <c r="L38" s="45"/>
       <c r="M38" s="46"/>
     </row>
-    <row r="39" spans="1:13" ht="15" customHeight="1">
-      <c r="A39" s="99"/>
+    <row r="39" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="97"/>
       <c r="B39" s="23"/>
-      <c r="C39" s="100" t="s">
-        <v>11</v>
-      </c>
-      <c r="D39" s="100"/>
+      <c r="C39" s="98" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" s="98"/>
       <c r="E39" s="24"/>
-      <c r="F39" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="G39" s="101"/>
+      <c r="F39" s="99" t="s">
+        <v>11</v>
+      </c>
+      <c r="G39" s="99"/>
       <c r="H39" s="25"/>
-      <c r="I39" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="J39" s="102"/>
+      <c r="I39" s="100" t="s">
+        <v>11</v>
+      </c>
+      <c r="J39" s="100"/>
       <c r="K39" s="26"/>
-      <c r="L39" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="M39" s="103"/>
-    </row>
-    <row r="40" spans="1:13">
-      <c r="A40" s="99"/>
+      <c r="L39" s="101" t="s">
+        <v>11</v>
+      </c>
+      <c r="M39" s="101"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A40" s="97"/>
       <c r="B40" s="27"/>
-      <c r="C40" s="100"/>
-      <c r="D40" s="100"/>
+      <c r="C40" s="98"/>
+      <c r="D40" s="98"/>
       <c r="E40" s="28"/>
-      <c r="F40" s="101"/>
-      <c r="G40" s="101"/>
+      <c r="F40" s="99"/>
+      <c r="G40" s="99"/>
       <c r="H40" s="29"/>
-      <c r="I40" s="102"/>
-      <c r="J40" s="102"/>
+      <c r="I40" s="100"/>
+      <c r="J40" s="100"/>
       <c r="K40" s="48"/>
-      <c r="L40" s="103"/>
-      <c r="M40" s="103"/>
-    </row>
-    <row r="41" spans="1:13">
-      <c r="A41" s="99"/>
+      <c r="L40" s="101"/>
+      <c r="M40" s="101"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A41" s="97"/>
       <c r="B41" s="31">
         <f>(B40-B39)</f>
         <v>0</v>
@@ -5724,66 +5728,6 @@
     </row>
   </sheetData>
   <mergeCells count="67">
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="C39:D40"/>
-    <mergeCell ref="F39:G40"/>
-    <mergeCell ref="I39:J40"/>
-    <mergeCell ref="L39:M40"/>
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="C36:D37"/>
-    <mergeCell ref="F36:G37"/>
-    <mergeCell ref="I36:J37"/>
-    <mergeCell ref="L36:M37"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="C33:D34"/>
-    <mergeCell ref="F33:G34"/>
-    <mergeCell ref="I33:J34"/>
-    <mergeCell ref="L33:M34"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="C30:D31"/>
-    <mergeCell ref="F30:G31"/>
-    <mergeCell ref="I30:J31"/>
-    <mergeCell ref="L30:M31"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="C27:D28"/>
-    <mergeCell ref="F27:G28"/>
-    <mergeCell ref="I27:J28"/>
-    <mergeCell ref="L27:M28"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="C24:D25"/>
-    <mergeCell ref="F24:G25"/>
-    <mergeCell ref="I24:J25"/>
-    <mergeCell ref="L24:M25"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="C21:D22"/>
-    <mergeCell ref="F21:G22"/>
-    <mergeCell ref="I21:J22"/>
-    <mergeCell ref="L21:M22"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="C18:D19"/>
-    <mergeCell ref="F18:G19"/>
-    <mergeCell ref="I18:J19"/>
-    <mergeCell ref="L18:M19"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="C15:D16"/>
-    <mergeCell ref="F15:G16"/>
-    <mergeCell ref="I15:J16"/>
-    <mergeCell ref="L15:M16"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="C12:D13"/>
-    <mergeCell ref="F12:G13"/>
-    <mergeCell ref="I12:J13"/>
-    <mergeCell ref="L12:M13"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="C9:D10"/>
-    <mergeCell ref="F9:G10"/>
-    <mergeCell ref="I9:J10"/>
-    <mergeCell ref="L9:M10"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="C6:D7"/>
-    <mergeCell ref="F6:G7"/>
-    <mergeCell ref="I6:J7"/>
-    <mergeCell ref="L6:M7"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="A3:A5"/>
@@ -5791,6 +5735,66 @@
     <mergeCell ref="F3:G4"/>
     <mergeCell ref="I3:J4"/>
     <mergeCell ref="L3:M4"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="C6:D7"/>
+    <mergeCell ref="F6:G7"/>
+    <mergeCell ref="I6:J7"/>
+    <mergeCell ref="L6:M7"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="C9:D10"/>
+    <mergeCell ref="F9:G10"/>
+    <mergeCell ref="I9:J10"/>
+    <mergeCell ref="L9:M10"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="C12:D13"/>
+    <mergeCell ref="F12:G13"/>
+    <mergeCell ref="I12:J13"/>
+    <mergeCell ref="L12:M13"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="C15:D16"/>
+    <mergeCell ref="F15:G16"/>
+    <mergeCell ref="I15:J16"/>
+    <mergeCell ref="L15:M16"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="C18:D19"/>
+    <mergeCell ref="F18:G19"/>
+    <mergeCell ref="I18:J19"/>
+    <mergeCell ref="L18:M19"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="C21:D22"/>
+    <mergeCell ref="F21:G22"/>
+    <mergeCell ref="I21:J22"/>
+    <mergeCell ref="L21:M22"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="C24:D25"/>
+    <mergeCell ref="F24:G25"/>
+    <mergeCell ref="I24:J25"/>
+    <mergeCell ref="L24:M25"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="C27:D28"/>
+    <mergeCell ref="F27:G28"/>
+    <mergeCell ref="I27:J28"/>
+    <mergeCell ref="L27:M28"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="C30:D31"/>
+    <mergeCell ref="F30:G31"/>
+    <mergeCell ref="I30:J31"/>
+    <mergeCell ref="L30:M31"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="C33:D34"/>
+    <mergeCell ref="F33:G34"/>
+    <mergeCell ref="I33:J34"/>
+    <mergeCell ref="L33:M34"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="C36:D37"/>
+    <mergeCell ref="F36:G37"/>
+    <mergeCell ref="I36:J37"/>
+    <mergeCell ref="L36:M37"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="C39:D40"/>
+    <mergeCell ref="F39:G40"/>
+    <mergeCell ref="I39:J40"/>
+    <mergeCell ref="L39:M40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
added a levelload trigger
</commit_message>
<xml_diff>
--- a/Zeitaufzeichnung_Ishjarta.xlsx
+++ b/Zeitaufzeichnung_Ishjarta.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fragon\Documents\GitHub\ishjarta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A647526A-0138-4E22-9EB2-BFE1AFF05803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CEF0788-CC64-4A09-B472-5C1135890103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="732" yWindow="732" windowWidth="17280" windowHeight="8880" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vorlage" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="42">
   <si>
     <t>Datum</t>
   </si>
@@ -470,6 +470,21 @@
       <t>Zeitaufzeichnung, Tutorial Level, Sprite Zeichnen</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t>Aufgabe:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">  Tutorial Level</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -5907,8 +5922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D6B74AA-FFCC-4E7B-951E-AF7C1087A71C}">
   <dimension ref="A1:O41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5978,11 +5993,11 @@
       </c>
       <c r="C2" s="10">
         <f t="array" ref="C2">SUM(B5:B41*(MOD(ROW(B5:B41)-2,3)=0))</f>
-        <v>0.3194444444444452</v>
+        <v>0.37500000000000078</v>
       </c>
       <c r="D2" s="11">
         <f>C2+Sprint_4!D2</f>
-        <v>2.6590277777777813</v>
+        <v>2.7145833333333371</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>6</v>
@@ -6022,7 +6037,7 @@
       </c>
       <c r="O2" s="22">
         <f>C2+F2+I2+L2</f>
-        <v>0.40277777777777923</v>
+        <v>0.45833333333333481</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -6058,7 +6073,7 @@
       </c>
       <c r="O3" s="22">
         <f>D2+G2+J2+M2</f>
-        <v>9.1763888888889067</v>
+        <v>9.2319444444444621</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -6514,10 +6529,14 @@
       <c r="M23" s="98"/>
     </row>
     <row r="24" spans="1:13" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="99"/>
-      <c r="B24" s="23"/>
+      <c r="A24" s="99">
+        <v>44617</v>
+      </c>
+      <c r="B24" s="23">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="C24" s="100" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D24" s="100"/>
       <c r="E24" s="24"/>
@@ -6538,7 +6557,9 @@
     </row>
     <row r="25" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="99"/>
-      <c r="B25" s="27"/>
+      <c r="B25" s="27">
+        <v>0.63888888888888895</v>
+      </c>
       <c r="C25" s="100"/>
       <c r="D25" s="100"/>
       <c r="E25" s="28"/>
@@ -6555,7 +6576,7 @@
       <c r="A26" s="99"/>
       <c r="B26" s="31">
         <f>(B25-B24)</f>
-        <v>0</v>
+        <v>5.555555555555558E-2</v>
       </c>
       <c r="C26" s="32"/>
       <c r="D26" s="33"/>

</xml_diff>

<commit_message>
added sprites and prefabs
</commit_message>
<xml_diff>
--- a/Zeitaufzeichnung_Ishjarta.xlsx
+++ b/Zeitaufzeichnung_Ishjarta.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danijel\Desktop\ishjarta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FFA3BC0-AD16-4998-857A-A36DF1E9B09C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD49EB10-6584-4478-9E79-2A6F61795C65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4457" yWindow="4457" windowWidth="24686" windowHeight="13140" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="47">
   <si>
     <t>Datum</t>
   </si>
@@ -552,6 +552,32 @@
   <si>
     <t>Aufgabe: Sprites Zeichnen</t>
   </si>
+  <si>
+    <r>
+      <t>Aufgabe:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Level Design</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -1372,6 +1398,12 @@
     <xf numFmtId="165" fontId="2" fillId="5" borderId="1" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="14" fontId="2" fillId="6" borderId="10" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1387,12 +1419,6 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="12" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="167" fontId="2" fillId="6" borderId="17" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1429,26 +1455,29 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="30" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="5" borderId="31" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="32" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="33" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="5" borderId="23" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="165" fontId="2" fillId="5" borderId="1" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="32" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="30" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="33" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="5" borderId="23" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="5" borderId="31" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1461,9 +1490,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -1878,7 +1904,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A1" s="104" t="s">
+      <c r="A1" s="99" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1917,13 +1943,13 @@
       <c r="M1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="105" t="s">
+      <c r="N1" s="100" t="s">
         <v>4</v>
       </c>
-      <c r="O1" s="105"/>
+      <c r="O1" s="100"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A2" s="104"/>
+      <c r="A2" s="99"/>
       <c r="B2" s="9" t="s">
         <v>5</v>
       </c>
@@ -1977,35 +2003,35 @@
       </c>
     </row>
     <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="99"/>
+      <c r="A3" s="101"/>
       <c r="B3" s="23">
         <v>0.33333333333333298</v>
       </c>
-      <c r="C3" s="100" t="s">
+      <c r="C3" s="102" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="100"/>
+      <c r="D3" s="102"/>
       <c r="E3" s="24">
         <v>0.33333333333333298</v>
       </c>
-      <c r="F3" s="101" t="s">
+      <c r="F3" s="103" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="101"/>
+      <c r="G3" s="103"/>
       <c r="H3" s="25">
         <v>0.33333333333333298</v>
       </c>
-      <c r="I3" s="102" t="s">
+      <c r="I3" s="104" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="102"/>
+      <c r="J3" s="104"/>
       <c r="K3" s="26">
         <v>0.33333333333333298</v>
       </c>
-      <c r="L3" s="103" t="s">
+      <c r="L3" s="105" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="103"/>
+      <c r="M3" s="105"/>
       <c r="N3" s="21" t="s">
         <v>10</v>
       </c>
@@ -2015,30 +2041,30 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A4" s="99"/>
+      <c r="A4" s="101"/>
       <c r="B4" s="27">
         <v>0.41666666666666702</v>
       </c>
-      <c r="C4" s="100"/>
-      <c r="D4" s="100"/>
+      <c r="C4" s="102"/>
+      <c r="D4" s="102"/>
       <c r="E4" s="28">
         <v>0.41666666666666702</v>
       </c>
-      <c r="F4" s="101"/>
-      <c r="G4" s="101"/>
+      <c r="F4" s="103"/>
+      <c r="G4" s="103"/>
       <c r="H4" s="29">
         <v>0.41666666666666702</v>
       </c>
-      <c r="I4" s="102"/>
-      <c r="J4" s="102"/>
+      <c r="I4" s="104"/>
+      <c r="J4" s="104"/>
       <c r="K4" s="30">
         <v>0.41666666666666702</v>
       </c>
-      <c r="L4" s="103"/>
-      <c r="M4" s="103"/>
+      <c r="L4" s="105"/>
+      <c r="M4" s="105"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A5" s="99"/>
+      <c r="A5" s="101"/>
       <c r="B5" s="31">
         <f>B4-B3</f>
         <v>8.3333333333334036E-2</v>
@@ -2065,45 +2091,45 @@
       <c r="M5" s="42"/>
     </row>
     <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="99"/>
+      <c r="A6" s="101"/>
       <c r="B6" s="23"/>
-      <c r="C6" s="100" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="100"/>
+      <c r="C6" s="102" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="102"/>
       <c r="E6" s="24"/>
-      <c r="F6" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="101"/>
+      <c r="F6" s="103" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="103"/>
       <c r="H6" s="25"/>
-      <c r="I6" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="J6" s="102"/>
+      <c r="I6" s="104" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="104"/>
       <c r="K6" s="43"/>
-      <c r="L6" s="103" t="s">
+      <c r="L6" s="105" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="103"/>
+      <c r="M6" s="105"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A7" s="99"/>
+      <c r="A7" s="101"/>
       <c r="B7" s="27"/>
-      <c r="C7" s="100"/>
-      <c r="D7" s="100"/>
+      <c r="C7" s="102"/>
+      <c r="D7" s="102"/>
       <c r="E7" s="28"/>
-      <c r="F7" s="101"/>
-      <c r="G7" s="101"/>
+      <c r="F7" s="103"/>
+      <c r="G7" s="103"/>
       <c r="H7" s="29"/>
-      <c r="I7" s="102"/>
-      <c r="J7" s="102"/>
+      <c r="I7" s="104"/>
+      <c r="J7" s="104"/>
       <c r="K7" s="30"/>
-      <c r="L7" s="103"/>
-      <c r="M7" s="103"/>
+      <c r="L7" s="105"/>
+      <c r="M7" s="105"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A8" s="99"/>
+      <c r="A8" s="101"/>
       <c r="B8" s="31">
         <f>B7-B6</f>
         <v>0</v>
@@ -2130,45 +2156,45 @@
       <c r="M8" s="46"/>
     </row>
     <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="99"/>
+      <c r="A9" s="101"/>
       <c r="B9" s="23"/>
-      <c r="C9" s="100" t="s">
+      <c r="C9" s="102" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="100"/>
+      <c r="D9" s="102"/>
       <c r="E9" s="24"/>
-      <c r="F9" s="101" t="s">
+      <c r="F9" s="103" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="101"/>
+      <c r="G9" s="103"/>
       <c r="H9" s="25"/>
-      <c r="I9" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="J9" s="102"/>
+      <c r="I9" s="104" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" s="104"/>
       <c r="K9" s="47"/>
-      <c r="L9" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="M9" s="103"/>
+      <c r="L9" s="105" t="s">
+        <v>11</v>
+      </c>
+      <c r="M9" s="105"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A10" s="99"/>
+      <c r="A10" s="101"/>
       <c r="B10" s="27"/>
-      <c r="C10" s="100"/>
-      <c r="D10" s="100"/>
+      <c r="C10" s="102"/>
+      <c r="D10" s="102"/>
       <c r="E10" s="28"/>
-      <c r="F10" s="101"/>
-      <c r="G10" s="101"/>
+      <c r="F10" s="103"/>
+      <c r="G10" s="103"/>
       <c r="H10" s="29"/>
-      <c r="I10" s="102"/>
-      <c r="J10" s="102"/>
+      <c r="I10" s="104"/>
+      <c r="J10" s="104"/>
       <c r="K10" s="30"/>
-      <c r="L10" s="103"/>
-      <c r="M10" s="103"/>
+      <c r="L10" s="105"/>
+      <c r="M10" s="105"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A11" s="99"/>
+      <c r="A11" s="101"/>
       <c r="B11" s="31">
         <f>(B10-B9)</f>
         <v>0</v>
@@ -2195,45 +2221,45 @@
       <c r="M11" s="46"/>
     </row>
     <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="99"/>
+      <c r="A12" s="101"/>
       <c r="B12" s="23"/>
-      <c r="C12" s="100" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="100"/>
+      <c r="C12" s="102" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="102"/>
       <c r="E12" s="24"/>
-      <c r="F12" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" s="101"/>
+      <c r="F12" s="103" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="103"/>
       <c r="H12" s="25"/>
-      <c r="I12" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="J12" s="102"/>
+      <c r="I12" s="104" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" s="104"/>
       <c r="K12" s="47"/>
-      <c r="L12" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="M12" s="103"/>
+      <c r="L12" s="105" t="s">
+        <v>11</v>
+      </c>
+      <c r="M12" s="105"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A13" s="99"/>
+      <c r="A13" s="101"/>
       <c r="B13" s="27"/>
-      <c r="C13" s="100"/>
-      <c r="D13" s="100"/>
+      <c r="C13" s="102"/>
+      <c r="D13" s="102"/>
       <c r="E13" s="28"/>
-      <c r="F13" s="101"/>
-      <c r="G13" s="101"/>
+      <c r="F13" s="103"/>
+      <c r="G13" s="103"/>
       <c r="H13" s="29"/>
-      <c r="I13" s="102"/>
-      <c r="J13" s="102"/>
+      <c r="I13" s="104"/>
+      <c r="J13" s="104"/>
       <c r="K13" s="48"/>
-      <c r="L13" s="103"/>
-      <c r="M13" s="103"/>
+      <c r="L13" s="105"/>
+      <c r="M13" s="105"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A14" s="99"/>
+      <c r="A14" s="101"/>
       <c r="B14" s="31">
         <f>(B13-B12)</f>
         <v>0</v>
@@ -2260,45 +2286,45 @@
       <c r="M14" s="50"/>
     </row>
     <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="99"/>
+      <c r="A15" s="101"/>
       <c r="B15" s="23"/>
-      <c r="C15" s="100" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="100"/>
+      <c r="C15" s="102" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="102"/>
       <c r="E15" s="24"/>
-      <c r="F15" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="G15" s="101"/>
+      <c r="F15" s="103" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="103"/>
       <c r="H15" s="25"/>
-      <c r="I15" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="J15" s="102"/>
+      <c r="I15" s="104" t="s">
+        <v>11</v>
+      </c>
+      <c r="J15" s="104"/>
       <c r="K15" s="26"/>
-      <c r="L15" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="M15" s="103"/>
+      <c r="L15" s="105" t="s">
+        <v>11</v>
+      </c>
+      <c r="M15" s="105"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A16" s="99"/>
+      <c r="A16" s="101"/>
       <c r="B16" s="27"/>
-      <c r="C16" s="100"/>
-      <c r="D16" s="100"/>
+      <c r="C16" s="102"/>
+      <c r="D16" s="102"/>
       <c r="E16" s="28"/>
-      <c r="F16" s="101"/>
-      <c r="G16" s="101"/>
+      <c r="F16" s="103"/>
+      <c r="G16" s="103"/>
       <c r="H16" s="29"/>
-      <c r="I16" s="102"/>
-      <c r="J16" s="102"/>
+      <c r="I16" s="104"/>
+      <c r="J16" s="104"/>
       <c r="K16" s="30"/>
-      <c r="L16" s="103"/>
-      <c r="M16" s="103"/>
+      <c r="L16" s="105"/>
+      <c r="M16" s="105"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A17" s="99"/>
+      <c r="A17" s="101"/>
       <c r="B17" s="31">
         <f>(B16-B15)</f>
         <v>0</v>
@@ -2325,45 +2351,45 @@
       <c r="M17" s="46"/>
     </row>
     <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="99"/>
+      <c r="A18" s="101"/>
       <c r="B18" s="23"/>
-      <c r="C18" s="100" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="100"/>
+      <c r="C18" s="102" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="102"/>
       <c r="E18" s="24"/>
-      <c r="F18" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="G18" s="101"/>
+      <c r="F18" s="103" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" s="103"/>
       <c r="H18" s="25"/>
-      <c r="I18" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="J18" s="102"/>
+      <c r="I18" s="104" t="s">
+        <v>11</v>
+      </c>
+      <c r="J18" s="104"/>
       <c r="K18" s="47"/>
-      <c r="L18" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="M18" s="103"/>
+      <c r="L18" s="105" t="s">
+        <v>11</v>
+      </c>
+      <c r="M18" s="105"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A19" s="99"/>
+      <c r="A19" s="101"/>
       <c r="B19" s="27"/>
-      <c r="C19" s="100"/>
-      <c r="D19" s="100"/>
+      <c r="C19" s="102"/>
+      <c r="D19" s="102"/>
       <c r="E19" s="28"/>
-      <c r="F19" s="101"/>
-      <c r="G19" s="101"/>
+      <c r="F19" s="103"/>
+      <c r="G19" s="103"/>
       <c r="H19" s="29"/>
-      <c r="I19" s="102"/>
-      <c r="J19" s="102"/>
+      <c r="I19" s="104"/>
+      <c r="J19" s="104"/>
       <c r="K19" s="30"/>
-      <c r="L19" s="103"/>
-      <c r="M19" s="103"/>
+      <c r="L19" s="105"/>
+      <c r="M19" s="105"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A20" s="99"/>
+      <c r="A20" s="101"/>
       <c r="B20" s="31">
         <f>(B19-B18)</f>
         <v>0</v>
@@ -2390,45 +2416,45 @@
       <c r="M20" s="46"/>
     </row>
     <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="99"/>
+      <c r="A21" s="101"/>
       <c r="B21" s="23"/>
-      <c r="C21" s="100" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" s="100"/>
+      <c r="C21" s="102" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="102"/>
       <c r="E21" s="24"/>
-      <c r="F21" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="G21" s="101"/>
+      <c r="F21" s="103" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" s="103"/>
       <c r="H21" s="25"/>
-      <c r="I21" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="J21" s="102"/>
+      <c r="I21" s="104" t="s">
+        <v>11</v>
+      </c>
+      <c r="J21" s="104"/>
       <c r="K21" s="26"/>
-      <c r="L21" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="M21" s="103"/>
+      <c r="L21" s="105" t="s">
+        <v>11</v>
+      </c>
+      <c r="M21" s="105"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A22" s="99"/>
+      <c r="A22" s="101"/>
       <c r="B22" s="27"/>
-      <c r="C22" s="100"/>
-      <c r="D22" s="100"/>
+      <c r="C22" s="102"/>
+      <c r="D22" s="102"/>
       <c r="E22" s="28"/>
-      <c r="F22" s="101"/>
-      <c r="G22" s="101"/>
+      <c r="F22" s="103"/>
+      <c r="G22" s="103"/>
       <c r="H22" s="29"/>
-      <c r="I22" s="102"/>
-      <c r="J22" s="102"/>
+      <c r="I22" s="104"/>
+      <c r="J22" s="104"/>
       <c r="K22" s="48"/>
-      <c r="L22" s="103"/>
-      <c r="M22" s="103"/>
+      <c r="L22" s="105"/>
+      <c r="M22" s="105"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A23" s="99"/>
+      <c r="A23" s="101"/>
       <c r="B23" s="31">
         <f>(B22-B21)</f>
         <v>0</v>
@@ -2455,45 +2481,45 @@
       <c r="M23" s="52"/>
     </row>
     <row r="24" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="99"/>
+      <c r="A24" s="101"/>
       <c r="B24" s="23"/>
-      <c r="C24" s="100" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" s="100"/>
+      <c r="C24" s="102" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="102"/>
       <c r="E24" s="24"/>
-      <c r="F24" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="G24" s="101"/>
+      <c r="F24" s="103" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" s="103"/>
       <c r="H24" s="25"/>
-      <c r="I24" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="J24" s="102"/>
+      <c r="I24" s="104" t="s">
+        <v>11</v>
+      </c>
+      <c r="J24" s="104"/>
       <c r="K24" s="26"/>
-      <c r="L24" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="M24" s="103"/>
+      <c r="L24" s="105" t="s">
+        <v>11</v>
+      </c>
+      <c r="M24" s="105"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A25" s="99"/>
+      <c r="A25" s="101"/>
       <c r="B25" s="27"/>
-      <c r="C25" s="100"/>
-      <c r="D25" s="100"/>
+      <c r="C25" s="102"/>
+      <c r="D25" s="102"/>
       <c r="E25" s="28"/>
-      <c r="F25" s="101"/>
-      <c r="G25" s="101"/>
+      <c r="F25" s="103"/>
+      <c r="G25" s="103"/>
       <c r="H25" s="29"/>
-      <c r="I25" s="102"/>
-      <c r="J25" s="102"/>
+      <c r="I25" s="104"/>
+      <c r="J25" s="104"/>
       <c r="K25" s="30"/>
-      <c r="L25" s="103"/>
-      <c r="M25" s="103"/>
+      <c r="L25" s="105"/>
+      <c r="M25" s="105"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A26" s="99"/>
+      <c r="A26" s="101"/>
       <c r="B26" s="31">
         <f>(B25-B24)</f>
         <v>0</v>
@@ -2520,45 +2546,45 @@
       <c r="M26" s="46"/>
     </row>
     <row r="27" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="99"/>
+      <c r="A27" s="101"/>
       <c r="B27" s="23"/>
-      <c r="C27" s="100" t="s">
-        <v>11</v>
-      </c>
-      <c r="D27" s="100"/>
+      <c r="C27" s="102" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="102"/>
       <c r="E27" s="24"/>
-      <c r="F27" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="G27" s="101"/>
+      <c r="F27" s="103" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" s="103"/>
       <c r="H27" s="25"/>
-      <c r="I27" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="J27" s="102"/>
+      <c r="I27" s="104" t="s">
+        <v>11</v>
+      </c>
+      <c r="J27" s="104"/>
       <c r="K27" s="47"/>
-      <c r="L27" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="M27" s="103"/>
+      <c r="L27" s="105" t="s">
+        <v>11</v>
+      </c>
+      <c r="M27" s="105"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A28" s="99"/>
+      <c r="A28" s="101"/>
       <c r="B28" s="27"/>
-      <c r="C28" s="100"/>
-      <c r="D28" s="100"/>
+      <c r="C28" s="102"/>
+      <c r="D28" s="102"/>
       <c r="E28" s="28"/>
-      <c r="F28" s="101"/>
-      <c r="G28" s="101"/>
+      <c r="F28" s="103"/>
+      <c r="G28" s="103"/>
       <c r="H28" s="29"/>
-      <c r="I28" s="102"/>
-      <c r="J28" s="102"/>
+      <c r="I28" s="104"/>
+      <c r="J28" s="104"/>
       <c r="K28" s="30"/>
-      <c r="L28" s="103"/>
-      <c r="M28" s="103"/>
+      <c r="L28" s="105"/>
+      <c r="M28" s="105"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A29" s="99"/>
+      <c r="A29" s="101"/>
       <c r="B29" s="31">
         <f>(B28-B27)</f>
         <v>0</v>
@@ -2585,45 +2611,45 @@
       <c r="M29" s="46"/>
     </row>
     <row r="30" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="99"/>
+      <c r="A30" s="101"/>
       <c r="B30" s="23"/>
-      <c r="C30" s="100" t="s">
-        <v>11</v>
-      </c>
-      <c r="D30" s="100"/>
+      <c r="C30" s="102" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" s="102"/>
       <c r="E30" s="24"/>
-      <c r="F30" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="G30" s="101"/>
+      <c r="F30" s="103" t="s">
+        <v>11</v>
+      </c>
+      <c r="G30" s="103"/>
       <c r="H30" s="25"/>
-      <c r="I30" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="J30" s="102"/>
+      <c r="I30" s="104" t="s">
+        <v>11</v>
+      </c>
+      <c r="J30" s="104"/>
       <c r="K30" s="26"/>
-      <c r="L30" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="M30" s="103"/>
+      <c r="L30" s="105" t="s">
+        <v>11</v>
+      </c>
+      <c r="M30" s="105"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A31" s="99"/>
+      <c r="A31" s="101"/>
       <c r="B31" s="27"/>
-      <c r="C31" s="100"/>
-      <c r="D31" s="100"/>
+      <c r="C31" s="102"/>
+      <c r="D31" s="102"/>
       <c r="E31" s="28"/>
-      <c r="F31" s="101"/>
-      <c r="G31" s="101"/>
+      <c r="F31" s="103"/>
+      <c r="G31" s="103"/>
       <c r="H31" s="29"/>
-      <c r="I31" s="102"/>
-      <c r="J31" s="102"/>
+      <c r="I31" s="104"/>
+      <c r="J31" s="104"/>
       <c r="K31" s="48"/>
-      <c r="L31" s="103"/>
-      <c r="M31" s="103"/>
+      <c r="L31" s="105"/>
+      <c r="M31" s="105"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A32" s="99"/>
+      <c r="A32" s="101"/>
       <c r="B32" s="31">
         <f>(B31-B30)</f>
         <v>0</v>
@@ -2650,45 +2676,45 @@
       <c r="M32" s="52"/>
     </row>
     <row r="33" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="99"/>
+      <c r="A33" s="101"/>
       <c r="B33" s="23"/>
-      <c r="C33" s="100" t="s">
-        <v>11</v>
-      </c>
-      <c r="D33" s="100"/>
+      <c r="C33" s="102" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="102"/>
       <c r="E33" s="24"/>
-      <c r="F33" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="G33" s="101"/>
+      <c r="F33" s="103" t="s">
+        <v>11</v>
+      </c>
+      <c r="G33" s="103"/>
       <c r="H33" s="25"/>
-      <c r="I33" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="J33" s="102"/>
+      <c r="I33" s="104" t="s">
+        <v>11</v>
+      </c>
+      <c r="J33" s="104"/>
       <c r="K33" s="26"/>
-      <c r="L33" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="M33" s="103"/>
+      <c r="L33" s="105" t="s">
+        <v>11</v>
+      </c>
+      <c r="M33" s="105"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A34" s="99"/>
+      <c r="A34" s="101"/>
       <c r="B34" s="27"/>
-      <c r="C34" s="100"/>
-      <c r="D34" s="100"/>
+      <c r="C34" s="102"/>
+      <c r="D34" s="102"/>
       <c r="E34" s="28"/>
-      <c r="F34" s="101"/>
-      <c r="G34" s="101"/>
+      <c r="F34" s="103"/>
+      <c r="G34" s="103"/>
       <c r="H34" s="29"/>
-      <c r="I34" s="102"/>
-      <c r="J34" s="102"/>
+      <c r="I34" s="104"/>
+      <c r="J34" s="104"/>
       <c r="K34" s="30"/>
-      <c r="L34" s="103"/>
-      <c r="M34" s="103"/>
+      <c r="L34" s="105"/>
+      <c r="M34" s="105"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A35" s="99"/>
+      <c r="A35" s="101"/>
       <c r="B35" s="31">
         <f>(B34-B33)</f>
         <v>0</v>
@@ -2715,45 +2741,45 @@
       <c r="M35" s="46"/>
     </row>
     <row r="36" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="99"/>
+      <c r="A36" s="101"/>
       <c r="B36" s="23"/>
-      <c r="C36" s="100" t="s">
-        <v>11</v>
-      </c>
-      <c r="D36" s="100"/>
+      <c r="C36" s="102" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" s="102"/>
       <c r="E36" s="24"/>
-      <c r="F36" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="G36" s="101"/>
+      <c r="F36" s="103" t="s">
+        <v>11</v>
+      </c>
+      <c r="G36" s="103"/>
       <c r="H36" s="25"/>
-      <c r="I36" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="J36" s="102"/>
+      <c r="I36" s="104" t="s">
+        <v>11</v>
+      </c>
+      <c r="J36" s="104"/>
       <c r="K36" s="47"/>
-      <c r="L36" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="M36" s="103"/>
+      <c r="L36" s="105" t="s">
+        <v>11</v>
+      </c>
+      <c r="M36" s="105"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A37" s="99"/>
+      <c r="A37" s="101"/>
       <c r="B37" s="27"/>
-      <c r="C37" s="100"/>
-      <c r="D37" s="100"/>
+      <c r="C37" s="102"/>
+      <c r="D37" s="102"/>
       <c r="E37" s="28"/>
-      <c r="F37" s="101"/>
-      <c r="G37" s="101"/>
+      <c r="F37" s="103"/>
+      <c r="G37" s="103"/>
       <c r="H37" s="29"/>
-      <c r="I37" s="102"/>
-      <c r="J37" s="102"/>
+      <c r="I37" s="104"/>
+      <c r="J37" s="104"/>
       <c r="K37" s="30"/>
-      <c r="L37" s="103"/>
-      <c r="M37" s="103"/>
+      <c r="L37" s="105"/>
+      <c r="M37" s="105"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A38" s="99"/>
+      <c r="A38" s="101"/>
       <c r="B38" s="31">
         <f>(B37-B36)</f>
         <v>0</v>
@@ -2780,45 +2806,45 @@
       <c r="M38" s="46"/>
     </row>
     <row r="39" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="99"/>
+      <c r="A39" s="101"/>
       <c r="B39" s="23"/>
-      <c r="C39" s="100" t="s">
-        <v>11</v>
-      </c>
-      <c r="D39" s="100"/>
+      <c r="C39" s="102" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" s="102"/>
       <c r="E39" s="24"/>
-      <c r="F39" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="G39" s="101"/>
+      <c r="F39" s="103" t="s">
+        <v>11</v>
+      </c>
+      <c r="G39" s="103"/>
       <c r="H39" s="25"/>
-      <c r="I39" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="J39" s="102"/>
+      <c r="I39" s="104" t="s">
+        <v>11</v>
+      </c>
+      <c r="J39" s="104"/>
       <c r="K39" s="26"/>
-      <c r="L39" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="M39" s="103"/>
+      <c r="L39" s="105" t="s">
+        <v>11</v>
+      </c>
+      <c r="M39" s="105"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A40" s="99"/>
+      <c r="A40" s="101"/>
       <c r="B40" s="27"/>
-      <c r="C40" s="100"/>
-      <c r="D40" s="100"/>
+      <c r="C40" s="102"/>
+      <c r="D40" s="102"/>
       <c r="E40" s="28"/>
-      <c r="F40" s="101"/>
-      <c r="G40" s="101"/>
+      <c r="F40" s="103"/>
+      <c r="G40" s="103"/>
       <c r="H40" s="29"/>
-      <c r="I40" s="102"/>
-      <c r="J40" s="102"/>
+      <c r="I40" s="104"/>
+      <c r="J40" s="104"/>
       <c r="K40" s="48"/>
-      <c r="L40" s="103"/>
-      <c r="M40" s="103"/>
+      <c r="L40" s="105"/>
+      <c r="M40" s="105"/>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A41" s="99"/>
+      <c r="A41" s="101"/>
       <c r="B41" s="31">
         <f>(B40-B39)</f>
         <v>0</v>
@@ -2846,6 +2872,66 @@
     </row>
   </sheetData>
   <mergeCells count="67">
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="C39:D40"/>
+    <mergeCell ref="F39:G40"/>
+    <mergeCell ref="I39:J40"/>
+    <mergeCell ref="L39:M40"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="C36:D37"/>
+    <mergeCell ref="F36:G37"/>
+    <mergeCell ref="I36:J37"/>
+    <mergeCell ref="L36:M37"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="C33:D34"/>
+    <mergeCell ref="F33:G34"/>
+    <mergeCell ref="I33:J34"/>
+    <mergeCell ref="L33:M34"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="C30:D31"/>
+    <mergeCell ref="F30:G31"/>
+    <mergeCell ref="I30:J31"/>
+    <mergeCell ref="L30:M31"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="C27:D28"/>
+    <mergeCell ref="F27:G28"/>
+    <mergeCell ref="I27:J28"/>
+    <mergeCell ref="L27:M28"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="C24:D25"/>
+    <mergeCell ref="F24:G25"/>
+    <mergeCell ref="I24:J25"/>
+    <mergeCell ref="L24:M25"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="C21:D22"/>
+    <mergeCell ref="F21:G22"/>
+    <mergeCell ref="I21:J22"/>
+    <mergeCell ref="L21:M22"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="C18:D19"/>
+    <mergeCell ref="F18:G19"/>
+    <mergeCell ref="I18:J19"/>
+    <mergeCell ref="L18:M19"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="C15:D16"/>
+    <mergeCell ref="F15:G16"/>
+    <mergeCell ref="I15:J16"/>
+    <mergeCell ref="L15:M16"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="C12:D13"/>
+    <mergeCell ref="F12:G13"/>
+    <mergeCell ref="I12:J13"/>
+    <mergeCell ref="L12:M13"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="C9:D10"/>
+    <mergeCell ref="F9:G10"/>
+    <mergeCell ref="I9:J10"/>
+    <mergeCell ref="L9:M10"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="C6:D7"/>
+    <mergeCell ref="F6:G7"/>
+    <mergeCell ref="I6:J7"/>
+    <mergeCell ref="L6:M7"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="A3:A5"/>
@@ -2853,66 +2939,6 @@
     <mergeCell ref="F3:G4"/>
     <mergeCell ref="I3:J4"/>
     <mergeCell ref="L3:M4"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="C6:D7"/>
-    <mergeCell ref="F6:G7"/>
-    <mergeCell ref="I6:J7"/>
-    <mergeCell ref="L6:M7"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="C9:D10"/>
-    <mergeCell ref="F9:G10"/>
-    <mergeCell ref="I9:J10"/>
-    <mergeCell ref="L9:M10"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="C12:D13"/>
-    <mergeCell ref="F12:G13"/>
-    <mergeCell ref="I12:J13"/>
-    <mergeCell ref="L12:M13"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="C15:D16"/>
-    <mergeCell ref="F15:G16"/>
-    <mergeCell ref="I15:J16"/>
-    <mergeCell ref="L15:M16"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="C18:D19"/>
-    <mergeCell ref="F18:G19"/>
-    <mergeCell ref="I18:J19"/>
-    <mergeCell ref="L18:M19"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="C21:D22"/>
-    <mergeCell ref="F21:G22"/>
-    <mergeCell ref="I21:J22"/>
-    <mergeCell ref="L21:M22"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="C24:D25"/>
-    <mergeCell ref="F24:G25"/>
-    <mergeCell ref="I24:J25"/>
-    <mergeCell ref="L24:M25"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="C27:D28"/>
-    <mergeCell ref="F27:G28"/>
-    <mergeCell ref="I27:J28"/>
-    <mergeCell ref="L27:M28"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="C30:D31"/>
-    <mergeCell ref="F30:G31"/>
-    <mergeCell ref="I30:J31"/>
-    <mergeCell ref="L30:M31"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="C33:D34"/>
-    <mergeCell ref="F33:G34"/>
-    <mergeCell ref="I33:J34"/>
-    <mergeCell ref="L33:M34"/>
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="C36:D37"/>
-    <mergeCell ref="F36:G37"/>
-    <mergeCell ref="I36:J37"/>
-    <mergeCell ref="L36:M37"/>
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="C39:D40"/>
-    <mergeCell ref="F39:G40"/>
-    <mergeCell ref="I39:J40"/>
-    <mergeCell ref="L39:M40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -3369,6 +3395,60 @@
     </row>
   </sheetData>
   <mergeCells count="63">
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="I20:I21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="E2:E3"/>
@@ -3378,60 +3458,6 @@
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="H4:I4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="I20:I21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="H22:I22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -3535,10 +3561,10 @@
       <c r="K2" s="26">
         <v>0.33333333333333298</v>
       </c>
-      <c r="L2" s="121" t="s">
+      <c r="L2" s="118" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="121"/>
+      <c r="M2" s="118"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A3" s="106"/>
@@ -3560,8 +3586,8 @@
       <c r="K3" s="30">
         <v>0.41666666666666702</v>
       </c>
-      <c r="L3" s="121"/>
-      <c r="M3" s="121"/>
+      <c r="L3" s="118"/>
+      <c r="M3" s="118"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A4" s="106"/>
@@ -3583,12 +3609,12 @@
       </c>
       <c r="I4" s="113"/>
       <c r="J4" s="113"/>
-      <c r="K4" s="124">
+      <c r="K4" s="119">
         <f>K3-K2</f>
         <v>8.3333333333334036E-2</v>
       </c>
-      <c r="L4" s="124"/>
-      <c r="M4" s="124"/>
+      <c r="L4" s="119"/>
+      <c r="M4" s="119"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A5" s="106">
@@ -3614,10 +3640,10 @@
       <c r="K5" s="43">
         <v>0.33333333333333298</v>
       </c>
-      <c r="L5" s="118" t="s">
+      <c r="L5" s="120" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="118"/>
+      <c r="M5" s="120"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A6" s="106"/>
@@ -3635,8 +3661,8 @@
       <c r="K6" s="30">
         <v>0.625</v>
       </c>
-      <c r="L6" s="118"/>
-      <c r="M6" s="118"/>
+      <c r="L6" s="120"/>
+      <c r="M6" s="120"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A7" s="106"/>
@@ -3693,10 +3719,10 @@
       <c r="K8" s="47">
         <v>0.77083333333333304</v>
       </c>
-      <c r="L8" s="120" t="s">
+      <c r="L8" s="121" t="s">
         <v>12</v>
       </c>
-      <c r="M8" s="120"/>
+      <c r="M8" s="121"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A9" s="106"/>
@@ -3718,8 +3744,8 @@
       <c r="K9" s="30">
         <v>0.91666666666666696</v>
       </c>
-      <c r="L9" s="120"/>
-      <c r="M9" s="120"/>
+      <c r="L9" s="121"/>
+      <c r="M9" s="121"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A10" s="106"/>
@@ -3849,10 +3875,10 @@
       </c>
       <c r="J14" s="117"/>
       <c r="K14" s="26"/>
-      <c r="L14" s="121" t="s">
+      <c r="L14" s="118" t="s">
         <v>12</v>
       </c>
-      <c r="M14" s="121"/>
+      <c r="M14" s="118"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A15" s="106"/>
@@ -3866,8 +3892,8 @@
       <c r="I15" s="117"/>
       <c r="J15" s="117"/>
       <c r="K15" s="30"/>
-      <c r="L15" s="121"/>
-      <c r="M15" s="121"/>
+      <c r="L15" s="118"/>
+      <c r="M15" s="118"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A16" s="106"/>
@@ -3914,10 +3940,10 @@
       </c>
       <c r="J17" s="117"/>
       <c r="K17" s="47"/>
-      <c r="L17" s="120" t="s">
+      <c r="L17" s="121" t="s">
         <v>12</v>
       </c>
-      <c r="M17" s="120"/>
+      <c r="M17" s="121"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A18" s="106"/>
@@ -3931,8 +3957,8 @@
       <c r="I18" s="117"/>
       <c r="J18" s="117"/>
       <c r="K18" s="30"/>
-      <c r="L18" s="120"/>
-      <c r="M18" s="120"/>
+      <c r="L18" s="121"/>
+      <c r="M18" s="121"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A19" s="106"/>
@@ -3979,10 +4005,10 @@
       </c>
       <c r="J20" s="117"/>
       <c r="K20" s="26"/>
-      <c r="L20" s="118" t="s">
+      <c r="L20" s="120" t="s">
         <v>12</v>
       </c>
-      <c r="M20" s="118"/>
+      <c r="M20" s="120"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A21" s="106"/>
@@ -3996,8 +4022,8 @@
       <c r="I21" s="117"/>
       <c r="J21" s="117"/>
       <c r="K21" s="48"/>
-      <c r="L21" s="118"/>
-      <c r="M21" s="118"/>
+      <c r="L21" s="120"/>
+      <c r="M21" s="120"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A22" s="106"/>
@@ -4019,15 +4045,69 @@
       </c>
       <c r="I22" s="113"/>
       <c r="J22" s="113"/>
-      <c r="K22" s="119">
+      <c r="K22" s="124">
         <f>K21-K20</f>
         <v>0</v>
       </c>
-      <c r="L22" s="119"/>
-      <c r="M22" s="119"/>
+      <c r="L22" s="124"/>
+      <c r="M22" s="124"/>
     </row>
   </sheetData>
   <mergeCells count="63">
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="C20:D21"/>
+    <mergeCell ref="F20:G21"/>
+    <mergeCell ref="I20:J21"/>
+    <mergeCell ref="L20:M21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="H22:J22"/>
+    <mergeCell ref="K22:M22"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="C17:D18"/>
+    <mergeCell ref="F17:G18"/>
+    <mergeCell ref="I17:J18"/>
+    <mergeCell ref="L17:M18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="K19:M19"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="C14:D15"/>
+    <mergeCell ref="F14:G15"/>
+    <mergeCell ref="I14:J15"/>
+    <mergeCell ref="L14:M15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="C11:D12"/>
+    <mergeCell ref="F11:G12"/>
+    <mergeCell ref="I11:J12"/>
+    <mergeCell ref="L11:M12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="C8:D9"/>
+    <mergeCell ref="F8:G9"/>
+    <mergeCell ref="I8:J9"/>
+    <mergeCell ref="L8:M9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="C5:D6"/>
+    <mergeCell ref="F5:G6"/>
+    <mergeCell ref="I5:J6"/>
+    <mergeCell ref="L5:M6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="K7:M7"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="C2:D3"/>
     <mergeCell ref="F2:G3"/>
@@ -4037,60 +4117,6 @@
     <mergeCell ref="E4:G4"/>
     <mergeCell ref="H4:J4"/>
     <mergeCell ref="K4:M4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="C5:D6"/>
-    <mergeCell ref="F5:G6"/>
-    <mergeCell ref="I5:J6"/>
-    <mergeCell ref="L5:M6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="C8:D9"/>
-    <mergeCell ref="F8:G9"/>
-    <mergeCell ref="I8:J9"/>
-    <mergeCell ref="L8:M9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="K10:M10"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="C11:D12"/>
-    <mergeCell ref="F11:G12"/>
-    <mergeCell ref="I11:J12"/>
-    <mergeCell ref="L11:M12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="K13:M13"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="C14:D15"/>
-    <mergeCell ref="F14:G15"/>
-    <mergeCell ref="I14:J15"/>
-    <mergeCell ref="L14:M15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="K16:M16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="C17:D18"/>
-    <mergeCell ref="F17:G18"/>
-    <mergeCell ref="I17:J18"/>
-    <mergeCell ref="L17:M18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="K19:M19"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="C20:D21"/>
-    <mergeCell ref="F20:G21"/>
-    <mergeCell ref="I20:J21"/>
-    <mergeCell ref="L20:M21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="H22:J22"/>
-    <mergeCell ref="K22:M22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -4119,7 +4145,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A1" s="129" t="s">
+      <c r="A1" s="125" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="77" t="s">
@@ -4161,7 +4187,7 @@
       <c r="N1" s="76"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A2" s="129"/>
+      <c r="A2" s="125"/>
       <c r="B2" s="85" t="s">
         <v>5</v>
       </c>
@@ -4208,63 +4234,63 @@
       </c>
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="99">
+      <c r="A3" s="101">
         <v>44571</v>
       </c>
       <c r="B3" s="23">
         <v>0.33333333333333298</v>
       </c>
-      <c r="C3" s="125" t="s">
+      <c r="C3" s="126" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="125"/>
+      <c r="D3" s="126"/>
       <c r="E3" s="24">
         <v>0.33333333333333298</v>
       </c>
-      <c r="F3" s="126" t="s">
+      <c r="F3" s="127" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="126"/>
+      <c r="G3" s="127"/>
       <c r="H3" s="25">
         <v>0.33333333333333298</v>
       </c>
-      <c r="I3" s="127" t="s">
+      <c r="I3" s="128" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="127"/>
+      <c r="J3" s="128"/>
       <c r="K3" s="26">
         <v>0.33333333333333298</v>
       </c>
-      <c r="L3" s="128" t="s">
+      <c r="L3" s="129" t="s">
         <v>21</v>
       </c>
-      <c r="M3" s="128"/>
+      <c r="M3" s="129"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A4" s="99"/>
+      <c r="A4" s="101"/>
       <c r="B4" s="27">
         <v>0.41666666666666702</v>
       </c>
-      <c r="C4" s="125"/>
-      <c r="D4" s="125"/>
+      <c r="C4" s="126"/>
+      <c r="D4" s="126"/>
       <c r="E4" s="28">
         <v>0.41666666666666702</v>
       </c>
-      <c r="F4" s="126"/>
-      <c r="G4" s="126"/>
+      <c r="F4" s="127"/>
+      <c r="G4" s="127"/>
       <c r="H4" s="29">
         <v>0.41666666666666702</v>
       </c>
-      <c r="I4" s="127"/>
-      <c r="J4" s="127"/>
+      <c r="I4" s="128"/>
+      <c r="J4" s="128"/>
       <c r="K4" s="30">
         <v>0.41666666666666702</v>
       </c>
-      <c r="L4" s="128"/>
-      <c r="M4" s="128"/>
+      <c r="L4" s="129"/>
+      <c r="M4" s="129"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A5" s="99"/>
+      <c r="A5" s="101"/>
       <c r="B5" s="31">
         <f>B4-B3</f>
         <v>8.3333333333334036E-2</v>
@@ -4291,63 +4317,63 @@
       <c r="M5" s="42"/>
     </row>
     <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="99">
+      <c r="A6" s="101">
         <v>44583</v>
       </c>
       <c r="B6" s="23">
         <v>0.79166666666666696</v>
       </c>
-      <c r="C6" s="125" t="s">
+      <c r="C6" s="126" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="125"/>
+      <c r="D6" s="126"/>
       <c r="E6" s="24">
         <v>0.82291666666666696</v>
       </c>
-      <c r="F6" s="126" t="s">
+      <c r="F6" s="127" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="126"/>
+      <c r="G6" s="127"/>
       <c r="H6" s="25">
         <v>0.79166666666666696</v>
       </c>
-      <c r="I6" s="127" t="s">
+      <c r="I6" s="128" t="s">
         <v>22</v>
       </c>
-      <c r="J6" s="127"/>
+      <c r="J6" s="128"/>
       <c r="K6" s="43">
         <v>0.79166666666666696</v>
       </c>
-      <c r="L6" s="128" t="s">
+      <c r="L6" s="129" t="s">
         <v>22</v>
       </c>
-      <c r="M6" s="128"/>
+      <c r="M6" s="129"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A7" s="99"/>
+      <c r="A7" s="101"/>
       <c r="B7" s="27">
         <v>0.89791666666666703</v>
       </c>
-      <c r="C7" s="125"/>
-      <c r="D7" s="125"/>
+      <c r="C7" s="126"/>
+      <c r="D7" s="126"/>
       <c r="E7" s="28">
         <v>0.89791666666666703</v>
       </c>
-      <c r="F7" s="126"/>
-      <c r="G7" s="126"/>
+      <c r="F7" s="127"/>
+      <c r="G7" s="127"/>
       <c r="H7" s="29">
         <v>0.89583333333333304</v>
       </c>
-      <c r="I7" s="127"/>
-      <c r="J7" s="127"/>
+      <c r="I7" s="128"/>
+      <c r="J7" s="128"/>
       <c r="K7" s="30">
         <v>0.89791666666666703</v>
       </c>
-      <c r="L7" s="128"/>
-      <c r="M7" s="128"/>
+      <c r="L7" s="129"/>
+      <c r="M7" s="129"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A8" s="99"/>
+      <c r="A8" s="101"/>
       <c r="B8" s="31">
         <f>B7-B6</f>
         <v>0.10625000000000007</v>
@@ -4374,63 +4400,63 @@
       <c r="M8" s="46"/>
     </row>
     <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="99">
+      <c r="A9" s="101">
         <v>44584</v>
       </c>
       <c r="B9" s="23">
         <v>0.75694444444444398</v>
       </c>
-      <c r="C9" s="125" t="s">
+      <c r="C9" s="126" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="125"/>
+      <c r="D9" s="126"/>
       <c r="E9" s="24">
         <v>0.75694444444444398</v>
       </c>
-      <c r="F9" s="126" t="s">
+      <c r="F9" s="127" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="126"/>
+      <c r="G9" s="127"/>
       <c r="H9" s="25">
         <v>0.75694444444444398</v>
       </c>
-      <c r="I9" s="127" t="s">
+      <c r="I9" s="128" t="s">
         <v>23</v>
       </c>
-      <c r="J9" s="127"/>
+      <c r="J9" s="128"/>
       <c r="K9" s="47">
         <v>0.75694444444444398</v>
       </c>
-      <c r="L9" s="128" t="s">
+      <c r="L9" s="129" t="s">
         <v>23</v>
       </c>
-      <c r="M9" s="128"/>
+      <c r="M9" s="129"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A10" s="99"/>
+      <c r="A10" s="101"/>
       <c r="B10" s="27">
         <v>0.83541666666666703</v>
       </c>
-      <c r="C10" s="125"/>
-      <c r="D10" s="125"/>
+      <c r="C10" s="126"/>
+      <c r="D10" s="126"/>
       <c r="E10" s="28">
         <v>0.83541666666666703</v>
       </c>
-      <c r="F10" s="126"/>
-      <c r="G10" s="126"/>
+      <c r="F10" s="127"/>
+      <c r="G10" s="127"/>
       <c r="H10" s="29">
         <v>0.83541666666666703</v>
       </c>
-      <c r="I10" s="127"/>
-      <c r="J10" s="127"/>
+      <c r="I10" s="128"/>
+      <c r="J10" s="128"/>
       <c r="K10" s="30">
         <v>0.83541666666666703</v>
       </c>
-      <c r="L10" s="128"/>
-      <c r="M10" s="128"/>
+      <c r="L10" s="129"/>
+      <c r="M10" s="129"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A11" s="99"/>
+      <c r="A11" s="101"/>
       <c r="B11" s="31">
         <f>(B10-B9)</f>
         <v>7.8472222222223054E-2</v>
@@ -4457,45 +4483,45 @@
       <c r="M11" s="46"/>
     </row>
     <row r="12" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="99"/>
+      <c r="A12" s="101"/>
       <c r="B12" s="23"/>
-      <c r="C12" s="125" t="s">
+      <c r="C12" s="126" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="125"/>
+      <c r="D12" s="126"/>
       <c r="E12" s="24"/>
-      <c r="F12" s="126" t="s">
+      <c r="F12" s="127" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="126"/>
+      <c r="G12" s="127"/>
       <c r="H12" s="25"/>
-      <c r="I12" s="127" t="s">
+      <c r="I12" s="128" t="s">
         <v>12</v>
       </c>
-      <c r="J12" s="127"/>
+      <c r="J12" s="128"/>
       <c r="K12" s="47"/>
-      <c r="L12" s="128" t="s">
+      <c r="L12" s="129" t="s">
         <v>12</v>
       </c>
-      <c r="M12" s="128"/>
+      <c r="M12" s="129"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A13" s="99"/>
+      <c r="A13" s="101"/>
       <c r="B13" s="27"/>
-      <c r="C13" s="125"/>
-      <c r="D13" s="125"/>
+      <c r="C13" s="126"/>
+      <c r="D13" s="126"/>
       <c r="E13" s="28"/>
-      <c r="F13" s="126"/>
-      <c r="G13" s="126"/>
+      <c r="F13" s="127"/>
+      <c r="G13" s="127"/>
       <c r="H13" s="29"/>
-      <c r="I13" s="127"/>
-      <c r="J13" s="127"/>
+      <c r="I13" s="128"/>
+      <c r="J13" s="128"/>
       <c r="K13" s="48"/>
-      <c r="L13" s="128"/>
-      <c r="M13" s="128"/>
+      <c r="L13" s="129"/>
+      <c r="M13" s="129"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A14" s="99"/>
+      <c r="A14" s="101"/>
       <c r="B14" s="31">
         <f>(B13-B12)</f>
         <v>0</v>
@@ -4522,45 +4548,45 @@
       <c r="M14" s="50"/>
     </row>
     <row r="15" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="99"/>
+      <c r="A15" s="101"/>
       <c r="B15" s="23"/>
-      <c r="C15" s="125" t="s">
+      <c r="C15" s="126" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="125"/>
+      <c r="D15" s="126"/>
       <c r="E15" s="24"/>
-      <c r="F15" s="126" t="s">
+      <c r="F15" s="127" t="s">
         <v>12</v>
       </c>
-      <c r="G15" s="126"/>
+      <c r="G15" s="127"/>
       <c r="H15" s="25"/>
-      <c r="I15" s="127" t="s">
+      <c r="I15" s="128" t="s">
         <v>12</v>
       </c>
-      <c r="J15" s="127"/>
+      <c r="J15" s="128"/>
       <c r="K15" s="26"/>
-      <c r="L15" s="128" t="s">
+      <c r="L15" s="129" t="s">
         <v>12</v>
       </c>
-      <c r="M15" s="128"/>
+      <c r="M15" s="129"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A16" s="99"/>
+      <c r="A16" s="101"/>
       <c r="B16" s="27"/>
-      <c r="C16" s="125"/>
-      <c r="D16" s="125"/>
+      <c r="C16" s="126"/>
+      <c r="D16" s="126"/>
       <c r="E16" s="28"/>
-      <c r="F16" s="126"/>
-      <c r="G16" s="126"/>
+      <c r="F16" s="127"/>
+      <c r="G16" s="127"/>
       <c r="H16" s="29"/>
-      <c r="I16" s="127"/>
-      <c r="J16" s="127"/>
+      <c r="I16" s="128"/>
+      <c r="J16" s="128"/>
       <c r="K16" s="30"/>
-      <c r="L16" s="128"/>
-      <c r="M16" s="128"/>
+      <c r="L16" s="129"/>
+      <c r="M16" s="129"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A17" s="99"/>
+      <c r="A17" s="101"/>
       <c r="B17" s="31">
         <f>(B16-B15)</f>
         <v>0</v>
@@ -4587,45 +4613,45 @@
       <c r="M17" s="46"/>
     </row>
     <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="99"/>
+      <c r="A18" s="101"/>
       <c r="B18" s="23"/>
-      <c r="C18" s="125" t="s">
+      <c r="C18" s="126" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="125"/>
+      <c r="D18" s="126"/>
       <c r="E18" s="24"/>
-      <c r="F18" s="126" t="s">
+      <c r="F18" s="127" t="s">
         <v>12</v>
       </c>
-      <c r="G18" s="126"/>
+      <c r="G18" s="127"/>
       <c r="H18" s="25"/>
-      <c r="I18" s="127" t="s">
+      <c r="I18" s="128" t="s">
         <v>12</v>
       </c>
-      <c r="J18" s="127"/>
+      <c r="J18" s="128"/>
       <c r="K18" s="47"/>
-      <c r="L18" s="128" t="s">
+      <c r="L18" s="129" t="s">
         <v>12</v>
       </c>
-      <c r="M18" s="128"/>
+      <c r="M18" s="129"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A19" s="99"/>
+      <c r="A19" s="101"/>
       <c r="B19" s="27"/>
-      <c r="C19" s="125"/>
-      <c r="D19" s="125"/>
+      <c r="C19" s="126"/>
+      <c r="D19" s="126"/>
       <c r="E19" s="28"/>
-      <c r="F19" s="126"/>
-      <c r="G19" s="126"/>
+      <c r="F19" s="127"/>
+      <c r="G19" s="127"/>
       <c r="H19" s="29"/>
-      <c r="I19" s="127"/>
-      <c r="J19" s="127"/>
+      <c r="I19" s="128"/>
+      <c r="J19" s="128"/>
       <c r="K19" s="30"/>
-      <c r="L19" s="128"/>
-      <c r="M19" s="128"/>
+      <c r="L19" s="129"/>
+      <c r="M19" s="129"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A20" s="99"/>
+      <c r="A20" s="101"/>
       <c r="B20" s="31">
         <f>(B19-B18)</f>
         <v>0</v>
@@ -4652,45 +4678,45 @@
       <c r="M20" s="46"/>
     </row>
     <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="99"/>
+      <c r="A21" s="101"/>
       <c r="B21" s="23"/>
-      <c r="C21" s="125" t="s">
+      <c r="C21" s="126" t="s">
         <v>12</v>
       </c>
-      <c r="D21" s="125"/>
+      <c r="D21" s="126"/>
       <c r="E21" s="24"/>
-      <c r="F21" s="126" t="s">
+      <c r="F21" s="127" t="s">
         <v>12</v>
       </c>
-      <c r="G21" s="126"/>
+      <c r="G21" s="127"/>
       <c r="H21" s="25"/>
-      <c r="I21" s="127" t="s">
+      <c r="I21" s="128" t="s">
         <v>12</v>
       </c>
-      <c r="J21" s="127"/>
+      <c r="J21" s="128"/>
       <c r="K21" s="26"/>
-      <c r="L21" s="128" t="s">
+      <c r="L21" s="129" t="s">
         <v>12</v>
       </c>
-      <c r="M21" s="128"/>
+      <c r="M21" s="129"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A22" s="99"/>
+      <c r="A22" s="101"/>
       <c r="B22" s="27"/>
-      <c r="C22" s="125"/>
-      <c r="D22" s="125"/>
+      <c r="C22" s="126"/>
+      <c r="D22" s="126"/>
       <c r="E22" s="28"/>
-      <c r="F22" s="126"/>
-      <c r="G22" s="126"/>
+      <c r="F22" s="127"/>
+      <c r="G22" s="127"/>
       <c r="H22" s="29"/>
-      <c r="I22" s="127"/>
-      <c r="J22" s="127"/>
+      <c r="I22" s="128"/>
+      <c r="J22" s="128"/>
       <c r="K22" s="48"/>
-      <c r="L22" s="128"/>
-      <c r="M22" s="128"/>
+      <c r="L22" s="129"/>
+      <c r="M22" s="129"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A23" s="99"/>
+      <c r="A23" s="101"/>
       <c r="B23" s="31">
         <f>(B22-B21)</f>
         <v>0</v>
@@ -4736,42 +4762,42 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="C3:D4"/>
-    <mergeCell ref="F3:G4"/>
-    <mergeCell ref="I3:J4"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="C21:D22"/>
+    <mergeCell ref="F21:G22"/>
+    <mergeCell ref="I21:J22"/>
+    <mergeCell ref="L21:M22"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="C18:D19"/>
+    <mergeCell ref="F18:G19"/>
+    <mergeCell ref="I18:J19"/>
+    <mergeCell ref="L18:M19"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="C15:D16"/>
+    <mergeCell ref="F15:G16"/>
+    <mergeCell ref="I15:J16"/>
+    <mergeCell ref="L15:M16"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="C12:D13"/>
+    <mergeCell ref="F12:G13"/>
+    <mergeCell ref="I12:J13"/>
+    <mergeCell ref="L12:M13"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="C9:D10"/>
+    <mergeCell ref="F9:G10"/>
+    <mergeCell ref="I9:J10"/>
+    <mergeCell ref="L9:M10"/>
     <mergeCell ref="L3:M4"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="C6:D7"/>
     <mergeCell ref="F6:G7"/>
     <mergeCell ref="I6:J7"/>
     <mergeCell ref="L6:M7"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="C9:D10"/>
-    <mergeCell ref="F9:G10"/>
-    <mergeCell ref="I9:J10"/>
-    <mergeCell ref="L9:M10"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="C12:D13"/>
-    <mergeCell ref="F12:G13"/>
-    <mergeCell ref="I12:J13"/>
-    <mergeCell ref="L12:M13"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="C15:D16"/>
-    <mergeCell ref="F15:G16"/>
-    <mergeCell ref="I15:J16"/>
-    <mergeCell ref="L15:M16"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="C18:D19"/>
-    <mergeCell ref="F18:G19"/>
-    <mergeCell ref="I18:J19"/>
-    <mergeCell ref="L18:M19"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="C21:D22"/>
-    <mergeCell ref="F21:G22"/>
-    <mergeCell ref="I21:J22"/>
-    <mergeCell ref="L21:M22"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="C3:D4"/>
+    <mergeCell ref="F3:G4"/>
+    <mergeCell ref="I3:J4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -4802,7 +4828,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A1" s="104" t="s">
+      <c r="A1" s="99" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -4841,13 +4867,13 @@
       <c r="M1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="105" t="s">
+      <c r="N1" s="100" t="s">
         <v>4</v>
       </c>
-      <c r="O1" s="105"/>
+      <c r="O1" s="100"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A2" s="104"/>
+      <c r="A2" s="99"/>
       <c r="B2" s="9" t="s">
         <v>5</v>
       </c>
@@ -4901,37 +4927,37 @@
       </c>
     </row>
     <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="99">
+      <c r="A3" s="101">
         <v>44585</v>
       </c>
       <c r="B3" s="23">
         <v>0.33333333333333298</v>
       </c>
-      <c r="C3" s="100" t="s">
+      <c r="C3" s="102" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="100"/>
+      <c r="D3" s="102"/>
       <c r="E3" s="24">
         <v>0.33333333333333298</v>
       </c>
-      <c r="F3" s="101" t="s">
+      <c r="F3" s="103" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="101"/>
+      <c r="G3" s="103"/>
       <c r="H3" s="25">
         <v>0.33333333333333298</v>
       </c>
-      <c r="I3" s="102" t="s">
+      <c r="I3" s="104" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="102"/>
+      <c r="J3" s="104"/>
       <c r="K3" s="26">
         <v>0.33333333333333298</v>
       </c>
-      <c r="L3" s="103" t="s">
+      <c r="L3" s="105" t="s">
         <v>24</v>
       </c>
-      <c r="M3" s="103"/>
+      <c r="M3" s="105"/>
       <c r="N3" s="21" t="s">
         <v>10</v>
       </c>
@@ -4941,30 +4967,30 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A4" s="99"/>
+      <c r="A4" s="101"/>
       <c r="B4" s="27">
         <v>0.41666666666666702</v>
       </c>
-      <c r="C4" s="100"/>
-      <c r="D4" s="100"/>
+      <c r="C4" s="102"/>
+      <c r="D4" s="102"/>
       <c r="E4" s="28">
         <v>0.41666666666666702</v>
       </c>
-      <c r="F4" s="101"/>
-      <c r="G4" s="101"/>
+      <c r="F4" s="103"/>
+      <c r="G4" s="103"/>
       <c r="H4" s="29">
         <v>0.41666666666666702</v>
       </c>
-      <c r="I4" s="102"/>
-      <c r="J4" s="102"/>
+      <c r="I4" s="104"/>
+      <c r="J4" s="104"/>
       <c r="K4" s="30">
         <v>0.41666666666666702</v>
       </c>
-      <c r="L4" s="103"/>
-      <c r="M4" s="103"/>
+      <c r="L4" s="105"/>
+      <c r="M4" s="105"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A5" s="99"/>
+      <c r="A5" s="101"/>
       <c r="B5" s="31">
         <f>B4-B3</f>
         <v>8.3333333333334036E-2</v>
@@ -4991,63 +5017,63 @@
       <c r="M5" s="42"/>
     </row>
     <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="99">
+      <c r="A6" s="101">
         <v>44585</v>
       </c>
       <c r="B6" s="23">
         <v>0.6875</v>
       </c>
-      <c r="C6" s="100" t="s">
+      <c r="C6" s="102" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="100"/>
+      <c r="D6" s="102"/>
       <c r="E6" s="24">
         <v>0.6875</v>
       </c>
-      <c r="F6" s="101" t="s">
+      <c r="F6" s="103" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="101"/>
+      <c r="G6" s="103"/>
       <c r="H6" s="25">
         <v>0.6875</v>
       </c>
-      <c r="I6" s="102" t="s">
+      <c r="I6" s="104" t="s">
         <v>25</v>
       </c>
-      <c r="J6" s="102"/>
+      <c r="J6" s="104"/>
       <c r="K6" s="43">
         <v>0.6875</v>
       </c>
-      <c r="L6" s="103" t="s">
+      <c r="L6" s="105" t="s">
         <v>26</v>
       </c>
-      <c r="M6" s="103"/>
+      <c r="M6" s="105"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A7" s="99"/>
+      <c r="A7" s="101"/>
       <c r="B7" s="27">
         <v>0.71875</v>
       </c>
-      <c r="C7" s="100"/>
-      <c r="D7" s="100"/>
+      <c r="C7" s="102"/>
+      <c r="D7" s="102"/>
       <c r="E7" s="28">
         <v>0.71875</v>
       </c>
-      <c r="F7" s="101"/>
-      <c r="G7" s="101"/>
+      <c r="F7" s="103"/>
+      <c r="G7" s="103"/>
       <c r="H7" s="29">
         <v>0.71875</v>
       </c>
-      <c r="I7" s="102"/>
-      <c r="J7" s="102"/>
+      <c r="I7" s="104"/>
+      <c r="J7" s="104"/>
       <c r="K7" s="30">
         <v>0.71875</v>
       </c>
-      <c r="L7" s="103"/>
-      <c r="M7" s="103"/>
+      <c r="L7" s="105"/>
+      <c r="M7" s="105"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A8" s="99"/>
+      <c r="A8" s="101"/>
       <c r="B8" s="31">
         <f>B7-B6</f>
         <v>3.125E-2</v>
@@ -5074,51 +5100,51 @@
       <c r="M8" s="46"/>
     </row>
     <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="99">
+      <c r="A9" s="101">
         <v>44586</v>
       </c>
       <c r="B9" s="23">
         <v>0.58333333333333304</v>
       </c>
-      <c r="C9" s="100" t="s">
+      <c r="C9" s="102" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="100"/>
+      <c r="D9" s="102"/>
       <c r="E9" s="24"/>
-      <c r="F9" s="101" t="s">
+      <c r="F9" s="103" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="101"/>
+      <c r="G9" s="103"/>
       <c r="H9" s="25"/>
-      <c r="I9" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="J9" s="102"/>
+      <c r="I9" s="104" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" s="104"/>
       <c r="K9" s="47"/>
-      <c r="L9" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="M9" s="103"/>
+      <c r="L9" s="105" t="s">
+        <v>11</v>
+      </c>
+      <c r="M9" s="105"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A10" s="99"/>
+      <c r="A10" s="101"/>
       <c r="B10" s="27">
         <v>0.6875</v>
       </c>
-      <c r="C10" s="100"/>
-      <c r="D10" s="100"/>
+      <c r="C10" s="102"/>
+      <c r="D10" s="102"/>
       <c r="E10" s="28"/>
-      <c r="F10" s="101"/>
-      <c r="G10" s="101"/>
+      <c r="F10" s="103"/>
+      <c r="G10" s="103"/>
       <c r="H10" s="29"/>
-      <c r="I10" s="102"/>
-      <c r="J10" s="102"/>
+      <c r="I10" s="104"/>
+      <c r="J10" s="104"/>
       <c r="K10" s="30"/>
-      <c r="L10" s="103"/>
-      <c r="M10" s="103"/>
+      <c r="L10" s="105"/>
+      <c r="M10" s="105"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A11" s="99"/>
+      <c r="A11" s="101"/>
       <c r="B11" s="31">
         <f>(B10-B9)</f>
         <v>0.10416666666666696</v>
@@ -5145,51 +5171,51 @@
       <c r="M11" s="46"/>
     </row>
     <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="99">
+      <c r="A12" s="101">
         <v>44588</v>
       </c>
       <c r="B12" s="23">
         <v>0.85416666666666696</v>
       </c>
-      <c r="C12" s="100" t="s">
+      <c r="C12" s="102" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="100"/>
+      <c r="D12" s="102"/>
       <c r="E12" s="24"/>
-      <c r="F12" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" s="101"/>
+      <c r="F12" s="103" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="103"/>
       <c r="H12" s="25"/>
-      <c r="I12" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="J12" s="102"/>
+      <c r="I12" s="104" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" s="104"/>
       <c r="K12" s="47"/>
-      <c r="L12" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="M12" s="103"/>
+      <c r="L12" s="105" t="s">
+        <v>11</v>
+      </c>
+      <c r="M12" s="105"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A13" s="99"/>
+      <c r="A13" s="101"/>
       <c r="B13" s="27">
         <v>0.89583333333333304</v>
       </c>
-      <c r="C13" s="100"/>
-      <c r="D13" s="100"/>
+      <c r="C13" s="102"/>
+      <c r="D13" s="102"/>
       <c r="E13" s="28"/>
-      <c r="F13" s="101"/>
-      <c r="G13" s="101"/>
+      <c r="F13" s="103"/>
+      <c r="G13" s="103"/>
       <c r="H13" s="29"/>
-      <c r="I13" s="102"/>
-      <c r="J13" s="102"/>
+      <c r="I13" s="104"/>
+      <c r="J13" s="104"/>
       <c r="K13" s="48"/>
-      <c r="L13" s="103"/>
-      <c r="M13" s="103"/>
+      <c r="L13" s="105"/>
+      <c r="M13" s="105"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A14" s="99"/>
+      <c r="A14" s="101"/>
       <c r="B14" s="31">
         <f>(B13-B12)</f>
         <v>4.1666666666666075E-2</v>
@@ -5216,51 +5242,51 @@
       <c r="M14" s="50"/>
     </row>
     <row r="15" spans="1:15" ht="13.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="99">
+      <c r="A15" s="101">
         <v>44591</v>
       </c>
       <c r="B15" s="23"/>
-      <c r="C15" s="100" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="100"/>
+      <c r="C15" s="102" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="102"/>
       <c r="E15" s="24"/>
-      <c r="F15" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="G15" s="101"/>
+      <c r="F15" s="103" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="103"/>
       <c r="H15" s="25"/>
-      <c r="I15" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="J15" s="102"/>
+      <c r="I15" s="104" t="s">
+        <v>11</v>
+      </c>
+      <c r="J15" s="104"/>
       <c r="K15" s="26">
         <v>0.33333333333333298</v>
       </c>
-      <c r="L15" s="103" t="s">
+      <c r="L15" s="105" t="s">
         <v>29</v>
       </c>
-      <c r="M15" s="103"/>
+      <c r="M15" s="105"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A16" s="99"/>
+      <c r="A16" s="101"/>
       <c r="B16" s="27"/>
-      <c r="C16" s="100"/>
-      <c r="D16" s="100"/>
+      <c r="C16" s="102"/>
+      <c r="D16" s="102"/>
       <c r="E16" s="28"/>
-      <c r="F16" s="101"/>
-      <c r="G16" s="101"/>
+      <c r="F16" s="103"/>
+      <c r="G16" s="103"/>
       <c r="H16" s="29"/>
-      <c r="I16" s="102"/>
-      <c r="J16" s="102"/>
+      <c r="I16" s="104"/>
+      <c r="J16" s="104"/>
       <c r="K16" s="30">
         <v>0.41666666666666702</v>
       </c>
-      <c r="L16" s="103"/>
-      <c r="M16" s="103"/>
+      <c r="L16" s="105"/>
+      <c r="M16" s="105"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A17" s="99"/>
+      <c r="A17" s="101"/>
       <c r="B17" s="31">
         <f>(B16-B15)</f>
         <v>0</v>
@@ -5287,63 +5313,63 @@
       <c r="M17" s="46"/>
     </row>
     <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="99">
+      <c r="A18" s="101">
         <v>44591</v>
       </c>
       <c r="B18" s="23">
         <v>0.70833333333333337</v>
       </c>
-      <c r="C18" s="100" t="s">
+      <c r="C18" s="102" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="100"/>
+      <c r="D18" s="102"/>
       <c r="E18" s="24">
         <v>0.70833333333333337</v>
       </c>
-      <c r="F18" s="101" t="s">
+      <c r="F18" s="103" t="s">
         <v>31</v>
       </c>
-      <c r="G18" s="101"/>
+      <c r="G18" s="103"/>
       <c r="H18" s="25">
         <v>0.61805555555555558</v>
       </c>
-      <c r="I18" s="102" t="s">
+      <c r="I18" s="104" t="s">
         <v>32</v>
       </c>
-      <c r="J18" s="102"/>
+      <c r="J18" s="104"/>
       <c r="K18" s="47">
         <v>0.70833333333333337</v>
       </c>
-      <c r="L18" s="103" t="s">
+      <c r="L18" s="105" t="s">
         <v>30</v>
       </c>
-      <c r="M18" s="103"/>
+      <c r="M18" s="105"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A19" s="99"/>
+      <c r="A19" s="101"/>
       <c r="B19" s="27">
         <v>0.92708333333333337</v>
       </c>
-      <c r="C19" s="100"/>
-      <c r="D19" s="100"/>
+      <c r="C19" s="102"/>
+      <c r="D19" s="102"/>
       <c r="E19" s="28">
         <v>0.92708333333333337</v>
       </c>
-      <c r="F19" s="101"/>
-      <c r="G19" s="101"/>
+      <c r="F19" s="103"/>
+      <c r="G19" s="103"/>
       <c r="H19" s="29">
         <v>0.92708333333333337</v>
       </c>
-      <c r="I19" s="102"/>
-      <c r="J19" s="102"/>
+      <c r="I19" s="104"/>
+      <c r="J19" s="104"/>
       <c r="K19" s="30">
         <v>0.92708333333333337</v>
       </c>
-      <c r="L19" s="103"/>
-      <c r="M19" s="103"/>
+      <c r="L19" s="105"/>
+      <c r="M19" s="105"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A20" s="99"/>
+      <c r="A20" s="101"/>
       <c r="B20" s="31">
         <f>(B19-B18)</f>
         <v>0.21875</v>
@@ -5370,63 +5396,63 @@
       <c r="M20" s="46"/>
     </row>
     <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="99">
+      <c r="A21" s="101">
         <v>44592</v>
       </c>
       <c r="B21" s="23">
         <v>0.375</v>
       </c>
-      <c r="C21" s="100" t="s">
+      <c r="C21" s="102" t="s">
         <v>30</v>
       </c>
-      <c r="D21" s="100"/>
+      <c r="D21" s="102"/>
       <c r="E21" s="24">
         <v>0.375</v>
       </c>
-      <c r="F21" s="101" t="s">
+      <c r="F21" s="103" t="s">
         <v>31</v>
       </c>
-      <c r="G21" s="101"/>
+      <c r="G21" s="103"/>
       <c r="H21" s="25">
         <v>0.375</v>
       </c>
-      <c r="I21" s="102" t="s">
+      <c r="I21" s="104" t="s">
         <v>32</v>
       </c>
-      <c r="J21" s="102"/>
+      <c r="J21" s="104"/>
       <c r="K21" s="26">
         <v>0.375</v>
       </c>
-      <c r="L21" s="103" t="s">
+      <c r="L21" s="105" t="s">
         <v>30</v>
       </c>
-      <c r="M21" s="103"/>
+      <c r="M21" s="105"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A22" s="99"/>
+      <c r="A22" s="101"/>
       <c r="B22" s="27">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C22" s="100"/>
-      <c r="D22" s="100"/>
+      <c r="C22" s="102"/>
+      <c r="D22" s="102"/>
       <c r="E22" s="28">
         <v>0.41666666666666669</v>
       </c>
-      <c r="F22" s="101"/>
-      <c r="G22" s="101"/>
+      <c r="F22" s="103"/>
+      <c r="G22" s="103"/>
       <c r="H22" s="29">
         <v>0.41666666666666669</v>
       </c>
-      <c r="I22" s="102"/>
-      <c r="J22" s="102"/>
+      <c r="I22" s="104"/>
+      <c r="J22" s="104"/>
       <c r="K22" s="48">
         <v>0.41666666666666669</v>
       </c>
-      <c r="L22" s="103"/>
-      <c r="M22" s="103"/>
+      <c r="L22" s="105"/>
+      <c r="M22" s="105"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A23" s="99"/>
+      <c r="A23" s="101"/>
       <c r="B23" s="31">
         <f>(B22-B21)</f>
         <v>4.1666666666666685E-2</v>
@@ -5453,63 +5479,63 @@
       <c r="M23" s="52"/>
     </row>
     <row r="24" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="99">
+      <c r="A24" s="101">
         <v>44592</v>
       </c>
       <c r="B24" s="23">
         <v>0.625</v>
       </c>
-      <c r="C24" s="100" t="s">
+      <c r="C24" s="102" t="s">
         <v>30</v>
       </c>
-      <c r="D24" s="100"/>
+      <c r="D24" s="102"/>
       <c r="E24" s="24">
         <v>0.625</v>
       </c>
-      <c r="F24" s="101" t="s">
+      <c r="F24" s="103" t="s">
         <v>31</v>
       </c>
-      <c r="G24" s="101"/>
+      <c r="G24" s="103"/>
       <c r="H24" s="25">
         <v>0.625</v>
       </c>
-      <c r="I24" s="102" t="s">
+      <c r="I24" s="104" t="s">
         <v>33</v>
       </c>
-      <c r="J24" s="102"/>
+      <c r="J24" s="104"/>
       <c r="K24" s="26">
         <v>0.625</v>
       </c>
-      <c r="L24" s="103" t="s">
+      <c r="L24" s="105" t="s">
         <v>34</v>
       </c>
-      <c r="M24" s="103"/>
+      <c r="M24" s="105"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A25" s="99"/>
+      <c r="A25" s="101"/>
       <c r="B25" s="27">
         <v>0.75</v>
       </c>
-      <c r="C25" s="100"/>
-      <c r="D25" s="100"/>
+      <c r="C25" s="102"/>
+      <c r="D25" s="102"/>
       <c r="E25" s="28">
         <v>0.75</v>
       </c>
-      <c r="F25" s="101"/>
-      <c r="G25" s="101"/>
+      <c r="F25" s="103"/>
+      <c r="G25" s="103"/>
       <c r="H25" s="29">
         <v>0.70833333333333337</v>
       </c>
-      <c r="I25" s="102"/>
-      <c r="J25" s="102"/>
+      <c r="I25" s="104"/>
+      <c r="J25" s="104"/>
       <c r="K25" s="30">
         <v>0.75</v>
       </c>
-      <c r="L25" s="103"/>
-      <c r="M25" s="103"/>
+      <c r="L25" s="105"/>
+      <c r="M25" s="105"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A26" s="99"/>
+      <c r="A26" s="101"/>
       <c r="B26" s="31">
         <f>(B25-B24)</f>
         <v>0.125</v>
@@ -5536,63 +5562,63 @@
       <c r="M26" s="46"/>
     </row>
     <row r="27" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="99">
+      <c r="A27" s="101">
         <v>44594</v>
       </c>
       <c r="B27" s="23">
         <v>0.5</v>
       </c>
-      <c r="C27" s="100" t="s">
-        <v>11</v>
-      </c>
-      <c r="D27" s="100"/>
+      <c r="C27" s="102" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="102"/>
       <c r="E27" s="24">
         <v>0.5</v>
       </c>
-      <c r="F27" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="G27" s="101"/>
+      <c r="F27" s="103" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" s="103"/>
       <c r="H27" s="25">
         <v>0.5</v>
       </c>
-      <c r="I27" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="J27" s="102"/>
+      <c r="I27" s="104" t="s">
+        <v>11</v>
+      </c>
+      <c r="J27" s="104"/>
       <c r="K27" s="47">
         <v>0.5</v>
       </c>
-      <c r="L27" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="M27" s="103"/>
+      <c r="L27" s="105" t="s">
+        <v>11</v>
+      </c>
+      <c r="M27" s="105"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A28" s="99"/>
+      <c r="A28" s="101"/>
       <c r="B28" s="27">
         <v>0.53125</v>
       </c>
-      <c r="C28" s="100"/>
-      <c r="D28" s="100"/>
+      <c r="C28" s="102"/>
+      <c r="D28" s="102"/>
       <c r="E28" s="28">
         <v>0.53125</v>
       </c>
-      <c r="F28" s="101"/>
-      <c r="G28" s="101"/>
+      <c r="F28" s="103"/>
+      <c r="G28" s="103"/>
       <c r="H28" s="29">
         <v>0.53125</v>
       </c>
-      <c r="I28" s="102"/>
-      <c r="J28" s="102"/>
+      <c r="I28" s="104"/>
+      <c r="J28" s="104"/>
       <c r="K28" s="30">
         <v>0.53125</v>
       </c>
-      <c r="L28" s="103"/>
-      <c r="M28" s="103"/>
+      <c r="L28" s="105"/>
+      <c r="M28" s="105"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A29" s="99"/>
+      <c r="A29" s="101"/>
       <c r="B29" s="31">
         <f>(B28-B27)</f>
         <v>3.125E-2</v>
@@ -5619,63 +5645,63 @@
       <c r="M29" s="46"/>
     </row>
     <row r="30" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="99">
+      <c r="A30" s="101">
         <v>44597</v>
       </c>
       <c r="B30" s="23">
         <v>0.75</v>
       </c>
-      <c r="C30" s="100" t="s">
+      <c r="C30" s="102" t="s">
         <v>37</v>
       </c>
-      <c r="D30" s="100"/>
+      <c r="D30" s="102"/>
       <c r="E30" s="24">
         <v>0.75</v>
       </c>
-      <c r="F30" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="G30" s="101"/>
+      <c r="F30" s="103" t="s">
+        <v>11</v>
+      </c>
+      <c r="G30" s="103"/>
       <c r="H30" s="25">
         <v>0.75</v>
       </c>
-      <c r="I30" s="102" t="s">
+      <c r="I30" s="104" t="s">
         <v>35</v>
       </c>
-      <c r="J30" s="102"/>
+      <c r="J30" s="104"/>
       <c r="K30" s="26">
         <v>0.75</v>
       </c>
-      <c r="L30" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="M30" s="103"/>
+      <c r="L30" s="105" t="s">
+        <v>11</v>
+      </c>
+      <c r="M30" s="105"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A31" s="99"/>
+      <c r="A31" s="101"/>
       <c r="B31" s="27">
         <v>0.95833333333333337</v>
       </c>
-      <c r="C31" s="100"/>
-      <c r="D31" s="100"/>
+      <c r="C31" s="102"/>
+      <c r="D31" s="102"/>
       <c r="E31" s="28">
         <v>0.95833333333333337</v>
       </c>
-      <c r="F31" s="101"/>
-      <c r="G31" s="101"/>
+      <c r="F31" s="103"/>
+      <c r="G31" s="103"/>
       <c r="H31" s="29">
         <v>0.9375</v>
       </c>
-      <c r="I31" s="102"/>
-      <c r="J31" s="102"/>
+      <c r="I31" s="104"/>
+      <c r="J31" s="104"/>
       <c r="K31" s="48">
         <v>0.95833333333333337</v>
       </c>
-      <c r="L31" s="103"/>
-      <c r="M31" s="103"/>
+      <c r="L31" s="105"/>
+      <c r="M31" s="105"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A32" s="99"/>
+      <c r="A32" s="101"/>
       <c r="B32" s="31">
         <f>(B31-B30)</f>
         <v>0.20833333333333337</v>
@@ -5702,59 +5728,59 @@
       <c r="M32" s="52"/>
     </row>
     <row r="33" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="99">
+      <c r="A33" s="101">
         <v>44598</v>
       </c>
       <c r="B33" s="23">
         <v>0.89583333333333337</v>
       </c>
-      <c r="C33" s="100" t="s">
+      <c r="C33" s="102" t="s">
         <v>38</v>
       </c>
-      <c r="D33" s="100"/>
+      <c r="D33" s="102"/>
       <c r="E33" s="24"/>
-      <c r="F33" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="G33" s="101"/>
+      <c r="F33" s="103" t="s">
+        <v>11</v>
+      </c>
+      <c r="G33" s="103"/>
       <c r="H33" s="25">
         <v>0.83333333333333337</v>
       </c>
-      <c r="I33" s="102" t="s">
+      <c r="I33" s="104" t="s">
         <v>35</v>
       </c>
-      <c r="J33" s="102"/>
+      <c r="J33" s="104"/>
       <c r="K33" s="26">
         <v>0.41666666666666669</v>
       </c>
-      <c r="L33" s="103" t="s">
+      <c r="L33" s="105" t="s">
         <v>36</v>
       </c>
-      <c r="M33" s="103"/>
+      <c r="M33" s="105"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A34" s="99"/>
+      <c r="A34" s="101"/>
       <c r="B34" s="27">
         <v>0.98611111111111116</v>
       </c>
-      <c r="C34" s="100"/>
-      <c r="D34" s="100"/>
+      <c r="C34" s="102"/>
+      <c r="D34" s="102"/>
       <c r="E34" s="28"/>
-      <c r="F34" s="101"/>
-      <c r="G34" s="101"/>
+      <c r="F34" s="103"/>
+      <c r="G34" s="103"/>
       <c r="H34" s="29">
         <v>1</v>
       </c>
-      <c r="I34" s="102"/>
-      <c r="J34" s="102"/>
+      <c r="I34" s="104"/>
+      <c r="J34" s="104"/>
       <c r="K34" s="30">
         <v>0.75</v>
       </c>
-      <c r="L34" s="103"/>
-      <c r="M34" s="103"/>
+      <c r="L34" s="105"/>
+      <c r="M34" s="105"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A35" s="99"/>
+      <c r="A35" s="101"/>
       <c r="B35" s="31">
         <f>(B34-B33)</f>
         <v>9.027777777777779E-2</v>
@@ -5781,45 +5807,45 @@
       <c r="M35" s="46"/>
     </row>
     <row r="36" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="99"/>
+      <c r="A36" s="101"/>
       <c r="B36" s="23"/>
-      <c r="C36" s="100" t="s">
-        <v>11</v>
-      </c>
-      <c r="D36" s="100"/>
+      <c r="C36" s="102" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" s="102"/>
       <c r="E36" s="24"/>
-      <c r="F36" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="G36" s="101"/>
+      <c r="F36" s="103" t="s">
+        <v>11</v>
+      </c>
+      <c r="G36" s="103"/>
       <c r="H36" s="25"/>
-      <c r="I36" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="J36" s="102"/>
+      <c r="I36" s="104" t="s">
+        <v>11</v>
+      </c>
+      <c r="J36" s="104"/>
       <c r="K36" s="47"/>
-      <c r="L36" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="M36" s="103"/>
+      <c r="L36" s="105" t="s">
+        <v>11</v>
+      </c>
+      <c r="M36" s="105"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A37" s="99"/>
+      <c r="A37" s="101"/>
       <c r="B37" s="27"/>
-      <c r="C37" s="100"/>
-      <c r="D37" s="100"/>
+      <c r="C37" s="102"/>
+      <c r="D37" s="102"/>
       <c r="E37" s="28"/>
-      <c r="F37" s="101"/>
-      <c r="G37" s="101"/>
+      <c r="F37" s="103"/>
+      <c r="G37" s="103"/>
       <c r="H37" s="29"/>
-      <c r="I37" s="102"/>
-      <c r="J37" s="102"/>
+      <c r="I37" s="104"/>
+      <c r="J37" s="104"/>
       <c r="K37" s="30"/>
-      <c r="L37" s="103"/>
-      <c r="M37" s="103"/>
+      <c r="L37" s="105"/>
+      <c r="M37" s="105"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A38" s="99"/>
+      <c r="A38" s="101"/>
       <c r="B38" s="31">
         <f>(B37-B36)</f>
         <v>0</v>
@@ -5846,45 +5872,45 @@
       <c r="M38" s="46"/>
     </row>
     <row r="39" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="99"/>
+      <c r="A39" s="101"/>
       <c r="B39" s="23"/>
-      <c r="C39" s="100" t="s">
-        <v>11</v>
-      </c>
-      <c r="D39" s="100"/>
+      <c r="C39" s="102" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" s="102"/>
       <c r="E39" s="24"/>
-      <c r="F39" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="G39" s="101"/>
+      <c r="F39" s="103" t="s">
+        <v>11</v>
+      </c>
+      <c r="G39" s="103"/>
       <c r="H39" s="25"/>
-      <c r="I39" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="J39" s="102"/>
+      <c r="I39" s="104" t="s">
+        <v>11</v>
+      </c>
+      <c r="J39" s="104"/>
       <c r="K39" s="26"/>
-      <c r="L39" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="M39" s="103"/>
+      <c r="L39" s="105" t="s">
+        <v>11</v>
+      </c>
+      <c r="M39" s="105"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A40" s="99"/>
+      <c r="A40" s="101"/>
       <c r="B40" s="27"/>
-      <c r="C40" s="100"/>
-      <c r="D40" s="100"/>
+      <c r="C40" s="102"/>
+      <c r="D40" s="102"/>
       <c r="E40" s="28"/>
-      <c r="F40" s="101"/>
-      <c r="G40" s="101"/>
+      <c r="F40" s="103"/>
+      <c r="G40" s="103"/>
       <c r="H40" s="29"/>
-      <c r="I40" s="102"/>
-      <c r="J40" s="102"/>
+      <c r="I40" s="104"/>
+      <c r="J40" s="104"/>
       <c r="K40" s="48"/>
-      <c r="L40" s="103"/>
-      <c r="M40" s="103"/>
+      <c r="L40" s="105"/>
+      <c r="M40" s="105"/>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A41" s="99"/>
+      <c r="A41" s="101"/>
       <c r="B41" s="31">
         <f>(B40-B39)</f>
         <v>0</v>
@@ -5912,6 +5938,66 @@
     </row>
   </sheetData>
   <mergeCells count="67">
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="C39:D40"/>
+    <mergeCell ref="F39:G40"/>
+    <mergeCell ref="I39:J40"/>
+    <mergeCell ref="L39:M40"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="C36:D37"/>
+    <mergeCell ref="F36:G37"/>
+    <mergeCell ref="I36:J37"/>
+    <mergeCell ref="L36:M37"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="C33:D34"/>
+    <mergeCell ref="F33:G34"/>
+    <mergeCell ref="I33:J34"/>
+    <mergeCell ref="L33:M34"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="C30:D31"/>
+    <mergeCell ref="F30:G31"/>
+    <mergeCell ref="I30:J31"/>
+    <mergeCell ref="L30:M31"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="C27:D28"/>
+    <mergeCell ref="F27:G28"/>
+    <mergeCell ref="I27:J28"/>
+    <mergeCell ref="L27:M28"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="C24:D25"/>
+    <mergeCell ref="F24:G25"/>
+    <mergeCell ref="I24:J25"/>
+    <mergeCell ref="L24:M25"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="C21:D22"/>
+    <mergeCell ref="F21:G22"/>
+    <mergeCell ref="I21:J22"/>
+    <mergeCell ref="L21:M22"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="C18:D19"/>
+    <mergeCell ref="F18:G19"/>
+    <mergeCell ref="I18:J19"/>
+    <mergeCell ref="L18:M19"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="C15:D16"/>
+    <mergeCell ref="F15:G16"/>
+    <mergeCell ref="I15:J16"/>
+    <mergeCell ref="L15:M16"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="C12:D13"/>
+    <mergeCell ref="F12:G13"/>
+    <mergeCell ref="I12:J13"/>
+    <mergeCell ref="L12:M13"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="C9:D10"/>
+    <mergeCell ref="F9:G10"/>
+    <mergeCell ref="I9:J10"/>
+    <mergeCell ref="L9:M10"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="C6:D7"/>
+    <mergeCell ref="F6:G7"/>
+    <mergeCell ref="I6:J7"/>
+    <mergeCell ref="L6:M7"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="A3:A5"/>
@@ -5919,66 +6005,6 @@
     <mergeCell ref="F3:G4"/>
     <mergeCell ref="I3:J4"/>
     <mergeCell ref="L3:M4"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="C6:D7"/>
-    <mergeCell ref="F6:G7"/>
-    <mergeCell ref="I6:J7"/>
-    <mergeCell ref="L6:M7"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="C9:D10"/>
-    <mergeCell ref="F9:G10"/>
-    <mergeCell ref="I9:J10"/>
-    <mergeCell ref="L9:M10"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="C12:D13"/>
-    <mergeCell ref="F12:G13"/>
-    <mergeCell ref="I12:J13"/>
-    <mergeCell ref="L12:M13"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="C15:D16"/>
-    <mergeCell ref="F15:G16"/>
-    <mergeCell ref="I15:J16"/>
-    <mergeCell ref="L15:M16"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="C18:D19"/>
-    <mergeCell ref="F18:G19"/>
-    <mergeCell ref="I18:J19"/>
-    <mergeCell ref="L18:M19"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="C21:D22"/>
-    <mergeCell ref="F21:G22"/>
-    <mergeCell ref="I21:J22"/>
-    <mergeCell ref="L21:M22"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="C24:D25"/>
-    <mergeCell ref="F24:G25"/>
-    <mergeCell ref="I24:J25"/>
-    <mergeCell ref="L24:M25"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="C27:D28"/>
-    <mergeCell ref="F27:G28"/>
-    <mergeCell ref="I27:J28"/>
-    <mergeCell ref="L27:M28"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="C30:D31"/>
-    <mergeCell ref="F30:G31"/>
-    <mergeCell ref="I30:J31"/>
-    <mergeCell ref="L30:M31"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="C33:D34"/>
-    <mergeCell ref="F33:G34"/>
-    <mergeCell ref="I33:J34"/>
-    <mergeCell ref="L33:M34"/>
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="C36:D37"/>
-    <mergeCell ref="F36:G37"/>
-    <mergeCell ref="I36:J37"/>
-    <mergeCell ref="L36:M37"/>
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="C39:D40"/>
-    <mergeCell ref="F39:G40"/>
-    <mergeCell ref="I39:J40"/>
-    <mergeCell ref="L39:M40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5990,7 +6016,7 @@
   <dimension ref="A1:O41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A23" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.69140625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -6009,7 +6035,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="104" t="s">
+      <c r="A1" s="99" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -6048,23 +6074,23 @@
       <c r="M1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="105" t="s">
+      <c r="N1" s="100" t="s">
         <v>4</v>
       </c>
-      <c r="O1" s="105"/>
+      <c r="O1" s="100"/>
     </row>
     <row r="2" spans="1:15" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="104"/>
+      <c r="A2" s="99"/>
       <c r="B2" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="10">
         <f t="array" ref="C2">SUM(B5:B41*(MOD(ROW(B5:B41)-2,3)=0))</f>
-        <v>1.1562500000000002</v>
+        <v>1.2187500000000002</v>
       </c>
       <c r="D2" s="11">
         <f>C2+Sprint_4!D2</f>
-        <v>3.4958333333333362</v>
+        <v>3.5583333333333362</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>6</v>
@@ -6104,66 +6130,66 @@
       </c>
       <c r="O2" s="22">
         <f>C2+F2+I2+L2</f>
-        <v>2.3854166666666674</v>
+        <v>2.4479166666666674</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="99">
+      <c r="A3" s="101">
         <v>44599</v>
       </c>
       <c r="B3" s="23">
         <v>0.33333333333333298</v>
       </c>
-      <c r="C3" s="100" t="s">
+      <c r="C3" s="102" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="100"/>
+      <c r="D3" s="102"/>
       <c r="E3" s="24"/>
-      <c r="F3" s="101" t="s">
+      <c r="F3" s="103" t="s">
         <v>39</v>
       </c>
-      <c r="G3" s="101"/>
+      <c r="G3" s="103"/>
       <c r="H3" s="25">
         <v>0.33333333333333298</v>
       </c>
-      <c r="I3" s="102" t="s">
+      <c r="I3" s="104" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="102"/>
+      <c r="J3" s="104"/>
       <c r="K3" s="26"/>
-      <c r="L3" s="103" t="s">
+      <c r="L3" s="105" t="s">
         <v>13</v>
       </c>
-      <c r="M3" s="103"/>
+      <c r="M3" s="105"/>
       <c r="N3" s="21" t="s">
         <v>10</v>
       </c>
       <c r="O3" s="22">
         <f>D2+G2+J2+M2</f>
-        <v>11.159027777777794</v>
+        <v>11.221527777777794</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="99"/>
+      <c r="A4" s="101"/>
       <c r="B4" s="27">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C4" s="100"/>
-      <c r="D4" s="100"/>
+      <c r="C4" s="102"/>
+      <c r="D4" s="102"/>
       <c r="E4" s="28"/>
-      <c r="F4" s="101"/>
-      <c r="G4" s="101"/>
+      <c r="F4" s="103"/>
+      <c r="G4" s="103"/>
       <c r="H4" s="29">
         <v>0.41666666666666702</v>
       </c>
-      <c r="I4" s="102"/>
-      <c r="J4" s="102"/>
+      <c r="I4" s="104"/>
+      <c r="J4" s="104"/>
       <c r="K4" s="30"/>
-      <c r="L4" s="103"/>
-      <c r="M4" s="103"/>
+      <c r="L4" s="105"/>
+      <c r="M4" s="105"/>
     </row>
     <row r="5" spans="1:15" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="99"/>
+      <c r="A5" s="101"/>
       <c r="B5" s="31">
         <f>B4-B3</f>
         <v>8.3333333333333703E-2</v>
@@ -6190,59 +6216,59 @@
       <c r="M5" s="42"/>
     </row>
     <row r="6" spans="1:15" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="99">
+      <c r="A6" s="101">
         <v>44599</v>
       </c>
       <c r="B6" s="23">
         <v>0.60763888888888895</v>
       </c>
-      <c r="C6" s="100" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="100"/>
+      <c r="C6" s="102" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="102"/>
       <c r="E6" s="24"/>
-      <c r="F6" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="101"/>
+      <c r="F6" s="103" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="103"/>
       <c r="H6" s="25">
         <v>0.60763888888888895</v>
       </c>
-      <c r="I6" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="J6" s="102"/>
+      <c r="I6" s="104" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="104"/>
       <c r="K6" s="43">
         <v>0.60763888888888895</v>
       </c>
-      <c r="L6" s="103" t="s">
+      <c r="L6" s="105" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="103"/>
+      <c r="M6" s="105"/>
     </row>
     <row r="7" spans="1:15" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="99"/>
+      <c r="A7" s="101"/>
       <c r="B7" s="27">
         <v>0.71875</v>
       </c>
-      <c r="C7" s="100"/>
-      <c r="D7" s="100"/>
+      <c r="C7" s="102"/>
+      <c r="D7" s="102"/>
       <c r="E7" s="28"/>
-      <c r="F7" s="101"/>
-      <c r="G7" s="101"/>
+      <c r="F7" s="103"/>
+      <c r="G7" s="103"/>
       <c r="H7" s="29">
         <v>0.71875</v>
       </c>
-      <c r="I7" s="102"/>
-      <c r="J7" s="102"/>
+      <c r="I7" s="104"/>
+      <c r="J7" s="104"/>
       <c r="K7" s="30">
         <v>0.71875</v>
       </c>
-      <c r="L7" s="103"/>
-      <c r="M7" s="103"/>
+      <c r="L7" s="105"/>
+      <c r="M7" s="105"/>
     </row>
     <row r="8" spans="1:15" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="99"/>
+      <c r="A8" s="101"/>
       <c r="B8" s="31">
         <f>B7-B6</f>
         <v>0.11111111111111105</v>
@@ -6269,59 +6295,59 @@
       <c r="M8" s="46"/>
     </row>
     <row r="9" spans="1:15" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="99">
+      <c r="A9" s="101">
         <v>44601</v>
       </c>
       <c r="B9" s="23">
         <v>0.49305555555555558</v>
       </c>
-      <c r="C9" s="100" t="s">
+      <c r="C9" s="102" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="100"/>
+      <c r="D9" s="102"/>
       <c r="E9" s="24"/>
-      <c r="F9" s="101" t="s">
+      <c r="F9" s="103" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="101"/>
+      <c r="G9" s="103"/>
       <c r="H9" s="25">
         <v>0.49305555555555558</v>
       </c>
-      <c r="I9" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="J9" s="102"/>
+      <c r="I9" s="104" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" s="104"/>
       <c r="K9" s="47">
         <v>0.49305555555555558</v>
       </c>
-      <c r="L9" s="103" t="s">
+      <c r="L9" s="105" t="s">
         <v>39</v>
       </c>
-      <c r="M9" s="103"/>
+      <c r="M9" s="105"/>
     </row>
     <row r="10" spans="1:15" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="99"/>
+      <c r="A10" s="101"/>
       <c r="B10" s="27">
         <v>0.52777777777777779</v>
       </c>
-      <c r="C10" s="100"/>
-      <c r="D10" s="100"/>
+      <c r="C10" s="102"/>
+      <c r="D10" s="102"/>
       <c r="E10" s="28"/>
-      <c r="F10" s="101"/>
-      <c r="G10" s="101"/>
+      <c r="F10" s="103"/>
+      <c r="G10" s="103"/>
       <c r="H10" s="29">
         <v>0.52777777777777779</v>
       </c>
-      <c r="I10" s="102"/>
-      <c r="J10" s="102"/>
+      <c r="I10" s="104"/>
+      <c r="J10" s="104"/>
       <c r="K10" s="30">
         <v>0.52777777777777779</v>
       </c>
-      <c r="L10" s="103"/>
-      <c r="M10" s="103"/>
+      <c r="L10" s="105"/>
+      <c r="M10" s="105"/>
     </row>
     <row r="11" spans="1:15" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="99"/>
+      <c r="A11" s="101"/>
       <c r="B11" s="31">
         <f>(B10-B9)</f>
         <v>3.472222222222221E-2</v>
@@ -6348,59 +6374,59 @@
       <c r="M11" s="46"/>
     </row>
     <row r="12" spans="1:15" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="99">
+      <c r="A12" s="101">
         <v>44606</v>
       </c>
       <c r="B12" s="23">
         <v>0.33333333333333331</v>
       </c>
-      <c r="C12" s="100" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="100"/>
+      <c r="C12" s="102" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="102"/>
       <c r="E12" s="24"/>
-      <c r="F12" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" s="101"/>
+      <c r="F12" s="103" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="103"/>
       <c r="H12" s="25">
         <v>0.33333333333333331</v>
       </c>
-      <c r="I12" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="J12" s="102"/>
+      <c r="I12" s="104" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" s="104"/>
       <c r="K12" s="47">
         <v>0.33333333333333331</v>
       </c>
-      <c r="L12" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="M12" s="103"/>
+      <c r="L12" s="105" t="s">
+        <v>11</v>
+      </c>
+      <c r="M12" s="105"/>
     </row>
     <row r="13" spans="1:15" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="99"/>
+      <c r="A13" s="101"/>
       <c r="B13" s="27">
         <v>0.40625</v>
       </c>
-      <c r="C13" s="100"/>
-      <c r="D13" s="100"/>
+      <c r="C13" s="102"/>
+      <c r="D13" s="102"/>
       <c r="E13" s="28"/>
-      <c r="F13" s="101"/>
-      <c r="G13" s="101"/>
+      <c r="F13" s="103"/>
+      <c r="G13" s="103"/>
       <c r="H13" s="29">
         <v>0.40625</v>
       </c>
-      <c r="I13" s="102"/>
-      <c r="J13" s="102"/>
+      <c r="I13" s="104"/>
+      <c r="J13" s="104"/>
       <c r="K13" s="48">
         <v>0.40625</v>
       </c>
-      <c r="L13" s="103"/>
-      <c r="M13" s="103"/>
+      <c r="L13" s="105"/>
+      <c r="M13" s="105"/>
     </row>
     <row r="14" spans="1:15" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="99"/>
+      <c r="A14" s="101"/>
       <c r="B14" s="31">
         <f>(B13-B12)</f>
         <v>7.2916666666666685E-2</v>
@@ -6427,59 +6453,59 @@
       <c r="M14" s="97"/>
     </row>
     <row r="15" spans="1:15" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="99">
+      <c r="A15" s="101">
         <v>44606</v>
       </c>
       <c r="B15" s="23">
         <v>0.60763888888888895</v>
       </c>
-      <c r="C15" s="100" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="100"/>
+      <c r="C15" s="102" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="102"/>
       <c r="E15" s="24"/>
-      <c r="F15" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="G15" s="101"/>
+      <c r="F15" s="103" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="103"/>
       <c r="H15" s="25">
         <v>0.60763888888888895</v>
       </c>
-      <c r="I15" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="J15" s="102"/>
+      <c r="I15" s="104" t="s">
+        <v>11</v>
+      </c>
+      <c r="J15" s="104"/>
       <c r="K15" s="26">
         <v>0.60763888888888895</v>
       </c>
-      <c r="L15" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="M15" s="103"/>
+      <c r="L15" s="105" t="s">
+        <v>11</v>
+      </c>
+      <c r="M15" s="105"/>
     </row>
     <row r="16" spans="1:15" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="99"/>
+      <c r="A16" s="101"/>
       <c r="B16" s="27">
         <v>0.71875</v>
       </c>
-      <c r="C16" s="100"/>
-      <c r="D16" s="100"/>
+      <c r="C16" s="102"/>
+      <c r="D16" s="102"/>
       <c r="E16" s="28"/>
-      <c r="F16" s="101"/>
-      <c r="G16" s="101"/>
+      <c r="F16" s="103"/>
+      <c r="G16" s="103"/>
       <c r="H16" s="29">
         <v>0.71875</v>
       </c>
-      <c r="I16" s="102"/>
-      <c r="J16" s="102"/>
+      <c r="I16" s="104"/>
+      <c r="J16" s="104"/>
       <c r="K16" s="30">
         <v>0.71875</v>
       </c>
-      <c r="L16" s="103"/>
-      <c r="M16" s="103"/>
+      <c r="L16" s="105"/>
+      <c r="M16" s="105"/>
     </row>
     <row r="17" spans="1:13" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="99"/>
+      <c r="A17" s="101"/>
       <c r="B17" s="31">
         <f>(B16-B15)</f>
         <v>0.11111111111111105</v>
@@ -6506,59 +6532,59 @@
       <c r="M17" s="46"/>
     </row>
     <row r="18" spans="1:13" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="99">
+      <c r="A18" s="101">
         <v>44608</v>
       </c>
       <c r="B18" s="23">
         <v>0.49305555555555558</v>
       </c>
-      <c r="C18" s="100" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="100"/>
+      <c r="C18" s="102" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="102"/>
       <c r="E18" s="24"/>
-      <c r="F18" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="G18" s="101"/>
+      <c r="F18" s="103" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" s="103"/>
       <c r="H18" s="25">
         <v>0.49305555555555558</v>
       </c>
-      <c r="I18" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="J18" s="102"/>
+      <c r="I18" s="104" t="s">
+        <v>11</v>
+      </c>
+      <c r="J18" s="104"/>
       <c r="K18" s="47">
         <v>0.49305555555555558</v>
       </c>
-      <c r="L18" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="M18" s="103"/>
+      <c r="L18" s="105" t="s">
+        <v>11</v>
+      </c>
+      <c r="M18" s="105"/>
     </row>
     <row r="19" spans="1:13" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="99"/>
+      <c r="A19" s="101"/>
       <c r="B19" s="27">
         <v>0.52777777777777779</v>
       </c>
-      <c r="C19" s="100"/>
-      <c r="D19" s="100"/>
+      <c r="C19" s="102"/>
+      <c r="D19" s="102"/>
       <c r="E19" s="28"/>
-      <c r="F19" s="101"/>
-      <c r="G19" s="101"/>
+      <c r="F19" s="103"/>
+      <c r="G19" s="103"/>
       <c r="H19" s="29">
         <v>0.52777777777777779</v>
       </c>
-      <c r="I19" s="102"/>
-      <c r="J19" s="102"/>
+      <c r="I19" s="104"/>
+      <c r="J19" s="104"/>
       <c r="K19" s="30">
         <v>0.52777777777777779</v>
       </c>
-      <c r="L19" s="103"/>
-      <c r="M19" s="103"/>
+      <c r="L19" s="105"/>
+      <c r="M19" s="105"/>
     </row>
     <row r="20" spans="1:13" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="99"/>
+      <c r="A20" s="101"/>
       <c r="B20" s="31">
         <f>(B19-B18)</f>
         <v>3.472222222222221E-2</v>
@@ -6585,51 +6611,51 @@
       <c r="M20" s="46"/>
     </row>
     <row r="21" spans="1:13" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="99">
+      <c r="A21" s="101">
         <v>44613</v>
       </c>
       <c r="B21" s="23">
         <v>0.66666666666666663</v>
       </c>
-      <c r="C21" s="100" t="s">
+      <c r="C21" s="102" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="100"/>
+      <c r="D21" s="102"/>
       <c r="E21" s="24"/>
-      <c r="F21" s="101" t="s">
+      <c r="F21" s="103" t="s">
         <v>39</v>
       </c>
-      <c r="G21" s="101"/>
+      <c r="G21" s="103"/>
       <c r="H21" s="25"/>
-      <c r="I21" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="J21" s="102"/>
+      <c r="I21" s="104" t="s">
+        <v>11</v>
+      </c>
+      <c r="J21" s="104"/>
       <c r="K21" s="26"/>
-      <c r="L21" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="M21" s="103"/>
+      <c r="L21" s="105" t="s">
+        <v>11</v>
+      </c>
+      <c r="M21" s="105"/>
     </row>
     <row r="22" spans="1:13" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="99"/>
+      <c r="A22" s="101"/>
       <c r="B22" s="27">
         <v>0.90277777777777779</v>
       </c>
-      <c r="C22" s="100"/>
-      <c r="D22" s="100"/>
+      <c r="C22" s="102"/>
+      <c r="D22" s="102"/>
       <c r="E22" s="28"/>
-      <c r="F22" s="101"/>
-      <c r="G22" s="101"/>
+      <c r="F22" s="103"/>
+      <c r="G22" s="103"/>
       <c r="H22" s="29"/>
-      <c r="I22" s="102"/>
-      <c r="J22" s="102"/>
+      <c r="I22" s="104"/>
+      <c r="J22" s="104"/>
       <c r="K22" s="48"/>
-      <c r="L22" s="103"/>
-      <c r="M22" s="103"/>
+      <c r="L22" s="105"/>
+      <c r="M22" s="105"/>
     </row>
     <row r="23" spans="1:13" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="99"/>
+      <c r="A23" s="101"/>
       <c r="B23" s="31">
         <f>(B22-B21)</f>
         <v>0.23611111111111116</v>
@@ -6656,55 +6682,55 @@
       <c r="M23" s="98"/>
     </row>
     <row r="24" spans="1:13" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="99">
+      <c r="A24" s="101">
         <v>44617</v>
       </c>
       <c r="B24" s="23">
         <v>0.58333333333333337</v>
       </c>
-      <c r="C24" s="100" t="s">
+      <c r="C24" s="102" t="s">
         <v>41</v>
       </c>
-      <c r="D24" s="100"/>
+      <c r="D24" s="102"/>
       <c r="E24" s="24"/>
-      <c r="F24" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="G24" s="101"/>
+      <c r="F24" s="103" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" s="103"/>
       <c r="H24" s="25"/>
-      <c r="I24" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="J24" s="102"/>
+      <c r="I24" s="104" t="s">
+        <v>11</v>
+      </c>
+      <c r="J24" s="104"/>
       <c r="K24" s="26">
         <v>0.54166666666666663</v>
       </c>
-      <c r="L24" s="103" t="s">
+      <c r="L24" s="105" t="s">
         <v>42</v>
       </c>
-      <c r="M24" s="103"/>
+      <c r="M24" s="105"/>
     </row>
     <row r="25" spans="1:13" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="99"/>
+      <c r="A25" s="101"/>
       <c r="B25" s="27">
         <v>0.63888888888888895</v>
       </c>
-      <c r="C25" s="100"/>
-      <c r="D25" s="100"/>
+      <c r="C25" s="102"/>
+      <c r="D25" s="102"/>
       <c r="E25" s="28"/>
-      <c r="F25" s="101"/>
-      <c r="G25" s="101"/>
+      <c r="F25" s="103"/>
+      <c r="G25" s="103"/>
       <c r="H25" s="29"/>
-      <c r="I25" s="102"/>
-      <c r="J25" s="102"/>
+      <c r="I25" s="104"/>
+      <c r="J25" s="104"/>
       <c r="K25" s="30">
         <v>0.66666666666666663</v>
       </c>
-      <c r="L25" s="103"/>
-      <c r="M25" s="103"/>
+      <c r="L25" s="105"/>
+      <c r="M25" s="105"/>
     </row>
     <row r="26" spans="1:13" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="99"/>
+      <c r="A26" s="101"/>
       <c r="B26" s="31">
         <f>(B25-B24)</f>
         <v>5.555555555555558E-2</v>
@@ -6731,51 +6757,51 @@
       <c r="M26" s="46"/>
     </row>
     <row r="27" spans="1:13" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="99">
+      <c r="A27" s="101">
         <v>44618</v>
       </c>
       <c r="B27" s="23"/>
-      <c r="C27" s="100" t="s">
-        <v>11</v>
-      </c>
-      <c r="D27" s="100"/>
+      <c r="C27" s="102" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="102"/>
       <c r="E27" s="24"/>
-      <c r="F27" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="G27" s="101"/>
+      <c r="F27" s="103" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" s="103"/>
       <c r="H27" s="25"/>
-      <c r="I27" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="J27" s="102"/>
+      <c r="I27" s="104" t="s">
+        <v>11</v>
+      </c>
+      <c r="J27" s="104"/>
       <c r="K27" s="47">
         <v>0.66666666666666663</v>
       </c>
-      <c r="L27" s="103" t="s">
+      <c r="L27" s="105" t="s">
         <v>43</v>
       </c>
-      <c r="M27" s="103"/>
+      <c r="M27" s="105"/>
     </row>
     <row r="28" spans="1:13" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="99"/>
+      <c r="A28" s="101"/>
       <c r="B28" s="27"/>
-      <c r="C28" s="100"/>
-      <c r="D28" s="100"/>
+      <c r="C28" s="102"/>
+      <c r="D28" s="102"/>
       <c r="E28" s="28"/>
-      <c r="F28" s="101"/>
-      <c r="G28" s="101"/>
+      <c r="F28" s="103"/>
+      <c r="G28" s="103"/>
       <c r="H28" s="29"/>
-      <c r="I28" s="102"/>
-      <c r="J28" s="102"/>
+      <c r="I28" s="104"/>
+      <c r="J28" s="104"/>
       <c r="K28" s="30">
         <v>0.79166666666666663</v>
       </c>
-      <c r="L28" s="103"/>
-      <c r="M28" s="103"/>
+      <c r="L28" s="105"/>
+      <c r="M28" s="105"/>
     </row>
     <row r="29" spans="1:13" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="99"/>
+      <c r="A29" s="101"/>
       <c r="B29" s="31">
         <f>(B28-B27)</f>
         <v>0</v>
@@ -6802,51 +6828,51 @@
       <c r="M29" s="46"/>
     </row>
     <row r="30" spans="1:13" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="99">
+      <c r="A30" s="101">
         <v>44619</v>
       </c>
       <c r="B30" s="23"/>
-      <c r="C30" s="100" t="s">
-        <v>11</v>
-      </c>
-      <c r="D30" s="100"/>
+      <c r="C30" s="102" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" s="102"/>
       <c r="E30" s="24"/>
-      <c r="F30" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="G30" s="101"/>
+      <c r="F30" s="103" t="s">
+        <v>11</v>
+      </c>
+      <c r="G30" s="103"/>
       <c r="H30" s="25"/>
-      <c r="I30" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="J30" s="102"/>
+      <c r="I30" s="104" t="s">
+        <v>11</v>
+      </c>
+      <c r="J30" s="104"/>
       <c r="K30" s="26">
         <v>0.33333333333333331</v>
       </c>
-      <c r="L30" s="103" t="s">
+      <c r="L30" s="105" t="s">
         <v>43</v>
       </c>
-      <c r="M30" s="103"/>
+      <c r="M30" s="105"/>
     </row>
     <row r="31" spans="1:13" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="99"/>
+      <c r="A31" s="101"/>
       <c r="B31" s="27"/>
-      <c r="C31" s="100"/>
-      <c r="D31" s="100"/>
+      <c r="C31" s="102"/>
+      <c r="D31" s="102"/>
       <c r="E31" s="28"/>
-      <c r="F31" s="101"/>
-      <c r="G31" s="101"/>
+      <c r="F31" s="103"/>
+      <c r="G31" s="103"/>
       <c r="H31" s="29"/>
-      <c r="I31" s="102"/>
-      <c r="J31" s="102"/>
+      <c r="I31" s="104"/>
+      <c r="J31" s="104"/>
       <c r="K31" s="48">
         <v>0.5</v>
       </c>
-      <c r="L31" s="103"/>
-      <c r="M31" s="103"/>
+      <c r="L31" s="105"/>
+      <c r="M31" s="105"/>
     </row>
     <row r="32" spans="1:13" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="99"/>
+      <c r="A32" s="101"/>
       <c r="B32" s="31">
         <f>(B31-B30)</f>
         <v>0</v>
@@ -6873,51 +6899,51 @@
       <c r="M32" s="98"/>
     </row>
     <row r="33" spans="1:13" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="99">
+      <c r="A33" s="101">
         <v>44620</v>
       </c>
       <c r="B33" s="23">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C33" s="100" t="s">
+      <c r="C33" s="102" t="s">
         <v>44</v>
       </c>
-      <c r="D33" s="100"/>
+      <c r="D33" s="102"/>
       <c r="E33" s="24"/>
-      <c r="F33" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="G33" s="101"/>
+      <c r="F33" s="103" t="s">
+        <v>11</v>
+      </c>
+      <c r="G33" s="103"/>
       <c r="H33" s="25"/>
-      <c r="I33" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="J33" s="102"/>
+      <c r="I33" s="104" t="s">
+        <v>11</v>
+      </c>
+      <c r="J33" s="104"/>
       <c r="K33" s="26"/>
-      <c r="L33" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="M33" s="103"/>
+      <c r="L33" s="105" t="s">
+        <v>11</v>
+      </c>
+      <c r="M33" s="105"/>
     </row>
     <row r="34" spans="1:13" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="99"/>
+      <c r="A34" s="101"/>
       <c r="B34" s="27">
         <v>0.625</v>
       </c>
-      <c r="C34" s="100"/>
-      <c r="D34" s="100"/>
+      <c r="C34" s="102"/>
+      <c r="D34" s="102"/>
       <c r="E34" s="28"/>
-      <c r="F34" s="101"/>
-      <c r="G34" s="101"/>
+      <c r="F34" s="103"/>
+      <c r="G34" s="103"/>
       <c r="H34" s="29"/>
-      <c r="I34" s="102"/>
-      <c r="J34" s="102"/>
+      <c r="I34" s="104"/>
+      <c r="J34" s="104"/>
       <c r="K34" s="30"/>
-      <c r="L34" s="103"/>
-      <c r="M34" s="103"/>
+      <c r="L34" s="105"/>
+      <c r="M34" s="105"/>
     </row>
     <row r="35" spans="1:13" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="99"/>
+      <c r="A35" s="101"/>
       <c r="B35" s="31">
         <f>(B34-B33)</f>
         <v>0.20833333333333331</v>
@@ -6944,51 +6970,51 @@
       <c r="M35" s="46"/>
     </row>
     <row r="36" spans="1:13" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="99">
+      <c r="A36" s="101">
         <v>44624</v>
       </c>
       <c r="B36" s="23">
         <v>0.70833333333333337</v>
       </c>
-      <c r="C36" s="100" t="s">
+      <c r="C36" s="102" t="s">
         <v>45</v>
       </c>
-      <c r="D36" s="100"/>
+      <c r="D36" s="102"/>
       <c r="E36" s="24"/>
-      <c r="F36" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="G36" s="101"/>
+      <c r="F36" s="103" t="s">
+        <v>11</v>
+      </c>
+      <c r="G36" s="103"/>
       <c r="H36" s="25"/>
-      <c r="I36" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="J36" s="102"/>
+      <c r="I36" s="104" t="s">
+        <v>11</v>
+      </c>
+      <c r="J36" s="104"/>
       <c r="K36" s="47"/>
-      <c r="L36" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="M36" s="103"/>
+      <c r="L36" s="105" t="s">
+        <v>11</v>
+      </c>
+      <c r="M36" s="105"/>
     </row>
     <row r="37" spans="1:13" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="99"/>
+      <c r="A37" s="101"/>
       <c r="B37" s="27">
         <v>0.91666666666666663</v>
       </c>
-      <c r="C37" s="100"/>
-      <c r="D37" s="100"/>
+      <c r="C37" s="102"/>
+      <c r="D37" s="102"/>
       <c r="E37" s="28"/>
-      <c r="F37" s="101"/>
-      <c r="G37" s="101"/>
+      <c r="F37" s="103"/>
+      <c r="G37" s="103"/>
       <c r="H37" s="29"/>
-      <c r="I37" s="102"/>
-      <c r="J37" s="102"/>
+      <c r="I37" s="104"/>
+      <c r="J37" s="104"/>
       <c r="K37" s="30"/>
-      <c r="L37" s="103"/>
-      <c r="M37" s="103"/>
+      <c r="L37" s="105"/>
+      <c r="M37" s="105"/>
     </row>
     <row r="38" spans="1:13" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="99"/>
+      <c r="A38" s="101"/>
       <c r="B38" s="31">
         <f>(B37-B36)</f>
         <v>0.20833333333333326</v>
@@ -7015,48 +7041,54 @@
       <c r="M38" s="46"/>
     </row>
     <row r="39" spans="1:13" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="99"/>
-      <c r="B39" s="23"/>
-      <c r="C39" s="100" t="s">
-        <v>11</v>
-      </c>
-      <c r="D39" s="100"/>
+      <c r="A39" s="101">
+        <v>44626</v>
+      </c>
+      <c r="B39" s="23">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C39" s="102" t="s">
+        <v>46</v>
+      </c>
+      <c r="D39" s="102"/>
       <c r="E39" s="24"/>
-      <c r="F39" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="G39" s="101"/>
+      <c r="F39" s="103" t="s">
+        <v>11</v>
+      </c>
+      <c r="G39" s="103"/>
       <c r="H39" s="25"/>
-      <c r="I39" s="102" t="s">
-        <v>11</v>
-      </c>
-      <c r="J39" s="102"/>
+      <c r="I39" s="104" t="s">
+        <v>11</v>
+      </c>
+      <c r="J39" s="104"/>
       <c r="K39" s="26"/>
-      <c r="L39" s="103" t="s">
-        <v>11</v>
-      </c>
-      <c r="M39" s="103"/>
+      <c r="L39" s="105" t="s">
+        <v>11</v>
+      </c>
+      <c r="M39" s="105"/>
     </row>
     <row r="40" spans="1:13" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="99"/>
-      <c r="B40" s="27"/>
-      <c r="C40" s="100"/>
-      <c r="D40" s="100"/>
+      <c r="A40" s="101"/>
+      <c r="B40" s="27">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="C40" s="102"/>
+      <c r="D40" s="102"/>
       <c r="E40" s="28"/>
-      <c r="F40" s="101"/>
-      <c r="G40" s="101"/>
+      <c r="F40" s="103"/>
+      <c r="G40" s="103"/>
       <c r="H40" s="29"/>
-      <c r="I40" s="102"/>
-      <c r="J40" s="102"/>
+      <c r="I40" s="104"/>
+      <c r="J40" s="104"/>
       <c r="K40" s="48"/>
-      <c r="L40" s="103"/>
-      <c r="M40" s="103"/>
+      <c r="L40" s="105"/>
+      <c r="M40" s="105"/>
     </row>
     <row r="41" spans="1:13" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="99"/>
+      <c r="A41" s="101"/>
       <c r="B41" s="31">
         <f>(B40-B39)</f>
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
       <c r="C41" s="32"/>
       <c r="D41" s="33"/>
@@ -7081,66 +7113,6 @@
     </row>
   </sheetData>
   <mergeCells count="67">
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="C36:D37"/>
-    <mergeCell ref="F36:G37"/>
-    <mergeCell ref="I36:J37"/>
-    <mergeCell ref="L36:M37"/>
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="C39:D40"/>
-    <mergeCell ref="F39:G40"/>
-    <mergeCell ref="I39:J40"/>
-    <mergeCell ref="L39:M40"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="C30:D31"/>
-    <mergeCell ref="F30:G31"/>
-    <mergeCell ref="I30:J31"/>
-    <mergeCell ref="L30:M31"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="C33:D34"/>
-    <mergeCell ref="F33:G34"/>
-    <mergeCell ref="I33:J34"/>
-    <mergeCell ref="L33:M34"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="C24:D25"/>
-    <mergeCell ref="F24:G25"/>
-    <mergeCell ref="I24:J25"/>
-    <mergeCell ref="L24:M25"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="C27:D28"/>
-    <mergeCell ref="F27:G28"/>
-    <mergeCell ref="I27:J28"/>
-    <mergeCell ref="L27:M28"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="C18:D19"/>
-    <mergeCell ref="F18:G19"/>
-    <mergeCell ref="I18:J19"/>
-    <mergeCell ref="L18:M19"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="C21:D22"/>
-    <mergeCell ref="F21:G22"/>
-    <mergeCell ref="I21:J22"/>
-    <mergeCell ref="L21:M22"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="C12:D13"/>
-    <mergeCell ref="F12:G13"/>
-    <mergeCell ref="I12:J13"/>
-    <mergeCell ref="L12:M13"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="C15:D16"/>
-    <mergeCell ref="F15:G16"/>
-    <mergeCell ref="I15:J16"/>
-    <mergeCell ref="L15:M16"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="C6:D7"/>
-    <mergeCell ref="F6:G7"/>
-    <mergeCell ref="I6:J7"/>
-    <mergeCell ref="L6:M7"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="C9:D10"/>
-    <mergeCell ref="F9:G10"/>
-    <mergeCell ref="I9:J10"/>
-    <mergeCell ref="L9:M10"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="A3:A5"/>
@@ -7148,6 +7120,66 @@
     <mergeCell ref="F3:G4"/>
     <mergeCell ref="I3:J4"/>
     <mergeCell ref="L3:M4"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="C9:D10"/>
+    <mergeCell ref="F9:G10"/>
+    <mergeCell ref="I9:J10"/>
+    <mergeCell ref="L9:M10"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="C6:D7"/>
+    <mergeCell ref="F6:G7"/>
+    <mergeCell ref="I6:J7"/>
+    <mergeCell ref="L6:M7"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="C15:D16"/>
+    <mergeCell ref="F15:G16"/>
+    <mergeCell ref="I15:J16"/>
+    <mergeCell ref="L15:M16"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="C12:D13"/>
+    <mergeCell ref="F12:G13"/>
+    <mergeCell ref="I12:J13"/>
+    <mergeCell ref="L12:M13"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="C21:D22"/>
+    <mergeCell ref="F21:G22"/>
+    <mergeCell ref="I21:J22"/>
+    <mergeCell ref="L21:M22"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="C18:D19"/>
+    <mergeCell ref="F18:G19"/>
+    <mergeCell ref="I18:J19"/>
+    <mergeCell ref="L18:M19"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="C27:D28"/>
+    <mergeCell ref="F27:G28"/>
+    <mergeCell ref="I27:J28"/>
+    <mergeCell ref="L27:M28"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="C24:D25"/>
+    <mergeCell ref="F24:G25"/>
+    <mergeCell ref="I24:J25"/>
+    <mergeCell ref="L24:M25"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="C33:D34"/>
+    <mergeCell ref="F33:G34"/>
+    <mergeCell ref="I33:J34"/>
+    <mergeCell ref="L33:M34"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="C30:D31"/>
+    <mergeCell ref="F30:G31"/>
+    <mergeCell ref="I30:J31"/>
+    <mergeCell ref="L30:M31"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="C39:D40"/>
+    <mergeCell ref="F39:G40"/>
+    <mergeCell ref="I39:J40"/>
+    <mergeCell ref="L39:M40"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="C36:D37"/>
+    <mergeCell ref="F36:G37"/>
+    <mergeCell ref="I36:J37"/>
+    <mergeCell ref="L36:M37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>